<commit_message>
Auto bold the column headers
</commit_message>
<xml_diff>
--- a/books_spreadsheet_out.xlsx
+++ b/books_spreadsheet_out.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\p\gls01_workspace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1547501D-1129-4E72-A9D8-8295D1A5A4AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F010CA82-7001-42E7-8DA7-41113A47230F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
     <t>original_language</t>
   </si>
   <si>
-    <t>book_title_flavor_for_translation</t>
+    <t>book_title_flavor</t>
   </si>
   <si>
     <t>translator_full_name</t>
@@ -171,17 +171,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -197,10 +189,8 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -223,11 +213,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,162 +534,159 @@
   <dimension ref="A1:AV1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="135.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" style="2" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="63.5703125" style="2" customWidth="1"/>
-    <col min="7" max="12" width="9.140625" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="64.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="35" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Y1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="Z1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AA1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AB1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AC1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AD1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AE1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AF1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AG1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AH1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AI1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AK1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AL1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AM1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AN1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AO1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AP1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="AR1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="3" t="s">
+      <c r="AS1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="3" t="s">
+      <c r="AT1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="3" t="s">
+      <c r="AU1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="3" t="s">
+      <c r="AV1" s="2" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refactoring works to book_title_set
</commit_message>
<xml_diff>
--- a/books_spreadsheet_out.xlsx
+++ b/books_spreadsheet_out.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -39,11 +39,20 @@
       <sz val="9"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="9"/>
+    </font>
+    <font>
       <b val="1"/>
       <sz val="9"/>
     </font>
     <font>
       <name val="Segoe UI Historic"/>
+      <sz val="9"/>
+    </font>
+    <font>
+      <name val="Tengwar Annatar"/>
       <sz val="9"/>
     </font>
   </fonts>
@@ -67,7 +76,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -77,12 +86,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -91,6 +94,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,10 +467,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AX5"/>
+  <dimension ref="A1:AX18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15.75" outlineLevelCol="0"/>
@@ -490,252 +501,252 @@
     <col width="32" customWidth="1" style="3" min="24" max="24"/>
     <col width="16.7109375" customWidth="1" style="3" min="25" max="25"/>
     <col width="34.42578125" customWidth="1" style="1" min="26" max="26"/>
-    <col width="9.140625" customWidth="1" style="1" min="27" max="41"/>
-    <col width="9.140625" customWidth="1" style="1" min="42" max="16384"/>
+    <col width="9.140625" customWidth="1" style="1" min="27" max="42"/>
+    <col width="9.140625" customWidth="1" style="1" min="43" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="inlineStr">
+      <c r="A1" s="8" t="inlineStr">
         <is>
           <t>format</t>
         </is>
       </c>
-      <c r="B1" s="7" t="inlineStr">
+      <c r="B1" s="8" t="inlineStr">
         <is>
           <t>materials</t>
         </is>
       </c>
-      <c r="C1" s="8" t="inlineStr">
+      <c r="C1" s="9" t="inlineStr">
         <is>
           <t>number_volumes</t>
         </is>
       </c>
-      <c r="D1" s="8" t="inlineStr">
+      <c r="D1" s="9" t="inlineStr">
         <is>
           <t>number_pages</t>
         </is>
       </c>
-      <c r="E1" s="8" t="inlineStr">
+      <c r="E1" s="9" t="inlineStr">
         <is>
           <t>weight</t>
         </is>
       </c>
-      <c r="F1" s="7" t="inlineStr">
+      <c r="F1" s="8" t="inlineStr">
         <is>
           <t>current_language</t>
         </is>
       </c>
-      <c r="G1" s="7" t="inlineStr">
+      <c r="G1" s="8" t="inlineStr">
         <is>
           <t>original_language</t>
         </is>
       </c>
-      <c r="H1" s="8" t="inlineStr">
+      <c r="H1" s="9" t="inlineStr">
         <is>
           <t>topic</t>
         </is>
       </c>
-      <c r="I1" s="8" t="inlineStr">
+      <c r="I1" s="9" t="inlineStr">
         <is>
           <t>topic_apparent</t>
         </is>
       </c>
-      <c r="J1" s="8" t="inlineStr">
+      <c r="J1" s="9" t="inlineStr">
         <is>
           <t>scope</t>
         </is>
       </c>
-      <c r="K1" s="8" t="inlineStr">
+      <c r="K1" s="9" t="inlineStr">
         <is>
           <t>scope_esoteric</t>
         </is>
       </c>
-      <c r="L1" s="8" t="inlineStr">
+      <c r="L1" s="9" t="inlineStr">
         <is>
           <t>complexity</t>
         </is>
       </c>
-      <c r="M1" s="7" t="inlineStr">
+      <c r="M1" s="8" t="inlineStr">
         <is>
           <t>complexity_esoteric</t>
         </is>
       </c>
-      <c r="N1" s="7" t="inlineStr">
+      <c r="N1" s="8" t="inlineStr">
         <is>
           <t>fraction_complete</t>
         </is>
       </c>
-      <c r="O1" s="7" t="inlineStr">
+      <c r="O1" s="8" t="inlineStr">
         <is>
           <t>market_value</t>
         </is>
       </c>
-      <c r="P1" s="7" t="inlineStr">
+      <c r="P1" s="8" t="inlineStr">
         <is>
           <t>book_title</t>
         </is>
       </c>
-      <c r="Q1" s="7" t="inlineStr">
+      <c r="Q1" s="8" t="inlineStr">
         <is>
           <t>author_full</t>
         </is>
       </c>
-      <c r="R1" s="7" t="inlineStr">
+      <c r="R1" s="8" t="inlineStr">
         <is>
           <t>translator_full_name</t>
         </is>
       </c>
-      <c r="S1" s="8" t="inlineStr">
+      <c r="S1" s="9" t="inlineStr">
         <is>
           <t>book_title_flavor</t>
         </is>
       </c>
-      <c r="T1" s="8" t="inlineStr">
+      <c r="T1" s="9" t="inlineStr">
         <is>
           <t>reading_time</t>
         </is>
       </c>
-      <c r="U1" s="8" t="inlineStr">
+      <c r="U1" s="9" t="inlineStr">
         <is>
           <t>reference_time</t>
         </is>
       </c>
-      <c r="V1" s="8" t="inlineStr">
+      <c r="V1" s="9" t="inlineStr">
         <is>
           <t>age_at_discovery</t>
         </is>
       </c>
-      <c r="W1" s="8" t="inlineStr">
+      <c r="W1" s="9" t="inlineStr">
         <is>
           <t>number_extant_copies</t>
         </is>
       </c>
-      <c r="X1" s="9" t="inlineStr">
+      <c r="X1" s="10" t="inlineStr">
         <is>
           <t>number_extant_available_to_place</t>
         </is>
       </c>
-      <c r="Y1" s="9" t="inlineStr">
+      <c r="Y1" s="10" t="inlineStr">
         <is>
           <t>rarity_modifier</t>
         </is>
       </c>
-      <c r="Z1" s="7" t="inlineStr">
+      <c r="Z1" s="8" t="inlineStr">
         <is>
           <t>libraries_it_is_in</t>
         </is>
       </c>
-      <c r="AA1" s="7" t="inlineStr">
+      <c r="AA1" s="8" t="inlineStr">
         <is>
           <t>author_epithet</t>
         </is>
       </c>
-      <c r="AB1" s="7" t="inlineStr">
+      <c r="AB1" s="8" t="inlineStr">
         <is>
           <t>author_name</t>
         </is>
       </c>
-      <c r="AC1" s="7" t="inlineStr">
+      <c r="AC1" s="8" t="inlineStr">
         <is>
           <t>author_nationality</t>
         </is>
       </c>
-      <c r="AD1" s="7" t="inlineStr">
+      <c r="AD1" s="8" t="inlineStr">
         <is>
           <t>author_title</t>
         </is>
       </c>
-      <c r="AE1" s="7" t="inlineStr">
+      <c r="AE1" s="8" t="inlineStr">
         <is>
           <t>author_sex</t>
         </is>
       </c>
-      <c r="AF1" s="7" t="inlineStr">
+      <c r="AF1" s="8" t="inlineStr">
         <is>
           <t>translator_name</t>
         </is>
       </c>
-      <c r="AG1" s="7" t="inlineStr">
+      <c r="AG1" s="8" t="inlineStr">
         <is>
           <t>translator_nationality</t>
         </is>
       </c>
-      <c r="AH1" s="7" t="inlineStr">
+      <c r="AH1" s="8" t="inlineStr">
         <is>
           <t>translator_sex</t>
         </is>
       </c>
-      <c r="AI1" s="7" t="inlineStr">
+      <c r="AI1" s="8" t="inlineStr">
         <is>
           <t>translator_title</t>
         </is>
       </c>
-      <c r="AJ1" s="7" t="inlineStr">
+      <c r="AJ1" s="8" t="inlineStr">
         <is>
           <t>weight_per_page</t>
         </is>
       </c>
-      <c r="AK1" s="7" t="inlineStr">
+      <c r="AK1" s="8" t="inlineStr">
         <is>
           <t>template</t>
         </is>
       </c>
-      <c r="AL1" s="7" t="inlineStr">
+      <c r="AL1" s="8" t="inlineStr">
         <is>
           <t>topic_title_form</t>
         </is>
       </c>
-      <c r="AM1" s="7" t="inlineStr">
+      <c r="AM1" s="8" t="inlineStr">
         <is>
           <t>cost_per_page</t>
         </is>
       </c>
-      <c r="AN1" s="7" t="inlineStr">
+      <c r="AN1" s="8" t="inlineStr">
         <is>
           <t>production_value</t>
         </is>
       </c>
-      <c r="AO1" s="7" t="inlineStr">
+      <c r="AO1" s="8" t="inlineStr">
         <is>
           <t>literary_value_base</t>
         </is>
       </c>
-      <c r="AP1" s="7" t="inlineStr">
+      <c r="AP1" s="8" t="inlineStr">
         <is>
           <t>literary_value_modified</t>
         </is>
       </c>
-      <c r="AQ1" s="7" t="inlineStr">
+      <c r="AQ1" s="8" t="inlineStr">
         <is>
           <t>esoteric_literary_value_base</t>
         </is>
       </c>
-      <c r="AR1" s="7" t="inlineStr">
+      <c r="AR1" s="8" t="inlineStr">
         <is>
           <t>esoteric_literary_value_modified</t>
         </is>
       </c>
-      <c r="AS1" s="7" t="inlineStr">
+      <c r="AS1" s="8" t="inlineStr">
         <is>
           <t>year_discovered</t>
         </is>
       </c>
-      <c r="AT1" s="7" t="inlineStr">
+      <c r="AT1" s="8" t="inlineStr">
         <is>
           <t>year_written</t>
         </is>
       </c>
-      <c r="AU1" s="7" t="inlineStr">
+      <c r="AU1" s="8" t="inlineStr">
         <is>
           <t>is_a_translation</t>
         </is>
       </c>
-      <c r="AV1" s="7" t="inlineStr">
+      <c r="AV1" s="8" t="inlineStr">
         <is>
           <t>book_type</t>
         </is>
       </c>
-      <c r="AW1" s="7" t="inlineStr">
+      <c r="AW1" s="8" t="inlineStr">
         <is>
           <t>final_title</t>
         </is>
@@ -761,33 +772,28 @@
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>333</v>
+        <v>666</v>
       </c>
       <c r="E2" t="n">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Classical</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Elvish</t>
+          <t>Regional</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Craft (brewing)</t>
+          <t>Loremastery</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Craft (brewing)</t>
+          <t>Loremastery</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
@@ -802,64 +808,64 @@
         <v>1</v>
       </c>
       <c r="O2" t="n">
-        <v>457</v>
+        <v>1579</v>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>Brewing, a Eclipsed Calculation</t>
+          <t>The Many Anger of The Chief Sinner and Loremastery</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Dr. Gregory Smith the Slim</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>Bob Dole</t>
-        </is>
-      </c>
-      <c r="S2" s="10" t="inlineStr">
-        <is>
-          <t>Nisl coacturos milium tigurinus veniam</t>
+          <t>Her Holiness Torvi Mortensdotter the Daring</t>
+        </is>
+      </c>
+      <c r="S2" s="11" t="inlineStr">
+        <is>
+          <t>Δ΄ εὐθείᾳ ᾖ κέντρον μίαν αὐτοῦ ἡμικύκλιον ἐστίν] με΄ αὐτὴν ἐκβαλλόμεναι ἐλάττονες σημεῖον</t>
         </is>
       </c>
       <c r="T2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="V2" t="n">
-        <v>94</v>
+        <v>47</v>
       </c>
       <c r="W2" t="n">
-        <v>47</v>
+        <v>2</v>
       </c>
       <c r="X2" t="n">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>the Slim</t>
+          <t>the Daring</t>
         </is>
       </c>
       <c r="AB2" t="inlineStr">
         <is>
-          <t>Gregory Smith</t>
+          <t>Torvi Mortensdotter</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_female</t>
         </is>
       </c>
       <c r="AD2" t="inlineStr">
         <is>
-          <t>Dr.</t>
+          <t>Her Holiness</t>
         </is>
       </c>
       <c r="AE2" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="AJ2" t="n">
@@ -867,25 +873,25 @@
       </c>
       <c r="AK2" t="inlineStr">
         <is>
-          <t>{topic}, a {adjective_1} {noun_1}</t>
+          <t>{the_1} {negative_1} of {person_evil} and {topic}</t>
         </is>
       </c>
       <c r="AL2" t="inlineStr">
         <is>
-          <t>Brewing</t>
+          <t>Loremastery</t>
         </is>
       </c>
       <c r="AM2" t="n">
         <v>0.37</v>
       </c>
       <c r="AN2" t="n">
-        <v>124</v>
+        <v>247</v>
       </c>
       <c r="AO2" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AP2" t="n">
-        <v>333</v>
+        <v>1332</v>
       </c>
       <c r="AQ2" t="n">
         <v>0</v>
@@ -900,7 +906,7 @@
         <v>0</v>
       </c>
       <c r="AU2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV2" t="inlineStr">
         <is>
@@ -916,36 +922,31 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Vellum</t>
+          <t>Parchment</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>500</v>
+        <v>1333</v>
       </c>
       <c r="E3" t="n">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Common</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Ancient</t>
+          <t>Classical</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Skirmishing</t>
+          <t>Knowledge (mathematics)</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Skirmishing</t>
+          <t>Knowledge (mathematics)</t>
         </is>
       </c>
       <c r="J3" t="n">
@@ -955,7 +956,7 @@
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>2</v>
+        <v>0.75</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
@@ -964,64 +965,54 @@
         <v>1</v>
       </c>
       <c r="O3" t="n">
-        <v>1195</v>
+        <v>1827</v>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Skirmishing and the Epochs</t>
+          <t>The Covetousness of Risha Chishti, in which case Discoursing on On the Solving of Equations is Given Particular Attention by Way of Instruction and Warning</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Dr. Gregory Smith the Slim</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>Bob Dole</t>
-        </is>
-      </c>
-      <c r="S3" s="10" t="inlineStr">
-        <is>
-          <t>Skirmishing and the Epochs</t>
+          <t>Fosca Suedia</t>
+        </is>
+      </c>
+      <c r="S3" s="11" t="inlineStr">
+        <is>
+          <t>Deligatam beatae metius opere cibaria incidit audacia ipsi indicium miserat filia educit sublati diurnisque contingant experiantur creatur intulisset iracundum petit accessisset valeat lacessere exploratores peritissimus singulos transisse</t>
         </is>
       </c>
       <c r="T3" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="U3" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="V3" t="n">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="W3" t="n">
-        <v>1</v>
+        <v>343</v>
       </c>
       <c r="X3" t="n">
-        <v>0</v>
+        <v>342</v>
       </c>
       <c r="Y3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA3" t="inlineStr">
-        <is>
-          <t>the Slim</t>
-        </is>
+        <v>0.02</v>
       </c>
       <c r="AB3" t="inlineStr">
         <is>
-          <t>Gregory Smith</t>
-        </is>
-      </c>
-      <c r="AD3" t="inlineStr">
-        <is>
-          <t>Dr.</t>
+          <t>Fosca Suedia</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>_names_roman_surnames</t>
         </is>
       </c>
       <c r="AE3" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="AJ3" t="n">
@@ -1029,25 +1020,25 @@
       </c>
       <c r="AK3" t="inlineStr">
         <is>
-          <t>{topic} and {noun_2}</t>
+          <t>{the_1} {negative_1} of {person_1}, in which case {conjunction_about} {topic} is Given Particular Attention by Way of Instruction and Warning</t>
         </is>
       </c>
       <c r="AL3" t="inlineStr">
         <is>
-          <t>Skirmishing</t>
+          <t>On the Solving of Equations</t>
         </is>
       </c>
       <c r="AM3" t="n">
-        <v>0.39</v>
+        <v>0.37</v>
       </c>
       <c r="AN3" t="n">
-        <v>195</v>
+        <v>494</v>
       </c>
       <c r="AO3" t="n">
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="AP3" t="n">
-        <v>1000</v>
+        <v>1333</v>
       </c>
       <c r="AQ3" t="n">
         <v>0</v>
@@ -1062,7 +1053,7 @@
         <v>0</v>
       </c>
       <c r="AU3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV3" t="inlineStr">
         <is>
@@ -1078,133 +1069,102 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Vellum</t>
+          <t>Parchment</t>
         </is>
       </c>
       <c r="C4" t="n">
         <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>500</v>
+        <v>333</v>
       </c>
       <c r="E4" t="n">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Classical</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Regional</t>
+          <t>Common</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Endurance</t>
+          <t>Esoteric: Judge’s Choice</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Endurance</t>
+          <t>Alertness</t>
         </is>
       </c>
       <c r="J4" t="n">
         <v>1</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N4" t="n">
         <v>1</v>
       </c>
       <c r="O4" t="n">
-        <v>1195</v>
+        <v>2122</v>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Initiating Endurance</t>
+          <t>The Accursed Wrongdoing of Aurèle Bellecourt, Considering Alertness</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Dr. Gregory Smith the Slim</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>The Reverend Bob Dole</t>
-        </is>
-      </c>
-      <c r="S4" s="10" t="inlineStr">
-        <is>
-          <t>Odio sapiente volutpat pons cultum biennium militum pila</t>
+          <t>His Holiness Aldric Magnan</t>
+        </is>
+      </c>
+      <c r="S4" s="11" t="inlineStr">
+        <is>
+          <t>The Accursed Wrongdoing of Aurèle Bellecourt, Considering Alertness</t>
         </is>
       </c>
       <c r="T4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V4" t="n">
-        <v>169</v>
+        <v>14</v>
       </c>
       <c r="W4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="X4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Y4" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z4" t="inlineStr"/>
-      <c r="AA4" t="inlineStr">
-        <is>
-          <t>the Slim</t>
-        </is>
+        <v>0.5</v>
       </c>
       <c r="AB4" t="inlineStr">
         <is>
-          <t>Gregory Smith</t>
+          <t>Aldric Magnan</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
         </is>
       </c>
       <c r="AD4" t="inlineStr">
         <is>
-          <t>Dr.</t>
+          <t>His Holiness</t>
         </is>
       </c>
       <c r="AE4" t="inlineStr">
         <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="AF4" t="inlineStr">
-        <is>
-          <t>Bob Dole</t>
-        </is>
-      </c>
-      <c r="AG4" t="inlineStr">
-        <is>
-          <t>Greek</t>
-        </is>
-      </c>
-      <c r="AH4" t="inlineStr">
-        <is>
           <t>Male</t>
-        </is>
-      </c>
-      <c r="AI4" t="inlineStr">
-        <is>
-          <t>The Reverend</t>
         </is>
       </c>
       <c r="AJ4" t="n">
@@ -1212,31 +1172,31 @@
       </c>
       <c r="AK4" t="inlineStr">
         <is>
-          <t>{verbing} {topic}</t>
+          <t>{the_1} {negative_1} of {person_1}, Considering {topic}</t>
         </is>
       </c>
       <c r="AL4" t="inlineStr">
         <is>
-          <t>Endurance</t>
+          <t>Alertness</t>
         </is>
       </c>
       <c r="AM4" t="n">
-        <v>0.39</v>
+        <v>0.37</v>
       </c>
       <c r="AN4" t="n">
-        <v>195</v>
+        <v>124</v>
       </c>
       <c r="AO4" t="n">
-        <v>1.25</v>
+        <v>2</v>
       </c>
       <c r="AP4" t="n">
-        <v>1000</v>
+        <v>333</v>
       </c>
       <c r="AQ4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR4" t="n">
-        <v>0</v>
+        <v>1665</v>
       </c>
       <c r="AS4" t="n">
         <v>0</v>
@@ -1245,53 +1205,47 @@
         <v>0</v>
       </c>
       <c r="AU4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV4" t="inlineStr">
         <is>
           <t>Standard</t>
         </is>
       </c>
-      <c r="AW4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Scroll</t>
+          <t>Codex</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Ordinary Papyrus</t>
+          <t>Parchment</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D5" t="n">
         <v>1000</v>
       </c>
       <c r="E5" t="n">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
           <t>Classical</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Regional</t>
-        </is>
-      </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Alchemy</t>
+          <t>Navigation</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Alchemy</t>
+          <t>Navigation</t>
         </is>
       </c>
       <c r="J5" t="n">
@@ -1310,26 +1264,21 @@
         <v>1</v>
       </c>
       <c r="O5" t="n">
-        <v>1310</v>
+        <v>1370</v>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>The Masked Orbit of Foreboding: Transmutation of the Elements</t>
+          <t>A Meditation on Navigation</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Dr. Gregory Smith the Slim</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>The Reverend Bob Dole</t>
-        </is>
-      </c>
-      <c r="S5" s="10" t="inlineStr">
-        <is>
-          <t>Fratri deperdere quibuscum concedere consederant ornamento mortem hostium deorum naviculam soluta esset nullis</t>
+          <t>Biyn Karlsson</t>
+        </is>
+      </c>
+      <c r="S5" s="11" t="inlineStr">
+        <is>
+          <t>Sollicitudin centum fiebat</t>
         </is>
       </c>
       <c r="T5" t="n">
@@ -1339,56 +1288,30 @@
         <v>5</v>
       </c>
       <c r="V5" t="n">
-        <v>478</v>
+        <v>22</v>
       </c>
       <c r="W5" t="n">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="X5" t="n">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="Z5" t="inlineStr"/>
-      <c r="AA5" t="inlineStr">
-        <is>
-          <t>the Slim</t>
-        </is>
+        <v>0.1</v>
       </c>
       <c r="AB5" t="inlineStr">
         <is>
-          <t>Gregory Smith</t>
-        </is>
-      </c>
-      <c r="AD5" t="inlineStr">
-        <is>
-          <t>Dr.</t>
+          <t>Biyn Karlsson</t>
+        </is>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_male</t>
         </is>
       </c>
       <c r="AE5" t="inlineStr">
         <is>
           <t>Male</t>
-        </is>
-      </c>
-      <c r="AF5" t="inlineStr">
-        <is>
-          <t>Bob Dole</t>
-        </is>
-      </c>
-      <c r="AG5" t="inlineStr">
-        <is>
-          <t>Greek</t>
-        </is>
-      </c>
-      <c r="AH5" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="AI5" t="inlineStr">
-        <is>
-          <t>The Reverend</t>
         </is>
       </c>
       <c r="AJ5" t="n">
@@ -1396,19 +1319,19 @@
       </c>
       <c r="AK5" t="inlineStr">
         <is>
-          <t>The {adjective_1} {noun_1} of {noun_2}: {topic}</t>
+          <t>{study_on} on {topic}</t>
         </is>
       </c>
       <c r="AL5" t="inlineStr">
         <is>
-          <t>Transmutation of the Elements</t>
+          <t>Navigation</t>
         </is>
       </c>
       <c r="AM5" t="n">
-        <v>0.31</v>
+        <v>0.37</v>
       </c>
       <c r="AN5" t="n">
-        <v>310</v>
+        <v>370</v>
       </c>
       <c r="AO5" t="n">
         <v>2</v>
@@ -1429,14 +1352,2072 @@
         <v>0</v>
       </c>
       <c r="AU5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV5" t="inlineStr">
         <is>
           <t>Standard</t>
         </is>
       </c>
-      <c r="AW5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>3</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E6" t="n">
+        <v>124</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Classical</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Craft (blacksmithing)</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Craft (blacksmithing)</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
+        <v>2</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>1</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>1</v>
+      </c>
+      <c r="O6" t="n">
+        <v>4780</v>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>Communication of Sergine Thibaut About Smithing</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>The Honorable Mégane Ballesdens</t>
+        </is>
+      </c>
+      <c r="S6" s="11" t="inlineStr">
+        <is>
+          <t>C convocatis audere perferre abditi eo vocibus gerendum</t>
+        </is>
+      </c>
+      <c r="T6" t="n">
+        <v>11</v>
+      </c>
+      <c r="U6" t="n">
+        <v>11</v>
+      </c>
+      <c r="V6" t="n">
+        <v>420</v>
+      </c>
+      <c r="W6" t="n">
+        <v>1</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t>Mégane Ballesdens</t>
+        </is>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AD6" t="inlineStr">
+        <is>
+          <t>The Honorable</t>
+        </is>
+      </c>
+      <c r="AE6" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ6" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK6" t="inlineStr">
+        <is>
+          <t>{communication} of {person_1} {conjunction_about} {topic}</t>
+        </is>
+      </c>
+      <c r="AL6" t="inlineStr">
+        <is>
+          <t>Smithing</t>
+        </is>
+      </c>
+      <c r="AM6" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>780</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP6" t="n">
+        <v>4000</v>
+      </c>
+      <c r="AQ6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV6" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>500</v>
+      </c>
+      <c r="E7" t="n">
+        <v>32</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Regional</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Contortionism</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Contortionism</t>
+        </is>
+      </c>
+      <c r="J7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>2</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>1</v>
+      </c>
+      <c r="O7" t="n">
+        <v>695</v>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>Journals of Fenal Taskin and Rufus Carisia Concerning Contortionism</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>Magister Luca Morris</t>
+        </is>
+      </c>
+      <c r="S7" s="11" t="inlineStr">
+        <is>
+          <t>Παραλληλόγραμμα εὐθείαις τεσσάρων μή ἰσοσκελὲς πλευραὶ ἡμίση μζ΄ ἐλάσσονες ς΄ ἄπειρον ὅλα γωνίαις ἑαυτῆς τάς ἐξ</t>
+        </is>
+      </c>
+      <c r="T7" t="n">
+        <v>2</v>
+      </c>
+      <c r="U7" t="n">
+        <v>2</v>
+      </c>
+      <c r="V7" t="n">
+        <v>39</v>
+      </c>
+      <c r="W7" t="n">
+        <v>95</v>
+      </c>
+      <c r="X7" t="n">
+        <v>94</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AB7" t="inlineStr">
+        <is>
+          <t>Luca Morris</t>
+        </is>
+      </c>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>_names_english_surnames</t>
+        </is>
+      </c>
+      <c r="AD7" t="inlineStr">
+        <is>
+          <t>Magister</t>
+        </is>
+      </c>
+      <c r="AE7" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ7" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK7" t="inlineStr">
+        <is>
+          <t>{communication} of {person_1} and {person_2} {conjunction_about} {topic}</t>
+        </is>
+      </c>
+      <c r="AL7" t="inlineStr">
+        <is>
+          <t>Contortionism</t>
+        </is>
+      </c>
+      <c r="AM7" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN7" t="n">
+        <v>195</v>
+      </c>
+      <c r="AO7" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AP7" t="n">
+        <v>500</v>
+      </c>
+      <c r="AQ7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV7" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="n">
+        <v>500</v>
+      </c>
+      <c r="E8" t="n">
+        <v>32</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Precise Shooting</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Precise Shooting</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>2</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>1</v>
+      </c>
+      <c r="O8" t="n">
+        <v>685</v>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>Maryvonne Brindeau and Wrongs: Aspects of Precise Shooting</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>Rune Mortensdotter</t>
+        </is>
+      </c>
+      <c r="S8" s="11" t="inlineStr">
+        <is>
+          <t>Maryvonne Brindeau and Wrongs: Aspects of Precise Shooting</t>
+        </is>
+      </c>
+      <c r="T8" t="n">
+        <v>2</v>
+      </c>
+      <c r="U8" t="n">
+        <v>2</v>
+      </c>
+      <c r="V8" t="n">
+        <v>39</v>
+      </c>
+      <c r="W8" t="n">
+        <v>33</v>
+      </c>
+      <c r="X8" t="n">
+        <v>32</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="AB8" t="inlineStr">
+        <is>
+          <t>Rune Mortensdotter</t>
+        </is>
+      </c>
+      <c r="AC8" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_female</t>
+        </is>
+      </c>
+      <c r="AE8" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ8" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK8" t="inlineStr">
+        <is>
+          <t>{person_1} and {negative_1}: Aspects of {topic}</t>
+        </is>
+      </c>
+      <c r="AL8" t="inlineStr">
+        <is>
+          <t>Precise Shooting</t>
+        </is>
+      </c>
+      <c r="AM8" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN8" t="n">
+        <v>185</v>
+      </c>
+      <c r="AO8" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AP8" t="n">
+        <v>500</v>
+      </c>
+      <c r="AQ8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV8" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>2</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E9" t="n">
+        <v>63</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Regional</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Contemplation</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Contemplation</t>
+        </is>
+      </c>
+      <c r="J9" t="n">
+        <v>1</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>1</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>1</v>
+      </c>
+      <c r="O9" t="n">
+        <v>1390</v>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>Transactions Apropos of Contemplation from Margaret Holderby</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>Orianne Leavitt</t>
+        </is>
+      </c>
+      <c r="S9" s="11" t="inlineStr">
+        <is>
+          <t>Ἐλάσσονας ἠιτήσθω ἑκατέρα παραβαλεῖν περιεχομένη τὰ δ΄ διπλάσια περιφερείας εἰσι παραλληλογράμμων ἴσα</t>
+        </is>
+      </c>
+      <c r="T9" t="n">
+        <v>5</v>
+      </c>
+      <c r="U9" t="n">
+        <v>5</v>
+      </c>
+      <c r="V9" t="n">
+        <v>32</v>
+      </c>
+      <c r="W9" t="n">
+        <v>36</v>
+      </c>
+      <c r="X9" t="n">
+        <v>35</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="AB9" t="inlineStr">
+        <is>
+          <t>Orianne Leavitt</t>
+        </is>
+      </c>
+      <c r="AC9" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AE9" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ9" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK9" t="inlineStr">
+        <is>
+          <t>{communication} {conjunction_about} {topic} {conjunction_by} {person_1}</t>
+        </is>
+      </c>
+      <c r="AL9" t="inlineStr">
+        <is>
+          <t>Contemplation</t>
+        </is>
+      </c>
+      <c r="AM9" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN9" t="n">
+        <v>390</v>
+      </c>
+      <c r="AO9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="AQ9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU9" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV9" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1500</v>
+      </c>
+      <c r="E10" t="n">
+        <v>93</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Regional</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Ambushing</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Ambushing</t>
+        </is>
+      </c>
+      <c r="J10" t="n">
+        <v>3</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>2</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>1</v>
+      </c>
+      <c r="O10" t="n">
+        <v>2055</v>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>Inquiries in Ambushing</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>Magister Hatem Abitbol III</t>
+        </is>
+      </c>
+      <c r="S10" s="11" t="inlineStr">
+        <is>
+          <t>Σχήματος πρὸς ιθ΄ ις΄ οὐθέν αἰτήματα ἰσόπλευρόν</t>
+        </is>
+      </c>
+      <c r="T10" t="n">
+        <v>8</v>
+      </c>
+      <c r="U10" t="n">
+        <v>8</v>
+      </c>
+      <c r="V10" t="n">
+        <v>38</v>
+      </c>
+      <c r="W10" t="n">
+        <v>66</v>
+      </c>
+      <c r="X10" t="n">
+        <v>65</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AA10" t="inlineStr">
+        <is>
+          <t>III</t>
+        </is>
+      </c>
+      <c r="AB10" t="inlineStr">
+        <is>
+          <t>Hatem Abitbol</t>
+        </is>
+      </c>
+      <c r="AC10" t="inlineStr">
+        <is>
+          <t>_names_arabic_surnames</t>
+        </is>
+      </c>
+      <c r="AD10" t="inlineStr">
+        <is>
+          <t>Magister</t>
+        </is>
+      </c>
+      <c r="AE10" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ10" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK10" t="inlineStr">
+        <is>
+          <t>{study_in} in {topic}</t>
+        </is>
+      </c>
+      <c r="AL10" t="inlineStr">
+        <is>
+          <t>Ambushing</t>
+        </is>
+      </c>
+      <c r="AM10" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN10" t="n">
+        <v>555</v>
+      </c>
+      <c r="AO10" t="n">
+        <v>4</v>
+      </c>
+      <c r="AP10" t="n">
+        <v>1500</v>
+      </c>
+      <c r="AQ10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV10" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>2</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1333</v>
+      </c>
+      <c r="E11" t="n">
+        <v>83</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Classical</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Labor (domestic)</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Labor (domestic)</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
+        <v>4</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>3</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="n">
+        <v>1</v>
+      </c>
+      <c r="O11" t="n">
+        <v>7159</v>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>Cleaning Mansions and the Centuries</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>Bodil Andreasdotter</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr"/>
+      <c r="S11" s="11" t="inlineStr">
+        <is>
+          <t>Absentisque mitterentur hic litteras circumveniretur purus vulnere mercatores imponere</t>
+        </is>
+      </c>
+      <c r="T11" t="n">
+        <v>7</v>
+      </c>
+      <c r="U11" t="n">
+        <v>7</v>
+      </c>
+      <c r="V11" t="n">
+        <v>20</v>
+      </c>
+      <c r="W11" t="n">
+        <v>4</v>
+      </c>
+      <c r="X11" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="Z11" t="inlineStr"/>
+      <c r="AA11" t="inlineStr"/>
+      <c r="AB11" t="inlineStr">
+        <is>
+          <t>Bodil Andreasdotter</t>
+        </is>
+      </c>
+      <c r="AC11" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_female</t>
+        </is>
+      </c>
+      <c r="AD11" t="inlineStr"/>
+      <c r="AE11" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AF11" t="inlineStr"/>
+      <c r="AG11" t="inlineStr"/>
+      <c r="AH11" t="inlineStr"/>
+      <c r="AI11" t="inlineStr"/>
+      <c r="AJ11" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK11" t="inlineStr">
+        <is>
+          <t>{topic} and {noun_2}</t>
+        </is>
+      </c>
+      <c r="AL11" t="inlineStr">
+        <is>
+          <t>Cleaning Mansions</t>
+        </is>
+      </c>
+      <c r="AM11" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN11" t="n">
+        <v>494</v>
+      </c>
+      <c r="AO11" t="n">
+        <v>10</v>
+      </c>
+      <c r="AP11" t="n">
+        <v>6665</v>
+      </c>
+      <c r="AQ11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU11" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV11" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" t="n">
+        <v>500</v>
+      </c>
+      <c r="E12" t="n">
+        <v>32</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
+      <c r="J12" t="n">
+        <v>1</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>2</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>1</v>
+      </c>
+      <c r="O12" t="n">
+        <v>685</v>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>Scrutiny of Engineering</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>Lana Wardak XIII</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr"/>
+      <c r="S12" s="11" t="inlineStr">
+        <is>
+          <t>Scrutiny of Engineering</t>
+        </is>
+      </c>
+      <c r="T12" t="n">
+        <v>2</v>
+      </c>
+      <c r="U12" t="n">
+        <v>2</v>
+      </c>
+      <c r="V12" t="n">
+        <v>41</v>
+      </c>
+      <c r="W12" t="n">
+        <v>90</v>
+      </c>
+      <c r="X12" t="n">
+        <v>89</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="Z12" t="inlineStr"/>
+      <c r="AA12" t="inlineStr">
+        <is>
+          <t>XIII</t>
+        </is>
+      </c>
+      <c r="AB12" t="inlineStr">
+        <is>
+          <t>Lana Wardak</t>
+        </is>
+      </c>
+      <c r="AC12" t="inlineStr">
+        <is>
+          <t>_names_arabic_surnames</t>
+        </is>
+      </c>
+      <c r="AD12" t="inlineStr"/>
+      <c r="AE12" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AF12" t="inlineStr"/>
+      <c r="AG12" t="inlineStr"/>
+      <c r="AH12" t="inlineStr"/>
+      <c r="AI12" t="inlineStr"/>
+      <c r="AJ12" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK12" t="inlineStr">
+        <is>
+          <t>{study_of} of {topic}</t>
+        </is>
+      </c>
+      <c r="AL12" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
+      <c r="AM12" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN12" t="n">
+        <v>185</v>
+      </c>
+      <c r="AO12" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AP12" t="n">
+        <v>500</v>
+      </c>
+      <c r="AQ12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU12" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV12" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>2</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E13" t="n">
+        <v>63</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Battle Magic</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Battle Magic</t>
+        </is>
+      </c>
+      <c r="J13" t="n">
+        <v>1</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>1</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>1</v>
+      </c>
+      <c r="O13" t="n">
+        <v>1390</v>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>The Guilt of The Chief Sinner on the Dire Subject of Sorcerie and the Field of Battle</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>His Lordship Dan Poncelet the Bearded</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr"/>
+      <c r="S13" s="11" t="inlineStr">
+        <is>
+          <t>The Guilt of The Chief Sinner on the Dire Subject of Sorcerie and the Field of Battle</t>
+        </is>
+      </c>
+      <c r="T13" t="n">
+        <v>5</v>
+      </c>
+      <c r="U13" t="n">
+        <v>5</v>
+      </c>
+      <c r="V13" t="n">
+        <v>34</v>
+      </c>
+      <c r="W13" t="n">
+        <v>81</v>
+      </c>
+      <c r="X13" t="n">
+        <v>80</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="Z13" t="inlineStr"/>
+      <c r="AA13" t="inlineStr">
+        <is>
+          <t>the Bearded</t>
+        </is>
+      </c>
+      <c r="AB13" t="inlineStr">
+        <is>
+          <t>Dan Poncelet</t>
+        </is>
+      </c>
+      <c r="AC13" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AD13" t="inlineStr">
+        <is>
+          <t>His Lordship</t>
+        </is>
+      </c>
+      <c r="AE13" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AF13" t="inlineStr"/>
+      <c r="AG13" t="inlineStr"/>
+      <c r="AH13" t="inlineStr"/>
+      <c r="AI13" t="inlineStr"/>
+      <c r="AJ13" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK13" t="inlineStr">
+        <is>
+          <t>{the_1} {negative_1} of {person_evil} on the Dire Subject of {topic}</t>
+        </is>
+      </c>
+      <c r="AL13" t="inlineStr">
+        <is>
+          <t>Sorcerie and the Field of Battle</t>
+        </is>
+      </c>
+      <c r="AM13" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN13" t="n">
+        <v>390</v>
+      </c>
+      <c r="AO13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP13" t="n">
+        <v>1000</v>
+      </c>
+      <c r="AQ13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU13" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV13" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" t="n">
+        <v>500</v>
+      </c>
+      <c r="E14" t="n">
+        <v>32</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Beast Friendship</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Beast Friendship</t>
+        </is>
+      </c>
+      <c r="J14" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>2</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>1</v>
+      </c>
+      <c r="O14" t="n">
+        <v>695</v>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>Communication of Ødger Berg and Maecia Trebulana Apropos of Friendship with the Beasts</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>Madam Rota Halvorsdotter</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr"/>
+      <c r="S14" s="11" t="inlineStr">
+        <is>
+          <t>Communication of Ødger Berg and Maecia Trebulana Apropos of Friendship with the Beasts</t>
+        </is>
+      </c>
+      <c r="T14" t="n">
+        <v>2</v>
+      </c>
+      <c r="U14" t="n">
+        <v>2</v>
+      </c>
+      <c r="V14" t="n">
+        <v>37</v>
+      </c>
+      <c r="W14" t="n">
+        <v>18</v>
+      </c>
+      <c r="X14" t="n">
+        <v>17</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="Z14" t="inlineStr"/>
+      <c r="AA14" t="inlineStr"/>
+      <c r="AB14" t="inlineStr">
+        <is>
+          <t>Rota Halvorsdotter</t>
+        </is>
+      </c>
+      <c r="AC14" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_female</t>
+        </is>
+      </c>
+      <c r="AD14" t="inlineStr">
+        <is>
+          <t>Madam</t>
+        </is>
+      </c>
+      <c r="AE14" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AF14" t="inlineStr"/>
+      <c r="AG14" t="inlineStr"/>
+      <c r="AH14" t="inlineStr"/>
+      <c r="AI14" t="inlineStr"/>
+      <c r="AJ14" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK14" t="inlineStr">
+        <is>
+          <t>{communication} of {person_1} and {person_2} {conjunction_about} {topic}</t>
+        </is>
+      </c>
+      <c r="AL14" t="inlineStr">
+        <is>
+          <t>Friendship with the Beasts</t>
+        </is>
+      </c>
+      <c r="AM14" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN14" t="n">
+        <v>195</v>
+      </c>
+      <c r="AO14" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AP14" t="n">
+        <v>500</v>
+      </c>
+      <c r="AQ14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU14" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV14" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" t="n">
+        <v>235</v>
+      </c>
+      <c r="E15" t="n">
+        <v>15</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Elvish</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Craft (leatherworking)</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Craft (leatherworking)</t>
+        </is>
+      </c>
+      <c r="J15" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>2</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="O15" t="n">
+        <v>562</v>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>Communication as Regards Leatherworking from Anouk Marchant</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>Kare Magnusdotter</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Arnaude Bozonnet</t>
+        </is>
+      </c>
+      <c r="S15" s="11" t="inlineStr">
+        <is>
+          <t>Communication as Regards Leatherworking from Anouk Marchant</t>
+        </is>
+      </c>
+      <c r="T15" t="n">
+        <v>1</v>
+      </c>
+      <c r="U15" t="n">
+        <v>1</v>
+      </c>
+      <c r="V15" t="n">
+        <v>50</v>
+      </c>
+      <c r="W15" t="n">
+        <v>1</v>
+      </c>
+      <c r="X15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z15" t="inlineStr"/>
+      <c r="AA15" t="inlineStr"/>
+      <c r="AB15" t="inlineStr">
+        <is>
+          <t>Kare Magnusdotter</t>
+        </is>
+      </c>
+      <c r="AC15" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_female</t>
+        </is>
+      </c>
+      <c r="AD15" t="inlineStr"/>
+      <c r="AE15" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AF15" t="inlineStr">
+        <is>
+          <t>Arnaude Bozonnet</t>
+        </is>
+      </c>
+      <c r="AG15" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AH15" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AI15" t="inlineStr"/>
+      <c r="AJ15" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK15" t="inlineStr">
+        <is>
+          <t>{communication} {conjunction_about} {topic} {conjunction_by} {person_1}</t>
+        </is>
+      </c>
+      <c r="AL15" t="inlineStr">
+        <is>
+          <t>Leatherworking</t>
+        </is>
+      </c>
+      <c r="AM15" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN15" t="n">
+        <v>195</v>
+      </c>
+      <c r="AO15" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AP15" t="n">
+        <v>1000</v>
+      </c>
+      <c r="AQ15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU15" t="b">
+        <v>1</v>
+      </c>
+      <c r="AV15" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" t="n">
+        <v>750</v>
+      </c>
+      <c r="E16" t="n">
+        <v>46</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Craft (baking)</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Craft (baking)</t>
+        </is>
+      </c>
+      <c r="J16" t="n">
+        <v>3</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>4</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>1</v>
+      </c>
+      <c r="O16" t="n">
+        <v>1043</v>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>The Lust of Vetrliði Nilsen, on the Subject of Baking</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>The Gracious Hugin Nielsen the Exquisite</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr"/>
+      <c r="S16" s="11" t="inlineStr">
+        <is>
+          <t>The Lust of Vetrliði Nilsen, on the Subject of Baking</t>
+        </is>
+      </c>
+      <c r="T16" t="n">
+        <v>4</v>
+      </c>
+      <c r="U16" t="n">
+        <v>4</v>
+      </c>
+      <c r="V16" t="n">
+        <v>20</v>
+      </c>
+      <c r="W16" t="n">
+        <v>206</v>
+      </c>
+      <c r="X16" t="n">
+        <v>205</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="Z16" t="inlineStr"/>
+      <c r="AA16" t="inlineStr">
+        <is>
+          <t>the Exquisite</t>
+        </is>
+      </c>
+      <c r="AB16" t="inlineStr">
+        <is>
+          <t>Hugin Nielsen</t>
+        </is>
+      </c>
+      <c r="AC16" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_male</t>
+        </is>
+      </c>
+      <c r="AD16" t="inlineStr">
+        <is>
+          <t>The Gracious</t>
+        </is>
+      </c>
+      <c r="AE16" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AF16" t="inlineStr"/>
+      <c r="AG16" t="inlineStr"/>
+      <c r="AH16" t="inlineStr"/>
+      <c r="AI16" t="inlineStr"/>
+      <c r="AJ16" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK16" t="inlineStr">
+        <is>
+          <t>{the_1} {negative_1} of {person_1}, on the Subject of {topic}</t>
+        </is>
+      </c>
+      <c r="AL16" t="inlineStr">
+        <is>
+          <t>Baking</t>
+        </is>
+      </c>
+      <c r="AM16" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN16" t="n">
+        <v>293</v>
+      </c>
+      <c r="AO16" t="n">
+        <v>5</v>
+      </c>
+      <c r="AP16" t="n">
+        <v>750</v>
+      </c>
+      <c r="AQ16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV16" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>2</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1333</v>
+      </c>
+      <c r="E17" t="n">
+        <v>83</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Classical</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Mapping</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Mapping</t>
+        </is>
+      </c>
+      <c r="J17" t="n">
+        <v>1</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O17" t="n">
+        <v>1853</v>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>The Damnable Evildoing of Steingrímr Petersen, Considering Mapping</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>Lord Alfarr Madsen</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr"/>
+      <c r="S17" s="11" t="inlineStr">
+        <is>
+          <t>Cursus subvexerat commutatione fecisse despiceret deleniti summo</t>
+        </is>
+      </c>
+      <c r="T17" t="n">
+        <v>7</v>
+      </c>
+      <c r="U17" t="n">
+        <v>7</v>
+      </c>
+      <c r="V17" t="n">
+        <v>107</v>
+      </c>
+      <c r="W17" t="n">
+        <v>12</v>
+      </c>
+      <c r="X17" t="n">
+        <v>11</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="Z17" t="inlineStr"/>
+      <c r="AA17" t="inlineStr"/>
+      <c r="AB17" t="inlineStr">
+        <is>
+          <t>Alfarr Madsen</t>
+        </is>
+      </c>
+      <c r="AC17" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_male</t>
+        </is>
+      </c>
+      <c r="AD17" t="inlineStr">
+        <is>
+          <t>Lord</t>
+        </is>
+      </c>
+      <c r="AE17" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AF17" t="inlineStr"/>
+      <c r="AG17" t="inlineStr"/>
+      <c r="AH17" t="inlineStr"/>
+      <c r="AI17" t="inlineStr"/>
+      <c r="AJ17" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK17" t="inlineStr">
+        <is>
+          <t>{the_1} {negative_1} of {person_1}, Considering {topic}</t>
+        </is>
+      </c>
+      <c r="AL17" t="inlineStr">
+        <is>
+          <t>Mapping</t>
+        </is>
+      </c>
+      <c r="AM17" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN17" t="n">
+        <v>520</v>
+      </c>
+      <c r="AO17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP17" t="n">
+        <v>1333</v>
+      </c>
+      <c r="AQ17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU17" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV17" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>2</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1333</v>
+      </c>
+      <c r="E18" t="n">
+        <v>83</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Elvish</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Esoteric: Theology</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Navigation</t>
+        </is>
+      </c>
+      <c r="J18" t="n">
+        <v>1</v>
+      </c>
+      <c r="K18" t="n">
+        <v>1</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="N18" t="n">
+        <v>1</v>
+      </c>
+      <c r="O18" t="n">
+        <v>8492</v>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>Navigation and the Generation</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>Baronness Isabel Baillieu the Gifted</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr"/>
+      <c r="S18" s="12" t="inlineStr">
+        <is>
+          <t>Brona gwanûr name goeoel nedhyr henneth</t>
+        </is>
+      </c>
+      <c r="T18" t="n">
+        <v>7</v>
+      </c>
+      <c r="U18" t="n">
+        <v>7</v>
+      </c>
+      <c r="V18" t="n">
+        <v>96</v>
+      </c>
+      <c r="W18" t="n">
+        <v>1</v>
+      </c>
+      <c r="X18" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z18" t="inlineStr"/>
+      <c r="AA18" t="inlineStr">
+        <is>
+          <t>the Gifted</t>
+        </is>
+      </c>
+      <c r="AB18" t="inlineStr">
+        <is>
+          <t>Isabel Baillieu</t>
+        </is>
+      </c>
+      <c r="AC18" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AD18" t="inlineStr">
+        <is>
+          <t>Baronness</t>
+        </is>
+      </c>
+      <c r="AE18" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AF18" t="inlineStr"/>
+      <c r="AG18" t="inlineStr"/>
+      <c r="AH18" t="inlineStr"/>
+      <c r="AI18" t="inlineStr"/>
+      <c r="AJ18" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK18" t="inlineStr">
+        <is>
+          <t>{topic} and {noun_2}</t>
+        </is>
+      </c>
+      <c r="AL18" t="inlineStr">
+        <is>
+          <t>Navigation</t>
+        </is>
+      </c>
+      <c r="AM18" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN18" t="n">
+        <v>494</v>
+      </c>
+      <c r="AO18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP18" t="n">
+        <v>1333</v>
+      </c>
+      <c r="AQ18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR18" t="n">
+        <v>6665</v>
+      </c>
+      <c r="AS18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV18" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Clean up double and single quotes 1
</commit_message>
<xml_diff>
--- a/books_spreadsheet_out.xlsx
+++ b/books_spreadsheet_out.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\p\gls01_workspace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A8D4D4-14AF-439C-B889-449F2FECC5F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C09F22-A050-4627-AC45-7EFCB779E7E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -547,7 +547,7 @@
   <dimension ref="A1:AX1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -583,8 +583,8 @@
     <col min="37" max="38" width="9.140625" style="1" customWidth="1"/>
     <col min="39" max="39" width="15.28515625" style="1" customWidth="1"/>
     <col min="40" max="40" width="13.7109375" style="1" customWidth="1"/>
-    <col min="41" max="56" width="9.140625" style="1" customWidth="1"/>
-    <col min="57" max="16384" width="9.140625" style="1"/>
+    <col min="41" max="57" width="9.140625" style="1" customWidth="1"/>
+    <col min="58" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Copy from source to dest works
</commit_message>
<xml_diff>
--- a/books_spreadsheet_out.xlsx
+++ b/books_spreadsheet_out.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\p\gls01_workspace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9A6172-7EB1-4E29-8953-29A312BD9529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D46FAB-7C1E-4AB3-9AB0-E199A7CD5A87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Book Hoard" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="GLS" localSheetId="0">'Book Hoard'!$A$1:$AV$1</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="148">
   <si>
     <t>format</t>
   </si>
@@ -850,7 +851,7 @@
   <dimension ref="A1:AX12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2506,4 +2507,1215 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E9323C4-DE08-41E4-A41E-07D43A3F2DD4}">
+  <dimension ref="A1:AX9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:50" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>500</v>
+      </c>
+      <c r="E1">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1"/>
+      <c r="H1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J1">
+        <v>1</v>
+      </c>
+      <c r="K1">
+        <v>0</v>
+      </c>
+      <c r="L1">
+        <v>2</v>
+      </c>
+      <c r="M1">
+        <v>0</v>
+      </c>
+      <c r="N1">
+        <v>1</v>
+      </c>
+      <c r="O1">
+        <v>810</v>
+      </c>
+      <c r="P1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>83</v>
+      </c>
+      <c r="R1"/>
+      <c r="S1" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="T1">
+        <v>3</v>
+      </c>
+      <c r="U1">
+        <v>3</v>
+      </c>
+      <c r="V1">
+        <v>45</v>
+      </c>
+      <c r="W1">
+        <v>1</v>
+      </c>
+      <c r="X1">
+        <v>0</v>
+      </c>
+      <c r="Y1">
+        <v>1</v>
+      </c>
+      <c r="Z1"/>
+      <c r="AA1"/>
+      <c r="AB1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF1"/>
+      <c r="AG1"/>
+      <c r="AH1"/>
+      <c r="AI1"/>
+      <c r="AJ1">
+        <v>0.06</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AM1">
+        <v>0.37</v>
+      </c>
+      <c r="AN1">
+        <v>185</v>
+      </c>
+      <c r="AO1">
+        <v>1.25</v>
+      </c>
+      <c r="AP1">
+        <v>625</v>
+      </c>
+      <c r="AQ1">
+        <v>0</v>
+      </c>
+      <c r="AR1">
+        <v>0</v>
+      </c>
+      <c r="AS1">
+        <v>0</v>
+      </c>
+      <c r="AT1">
+        <v>0</v>
+      </c>
+      <c r="AU1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AX1"/>
+    </row>
+    <row r="2" spans="1:50" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>1000</v>
+      </c>
+      <c r="E2">
+        <v>63</v>
+      </c>
+      <c r="F2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2"/>
+      <c r="H2" t="s">
+        <v>89</v>
+      </c>
+      <c r="I2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>440</v>
+      </c>
+      <c r="P2" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>91</v>
+      </c>
+      <c r="R2"/>
+      <c r="S2" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="T2">
+        <v>6</v>
+      </c>
+      <c r="U2">
+        <v>6</v>
+      </c>
+      <c r="V2">
+        <v>81</v>
+      </c>
+      <c r="W2">
+        <v>227</v>
+      </c>
+      <c r="X2">
+        <v>226</v>
+      </c>
+      <c r="Y2">
+        <v>0.05</v>
+      </c>
+      <c r="Z2"/>
+      <c r="AA2"/>
+      <c r="AB2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>94</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF2"/>
+      <c r="AG2"/>
+      <c r="AH2"/>
+      <c r="AI2"/>
+      <c r="AJ2">
+        <v>0.06</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AM2">
+        <v>0.39</v>
+      </c>
+      <c r="AN2">
+        <v>390</v>
+      </c>
+      <c r="AO2">
+        <v>1</v>
+      </c>
+      <c r="AP2">
+        <v>50</v>
+      </c>
+      <c r="AQ2">
+        <v>0</v>
+      </c>
+      <c r="AR2">
+        <v>0</v>
+      </c>
+      <c r="AS2">
+        <v>0</v>
+      </c>
+      <c r="AT2">
+        <v>0</v>
+      </c>
+      <c r="AU2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>97</v>
+      </c>
+      <c r="AX2"/>
+    </row>
+    <row r="3" spans="1:50" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>667</v>
+      </c>
+      <c r="E3">
+        <v>43</v>
+      </c>
+      <c r="F3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3"/>
+      <c r="H3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I3" t="s">
+        <v>98</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>3</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>798</v>
+      </c>
+      <c r="P3" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>100</v>
+      </c>
+      <c r="R3"/>
+      <c r="S3" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="T3">
+        <v>4</v>
+      </c>
+      <c r="U3">
+        <v>4</v>
+      </c>
+      <c r="V3">
+        <v>66</v>
+      </c>
+      <c r="W3">
+        <v>21</v>
+      </c>
+      <c r="X3">
+        <v>20</v>
+      </c>
+      <c r="Y3">
+        <v>0.33</v>
+      </c>
+      <c r="Z3"/>
+      <c r="AA3"/>
+      <c r="AB3" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD3"/>
+      <c r="AE3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF3"/>
+      <c r="AG3"/>
+      <c r="AH3"/>
+      <c r="AI3"/>
+      <c r="AJ3">
+        <v>0.06</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>102</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>103</v>
+      </c>
+      <c r="AM3">
+        <v>0.37</v>
+      </c>
+      <c r="AN3">
+        <v>247</v>
+      </c>
+      <c r="AO3">
+        <v>2.5</v>
+      </c>
+      <c r="AP3">
+        <v>551</v>
+      </c>
+      <c r="AQ3">
+        <v>0</v>
+      </c>
+      <c r="AR3">
+        <v>0</v>
+      </c>
+      <c r="AS3">
+        <v>0</v>
+      </c>
+      <c r="AT3">
+        <v>0</v>
+      </c>
+      <c r="AU3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AX3"/>
+    </row>
+    <row r="4" spans="1:50" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>500</v>
+      </c>
+      <c r="E4">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4"/>
+      <c r="H4" t="s">
+        <v>105</v>
+      </c>
+      <c r="I4" t="s">
+        <v>105</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>508</v>
+      </c>
+      <c r="P4" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>107</v>
+      </c>
+      <c r="R4"/>
+      <c r="S4" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="T4">
+        <v>3</v>
+      </c>
+      <c r="U4">
+        <v>3</v>
+      </c>
+      <c r="V4">
+        <v>64</v>
+      </c>
+      <c r="W4">
+        <v>2</v>
+      </c>
+      <c r="X4">
+        <v>1</v>
+      </c>
+      <c r="Y4">
+        <v>0.5</v>
+      </c>
+      <c r="Z4"/>
+      <c r="AA4"/>
+      <c r="AB4" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD4"/>
+      <c r="AE4" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF4"/>
+      <c r="AG4"/>
+      <c r="AH4"/>
+      <c r="AI4"/>
+      <c r="AJ4">
+        <v>0.06</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>109</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>105</v>
+      </c>
+      <c r="AM4">
+        <v>0.39</v>
+      </c>
+      <c r="AN4">
+        <v>195</v>
+      </c>
+      <c r="AO4">
+        <v>1.25</v>
+      </c>
+      <c r="AP4">
+        <v>313</v>
+      </c>
+      <c r="AQ4">
+        <v>0</v>
+      </c>
+      <c r="AR4">
+        <v>0</v>
+      </c>
+      <c r="AS4">
+        <v>0</v>
+      </c>
+      <c r="AT4">
+        <v>0</v>
+      </c>
+      <c r="AU4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>110</v>
+      </c>
+      <c r="AX4"/>
+    </row>
+    <row r="5" spans="1:50" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>1334</v>
+      </c>
+      <c r="E5">
+        <v>84</v>
+      </c>
+      <c r="F5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G5"/>
+      <c r="H5" t="s">
+        <v>111</v>
+      </c>
+      <c r="I5" t="s">
+        <v>111</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0.75</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>855</v>
+      </c>
+      <c r="P5" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>113</v>
+      </c>
+      <c r="R5"/>
+      <c r="S5" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="T5">
+        <v>8</v>
+      </c>
+      <c r="U5">
+        <v>8</v>
+      </c>
+      <c r="V5">
+        <v>31</v>
+      </c>
+      <c r="W5">
+        <v>38</v>
+      </c>
+      <c r="X5">
+        <v>37</v>
+      </c>
+      <c r="Y5">
+        <v>0.25</v>
+      </c>
+      <c r="Z5"/>
+      <c r="AA5"/>
+      <c r="AB5" t="s">
+        <v>115</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>116</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF5"/>
+      <c r="AG5"/>
+      <c r="AH5"/>
+      <c r="AI5"/>
+      <c r="AJ5">
+        <v>0.06</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>118</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>119</v>
+      </c>
+      <c r="AM5">
+        <v>0.39</v>
+      </c>
+      <c r="AN5">
+        <v>521</v>
+      </c>
+      <c r="AO5">
+        <v>1</v>
+      </c>
+      <c r="AP5">
+        <v>334</v>
+      </c>
+      <c r="AQ5">
+        <v>0</v>
+      </c>
+      <c r="AR5">
+        <v>0</v>
+      </c>
+      <c r="AS5">
+        <v>0</v>
+      </c>
+      <c r="AT5">
+        <v>0</v>
+      </c>
+      <c r="AU5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AW5" t="s">
+        <v>120</v>
+      </c>
+      <c r="AX5"/>
+    </row>
+    <row r="6" spans="1:50" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>1000</v>
+      </c>
+      <c r="E6">
+        <v>68</v>
+      </c>
+      <c r="F6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6"/>
+      <c r="H6" t="s">
+        <v>121</v>
+      </c>
+      <c r="I6" t="s">
+        <v>121</v>
+      </c>
+      <c r="J6">
+        <v>2</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>2</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1040</v>
+      </c>
+      <c r="P6" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>123</v>
+      </c>
+      <c r="R6"/>
+      <c r="S6" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="T6">
+        <v>6</v>
+      </c>
+      <c r="U6">
+        <v>6</v>
+      </c>
+      <c r="V6">
+        <v>864</v>
+      </c>
+      <c r="W6">
+        <v>9</v>
+      </c>
+      <c r="X6">
+        <v>8</v>
+      </c>
+      <c r="Y6">
+        <v>0.33</v>
+      </c>
+      <c r="Z6"/>
+      <c r="AA6"/>
+      <c r="AB6" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD6"/>
+      <c r="AE6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF6"/>
+      <c r="AG6"/>
+      <c r="AH6"/>
+      <c r="AI6"/>
+      <c r="AJ6">
+        <v>0.06</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>125</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>121</v>
+      </c>
+      <c r="AM6">
+        <v>0.38</v>
+      </c>
+      <c r="AN6">
+        <v>380</v>
+      </c>
+      <c r="AO6">
+        <v>2</v>
+      </c>
+      <c r="AP6">
+        <v>660</v>
+      </c>
+      <c r="AQ6">
+        <v>0</v>
+      </c>
+      <c r="AR6">
+        <v>0</v>
+      </c>
+      <c r="AS6">
+        <v>0</v>
+      </c>
+      <c r="AT6">
+        <v>0</v>
+      </c>
+      <c r="AU6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AW6" t="s">
+        <v>126</v>
+      </c>
+      <c r="AX6"/>
+    </row>
+    <row r="7" spans="1:50" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>667</v>
+      </c>
+      <c r="E7">
+        <v>43</v>
+      </c>
+      <c r="F7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7"/>
+      <c r="H7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I7" t="s">
+        <v>127</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>3</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>664</v>
+      </c>
+      <c r="P7" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>129</v>
+      </c>
+      <c r="R7"/>
+      <c r="S7" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="T7">
+        <v>4</v>
+      </c>
+      <c r="U7">
+        <v>4</v>
+      </c>
+      <c r="V7">
+        <v>43</v>
+      </c>
+      <c r="W7">
+        <v>36</v>
+      </c>
+      <c r="X7">
+        <v>35</v>
+      </c>
+      <c r="Y7">
+        <v>0.25</v>
+      </c>
+      <c r="Z7"/>
+      <c r="AA7"/>
+      <c r="AB7" t="s">
+        <v>129</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>116</v>
+      </c>
+      <c r="AD7"/>
+      <c r="AE7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF7"/>
+      <c r="AG7"/>
+      <c r="AH7"/>
+      <c r="AI7"/>
+      <c r="AJ7">
+        <v>0.06</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>127</v>
+      </c>
+      <c r="AM7">
+        <v>0.37</v>
+      </c>
+      <c r="AN7">
+        <v>247</v>
+      </c>
+      <c r="AO7">
+        <v>2.5</v>
+      </c>
+      <c r="AP7">
+        <v>417</v>
+      </c>
+      <c r="AQ7">
+        <v>0</v>
+      </c>
+      <c r="AR7">
+        <v>0</v>
+      </c>
+      <c r="AS7">
+        <v>0</v>
+      </c>
+      <c r="AT7">
+        <v>0</v>
+      </c>
+      <c r="AU7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV7" t="s">
+        <v>57</v>
+      </c>
+      <c r="AW7" t="s">
+        <v>131</v>
+      </c>
+      <c r="AX7"/>
+    </row>
+    <row r="8" spans="1:50" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>185</v>
+      </c>
+      <c r="E8">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
+        <v>88</v>
+      </c>
+      <c r="G8"/>
+      <c r="H8" t="s">
+        <v>132</v>
+      </c>
+      <c r="I8" t="s">
+        <v>132</v>
+      </c>
+      <c r="J8">
+        <v>0.5</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>2</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0.37</v>
+      </c>
+      <c r="O8">
+        <v>96</v>
+      </c>
+      <c r="P8" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>134</v>
+      </c>
+      <c r="R8"/>
+      <c r="S8" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+      <c r="U8">
+        <v>1</v>
+      </c>
+      <c r="V8">
+        <v>18</v>
+      </c>
+      <c r="W8">
+        <v>84</v>
+      </c>
+      <c r="X8">
+        <v>83</v>
+      </c>
+      <c r="Y8">
+        <v>0.1</v>
+      </c>
+      <c r="Z8"/>
+      <c r="AA8" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>137</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD8"/>
+      <c r="AE8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF8"/>
+      <c r="AG8"/>
+      <c r="AH8"/>
+      <c r="AI8"/>
+      <c r="AJ8">
+        <v>0.06</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>138</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>139</v>
+      </c>
+      <c r="AM8">
+        <v>0.39</v>
+      </c>
+      <c r="AN8">
+        <v>195</v>
+      </c>
+      <c r="AO8">
+        <v>1.25</v>
+      </c>
+      <c r="AP8">
+        <v>63</v>
+      </c>
+      <c r="AQ8">
+        <v>0</v>
+      </c>
+      <c r="AR8">
+        <v>0</v>
+      </c>
+      <c r="AS8">
+        <v>0</v>
+      </c>
+      <c r="AT8">
+        <v>0</v>
+      </c>
+      <c r="AU8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AW8" t="s">
+        <v>140</v>
+      </c>
+      <c r="AX8"/>
+    </row>
+    <row r="9" spans="1:50" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>1000</v>
+      </c>
+      <c r="E9">
+        <v>303</v>
+      </c>
+      <c r="F9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9"/>
+      <c r="H9" t="s">
+        <v>142</v>
+      </c>
+      <c r="I9" t="s">
+        <v>142</v>
+      </c>
+      <c r="J9">
+        <v>3</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>3</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>30710</v>
+      </c>
+      <c r="P9" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>144</v>
+      </c>
+      <c r="R9"/>
+      <c r="S9" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="T9">
+        <v>6</v>
+      </c>
+      <c r="U9">
+        <v>6</v>
+      </c>
+      <c r="V9">
+        <v>83</v>
+      </c>
+      <c r="W9">
+        <v>78</v>
+      </c>
+      <c r="X9">
+        <v>77</v>
+      </c>
+      <c r="Y9">
+        <v>0.1</v>
+      </c>
+      <c r="Z9"/>
+      <c r="AA9"/>
+      <c r="AB9" t="s">
+        <v>144</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>145</v>
+      </c>
+      <c r="AD9"/>
+      <c r="AE9" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF9"/>
+      <c r="AG9"/>
+      <c r="AH9"/>
+      <c r="AI9"/>
+      <c r="AJ9">
+        <v>0.3</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>146</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>142</v>
+      </c>
+      <c r="AM9">
+        <v>30.31</v>
+      </c>
+      <c r="AN9">
+        <v>30310</v>
+      </c>
+      <c r="AO9">
+        <v>4</v>
+      </c>
+      <c r="AP9">
+        <v>400</v>
+      </c>
+      <c r="AQ9">
+        <v>0</v>
+      </c>
+      <c r="AR9">
+        <v>0</v>
+      </c>
+      <c r="AS9">
+        <v>0</v>
+      </c>
+      <c r="AT9">
+        <v>0</v>
+      </c>
+      <c r="AU9" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AW9" t="s">
+        <v>147</v>
+      </c>
+      <c r="AX9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Works up to DEFAULT_EXCEL_FONT
</commit_message>
<xml_diff>
--- a/books_spreadsheet_out.xlsx
+++ b/books_spreadsheet_out.xlsx
@@ -461,7 +461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AX11"/>
+  <dimension ref="A1:AX21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -784,7 +784,6 @@
           <t>Regional</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
           <t>Battle Magic</t>
@@ -823,7 +822,6 @@
           <t>Cédric Chappuis</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr"/>
       <c r="S2" s="10" t="inlineStr">
         <is>
           <t>Ἄπειρον γωνίας γραμμή ἑκατέρᾳ] περατουμένη περιεχόμενα αἰτήματα ἀμβλεῖα λοιπαῖς ἀπὸ βάσει μόνον διαστήματι</t>
@@ -847,8 +845,6 @@
       <c r="Y2" t="n">
         <v>0.5</v>
       </c>
-      <c r="Z2" t="inlineStr"/>
-      <c r="AA2" t="inlineStr"/>
       <c r="AB2" t="inlineStr">
         <is>
           <t>Cédric Chappuis</t>
@@ -859,16 +855,11 @@
           <t>_names_french_surnames</t>
         </is>
       </c>
-      <c r="AD2" t="inlineStr"/>
       <c r="AE2" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
-      <c r="AF2" t="inlineStr"/>
-      <c r="AG2" t="inlineStr"/>
-      <c r="AH2" t="inlineStr"/>
-      <c r="AI2" t="inlineStr"/>
       <c r="AJ2" t="n">
         <v>0.06</v>
       </c>
@@ -919,7 +910,6 @@
           <t>15ebc13e-078c-46c6-81f6-518f6e901025</t>
         </is>
       </c>
-      <c r="AX2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -946,7 +936,6 @@
           <t>Common</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
           <t>Familiar</t>
@@ -985,7 +974,6 @@
           <t>Cynemær Punches</t>
         </is>
       </c>
-      <c r="R3" t="inlineStr"/>
       <c r="S3" s="10" t="inlineStr">
         <is>
           <t>Exchanges Apropos of Familiar by Bude Morgan</t>
@@ -1009,8 +997,6 @@
       <c r="Y3" t="n">
         <v>0.05</v>
       </c>
-      <c r="Z3" t="inlineStr"/>
-      <c r="AA3" t="inlineStr"/>
       <c r="AB3" t="inlineStr">
         <is>
           <t>Cynemær Punches</t>
@@ -1021,16 +1007,11 @@
           <t>_names_anglo_saxon_surnames</t>
         </is>
       </c>
-      <c r="AD3" t="inlineStr"/>
       <c r="AE3" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
-      <c r="AF3" t="inlineStr"/>
-      <c r="AG3" t="inlineStr"/>
-      <c r="AH3" t="inlineStr"/>
-      <c r="AI3" t="inlineStr"/>
       <c r="AJ3" t="n">
         <v>0.06</v>
       </c>
@@ -1081,7 +1062,6 @@
           <t>f739d418-26cf-412a-b88a-8747db083ec3</t>
         </is>
       </c>
-      <c r="AX3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1108,7 +1088,6 @@
           <t>Ancient</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
           <t>Trapping</t>
@@ -1147,7 +1126,6 @@
           <t>Hallbjǫrn Thomsen</t>
         </is>
       </c>
-      <c r="R4" t="inlineStr"/>
       <c r="S4" s="10" t="inlineStr">
         <is>
           <t>𐎬𐎨 𐎫𐎨𐎡𐎤𐎱𐎮 𐎵𐎤𐎫 𐎬𐎸𐎽 𐎬𐎠𐎦𐎭𐎠 𐎯𐎱𐎮𐎨𐎭 𐎱𐎨𐎽𐎸𐎽 𐎠𐎸𐎦𐎸</t>
@@ -1171,8 +1149,6 @@
       <c r="Y4" t="n">
         <v>0.25</v>
       </c>
-      <c r="Z4" t="inlineStr"/>
-      <c r="AA4" t="inlineStr"/>
       <c r="AB4" t="inlineStr">
         <is>
           <t>Hallbjǫrn Thomsen</t>
@@ -1183,16 +1159,11 @@
           <t>_names_norse_surnames_male</t>
         </is>
       </c>
-      <c r="AD4" t="inlineStr"/>
       <c r="AE4" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
-      <c r="AF4" t="inlineStr"/>
-      <c r="AG4" t="inlineStr"/>
-      <c r="AH4" t="inlineStr"/>
-      <c r="AI4" t="inlineStr"/>
       <c r="AJ4" t="n">
         <v>0.06</v>
       </c>
@@ -1243,7 +1214,6 @@
           <t>bc4a811c-671b-4617-b8a9-4f0d85c16781</t>
         </is>
       </c>
-      <c r="AX4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1270,7 +1240,6 @@
           <t>Classical</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr">
         <is>
           <t>Performance (singing)</t>
@@ -1309,7 +1278,6 @@
           <t>Doctor Amal Al-Hazmi</t>
         </is>
       </c>
-      <c r="R5" t="inlineStr"/>
       <c r="S5" s="10" t="inlineStr">
         <is>
           <t>Fraternum facere ignovisset dolore</t>
@@ -1333,8 +1301,6 @@
       <c r="Y5" t="n">
         <v>0.25</v>
       </c>
-      <c r="Z5" t="inlineStr"/>
-      <c r="AA5" t="inlineStr"/>
       <c r="AB5" t="inlineStr">
         <is>
           <t>Amal Al-Hazmi</t>
@@ -1355,10 +1321,6 @@
           <t>Female</t>
         </is>
       </c>
-      <c r="AF5" t="inlineStr"/>
-      <c r="AG5" t="inlineStr"/>
-      <c r="AH5" t="inlineStr"/>
-      <c r="AI5" t="inlineStr"/>
       <c r="AJ5" t="n">
         <v>0.06</v>
       </c>
@@ -1409,7 +1371,6 @@
           <t>8be91e0c-4b52-45bc-9b09-bd3da5c9019a</t>
         </is>
       </c>
-      <c r="AX5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1436,7 +1397,6 @@
           <t>Classical</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
           <t>Esoteric: Apostasy</t>
@@ -1475,7 +1435,6 @@
           <t>Amira Ahmadi</t>
         </is>
       </c>
-      <c r="R6" t="inlineStr"/>
       <c r="S6" s="10" t="inlineStr">
         <is>
           <t>Mandatis cupiditas militibus coepit pilis omnemque nuntiato accumsan liberius itinere imperia cruciatusque reliquorum moribus verbigenus</t>
@@ -1499,8 +1458,6 @@
       <c r="Y6" t="n">
         <v>0</v>
       </c>
-      <c r="Z6" t="inlineStr"/>
-      <c r="AA6" t="inlineStr"/>
       <c r="AB6" t="inlineStr">
         <is>
           <t>Amira Ahmadi</t>
@@ -1511,16 +1468,11 @@
           <t>_names_arabic_surnames</t>
         </is>
       </c>
-      <c r="AD6" t="inlineStr"/>
       <c r="AE6" t="inlineStr">
         <is>
           <t>Female</t>
         </is>
       </c>
-      <c r="AF6" t="inlineStr"/>
-      <c r="AG6" t="inlineStr"/>
-      <c r="AH6" t="inlineStr"/>
-      <c r="AI6" t="inlineStr"/>
       <c r="AJ6" t="n">
         <v>0.06</v>
       </c>
@@ -1571,7 +1523,6 @@
           <t>b0b10d4d-851b-4602-9cc2-8b62050431f0</t>
         </is>
       </c>
-      <c r="AX6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1598,7 +1549,6 @@
           <t>Common</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr">
         <is>
           <t>Craft (scrivening)</t>
@@ -1637,7 +1587,6 @@
           <t>Marilène Doux</t>
         </is>
       </c>
-      <c r="R7" t="inlineStr"/>
       <c r="S7" s="10" t="inlineStr">
         <is>
           <t>The Regrettable Violations of The Chief Sinner on the Dire Subject of Scrivening</t>
@@ -1661,8 +1610,6 @@
       <c r="Y7" t="n">
         <v>0.25</v>
       </c>
-      <c r="Z7" t="inlineStr"/>
-      <c r="AA7" t="inlineStr"/>
       <c r="AB7" t="inlineStr">
         <is>
           <t>Marilène Doux</t>
@@ -1673,16 +1620,11 @@
           <t>_names_french_surnames</t>
         </is>
       </c>
-      <c r="AD7" t="inlineStr"/>
       <c r="AE7" t="inlineStr">
         <is>
           <t>Female</t>
         </is>
       </c>
-      <c r="AF7" t="inlineStr"/>
-      <c r="AG7" t="inlineStr"/>
-      <c r="AH7" t="inlineStr"/>
-      <c r="AI7" t="inlineStr"/>
       <c r="AJ7" t="n">
         <v>0.06</v>
       </c>
@@ -1733,7 +1675,6 @@
           <t>e5693347-9b78-49d6-98d8-db476443f9d9</t>
         </is>
       </c>
-      <c r="AX7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1760,7 +1701,6 @@
           <t>Common</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr">
         <is>
           <t>Weapon Focus</t>
@@ -1799,7 +1739,6 @@
           <t>Doctor Raja Al-Zayani</t>
         </is>
       </c>
-      <c r="R8" t="inlineStr"/>
       <c r="S8" s="10" t="inlineStr">
         <is>
           <t>Ásketill Eriksdotter and Corruptions: Aspects of Weapon Focuing</t>
@@ -1823,8 +1762,6 @@
       <c r="Y8" t="n">
         <v>1</v>
       </c>
-      <c r="Z8" t="inlineStr"/>
-      <c r="AA8" t="inlineStr"/>
       <c r="AB8" t="inlineStr">
         <is>
           <t>Raja Al-Zayani</t>
@@ -1845,10 +1782,6 @@
           <t>Female</t>
         </is>
       </c>
-      <c r="AF8" t="inlineStr"/>
-      <c r="AG8" t="inlineStr"/>
-      <c r="AH8" t="inlineStr"/>
-      <c r="AI8" t="inlineStr"/>
       <c r="AJ8" t="n">
         <v>0.06</v>
       </c>
@@ -1899,7 +1832,6 @@
           <t>1bddc2f1-8051-41b0-bd78-f069cd8daf2c</t>
         </is>
       </c>
-      <c r="AX8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1926,7 +1858,6 @@
           <t>Common</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr">
         <is>
           <t>Profession (chamberlain)</t>
@@ -1965,7 +1896,6 @@
           <t>Decima Suetonia</t>
         </is>
       </c>
-      <c r="R9" t="inlineStr"/>
       <c r="S9" s="10" t="inlineStr">
         <is>
           <t>Chamberlain's Craft, a Malignant Discernment</t>
@@ -1989,8 +1919,6 @@
       <c r="Y9" t="n">
         <v>1</v>
       </c>
-      <c r="Z9" t="inlineStr"/>
-      <c r="AA9" t="inlineStr"/>
       <c r="AB9" t="inlineStr">
         <is>
           <t>Decima Suetonia</t>
@@ -2001,16 +1929,11 @@
           <t>_names_roman_surnames</t>
         </is>
       </c>
-      <c r="AD9" t="inlineStr"/>
       <c r="AE9" t="inlineStr">
         <is>
           <t>Female</t>
         </is>
       </c>
-      <c r="AF9" t="inlineStr"/>
-      <c r="AG9" t="inlineStr"/>
-      <c r="AH9" t="inlineStr"/>
-      <c r="AI9" t="inlineStr"/>
       <c r="AJ9" t="n">
         <v>0.06</v>
       </c>
@@ -2061,7 +1984,6 @@
           <t>7fd917b6-1416-41c2-9221-ebb855335d90</t>
         </is>
       </c>
-      <c r="AX9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -2088,7 +2010,6 @@
           <t>Common</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
         <is>
           <t>Profession (lawyer)</t>
@@ -2127,7 +2048,6 @@
           <t>Her Honor Anaëlle Mandrillon</t>
         </is>
       </c>
-      <c r="R10" t="inlineStr"/>
       <c r="S10" s="10" t="inlineStr">
         <is>
           <t>Lawyering, a Mystic Winding</t>
@@ -2151,8 +2071,6 @@
       <c r="Y10" t="n">
         <v>0.01</v>
       </c>
-      <c r="Z10" t="inlineStr"/>
-      <c r="AA10" t="inlineStr"/>
       <c r="AB10" t="inlineStr">
         <is>
           <t>Anaëlle Mandrillon</t>
@@ -2173,10 +2091,6 @@
           <t>Female</t>
         </is>
       </c>
-      <c r="AF10" t="inlineStr"/>
-      <c r="AG10" t="inlineStr"/>
-      <c r="AH10" t="inlineStr"/>
-      <c r="AI10" t="inlineStr"/>
       <c r="AJ10" t="n">
         <v>0.06</v>
       </c>
@@ -2227,7 +2141,6 @@
           <t>ce4ced62-ed36-4033-b81c-7e33e675d538</t>
         </is>
       </c>
-      <c r="AX10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -2254,7 +2167,6 @@
           <t>Elvish</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr">
         <is>
           <t>Running</t>
@@ -2293,7 +2205,6 @@
           <t>Finnr Nielsen</t>
         </is>
       </c>
-      <c r="R11" t="inlineStr"/>
       <c r="S11" s="11" t="inlineStr">
         <is>
           <t>Si gollor drû nostor gwirith ferais iell eredh uireb than</t>
@@ -2317,8 +2228,6 @@
       <c r="Y11" t="n">
         <v>0.02</v>
       </c>
-      <c r="Z11" t="inlineStr"/>
-      <c r="AA11" t="inlineStr"/>
       <c r="AB11" t="inlineStr">
         <is>
           <t>Finnr Nielsen</t>
@@ -2329,16 +2238,11 @@
           <t>_names_norse_surnames_male</t>
         </is>
       </c>
-      <c r="AD11" t="inlineStr"/>
       <c r="AE11" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
-      <c r="AF11" t="inlineStr"/>
-      <c r="AG11" t="inlineStr"/>
-      <c r="AH11" t="inlineStr"/>
-      <c r="AI11" t="inlineStr"/>
       <c r="AJ11" t="n">
         <v>0.06</v>
       </c>
@@ -2389,7 +2293,1646 @@
           <t>3c7a2683-6e0c-4ca9-88f0-06b43de77888</t>
         </is>
       </c>
-      <c r="AX11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" t="n">
+        <v>667</v>
+      </c>
+      <c r="E12" t="n">
+        <v>43</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Performance (dancing)</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Performance (dancing)</t>
+        </is>
+      </c>
+      <c r="J12" t="n">
+        <v>2</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>3</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>1</v>
+      </c>
+      <c r="O12" t="n">
+        <v>1095</v>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>The Veniality of Fernand Delavigne, on the Subject of Dancing</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>Her Ladyship Jocelin Massis</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr"/>
+      <c r="S12" s="10" t="inlineStr">
+        <is>
+          <t>The Veniality of Fernand Delavigne, on the Subject of Dancing</t>
+        </is>
+      </c>
+      <c r="T12" t="n">
+        <v>4</v>
+      </c>
+      <c r="U12" t="n">
+        <v>4</v>
+      </c>
+      <c r="V12" t="n">
+        <v>44</v>
+      </c>
+      <c r="W12" t="n">
+        <v>5</v>
+      </c>
+      <c r="X12" t="n">
+        <v>4</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="Z12" t="inlineStr"/>
+      <c r="AA12" t="inlineStr"/>
+      <c r="AB12" t="inlineStr">
+        <is>
+          <t>Jocelin Massis</t>
+        </is>
+      </c>
+      <c r="AC12" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AD12" t="inlineStr">
+        <is>
+          <t>Her Ladyship</t>
+        </is>
+      </c>
+      <c r="AE12" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AF12" t="inlineStr"/>
+      <c r="AG12" t="inlineStr"/>
+      <c r="AH12" t="inlineStr"/>
+      <c r="AI12" t="inlineStr"/>
+      <c r="AJ12" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK12" t="inlineStr">
+        <is>
+          <t>{the_1} {negative_1} of {person_1}, on the Subject of {topic}</t>
+        </is>
+      </c>
+      <c r="AL12" t="inlineStr">
+        <is>
+          <t>Dancing</t>
+        </is>
+      </c>
+      <c r="AM12" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN12" t="n">
+        <v>261</v>
+      </c>
+      <c r="AO12" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="AP12" t="n">
+        <v>834</v>
+      </c>
+      <c r="AQ12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU12" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV12" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW12" t="inlineStr">
+        <is>
+          <t>eaf0b5c0-e297-4c2d-87d2-c004c1624a54</t>
+        </is>
+      </c>
+      <c r="AX12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>2</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E13" t="n">
+        <v>63</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Regional</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Knowledge (history)</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Knowledge (history)</t>
+        </is>
+      </c>
+      <c r="J13" t="n">
+        <v>1</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>1</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>1</v>
+      </c>
+      <c r="O13" t="n">
+        <v>440</v>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>The Necromantic Jaunt: Concert of Rome</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>Guðríðr Nilsson</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr"/>
+      <c r="S13" s="10" t="inlineStr">
+        <is>
+          <t>Περιφερείας θέσθαι λοιπὴν περιεχόμενα γραμμαὶ περιφέρειαν]</t>
+        </is>
+      </c>
+      <c r="T13" t="n">
+        <v>6</v>
+      </c>
+      <c r="U13" t="n">
+        <v>6</v>
+      </c>
+      <c r="V13" t="n">
+        <v>50</v>
+      </c>
+      <c r="W13" t="n">
+        <v>194</v>
+      </c>
+      <c r="X13" t="n">
+        <v>193</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="Z13" t="inlineStr"/>
+      <c r="AA13" t="inlineStr"/>
+      <c r="AB13" t="inlineStr">
+        <is>
+          <t>Guðríðr Nilsson</t>
+        </is>
+      </c>
+      <c r="AC13" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_male</t>
+        </is>
+      </c>
+      <c r="AD13" t="inlineStr"/>
+      <c r="AE13" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AF13" t="inlineStr"/>
+      <c r="AG13" t="inlineStr"/>
+      <c r="AH13" t="inlineStr"/>
+      <c r="AI13" t="inlineStr"/>
+      <c r="AJ13" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK13" t="inlineStr">
+        <is>
+          <t>The {adjective_1} {noun_1}: {history_of} {place_city}</t>
+        </is>
+      </c>
+      <c r="AL13" t="inlineStr">
+        <is>
+          <t>History</t>
+        </is>
+      </c>
+      <c r="AM13" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN13" t="n">
+        <v>390</v>
+      </c>
+      <c r="AO13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP13" t="n">
+        <v>50</v>
+      </c>
+      <c r="AQ13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU13" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV13" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW13" t="inlineStr">
+        <is>
+          <t>863f667e-8bfe-4c07-a821-816a610860cf</t>
+        </is>
+      </c>
+      <c r="AX13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" t="n">
+        <v>750</v>
+      </c>
+      <c r="E14" t="n">
+        <v>47</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Regional</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Esoteric: Judge’s Choice</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Craft (wheelwright)</t>
+        </is>
+      </c>
+      <c r="J14" t="n">
+        <v>3</v>
+      </c>
+      <c r="K14" t="n">
+        <v>1</v>
+      </c>
+      <c r="L14" t="n">
+        <v>4</v>
+      </c>
+      <c r="M14" t="n">
+        <v>2</v>
+      </c>
+      <c r="N14" t="n">
+        <v>1</v>
+      </c>
+      <c r="O14" t="n">
+        <v>4966</v>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>The Imperfection of Hervé Delevingne, on the Subject of Wheelwrighting</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>Rasheed Baba</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr"/>
+      <c r="S14" s="10" t="inlineStr">
+        <is>
+          <t>Ἐλάσσονες πρὸς ἐφ' τὰ μόνας ἀναγράψαι ἐπιφάνειά δοθείσῃ κέντρον ὀρθαῖς δίχα γραμμὴ πλευραῖς ἴσα</t>
+        </is>
+      </c>
+      <c r="T14" t="n">
+        <v>5</v>
+      </c>
+      <c r="U14" t="n">
+        <v>5</v>
+      </c>
+      <c r="V14" t="n">
+        <v>17</v>
+      </c>
+      <c r="W14" t="n">
+        <v>27</v>
+      </c>
+      <c r="X14" t="n">
+        <v>26</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="Z14" t="inlineStr"/>
+      <c r="AA14" t="inlineStr"/>
+      <c r="AB14" t="inlineStr">
+        <is>
+          <t>Rasheed Baba</t>
+        </is>
+      </c>
+      <c r="AC14" t="inlineStr">
+        <is>
+          <t>_names_arabic_surnames</t>
+        </is>
+      </c>
+      <c r="AD14" t="inlineStr"/>
+      <c r="AE14" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AF14" t="inlineStr"/>
+      <c r="AG14" t="inlineStr"/>
+      <c r="AH14" t="inlineStr"/>
+      <c r="AI14" t="inlineStr"/>
+      <c r="AJ14" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK14" t="inlineStr">
+        <is>
+          <t>{the_1} {negative_1} of {person_1}, on the Subject of {topic}</t>
+        </is>
+      </c>
+      <c r="AL14" t="inlineStr">
+        <is>
+          <t>Wheelwrighting</t>
+        </is>
+      </c>
+      <c r="AM14" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN14" t="n">
+        <v>278</v>
+      </c>
+      <c r="AO14" t="n">
+        <v>5</v>
+      </c>
+      <c r="AP14" t="n">
+        <v>938</v>
+      </c>
+      <c r="AQ14" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AR14" t="n">
+        <v>3750</v>
+      </c>
+      <c r="AS14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU14" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV14" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW14" t="inlineStr">
+        <is>
+          <t>33862c9a-c4ed-4ca2-85f7-3920259b8ec5</t>
+        </is>
+      </c>
+      <c r="AX14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Tablet</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Clay</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E15" t="n">
+        <v>750</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Elvish</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Craft (rune-carving)</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Craft (rune-carving)</t>
+        </is>
+      </c>
+      <c r="J15" t="n">
+        <v>3</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>3</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
+        <v>1</v>
+      </c>
+      <c r="O15" t="n">
+        <v>2120</v>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>Initiating Rune-Carving</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>The Venerable Océane Pechet</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr"/>
+      <c r="S15" s="11" t="inlineStr">
+        <is>
+          <t>Loch cerain brîg rhass helch celebrin</t>
+        </is>
+      </c>
+      <c r="T15" t="n">
+        <v>6</v>
+      </c>
+      <c r="U15" t="n">
+        <v>6</v>
+      </c>
+      <c r="V15" t="n">
+        <v>1477</v>
+      </c>
+      <c r="W15" t="n">
+        <v>13</v>
+      </c>
+      <c r="X15" t="n">
+        <v>12</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="Z15" t="inlineStr"/>
+      <c r="AA15" t="inlineStr"/>
+      <c r="AB15" t="inlineStr">
+        <is>
+          <t>Océane Pechet</t>
+        </is>
+      </c>
+      <c r="AC15" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AD15" t="inlineStr">
+        <is>
+          <t>The Venerable</t>
+        </is>
+      </c>
+      <c r="AE15" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AF15" t="inlineStr"/>
+      <c r="AG15" t="inlineStr"/>
+      <c r="AH15" t="inlineStr"/>
+      <c r="AI15" t="inlineStr"/>
+      <c r="AJ15" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="AK15" t="inlineStr">
+        <is>
+          <t>{verbing} {topic}</t>
+        </is>
+      </c>
+      <c r="AL15" t="inlineStr">
+        <is>
+          <t>Rune-Carving</t>
+        </is>
+      </c>
+      <c r="AM15" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="AN15" t="n">
+        <v>800</v>
+      </c>
+      <c r="AO15" t="n">
+        <v>4</v>
+      </c>
+      <c r="AP15" t="n">
+        <v>1320</v>
+      </c>
+      <c r="AQ15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU15" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV15" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW15" t="inlineStr">
+        <is>
+          <t>7eb8708d-a580-4660-83c8-671a4fd38f65</t>
+        </is>
+      </c>
+      <c r="AX15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E16" t="n">
+        <v>63</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Collegiate Wizardry</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Collegiate Wizardry</t>
+        </is>
+      </c>
+      <c r="J16" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>1</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>1</v>
+      </c>
+      <c r="O16" t="n">
+        <v>1370</v>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>Chronicles of The Dark Lord with emphasis upon Collegiate Wizardry</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>Ælfsige Lee</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr"/>
+      <c r="S16" s="10" t="inlineStr">
+        <is>
+          <t>Chronicles of The Dark Lord with emphasis upon Collegiate Wizardry</t>
+        </is>
+      </c>
+      <c r="T16" t="n">
+        <v>6</v>
+      </c>
+      <c r="U16" t="n">
+        <v>6</v>
+      </c>
+      <c r="V16" t="n">
+        <v>96</v>
+      </c>
+      <c r="W16" t="n">
+        <v>1</v>
+      </c>
+      <c r="X16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z16" t="inlineStr"/>
+      <c r="AA16" t="inlineStr"/>
+      <c r="AB16" t="inlineStr">
+        <is>
+          <t>Ælfsige Lee</t>
+        </is>
+      </c>
+      <c r="AC16" t="inlineStr">
+        <is>
+          <t>_names_anglo_saxon_surnames</t>
+        </is>
+      </c>
+      <c r="AD16" t="inlineStr"/>
+      <c r="AE16" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AF16" t="inlineStr"/>
+      <c r="AG16" t="inlineStr"/>
+      <c r="AH16" t="inlineStr"/>
+      <c r="AI16" t="inlineStr"/>
+      <c r="AJ16" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK16" t="inlineStr">
+        <is>
+          <t>{biography_starter} of {person_evil} with emphasis upon {topic}</t>
+        </is>
+      </c>
+      <c r="AL16" t="inlineStr">
+        <is>
+          <t>Collegiate Wizardry</t>
+        </is>
+      </c>
+      <c r="AM16" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN16" t="n">
+        <v>370</v>
+      </c>
+      <c r="AO16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP16" t="n">
+        <v>1000</v>
+      </c>
+      <c r="AQ16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV16" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW16" t="inlineStr">
+        <is>
+          <t>fa1c1f29-e55b-4df1-b255-90a5e7db2571</t>
+        </is>
+      </c>
+      <c r="AX16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" t="n">
+        <v>500</v>
+      </c>
+      <c r="E17" t="n">
+        <v>32</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Lockpicking</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Lockpicking</t>
+        </is>
+      </c>
+      <c r="J17" t="n">
+        <v>1</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" t="n">
+        <v>2</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O17" t="n">
+        <v>402</v>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>The Orphic Migration of Qualms: Lockpicking</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>Stigr Madsen</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr"/>
+      <c r="S17" s="10" t="inlineStr">
+        <is>
+          <t>The Orphic Migration of Qualms: Lockpicking</t>
+        </is>
+      </c>
+      <c r="T17" t="n">
+        <v>3</v>
+      </c>
+      <c r="U17" t="n">
+        <v>3</v>
+      </c>
+      <c r="V17" t="n">
+        <v>31</v>
+      </c>
+      <c r="W17" t="n">
+        <v>18</v>
+      </c>
+      <c r="X17" t="n">
+        <v>17</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="Z17" t="inlineStr"/>
+      <c r="AA17" t="inlineStr"/>
+      <c r="AB17" t="inlineStr">
+        <is>
+          <t>Stigr Madsen</t>
+        </is>
+      </c>
+      <c r="AC17" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_male</t>
+        </is>
+      </c>
+      <c r="AD17" t="inlineStr"/>
+      <c r="AE17" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AF17" t="inlineStr"/>
+      <c r="AG17" t="inlineStr"/>
+      <c r="AH17" t="inlineStr"/>
+      <c r="AI17" t="inlineStr"/>
+      <c r="AJ17" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK17" t="inlineStr">
+        <is>
+          <t>The {adjective_1} {noun_1} of {noun_2}: {topic}</t>
+        </is>
+      </c>
+      <c r="AL17" t="inlineStr">
+        <is>
+          <t>Lockpicking</t>
+        </is>
+      </c>
+      <c r="AM17" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN17" t="n">
+        <v>195</v>
+      </c>
+      <c r="AO17" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AP17" t="n">
+        <v>207</v>
+      </c>
+      <c r="AQ17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU17" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV17" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW17" t="inlineStr">
+        <is>
+          <t>2f082724-75a5-480f-8d79-b472b9364bfa</t>
+        </is>
+      </c>
+      <c r="AX17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Scroll</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Fine Papyrus</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>4</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E18" t="n">
+        <v>68</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Elvish</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Acrobatics</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Acrobatics</t>
+        </is>
+      </c>
+      <c r="J18" t="n">
+        <v>1</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" t="n">
+        <v>1</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" t="n">
+        <v>1</v>
+      </c>
+      <c r="O18" t="n">
+        <v>430</v>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>Correspondence in the Matter of Tumbling by Dimitri Hébras</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>Ismaël Lebas</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr"/>
+      <c r="S18" s="11" t="inlineStr">
+        <is>
+          <t>Gwilith doer curunír gwann mâl hwiniol rîf sautha haim aeruil uidafnen</t>
+        </is>
+      </c>
+      <c r="T18" t="n">
+        <v>6</v>
+      </c>
+      <c r="U18" t="n">
+        <v>6</v>
+      </c>
+      <c r="V18" t="n">
+        <v>1641</v>
+      </c>
+      <c r="W18" t="n">
+        <v>64</v>
+      </c>
+      <c r="X18" t="n">
+        <v>63</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="Z18" t="inlineStr"/>
+      <c r="AA18" t="inlineStr"/>
+      <c r="AB18" t="inlineStr">
+        <is>
+          <t>Ismaël Lebas</t>
+        </is>
+      </c>
+      <c r="AC18" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AD18" t="inlineStr"/>
+      <c r="AE18" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AF18" t="inlineStr"/>
+      <c r="AG18" t="inlineStr"/>
+      <c r="AH18" t="inlineStr"/>
+      <c r="AI18" t="inlineStr"/>
+      <c r="AJ18" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK18" t="inlineStr">
+        <is>
+          <t>{communication} {conjunction_about} {topic} {conjunction_by} {person_1}</t>
+        </is>
+      </c>
+      <c r="AL18" t="inlineStr">
+        <is>
+          <t>Tumbling</t>
+        </is>
+      </c>
+      <c r="AM18" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AN18" t="n">
+        <v>330</v>
+      </c>
+      <c r="AO18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP18" t="n">
+        <v>100</v>
+      </c>
+      <c r="AQ18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV18" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW18" t="inlineStr">
+        <is>
+          <t>c799abd3-1568-4cf7-b204-9db28078ec88</t>
+        </is>
+      </c>
+      <c r="AX18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>2</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E19" t="n">
+        <v>63</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Classical</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Craft (tinkering)</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Craft (tinkering)</t>
+        </is>
+      </c>
+      <c r="J19" t="n">
+        <v>3</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" t="n">
+        <v>3</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0</v>
+      </c>
+      <c r="N19" t="n">
+        <v>1</v>
+      </c>
+      <c r="O19" t="n">
+        <v>1710</v>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>Judging Tinkering</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>Duchess Cosette d'Aguesseau</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr"/>
+      <c r="S19" s="10" t="inlineStr">
+        <is>
+          <t>Diuturnitate itinere corrupti culpa</t>
+        </is>
+      </c>
+      <c r="T19" t="n">
+        <v>6</v>
+      </c>
+      <c r="U19" t="n">
+        <v>6</v>
+      </c>
+      <c r="V19" t="n">
+        <v>60</v>
+      </c>
+      <c r="W19" t="n">
+        <v>20</v>
+      </c>
+      <c r="X19" t="n">
+        <v>19</v>
+      </c>
+      <c r="Y19" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="Z19" t="inlineStr"/>
+      <c r="AA19" t="inlineStr"/>
+      <c r="AB19" t="inlineStr">
+        <is>
+          <t>Cosette d'Aguesseau</t>
+        </is>
+      </c>
+      <c r="AC19" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AD19" t="inlineStr">
+        <is>
+          <t>Duchess</t>
+        </is>
+      </c>
+      <c r="AE19" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AF19" t="inlineStr"/>
+      <c r="AG19" t="inlineStr"/>
+      <c r="AH19" t="inlineStr"/>
+      <c r="AI19" t="inlineStr"/>
+      <c r="AJ19" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK19" t="inlineStr">
+        <is>
+          <t>{verbing} {topic}</t>
+        </is>
+      </c>
+      <c r="AL19" t="inlineStr">
+        <is>
+          <t>Tinkering</t>
+        </is>
+      </c>
+      <c r="AM19" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN19" t="n">
+        <v>390</v>
+      </c>
+      <c r="AO19" t="n">
+        <v>4</v>
+      </c>
+      <c r="AP19" t="n">
+        <v>1320</v>
+      </c>
+      <c r="AQ19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV19" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW19" t="inlineStr">
+        <is>
+          <t>af34b88c-d9aa-4653-9abe-0058856b1f37</t>
+        </is>
+      </c>
+      <c r="AX19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" t="n">
+        <v>500</v>
+      </c>
+      <c r="E20" t="n">
+        <v>32</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Craft (fletching)</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Craft (fletching)</t>
+        </is>
+      </c>
+      <c r="J20" t="n">
+        <v>1</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" t="n">
+        <v>2</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" t="n">
+        <v>1</v>
+      </c>
+      <c r="O20" t="n">
+        <v>402</v>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>The Faults of Lucia Simplicinia, Considering Fletching</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>Eugénie Grose le Petit</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr"/>
+      <c r="S20" s="10" t="inlineStr">
+        <is>
+          <t>The Faults of Lucia Simplicinia, Considering Fletching</t>
+        </is>
+      </c>
+      <c r="T20" t="n">
+        <v>3</v>
+      </c>
+      <c r="U20" t="n">
+        <v>3</v>
+      </c>
+      <c r="V20" t="n">
+        <v>42</v>
+      </c>
+      <c r="W20" t="n">
+        <v>24</v>
+      </c>
+      <c r="X20" t="n">
+        <v>23</v>
+      </c>
+      <c r="Y20" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="Z20" t="inlineStr"/>
+      <c r="AA20" t="inlineStr">
+        <is>
+          <t>le Petit</t>
+        </is>
+      </c>
+      <c r="AB20" t="inlineStr">
+        <is>
+          <t>Eugénie Grose</t>
+        </is>
+      </c>
+      <c r="AC20" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AD20" t="inlineStr"/>
+      <c r="AE20" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AF20" t="inlineStr"/>
+      <c r="AG20" t="inlineStr"/>
+      <c r="AH20" t="inlineStr"/>
+      <c r="AI20" t="inlineStr"/>
+      <c r="AJ20" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK20" t="inlineStr">
+        <is>
+          <t>{the_1} {negative_1} of {person_1}, Considering {topic}</t>
+        </is>
+      </c>
+      <c r="AL20" t="inlineStr">
+        <is>
+          <t>Fletching</t>
+        </is>
+      </c>
+      <c r="AM20" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN20" t="n">
+        <v>195</v>
+      </c>
+      <c r="AO20" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AP20" t="n">
+        <v>207</v>
+      </c>
+      <c r="AQ20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU20" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV20" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW20" t="inlineStr">
+        <is>
+          <t>f8fbadee-377c-4c3e-bcfd-93fd736a5826</t>
+        </is>
+      </c>
+      <c r="AX20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>2</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1334</v>
+      </c>
+      <c r="E21" t="n">
+        <v>84</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Classical</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
+      <c r="J21" t="n">
+        <v>1</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" t="n">
+        <v>1</v>
+      </c>
+      <c r="O21" t="n">
+        <v>1828</v>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>Transactions of Æthelthryth Hollyngworth Relating to Engineering</t>
+        </is>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>Doctor Gunnar Halvorsen</t>
+        </is>
+      </c>
+      <c r="R21" t="inlineStr"/>
+      <c r="S21" s="10" t="inlineStr">
+        <is>
+          <t>Capta contulerunt tabernaculis redderet ascendere ingenti commutato</t>
+        </is>
+      </c>
+      <c r="T21" t="n">
+        <v>8</v>
+      </c>
+      <c r="U21" t="n">
+        <v>8</v>
+      </c>
+      <c r="V21" t="n">
+        <v>368</v>
+      </c>
+      <c r="W21" t="n">
+        <v>1</v>
+      </c>
+      <c r="X21" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z21" t="inlineStr"/>
+      <c r="AA21" t="inlineStr"/>
+      <c r="AB21" t="inlineStr">
+        <is>
+          <t>Gunnar Halvorsen</t>
+        </is>
+      </c>
+      <c r="AC21" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_male</t>
+        </is>
+      </c>
+      <c r="AD21" t="inlineStr">
+        <is>
+          <t>Doctor</t>
+        </is>
+      </c>
+      <c r="AE21" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AF21" t="inlineStr"/>
+      <c r="AG21" t="inlineStr"/>
+      <c r="AH21" t="inlineStr"/>
+      <c r="AI21" t="inlineStr"/>
+      <c r="AJ21" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK21" t="inlineStr">
+        <is>
+          <t>{communication} of {person_1} {conjunction_about} {topic}</t>
+        </is>
+      </c>
+      <c r="AL21" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
+      <c r="AM21" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN21" t="n">
+        <v>494</v>
+      </c>
+      <c r="AO21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP21" t="n">
+        <v>1334</v>
+      </c>
+      <c r="AQ21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV21" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW21" t="inlineStr">
+        <is>
+          <t>6a09d45a-898e-49b6-a0e2-65457d1e6b4a</t>
+        </is>
+      </c>
+      <c r="AX21" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Works after DEFAULT FONT material
</commit_message>
<xml_diff>
--- a/books_spreadsheet_out.xlsx
+++ b/books_spreadsheet_out.xlsx
@@ -461,7 +461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AX21"/>
+  <dimension ref="A1:AX31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2319,7 +2319,6 @@
           <t>Common</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
         <is>
           <t>Performance (dancing)</t>
@@ -2358,7 +2357,6 @@
           <t>Her Ladyship Jocelin Massis</t>
         </is>
       </c>
-      <c r="R12" t="inlineStr"/>
       <c r="S12" s="10" t="inlineStr">
         <is>
           <t>The Veniality of Fernand Delavigne, on the Subject of Dancing</t>
@@ -2382,8 +2380,6 @@
       <c r="Y12" t="n">
         <v>0.5</v>
       </c>
-      <c r="Z12" t="inlineStr"/>
-      <c r="AA12" t="inlineStr"/>
       <c r="AB12" t="inlineStr">
         <is>
           <t>Jocelin Massis</t>
@@ -2404,10 +2400,6 @@
           <t>Female</t>
         </is>
       </c>
-      <c r="AF12" t="inlineStr"/>
-      <c r="AG12" t="inlineStr"/>
-      <c r="AH12" t="inlineStr"/>
-      <c r="AI12" t="inlineStr"/>
       <c r="AJ12" t="n">
         <v>0.06</v>
       </c>
@@ -2458,7 +2450,6 @@
           <t>eaf0b5c0-e297-4c2d-87d2-c004c1624a54</t>
         </is>
       </c>
-      <c r="AX12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2485,7 +2476,6 @@
           <t>Regional</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr">
         <is>
           <t>Knowledge (history)</t>
@@ -2524,7 +2514,6 @@
           <t>Guðríðr Nilsson</t>
         </is>
       </c>
-      <c r="R13" t="inlineStr"/>
       <c r="S13" s="10" t="inlineStr">
         <is>
           <t>Περιφερείας θέσθαι λοιπὴν περιεχόμενα γραμμαὶ περιφέρειαν]</t>
@@ -2548,8 +2537,6 @@
       <c r="Y13" t="n">
         <v>0.05</v>
       </c>
-      <c r="Z13" t="inlineStr"/>
-      <c r="AA13" t="inlineStr"/>
       <c r="AB13" t="inlineStr">
         <is>
           <t>Guðríðr Nilsson</t>
@@ -2560,16 +2547,11 @@
           <t>_names_norse_surnames_male</t>
         </is>
       </c>
-      <c r="AD13" t="inlineStr"/>
       <c r="AE13" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
-      <c r="AF13" t="inlineStr"/>
-      <c r="AG13" t="inlineStr"/>
-      <c r="AH13" t="inlineStr"/>
-      <c r="AI13" t="inlineStr"/>
       <c r="AJ13" t="n">
         <v>0.06</v>
       </c>
@@ -2620,7 +2602,6 @@
           <t>863f667e-8bfe-4c07-a821-816a610860cf</t>
         </is>
       </c>
-      <c r="AX13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2647,7 +2628,6 @@
           <t>Regional</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr">
         <is>
           <t>Esoteric: Judge’s Choice</t>
@@ -2686,7 +2666,6 @@
           <t>Rasheed Baba</t>
         </is>
       </c>
-      <c r="R14" t="inlineStr"/>
       <c r="S14" s="10" t="inlineStr">
         <is>
           <t>Ἐλάσσονες πρὸς ἐφ' τὰ μόνας ἀναγράψαι ἐπιφάνειά δοθείσῃ κέντρον ὀρθαῖς δίχα γραμμὴ πλευραῖς ἴσα</t>
@@ -2710,8 +2689,6 @@
       <c r="Y14" t="n">
         <v>0.25</v>
       </c>
-      <c r="Z14" t="inlineStr"/>
-      <c r="AA14" t="inlineStr"/>
       <c r="AB14" t="inlineStr">
         <is>
           <t>Rasheed Baba</t>
@@ -2722,16 +2699,11 @@
           <t>_names_arabic_surnames</t>
         </is>
       </c>
-      <c r="AD14" t="inlineStr"/>
       <c r="AE14" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
-      <c r="AF14" t="inlineStr"/>
-      <c r="AG14" t="inlineStr"/>
-      <c r="AH14" t="inlineStr"/>
-      <c r="AI14" t="inlineStr"/>
       <c r="AJ14" t="n">
         <v>0.06</v>
       </c>
@@ -2782,7 +2754,6 @@
           <t>33862c9a-c4ed-4ca2-85f7-3920259b8ec5</t>
         </is>
       </c>
-      <c r="AX14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2809,7 +2780,6 @@
           <t>Elvish</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr">
         <is>
           <t>Craft (rune-carving)</t>
@@ -2848,7 +2818,6 @@
           <t>The Venerable Océane Pechet</t>
         </is>
       </c>
-      <c r="R15" t="inlineStr"/>
       <c r="S15" s="11" t="inlineStr">
         <is>
           <t>Loch cerain brîg rhass helch celebrin</t>
@@ -2872,8 +2841,6 @@
       <c r="Y15" t="n">
         <v>0.33</v>
       </c>
-      <c r="Z15" t="inlineStr"/>
-      <c r="AA15" t="inlineStr"/>
       <c r="AB15" t="inlineStr">
         <is>
           <t>Océane Pechet</t>
@@ -2894,10 +2861,6 @@
           <t>Female</t>
         </is>
       </c>
-      <c r="AF15" t="inlineStr"/>
-      <c r="AG15" t="inlineStr"/>
-      <c r="AH15" t="inlineStr"/>
-      <c r="AI15" t="inlineStr"/>
       <c r="AJ15" t="n">
         <v>0.75</v>
       </c>
@@ -2948,7 +2911,6 @@
           <t>7eb8708d-a580-4660-83c8-671a4fd38f65</t>
         </is>
       </c>
-      <c r="AX15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2975,7 +2937,6 @@
           <t>Common</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr">
         <is>
           <t>Collegiate Wizardry</t>
@@ -3014,7 +2975,6 @@
           <t>Ælfsige Lee</t>
         </is>
       </c>
-      <c r="R16" t="inlineStr"/>
       <c r="S16" s="10" t="inlineStr">
         <is>
           <t>Chronicles of The Dark Lord with emphasis upon Collegiate Wizardry</t>
@@ -3038,8 +2998,6 @@
       <c r="Y16" t="n">
         <v>1</v>
       </c>
-      <c r="Z16" t="inlineStr"/>
-      <c r="AA16" t="inlineStr"/>
       <c r="AB16" t="inlineStr">
         <is>
           <t>Ælfsige Lee</t>
@@ -3050,16 +3008,11 @@
           <t>_names_anglo_saxon_surnames</t>
         </is>
       </c>
-      <c r="AD16" t="inlineStr"/>
       <c r="AE16" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
-      <c r="AF16" t="inlineStr"/>
-      <c r="AG16" t="inlineStr"/>
-      <c r="AH16" t="inlineStr"/>
-      <c r="AI16" t="inlineStr"/>
       <c r="AJ16" t="n">
         <v>0.06</v>
       </c>
@@ -3110,7 +3063,6 @@
           <t>fa1c1f29-e55b-4df1-b255-90a5e7db2571</t>
         </is>
       </c>
-      <c r="AX16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -3137,7 +3089,6 @@
           <t>Common</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr">
         <is>
           <t>Lockpicking</t>
@@ -3176,7 +3127,6 @@
           <t>Stigr Madsen</t>
         </is>
       </c>
-      <c r="R17" t="inlineStr"/>
       <c r="S17" s="10" t="inlineStr">
         <is>
           <t>The Orphic Migration of Qualms: Lockpicking</t>
@@ -3200,8 +3150,6 @@
       <c r="Y17" t="n">
         <v>0.33</v>
       </c>
-      <c r="Z17" t="inlineStr"/>
-      <c r="AA17" t="inlineStr"/>
       <c r="AB17" t="inlineStr">
         <is>
           <t>Stigr Madsen</t>
@@ -3212,16 +3160,11 @@
           <t>_names_norse_surnames_male</t>
         </is>
       </c>
-      <c r="AD17" t="inlineStr"/>
       <c r="AE17" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
-      <c r="AF17" t="inlineStr"/>
-      <c r="AG17" t="inlineStr"/>
-      <c r="AH17" t="inlineStr"/>
-      <c r="AI17" t="inlineStr"/>
       <c r="AJ17" t="n">
         <v>0.06</v>
       </c>
@@ -3272,7 +3215,6 @@
           <t>2f082724-75a5-480f-8d79-b472b9364bfa</t>
         </is>
       </c>
-      <c r="AX17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -3299,7 +3241,6 @@
           <t>Elvish</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr">
         <is>
           <t>Acrobatics</t>
@@ -3338,7 +3279,6 @@
           <t>Ismaël Lebas</t>
         </is>
       </c>
-      <c r="R18" t="inlineStr"/>
       <c r="S18" s="11" t="inlineStr">
         <is>
           <t>Gwilith doer curunír gwann mâl hwiniol rîf sautha haim aeruil uidafnen</t>
@@ -3362,8 +3302,6 @@
       <c r="Y18" t="n">
         <v>0.1</v>
       </c>
-      <c r="Z18" t="inlineStr"/>
-      <c r="AA18" t="inlineStr"/>
       <c r="AB18" t="inlineStr">
         <is>
           <t>Ismaël Lebas</t>
@@ -3374,16 +3312,11 @@
           <t>_names_french_surnames</t>
         </is>
       </c>
-      <c r="AD18" t="inlineStr"/>
       <c r="AE18" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
-      <c r="AF18" t="inlineStr"/>
-      <c r="AG18" t="inlineStr"/>
-      <c r="AH18" t="inlineStr"/>
-      <c r="AI18" t="inlineStr"/>
       <c r="AJ18" t="n">
         <v>0.06</v>
       </c>
@@ -3434,7 +3367,6 @@
           <t>c799abd3-1568-4cf7-b204-9db28078ec88</t>
         </is>
       </c>
-      <c r="AX18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -3461,7 +3393,6 @@
           <t>Classical</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr">
         <is>
           <t>Craft (tinkering)</t>
@@ -3500,7 +3431,6 @@
           <t>Duchess Cosette d'Aguesseau</t>
         </is>
       </c>
-      <c r="R19" t="inlineStr"/>
       <c r="S19" s="10" t="inlineStr">
         <is>
           <t>Diuturnitate itinere corrupti culpa</t>
@@ -3524,8 +3454,6 @@
       <c r="Y19" t="n">
         <v>0.33</v>
       </c>
-      <c r="Z19" t="inlineStr"/>
-      <c r="AA19" t="inlineStr"/>
       <c r="AB19" t="inlineStr">
         <is>
           <t>Cosette d'Aguesseau</t>
@@ -3546,10 +3474,6 @@
           <t>Female</t>
         </is>
       </c>
-      <c r="AF19" t="inlineStr"/>
-      <c r="AG19" t="inlineStr"/>
-      <c r="AH19" t="inlineStr"/>
-      <c r="AI19" t="inlineStr"/>
       <c r="AJ19" t="n">
         <v>0.06</v>
       </c>
@@ -3600,7 +3524,6 @@
           <t>af34b88c-d9aa-4653-9abe-0058856b1f37</t>
         </is>
       </c>
-      <c r="AX19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -3627,7 +3550,6 @@
           <t>Common</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr">
         <is>
           <t>Craft (fletching)</t>
@@ -3666,7 +3588,6 @@
           <t>Eugénie Grose le Petit</t>
         </is>
       </c>
-      <c r="R20" t="inlineStr"/>
       <c r="S20" s="10" t="inlineStr">
         <is>
           <t>The Faults of Lucia Simplicinia, Considering Fletching</t>
@@ -3690,7 +3611,6 @@
       <c r="Y20" t="n">
         <v>0.33</v>
       </c>
-      <c r="Z20" t="inlineStr"/>
       <c r="AA20" t="inlineStr">
         <is>
           <t>le Petit</t>
@@ -3706,16 +3626,11 @@
           <t>_names_french_surnames</t>
         </is>
       </c>
-      <c r="AD20" t="inlineStr"/>
       <c r="AE20" t="inlineStr">
         <is>
           <t>Female</t>
         </is>
       </c>
-      <c r="AF20" t="inlineStr"/>
-      <c r="AG20" t="inlineStr"/>
-      <c r="AH20" t="inlineStr"/>
-      <c r="AI20" t="inlineStr"/>
       <c r="AJ20" t="n">
         <v>0.06</v>
       </c>
@@ -3766,7 +3681,6 @@
           <t>f8fbadee-377c-4c3e-bcfd-93fd736a5826</t>
         </is>
       </c>
-      <c r="AX20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -3793,7 +3707,6 @@
           <t>Classical</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr">
         <is>
           <t>Engineering</t>
@@ -3832,7 +3745,6 @@
           <t>Doctor Gunnar Halvorsen</t>
         </is>
       </c>
-      <c r="R21" t="inlineStr"/>
       <c r="S21" s="10" t="inlineStr">
         <is>
           <t>Capta contulerunt tabernaculis redderet ascendere ingenti commutato</t>
@@ -3856,8 +3768,6 @@
       <c r="Y21" t="n">
         <v>1</v>
       </c>
-      <c r="Z21" t="inlineStr"/>
-      <c r="AA21" t="inlineStr"/>
       <c r="AB21" t="inlineStr">
         <is>
           <t>Gunnar Halvorsen</t>
@@ -3878,10 +3788,6 @@
           <t>Male</t>
         </is>
       </c>
-      <c r="AF21" t="inlineStr"/>
-      <c r="AG21" t="inlineStr"/>
-      <c r="AH21" t="inlineStr"/>
-      <c r="AI21" t="inlineStr"/>
       <c r="AJ21" t="n">
         <v>0.06</v>
       </c>
@@ -3932,7 +3838,1646 @@
           <t>6a09d45a-898e-49b6-a0e2-65457d1e6b4a</t>
         </is>
       </c>
-      <c r="AX21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>2</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1334</v>
+      </c>
+      <c r="E22" t="n">
+        <v>84</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Regional</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Black Lore of Zahar</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Black Lore of Zahar</t>
+        </is>
+      </c>
+      <c r="J22" t="n">
+        <v>1</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0</v>
+      </c>
+      <c r="N22" t="n">
+        <v>1</v>
+      </c>
+      <c r="O22" t="n">
+        <v>535</v>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>Condemnation of Bahruz the Prophet and Black Lore</t>
+        </is>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>Cécile Rigal</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr"/>
+      <c r="S22" s="10" t="inlineStr">
+        <is>
+          <t>Τοῖς ἐὰν κύκλον κάθετος μείζων ἔχουσαι εἶναι ια΄ συσταθῶσιν πλευρὰ περιέχουσιν τὸ μβ΄</t>
+        </is>
+      </c>
+      <c r="T22" t="n">
+        <v>8</v>
+      </c>
+      <c r="U22" t="n">
+        <v>8</v>
+      </c>
+      <c r="V22" t="n">
+        <v>44</v>
+      </c>
+      <c r="W22" t="n">
+        <v>587</v>
+      </c>
+      <c r="X22" t="n">
+        <v>586</v>
+      </c>
+      <c r="Y22" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="Z22" t="inlineStr"/>
+      <c r="AA22" t="inlineStr"/>
+      <c r="AB22" t="inlineStr">
+        <is>
+          <t>Cécile Rigal</t>
+        </is>
+      </c>
+      <c r="AC22" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AD22" t="inlineStr"/>
+      <c r="AE22" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AF22" t="inlineStr"/>
+      <c r="AG22" t="inlineStr"/>
+      <c r="AH22" t="inlineStr"/>
+      <c r="AI22" t="inlineStr"/>
+      <c r="AJ22" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK22" t="inlineStr">
+        <is>
+          <t>{biography_starter} of {person_famous} and {topic}</t>
+        </is>
+      </c>
+      <c r="AL22" t="inlineStr">
+        <is>
+          <t>Black Lore</t>
+        </is>
+      </c>
+      <c r="AM22" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN22" t="n">
+        <v>521</v>
+      </c>
+      <c r="AO22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP22" t="n">
+        <v>14</v>
+      </c>
+      <c r="AQ22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU22" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV22" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW22" t="inlineStr">
+        <is>
+          <t>be3cab4c-00c9-423f-9c29-823ca79f2694</t>
+        </is>
+      </c>
+      <c r="AX22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Scroll</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Fine Papyrus</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>4</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E23" t="n">
+        <v>68</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Ancient</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Esoteric: Loremastery</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Mimicry</t>
+        </is>
+      </c>
+      <c r="J23" t="n">
+        <v>4</v>
+      </c>
+      <c r="K23" t="n">
+        <v>2</v>
+      </c>
+      <c r="L23" t="n">
+        <v>4</v>
+      </c>
+      <c r="M23" t="n">
+        <v>5</v>
+      </c>
+      <c r="N23" t="n">
+        <v>1</v>
+      </c>
+      <c r="O23" t="n">
+        <v>23631</v>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>Epistles of Lilou Guérillot and Godric Holderness in the Matter of Mimicry</t>
+        </is>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>His Grace Benjamin Mercier</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr"/>
+      <c r="S23" s="10" t="inlineStr">
+        <is>
+          <t>𐎬𐎸𐎽 𐎫𐎸𐎢𐏂𐎸𐎽 𐎬𐎠𐎸𐎱𐎨𐎽 𐎽𐎮𐎣𐎠𐎫𐎤𐎽 𐎤𐎦𐎤𐏂 𐎱𐎸𐏂𐎱𐎸𐎬 𐎥𐎠</t>
+        </is>
+      </c>
+      <c r="T23" t="n">
+        <v>6</v>
+      </c>
+      <c r="U23" t="n">
+        <v>6</v>
+      </c>
+      <c r="V23" t="n">
+        <v>770</v>
+      </c>
+      <c r="W23" t="n">
+        <v>13</v>
+      </c>
+      <c r="X23" t="n">
+        <v>12</v>
+      </c>
+      <c r="Y23" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="Z23" t="inlineStr"/>
+      <c r="AA23" t="inlineStr"/>
+      <c r="AB23" t="inlineStr">
+        <is>
+          <t>Benjamin Mercier</t>
+        </is>
+      </c>
+      <c r="AC23" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AD23" t="inlineStr">
+        <is>
+          <t>His Grace</t>
+        </is>
+      </c>
+      <c r="AE23" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AF23" t="inlineStr"/>
+      <c r="AG23" t="inlineStr"/>
+      <c r="AH23" t="inlineStr"/>
+      <c r="AI23" t="inlineStr"/>
+      <c r="AJ23" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK23" t="inlineStr">
+        <is>
+          <t>{communication} of {person_1} and {person_2} {conjunction_about} {topic}</t>
+        </is>
+      </c>
+      <c r="AL23" t="inlineStr">
+        <is>
+          <t>Mimicry</t>
+        </is>
+      </c>
+      <c r="AM23" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AN23" t="n">
+        <v>330</v>
+      </c>
+      <c r="AO23" t="n">
+        <v>10</v>
+      </c>
+      <c r="AP23" t="n">
+        <v>3301</v>
+      </c>
+      <c r="AQ23" t="n">
+        <v>10</v>
+      </c>
+      <c r="AR23" t="n">
+        <v>20000</v>
+      </c>
+      <c r="AS23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU23" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV23" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW23" t="inlineStr">
+        <is>
+          <t>9683b8c0-67c2-4077-9f48-ca8d0bc1d682</t>
+        </is>
+      </c>
+      <c r="AX23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Silver Foil</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" t="n">
+        <v>667</v>
+      </c>
+      <c r="E24" t="n">
+        <v>103</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Regional</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Navigation</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Navigation</t>
+        </is>
+      </c>
+      <c r="J24" t="n">
+        <v>2</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" t="n">
+        <v>3</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0</v>
+      </c>
+      <c r="N24" t="n">
+        <v>1</v>
+      </c>
+      <c r="O24" t="n">
+        <v>1759</v>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>Investigation of Navigation</t>
+        </is>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>Doctor Molde Pedersen</t>
+        </is>
+      </c>
+      <c r="R24" t="inlineStr"/>
+      <c r="S24" s="10" t="inlineStr">
+        <is>
+          <t>Σημείοις σημεῖα ἔσονται οὗ κέντρου</t>
+        </is>
+      </c>
+      <c r="T24" t="n">
+        <v>4</v>
+      </c>
+      <c r="U24" t="n">
+        <v>4</v>
+      </c>
+      <c r="V24" t="n">
+        <v>14</v>
+      </c>
+      <c r="W24" t="n">
+        <v>10</v>
+      </c>
+      <c r="X24" t="n">
+        <v>9</v>
+      </c>
+      <c r="Y24" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="Z24" t="inlineStr"/>
+      <c r="AA24" t="inlineStr"/>
+      <c r="AB24" t="inlineStr">
+        <is>
+          <t>Molde Pedersen</t>
+        </is>
+      </c>
+      <c r="AC24" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_male</t>
+        </is>
+      </c>
+      <c r="AD24" t="inlineStr">
+        <is>
+          <t>Doctor</t>
+        </is>
+      </c>
+      <c r="AE24" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AF24" t="inlineStr"/>
+      <c r="AG24" t="inlineStr"/>
+      <c r="AH24" t="inlineStr"/>
+      <c r="AI24" t="inlineStr"/>
+      <c r="AJ24" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="AK24" t="inlineStr">
+        <is>
+          <t>{study_of} of {topic}</t>
+        </is>
+      </c>
+      <c r="AL24" t="inlineStr">
+        <is>
+          <t>Navigation</t>
+        </is>
+      </c>
+      <c r="AM24" t="n">
+        <v>1.81</v>
+      </c>
+      <c r="AN24" t="n">
+        <v>1208</v>
+      </c>
+      <c r="AO24" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="AP24" t="n">
+        <v>551</v>
+      </c>
+      <c r="AQ24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU24" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV24" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW24" t="inlineStr">
+        <is>
+          <t>9b3f69f1-4972-4232-9ac8-d0f7594a2ecb</t>
+        </is>
+      </c>
+      <c r="AX24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>2</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E25" t="n">
+        <v>63</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Regional</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Mimicry</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Mimicry</t>
+        </is>
+      </c>
+      <c r="J25" t="n">
+        <v>1</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0</v>
+      </c>
+      <c r="L25" t="n">
+        <v>1</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0</v>
+      </c>
+      <c r="N25" t="n">
+        <v>1</v>
+      </c>
+      <c r="O25" t="n">
+        <v>870</v>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>Exchanges of Völund Olofsson in Regard to Mimicry</t>
+        </is>
+      </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>Benoît Cantin</t>
+        </is>
+      </c>
+      <c r="R25" t="inlineStr"/>
+      <c r="S25" s="10" t="inlineStr">
+        <is>
+          <t>Ὀρθὴ ἀνίσων γραμμῆς ἐναλλὰξ οὗ τῷ ἀπλατές κειμένων κοιναί</t>
+        </is>
+      </c>
+      <c r="T25" t="n">
+        <v>6</v>
+      </c>
+      <c r="U25" t="n">
+        <v>6</v>
+      </c>
+      <c r="V25" t="n">
+        <v>12</v>
+      </c>
+      <c r="W25" t="n">
+        <v>4</v>
+      </c>
+      <c r="X25" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y25" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="Z25" t="inlineStr"/>
+      <c r="AA25" t="inlineStr"/>
+      <c r="AB25" t="inlineStr">
+        <is>
+          <t>Benoît Cantin</t>
+        </is>
+      </c>
+      <c r="AC25" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AD25" t="inlineStr"/>
+      <c r="AE25" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AF25" t="inlineStr"/>
+      <c r="AG25" t="inlineStr"/>
+      <c r="AH25" t="inlineStr"/>
+      <c r="AI25" t="inlineStr"/>
+      <c r="AJ25" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK25" t="inlineStr">
+        <is>
+          <t>{communication} of {person_1} {conjunction_about} {topic}</t>
+        </is>
+      </c>
+      <c r="AL25" t="inlineStr">
+        <is>
+          <t>Mimicry</t>
+        </is>
+      </c>
+      <c r="AM25" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN25" t="n">
+        <v>370</v>
+      </c>
+      <c r="AO25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP25" t="n">
+        <v>500</v>
+      </c>
+      <c r="AQ25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU25" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV25" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW25" t="inlineStr">
+        <is>
+          <t>965eeb24-115a-4537-9f60-6fb1fc64032b</t>
+        </is>
+      </c>
+      <c r="AX25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" t="n">
+        <v>667</v>
+      </c>
+      <c r="E26" t="n">
+        <v>43</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Trap Finding</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Trap Finding</t>
+        </is>
+      </c>
+      <c r="J26" t="n">
+        <v>2</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0</v>
+      </c>
+      <c r="L26" t="n">
+        <v>3</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0</v>
+      </c>
+      <c r="N26" t="n">
+        <v>1</v>
+      </c>
+      <c r="O26" t="n">
+        <v>664</v>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>Survey of Trap Finding</t>
+        </is>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>Her Ladyship Madeleine Bélanger</t>
+        </is>
+      </c>
+      <c r="R26" t="inlineStr"/>
+      <c r="S26" s="10" t="inlineStr">
+        <is>
+          <t>Survey of Trap Finding</t>
+        </is>
+      </c>
+      <c r="T26" t="n">
+        <v>4</v>
+      </c>
+      <c r="U26" t="n">
+        <v>4</v>
+      </c>
+      <c r="V26" t="n">
+        <v>46</v>
+      </c>
+      <c r="W26" t="n">
+        <v>29</v>
+      </c>
+      <c r="X26" t="n">
+        <v>28</v>
+      </c>
+      <c r="Y26" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="Z26" t="inlineStr"/>
+      <c r="AA26" t="inlineStr"/>
+      <c r="AB26" t="inlineStr">
+        <is>
+          <t>Madeleine Bélanger</t>
+        </is>
+      </c>
+      <c r="AC26" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AD26" t="inlineStr">
+        <is>
+          <t>Her Ladyship</t>
+        </is>
+      </c>
+      <c r="AE26" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AF26" t="inlineStr"/>
+      <c r="AG26" t="inlineStr"/>
+      <c r="AH26" t="inlineStr"/>
+      <c r="AI26" t="inlineStr"/>
+      <c r="AJ26" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK26" t="inlineStr">
+        <is>
+          <t>{study_of} of {topic}</t>
+        </is>
+      </c>
+      <c r="AL26" t="inlineStr">
+        <is>
+          <t>Trap Finding</t>
+        </is>
+      </c>
+      <c r="AM26" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN26" t="n">
+        <v>247</v>
+      </c>
+      <c r="AO26" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="AP26" t="n">
+        <v>417</v>
+      </c>
+      <c r="AQ26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU26" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV26" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW26" t="inlineStr">
+        <is>
+          <t>ee19b6cd-0ce3-433a-9a3c-ecf69fb518a8</t>
+        </is>
+      </c>
+      <c r="AX26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Scroll</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Ordinary Papyrus</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>6</v>
+      </c>
+      <c r="D27" t="n">
+        <v>1334</v>
+      </c>
+      <c r="E27" t="n">
+        <v>93</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Magical Engineering</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Magical Engineering</t>
+        </is>
+      </c>
+      <c r="J27" t="n">
+        <v>1</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0</v>
+      </c>
+      <c r="L27" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0</v>
+      </c>
+      <c r="N27" t="n">
+        <v>1</v>
+      </c>
+      <c r="O27" t="n">
+        <v>1081</v>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>Setting Forth For Magical Engineering</t>
+        </is>
+      </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>Wilburh Pontius</t>
+        </is>
+      </c>
+      <c r="R27" t="inlineStr"/>
+      <c r="S27" s="10" t="inlineStr">
+        <is>
+          <t>Setting Forth For Magical Engineering</t>
+        </is>
+      </c>
+      <c r="T27" t="n">
+        <v>8</v>
+      </c>
+      <c r="U27" t="n">
+        <v>8</v>
+      </c>
+      <c r="V27" t="n">
+        <v>17</v>
+      </c>
+      <c r="W27" t="n">
+        <v>3</v>
+      </c>
+      <c r="X27" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="Z27" t="inlineStr"/>
+      <c r="AA27" t="inlineStr"/>
+      <c r="AB27" t="inlineStr">
+        <is>
+          <t>Wilburh Pontius</t>
+        </is>
+      </c>
+      <c r="AC27" t="inlineStr">
+        <is>
+          <t>_names_anglo_saxon_surnames</t>
+        </is>
+      </c>
+      <c r="AD27" t="inlineStr"/>
+      <c r="AE27" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AF27" t="inlineStr"/>
+      <c r="AG27" t="inlineStr"/>
+      <c r="AH27" t="inlineStr"/>
+      <c r="AI27" t="inlineStr"/>
+      <c r="AJ27" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK27" t="inlineStr">
+        <is>
+          <t>{verbing} {topic}</t>
+        </is>
+      </c>
+      <c r="AL27" t="inlineStr">
+        <is>
+          <t>Magical Engineering</t>
+        </is>
+      </c>
+      <c r="AM27" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AN27" t="n">
+        <v>414</v>
+      </c>
+      <c r="AO27" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP27" t="n">
+        <v>667</v>
+      </c>
+      <c r="AQ27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU27" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV27" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW27" t="inlineStr">
+        <is>
+          <t>e837b42f-1968-4517-ae93-392d36e311bf</t>
+        </is>
+      </c>
+      <c r="AX27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>2</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1334</v>
+      </c>
+      <c r="E28" t="n">
+        <v>84</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Seduction</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Seduction</t>
+        </is>
+      </c>
+      <c r="J28" t="n">
+        <v>1</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0</v>
+      </c>
+      <c r="N28" t="n">
+        <v>1</v>
+      </c>
+      <c r="O28" t="n">
+        <v>962</v>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>Correspondence of Fleur Dufour-Lapointe Germane to Seducing</t>
+        </is>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>Ase Jonsdotter the Motionless</t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr"/>
+      <c r="S28" s="10" t="inlineStr">
+        <is>
+          <t>Correspondence of Fleur Dufour-Lapointe Germane to Seducing</t>
+        </is>
+      </c>
+      <c r="T28" t="n">
+        <v>8</v>
+      </c>
+      <c r="U28" t="n">
+        <v>8</v>
+      </c>
+      <c r="V28" t="n">
+        <v>32</v>
+      </c>
+      <c r="W28" t="n">
+        <v>13</v>
+      </c>
+      <c r="X28" t="n">
+        <v>12</v>
+      </c>
+      <c r="Y28" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="Z28" t="inlineStr"/>
+      <c r="AA28" t="inlineStr">
+        <is>
+          <t>the Motionless</t>
+        </is>
+      </c>
+      <c r="AB28" t="inlineStr">
+        <is>
+          <t>Ase Jonsdotter</t>
+        </is>
+      </c>
+      <c r="AC28" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_female</t>
+        </is>
+      </c>
+      <c r="AD28" t="inlineStr"/>
+      <c r="AE28" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AF28" t="inlineStr"/>
+      <c r="AG28" t="inlineStr"/>
+      <c r="AH28" t="inlineStr"/>
+      <c r="AI28" t="inlineStr"/>
+      <c r="AJ28" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK28" t="inlineStr">
+        <is>
+          <t>{communication} of {person_1} {conjunction_about} {topic}</t>
+        </is>
+      </c>
+      <c r="AL28" t="inlineStr">
+        <is>
+          <t>Seducing</t>
+        </is>
+      </c>
+      <c r="AM28" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN28" t="n">
+        <v>521</v>
+      </c>
+      <c r="AO28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP28" t="n">
+        <v>441</v>
+      </c>
+      <c r="AQ28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU28" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV28" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW28" t="inlineStr">
+        <is>
+          <t>85d73445-c3b5-43a7-aaa5-c5c9249cae55</t>
+        </is>
+      </c>
+      <c r="AX28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Scroll</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>6</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1500</v>
+      </c>
+      <c r="E29" t="n">
+        <v>102</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Ancient</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Craft (blacksmithing)</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Craft (blacksmithing)</t>
+        </is>
+      </c>
+      <c r="J29" t="n">
+        <v>3</v>
+      </c>
+      <c r="K29" t="n">
+        <v>0</v>
+      </c>
+      <c r="L29" t="n">
+        <v>2</v>
+      </c>
+      <c r="M29" t="n">
+        <v>0</v>
+      </c>
+      <c r="N29" t="n">
+        <v>1</v>
+      </c>
+      <c r="O29" t="n">
+        <v>3570</v>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>Rumination on Blacksmithing</t>
+        </is>
+      </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>Blandine Cloutier</t>
+        </is>
+      </c>
+      <c r="R29" t="inlineStr"/>
+      <c r="S29" s="10" t="inlineStr">
+        <is>
+          <t>𐎠 𐎨𐎯𐎽𐎸𐎬 𐎥𐎱𐎨𐎭𐎦𐎨𐎫𐎫𐎠 𐎰𐎸𐎨𐎽𐎰𐎸𐎤 𐎮𐎱𐎢𐎨 𐎭𐎮𐎭</t>
+        </is>
+      </c>
+      <c r="T29" t="n">
+        <v>9</v>
+      </c>
+      <c r="U29" t="n">
+        <v>9</v>
+      </c>
+      <c r="V29" t="n">
+        <v>532</v>
+      </c>
+      <c r="W29" t="n">
+        <v>5</v>
+      </c>
+      <c r="X29" t="n">
+        <v>4</v>
+      </c>
+      <c r="Y29" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="Z29" t="inlineStr"/>
+      <c r="AA29" t="inlineStr"/>
+      <c r="AB29" t="inlineStr">
+        <is>
+          <t>Blandine Cloutier</t>
+        </is>
+      </c>
+      <c r="AC29" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AD29" t="inlineStr"/>
+      <c r="AE29" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AF29" t="inlineStr"/>
+      <c r="AG29" t="inlineStr"/>
+      <c r="AH29" t="inlineStr"/>
+      <c r="AI29" t="inlineStr"/>
+      <c r="AJ29" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK29" t="inlineStr">
+        <is>
+          <t>{study_on} on {topic}</t>
+        </is>
+      </c>
+      <c r="AL29" t="inlineStr">
+        <is>
+          <t>Blacksmithing</t>
+        </is>
+      </c>
+      <c r="AM29" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="AN29" t="n">
+        <v>570</v>
+      </c>
+      <c r="AO29" t="n">
+        <v>4</v>
+      </c>
+      <c r="AP29" t="n">
+        <v>3000</v>
+      </c>
+      <c r="AQ29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU29" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV29" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW29" t="inlineStr">
+        <is>
+          <t>f2db3f73-ba70-466b-a5a0-a4ae6ffdabaf</t>
+        </is>
+      </c>
+      <c r="AX29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>2</v>
+      </c>
+      <c r="D30" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E30" t="n">
+        <v>63</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Land Surveying</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Land Surveying</t>
+        </is>
+      </c>
+      <c r="J30" t="n">
+        <v>3</v>
+      </c>
+      <c r="K30" t="n">
+        <v>0</v>
+      </c>
+      <c r="L30" t="n">
+        <v>3</v>
+      </c>
+      <c r="M30" t="n">
+        <v>0</v>
+      </c>
+      <c r="N30" t="n">
+        <v>1</v>
+      </c>
+      <c r="O30" t="n">
+        <v>2370</v>
+      </c>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>Land Surveying and Trembling</t>
+        </is>
+      </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>Adrienne Darche</t>
+        </is>
+      </c>
+      <c r="R30" t="inlineStr"/>
+      <c r="S30" s="10" t="inlineStr">
+        <is>
+          <t>Land Surveying and Trembling</t>
+        </is>
+      </c>
+      <c r="T30" t="n">
+        <v>6</v>
+      </c>
+      <c r="U30" t="n">
+        <v>6</v>
+      </c>
+      <c r="V30" t="n">
+        <v>31</v>
+      </c>
+      <c r="W30" t="n">
+        <v>2</v>
+      </c>
+      <c r="X30" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y30" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="Z30" t="inlineStr"/>
+      <c r="AA30" t="inlineStr"/>
+      <c r="AB30" t="inlineStr">
+        <is>
+          <t>Adrienne Darche</t>
+        </is>
+      </c>
+      <c r="AC30" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AD30" t="inlineStr"/>
+      <c r="AE30" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AF30" t="inlineStr"/>
+      <c r="AG30" t="inlineStr"/>
+      <c r="AH30" t="inlineStr"/>
+      <c r="AI30" t="inlineStr"/>
+      <c r="AJ30" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK30" t="inlineStr">
+        <is>
+          <t>{topic} and {noun_2}</t>
+        </is>
+      </c>
+      <c r="AL30" t="inlineStr">
+        <is>
+          <t>Land Surveying</t>
+        </is>
+      </c>
+      <c r="AM30" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN30" t="n">
+        <v>370</v>
+      </c>
+      <c r="AO30" t="n">
+        <v>4</v>
+      </c>
+      <c r="AP30" t="n">
+        <v>2000</v>
+      </c>
+      <c r="AQ30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU30" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV30" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW30" t="inlineStr">
+        <is>
+          <t>54c9df47-2e32-4087-8fa1-9895cfe1a0de</t>
+        </is>
+      </c>
+      <c r="AX30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" t="n">
+        <v>500</v>
+      </c>
+      <c r="E31" t="n">
+        <v>32</v>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Classical</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
+      <c r="J31" t="n">
+        <v>1</v>
+      </c>
+      <c r="K31" t="n">
+        <v>0</v>
+      </c>
+      <c r="L31" t="n">
+        <v>2</v>
+      </c>
+      <c r="M31" t="n">
+        <v>0</v>
+      </c>
+      <c r="N31" t="n">
+        <v>1</v>
+      </c>
+      <c r="O31" t="n">
+        <v>820</v>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>The Gladsome Progress: Engineering</t>
+        </is>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>Baron Wynnstan Sherman</t>
+        </is>
+      </c>
+      <c r="R31" t="inlineStr"/>
+      <c r="S31" s="10" t="inlineStr">
+        <is>
+          <t>Locus disciplina phalanga</t>
+        </is>
+      </c>
+      <c r="T31" t="n">
+        <v>3</v>
+      </c>
+      <c r="U31" t="n">
+        <v>3</v>
+      </c>
+      <c r="V31" t="n">
+        <v>23</v>
+      </c>
+      <c r="W31" t="n">
+        <v>1</v>
+      </c>
+      <c r="X31" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y31" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z31" t="inlineStr"/>
+      <c r="AA31" t="inlineStr"/>
+      <c r="AB31" t="inlineStr">
+        <is>
+          <t>Wynnstan Sherman</t>
+        </is>
+      </c>
+      <c r="AC31" t="inlineStr">
+        <is>
+          <t>_names_anglo_saxon_surnames</t>
+        </is>
+      </c>
+      <c r="AD31" t="inlineStr">
+        <is>
+          <t>Baron</t>
+        </is>
+      </c>
+      <c r="AE31" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AF31" t="inlineStr"/>
+      <c r="AG31" t="inlineStr"/>
+      <c r="AH31" t="inlineStr"/>
+      <c r="AI31" t="inlineStr"/>
+      <c r="AJ31" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK31" t="inlineStr">
+        <is>
+          <t>The {adjective_1} {noun_1}: {topic}</t>
+        </is>
+      </c>
+      <c r="AL31" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
+      <c r="AM31" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN31" t="n">
+        <v>195</v>
+      </c>
+      <c r="AO31" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AP31" t="n">
+        <v>625</v>
+      </c>
+      <c r="AQ31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU31" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV31" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW31" t="inlineStr">
+        <is>
+          <t>c33c2549-5dcf-4eec-ae0a-c0be3bce5038</t>
+        </is>
+      </c>
+      <c r="AX31" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Refactor global variables into settings all works!
</commit_message>
<xml_diff>
--- a/books_spreadsheet_out.xlsx
+++ b/books_spreadsheet_out.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\p\gls01_workspace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EECF8F1-264E-4B92-8835-19C32A98B450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6004F33F-6F49-461E-BFC4-44AA8267FAC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -581,8 +581,8 @@
     <col min="41" max="48" width="9.140625" style="1" customWidth="1"/>
     <col min="49" max="49" width="37.140625" style="1" customWidth="1"/>
     <col min="50" max="50" width="18.140625" style="1" customWidth="1"/>
-    <col min="51" max="63" width="9.140625" style="1" customWidth="1"/>
-    <col min="64" max="16384" width="9.140625" style="1"/>
+    <col min="51" max="64" width="9.140625" style="1" customWidth="1"/>
+    <col min="65" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Trying to do installer
</commit_message>
<xml_diff>
--- a/books_spreadsheet_out.xlsx
+++ b/books_spreadsheet_out.xlsx
@@ -466,7 +466,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AX259"/>
+  <dimension ref="A1:AX282"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -42170,6 +42170,3702 @@
         </is>
       </c>
     </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>Scroll</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>Fine Papyrus</t>
+        </is>
+      </c>
+      <c r="C260" t="n">
+        <v>2</v>
+      </c>
+      <c r="D260" t="n">
+        <v>500</v>
+      </c>
+      <c r="E260" t="n">
+        <v>34</v>
+      </c>
+      <c r="F260" t="inlineStr">
+        <is>
+          <t>Dwarven</t>
+        </is>
+      </c>
+      <c r="H260" t="inlineStr">
+        <is>
+          <t>Ambushing</t>
+        </is>
+      </c>
+      <c r="I260" t="inlineStr">
+        <is>
+          <t>Ambushing</t>
+        </is>
+      </c>
+      <c r="J260" t="n">
+        <v>1</v>
+      </c>
+      <c r="K260" t="n">
+        <v>0</v>
+      </c>
+      <c r="L260" t="n">
+        <v>2</v>
+      </c>
+      <c r="M260" t="n">
+        <v>0</v>
+      </c>
+      <c r="N260" t="n">
+        <v>1</v>
+      </c>
+      <c r="O260" t="n">
+        <v>322</v>
+      </c>
+      <c r="P260" t="inlineStr">
+        <is>
+          <t>Ambushing and Hungriness</t>
+        </is>
+      </c>
+      <c r="Q260" t="inlineStr">
+        <is>
+          <t>Horatius Cornelia</t>
+        </is>
+      </c>
+      <c r="S260" s="12" t="inlineStr">
+        <is>
+          <t>ᛟᚱᚾᚨᚱᛖ ᚲᚱᚨᛊ ᛊᛟᛚᛚᛁᚲᛁᛏᚢᛞᛁᚾ ᚾᛖᚲᚢᛖ ᛈᚺᚨᛊᛖᛚᛚᚢᛊ ᛖᚾᛁᛗ ᛈᚢᛚᚢᛁᚾᚨᚱ</t>
+        </is>
+      </c>
+      <c r="T260" t="n">
+        <v>3</v>
+      </c>
+      <c r="U260" t="n">
+        <v>3</v>
+      </c>
+      <c r="V260" t="n">
+        <v>480</v>
+      </c>
+      <c r="W260" t="n">
+        <v>46</v>
+      </c>
+      <c r="X260" t="n">
+        <v>45</v>
+      </c>
+      <c r="Y260" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="AB260" t="inlineStr">
+        <is>
+          <t>Horatius Cornelia</t>
+        </is>
+      </c>
+      <c r="AC260" t="inlineStr">
+        <is>
+          <t>_names_roman_surnames</t>
+        </is>
+      </c>
+      <c r="AE260" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ260" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK260" t="inlineStr">
+        <is>
+          <t>{topic} and {noun_2}</t>
+        </is>
+      </c>
+      <c r="AL260" t="inlineStr">
+        <is>
+          <t>Ambushing</t>
+        </is>
+      </c>
+      <c r="AM260" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AN260" t="n">
+        <v>165</v>
+      </c>
+      <c r="AO260" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AP260" t="n">
+        <v>157</v>
+      </c>
+      <c r="AQ260" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR260" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS260" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT260" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU260" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV260" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW260" t="inlineStr">
+        <is>
+          <t>8c9f8771-c34d-42f5-a8ed-aa5db96491d8</t>
+        </is>
+      </c>
+      <c r="AX260" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C261" t="n">
+        <v>1</v>
+      </c>
+      <c r="D261" t="n">
+        <v>500</v>
+      </c>
+      <c r="E261" t="n">
+        <v>32</v>
+      </c>
+      <c r="F261" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H261" t="inlineStr">
+        <is>
+          <t>Elementalism</t>
+        </is>
+      </c>
+      <c r="I261" t="inlineStr">
+        <is>
+          <t>Elementalism</t>
+        </is>
+      </c>
+      <c r="J261" t="n">
+        <v>1</v>
+      </c>
+      <c r="K261" t="n">
+        <v>0</v>
+      </c>
+      <c r="L261" t="n">
+        <v>2</v>
+      </c>
+      <c r="M261" t="n">
+        <v>0</v>
+      </c>
+      <c r="N261" t="n">
+        <v>1</v>
+      </c>
+      <c r="O261" t="n">
+        <v>402</v>
+      </c>
+      <c r="P261" t="inlineStr">
+        <is>
+          <t>Trial of The Temptress with emphasis upon Elementalism</t>
+        </is>
+      </c>
+      <c r="Q261" t="inlineStr">
+        <is>
+          <t>Eindriði Johansen</t>
+        </is>
+      </c>
+      <c r="S261" s="10" t="inlineStr">
+        <is>
+          <t>Trial of The Temptress with emphasis upon Elementalism</t>
+        </is>
+      </c>
+      <c r="T261" t="n">
+        <v>3</v>
+      </c>
+      <c r="U261" t="n">
+        <v>3</v>
+      </c>
+      <c r="V261" t="n">
+        <v>8</v>
+      </c>
+      <c r="W261" t="n">
+        <v>12</v>
+      </c>
+      <c r="X261" t="n">
+        <v>11</v>
+      </c>
+      <c r="Y261" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AB261" t="inlineStr">
+        <is>
+          <t>Eindriði Johansen</t>
+        </is>
+      </c>
+      <c r="AC261" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_male</t>
+        </is>
+      </c>
+      <c r="AE261" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ261" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK261" t="inlineStr">
+        <is>
+          <t>{biography_starter} of {person_evil} with emphasis upon {topic}</t>
+        </is>
+      </c>
+      <c r="AL261" t="inlineStr">
+        <is>
+          <t>Elementalism</t>
+        </is>
+      </c>
+      <c r="AM261" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN261" t="n">
+        <v>195</v>
+      </c>
+      <c r="AO261" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AP261" t="n">
+        <v>207</v>
+      </c>
+      <c r="AQ261" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR261" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS261" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT261" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU261" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV261" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW261" t="inlineStr">
+        <is>
+          <t>d431da42-9656-4881-a81a-8ded6d8087cd</t>
+        </is>
+      </c>
+      <c r="AX261" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C262" t="n">
+        <v>2</v>
+      </c>
+      <c r="D262" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E262" t="n">
+        <v>63</v>
+      </c>
+      <c r="F262" t="inlineStr">
+        <is>
+          <t>Regional</t>
+        </is>
+      </c>
+      <c r="H262" t="inlineStr">
+        <is>
+          <t>Esoteric: Judge’s Choice</t>
+        </is>
+      </c>
+      <c r="I262" t="inlineStr">
+        <is>
+          <t>Theology</t>
+        </is>
+      </c>
+      <c r="J262" t="n">
+        <v>2</v>
+      </c>
+      <c r="K262" t="n">
+        <v>1</v>
+      </c>
+      <c r="L262" t="n">
+        <v>2</v>
+      </c>
+      <c r="M262" t="n">
+        <v>2</v>
+      </c>
+      <c r="N262" t="n">
+        <v>1</v>
+      </c>
+      <c r="O262" t="n">
+        <v>12370</v>
+      </c>
+      <c r="P262" t="inlineStr">
+        <is>
+          <t>The Passion of Bahak the Preacher and Theology</t>
+        </is>
+      </c>
+      <c r="Q262" t="inlineStr">
+        <is>
+          <t>Diodore Jousset</t>
+        </is>
+      </c>
+      <c r="S262" s="10" t="inlineStr">
+        <is>
+          <t>Κεῖται ἰσοσκελὲς εἰσίν δοθέντος λοιπῶν ἠγμένη ἐστίν] ἑαυτῆς σημείῳ προσπίπτουσαι</t>
+        </is>
+      </c>
+      <c r="T262" t="n">
+        <v>6</v>
+      </c>
+      <c r="U262" t="n">
+        <v>6</v>
+      </c>
+      <c r="V262" t="n">
+        <v>12</v>
+      </c>
+      <c r="W262" t="n">
+        <v>1</v>
+      </c>
+      <c r="X262" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y262" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB262" t="inlineStr">
+        <is>
+          <t>Diodore Jousset</t>
+        </is>
+      </c>
+      <c r="AC262" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AE262" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ262" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK262" t="inlineStr">
+        <is>
+          <t>{biography_starter} of {person_famous} and {topic}</t>
+        </is>
+      </c>
+      <c r="AL262" t="inlineStr">
+        <is>
+          <t>Theology</t>
+        </is>
+      </c>
+      <c r="AM262" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN262" t="n">
+        <v>370</v>
+      </c>
+      <c r="AO262" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP262" t="n">
+        <v>2000</v>
+      </c>
+      <c r="AQ262" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AR262" t="n">
+        <v>10000</v>
+      </c>
+      <c r="AS262" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT262" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU262" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV262" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW262" t="inlineStr">
+        <is>
+          <t>7496e179-1159-4b83-91b8-51282c3b01e9</t>
+        </is>
+      </c>
+      <c r="AX262" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C263" t="n">
+        <v>1</v>
+      </c>
+      <c r="D263" t="n">
+        <v>750</v>
+      </c>
+      <c r="E263" t="n">
+        <v>47</v>
+      </c>
+      <c r="F263" t="inlineStr">
+        <is>
+          <t>Ancient</t>
+        </is>
+      </c>
+      <c r="H263" t="inlineStr">
+        <is>
+          <t>Performance (storytelling)</t>
+        </is>
+      </c>
+      <c r="I263" t="inlineStr">
+        <is>
+          <t>Performance (storytelling)</t>
+        </is>
+      </c>
+      <c r="J263" t="n">
+        <v>3</v>
+      </c>
+      <c r="K263" t="n">
+        <v>0</v>
+      </c>
+      <c r="L263" t="n">
+        <v>4</v>
+      </c>
+      <c r="M263" t="n">
+        <v>0</v>
+      </c>
+      <c r="N263" t="n">
+        <v>1</v>
+      </c>
+      <c r="O263" t="n">
+        <v>1516</v>
+      </c>
+      <c r="P263" t="inlineStr">
+        <is>
+          <t>Ruminations in Storytelling</t>
+        </is>
+      </c>
+      <c r="Q263" t="inlineStr">
+        <is>
+          <t>His Holiness Fróði Lindberg the Chaste</t>
+        </is>
+      </c>
+      <c r="S263" s="10" t="inlineStr">
+        <is>
+          <t>𐎯𐎱𐎤𐏂𐎨𐎸𐎬 𐎨𐎭𐏂𐎤𐎦𐎤𐎱 𐎵𐎨𐎵𐎤𐎱𐎱𐎠 𐎤𐏍 𐎽𐎮𐎣𐎠𐎫𐎤𐎽</t>
+        </is>
+      </c>
+      <c r="T263" t="n">
+        <v>5</v>
+      </c>
+      <c r="U263" t="n">
+        <v>5</v>
+      </c>
+      <c r="V263" t="n">
+        <v>575</v>
+      </c>
+      <c r="W263" t="n">
+        <v>8</v>
+      </c>
+      <c r="X263" t="n">
+        <v>7</v>
+      </c>
+      <c r="Y263" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AA263" t="inlineStr">
+        <is>
+          <t>the Chaste</t>
+        </is>
+      </c>
+      <c r="AB263" t="inlineStr">
+        <is>
+          <t>Fróði Lindberg</t>
+        </is>
+      </c>
+      <c r="AC263" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_male</t>
+        </is>
+      </c>
+      <c r="AD263" t="inlineStr">
+        <is>
+          <t>His Holiness</t>
+        </is>
+      </c>
+      <c r="AE263" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ263" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK263" t="inlineStr">
+        <is>
+          <t>{study_in} in {topic}</t>
+        </is>
+      </c>
+      <c r="AL263" t="inlineStr">
+        <is>
+          <t>Storytelling</t>
+        </is>
+      </c>
+      <c r="AM263" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN263" t="n">
+        <v>278</v>
+      </c>
+      <c r="AO263" t="n">
+        <v>5</v>
+      </c>
+      <c r="AP263" t="n">
+        <v>1238</v>
+      </c>
+      <c r="AQ263" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR263" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS263" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT263" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU263" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV263" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW263" t="inlineStr">
+        <is>
+          <t>6bbc9406-e32b-4a8c-9137-1c09c8beca05</t>
+        </is>
+      </c>
+      <c r="AX263" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C264" t="n">
+        <v>2</v>
+      </c>
+      <c r="D264" t="n">
+        <v>1334</v>
+      </c>
+      <c r="E264" t="n">
+        <v>84</v>
+      </c>
+      <c r="F264" t="inlineStr">
+        <is>
+          <t>Classical</t>
+        </is>
+      </c>
+      <c r="H264" t="inlineStr">
+        <is>
+          <t>Loremastery</t>
+        </is>
+      </c>
+      <c r="I264" t="inlineStr">
+        <is>
+          <t>Loremastery</t>
+        </is>
+      </c>
+      <c r="J264" t="n">
+        <v>1</v>
+      </c>
+      <c r="K264" t="n">
+        <v>0</v>
+      </c>
+      <c r="L264" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="M264" t="n">
+        <v>0</v>
+      </c>
+      <c r="N264" t="n">
+        <v>1</v>
+      </c>
+      <c r="O264" t="n">
+        <v>494</v>
+      </c>
+      <c r="P264" t="inlineStr">
+        <is>
+          <t>Surveying Loremastery: a Pressing Exposition</t>
+        </is>
+      </c>
+      <c r="Q264" t="inlineStr">
+        <is>
+          <t>Tamara Naeemi</t>
+        </is>
+      </c>
+      <c r="S264" s="10" t="inlineStr">
+        <is>
+          <t>Optimum remuneraturum utrum castra noctis exploratoribus</t>
+        </is>
+      </c>
+      <c r="T264" t="n">
+        <v>8</v>
+      </c>
+      <c r="U264" t="n">
+        <v>8</v>
+      </c>
+      <c r="V264" t="n">
+        <v>1</v>
+      </c>
+      <c r="W264" t="n">
+        <v>1843</v>
+      </c>
+      <c r="X264" t="n">
+        <v>1842</v>
+      </c>
+      <c r="Y264" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB264" t="inlineStr">
+        <is>
+          <t>Tamara Naeemi</t>
+        </is>
+      </c>
+      <c r="AC264" t="inlineStr">
+        <is>
+          <t>_names_arabic_surnames</t>
+        </is>
+      </c>
+      <c r="AE264" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ264" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK264" t="inlineStr">
+        <is>
+          <t>{verbing} {topic}: a {adjective_1} {noun_1}</t>
+        </is>
+      </c>
+      <c r="AL264" t="inlineStr">
+        <is>
+          <t>Loremastery</t>
+        </is>
+      </c>
+      <c r="AM264" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN264" t="n">
+        <v>494</v>
+      </c>
+      <c r="AO264" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP264" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ264" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR264" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS264" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT264" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU264" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV264" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW264" t="inlineStr">
+        <is>
+          <t>6b1974c7-8d07-40eb-846b-4e1a367c476d</t>
+        </is>
+      </c>
+      <c r="AX264" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C265" t="n">
+        <v>2</v>
+      </c>
+      <c r="D265" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E265" t="n">
+        <v>63</v>
+      </c>
+      <c r="F265" t="inlineStr">
+        <is>
+          <t>Regional</t>
+        </is>
+      </c>
+      <c r="H265" t="inlineStr">
+        <is>
+          <t>Knowledge (occult)</t>
+        </is>
+      </c>
+      <c r="I265" t="inlineStr">
+        <is>
+          <t>Knowledge (occult)</t>
+        </is>
+      </c>
+      <c r="J265" t="n">
+        <v>1</v>
+      </c>
+      <c r="K265" t="n">
+        <v>0</v>
+      </c>
+      <c r="L265" t="n">
+        <v>1</v>
+      </c>
+      <c r="M265" t="n">
+        <v>0</v>
+      </c>
+      <c r="N265" t="n">
+        <v>1</v>
+      </c>
+      <c r="O265" t="n">
+        <v>1390</v>
+      </c>
+      <c r="P265" t="inlineStr">
+        <is>
+          <t>Darby Nilsdotter and Misdeeds: Aspects of Occult Knowledge</t>
+        </is>
+      </c>
+      <c r="Q265" t="inlineStr">
+        <is>
+          <t>Marcella Laronia</t>
+        </is>
+      </c>
+      <c r="S265" s="10" t="inlineStr">
+        <is>
+          <t>Ὃ σημεῖα ἔσονται οὗ ἄλλαι λ΄ συμπίπτειν ῥόμβος ποιῇ διάμετρον ἀπλατές ταῖς τῶν</t>
+        </is>
+      </c>
+      <c r="T265" t="n">
+        <v>6</v>
+      </c>
+      <c r="U265" t="n">
+        <v>6</v>
+      </c>
+      <c r="V265" t="n">
+        <v>39</v>
+      </c>
+      <c r="W265" t="n">
+        <v>1</v>
+      </c>
+      <c r="X265" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y265" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB265" t="inlineStr">
+        <is>
+          <t>Marcella Laronia</t>
+        </is>
+      </c>
+      <c r="AC265" t="inlineStr">
+        <is>
+          <t>_names_roman_surnames</t>
+        </is>
+      </c>
+      <c r="AE265" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ265" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK265" t="inlineStr">
+        <is>
+          <t>{person_1} and {negative_1}: Aspects of {topic}</t>
+        </is>
+      </c>
+      <c r="AL265" t="inlineStr">
+        <is>
+          <t>Occult Knowledge</t>
+        </is>
+      </c>
+      <c r="AM265" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN265" t="n">
+        <v>390</v>
+      </c>
+      <c r="AO265" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP265" t="n">
+        <v>1000</v>
+      </c>
+      <c r="AQ265" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR265" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS265" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT265" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU265" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV265" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW265" t="inlineStr">
+        <is>
+          <t>da0a5bac-4d66-48ec-bdc6-bc8ae36227d2</t>
+        </is>
+      </c>
+      <c r="AX265" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C266" t="n">
+        <v>1</v>
+      </c>
+      <c r="D266" t="n">
+        <v>334</v>
+      </c>
+      <c r="E266" t="n">
+        <v>23</v>
+      </c>
+      <c r="F266" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H266" t="inlineStr">
+        <is>
+          <t>Profession (lawyer)</t>
+        </is>
+      </c>
+      <c r="I266" t="inlineStr">
+        <is>
+          <t>Profession (lawyer)</t>
+        </is>
+      </c>
+      <c r="J266" t="n">
+        <v>1</v>
+      </c>
+      <c r="K266" t="n">
+        <v>0</v>
+      </c>
+      <c r="L266" t="n">
+        <v>3</v>
+      </c>
+      <c r="M266" t="n">
+        <v>0</v>
+      </c>
+      <c r="N266" t="n">
+        <v>1</v>
+      </c>
+      <c r="O266" t="n">
+        <v>465</v>
+      </c>
+      <c r="P266" t="inlineStr">
+        <is>
+          <t>Crimes of Eydís Olsdotter and Advocacy</t>
+        </is>
+      </c>
+      <c r="Q266" t="inlineStr">
+        <is>
+          <t>Josselin Deydier</t>
+        </is>
+      </c>
+      <c r="S266" s="10" t="inlineStr">
+        <is>
+          <t>Crimes of Eydís Olsdotter and Advocacy</t>
+        </is>
+      </c>
+      <c r="T266" t="n">
+        <v>2</v>
+      </c>
+      <c r="U266" t="n">
+        <v>2</v>
+      </c>
+      <c r="V266" t="n">
+        <v>64</v>
+      </c>
+      <c r="W266" t="n">
+        <v>5</v>
+      </c>
+      <c r="X266" t="n">
+        <v>4</v>
+      </c>
+      <c r="Y266" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AB266" t="inlineStr">
+        <is>
+          <t>Josselin Deydier</t>
+        </is>
+      </c>
+      <c r="AC266" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AE266" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ266" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK266" t="inlineStr">
+        <is>
+          <t>{biography_starter} of {person_1} and {topic}</t>
+        </is>
+      </c>
+      <c r="AL266" t="inlineStr">
+        <is>
+          <t>Advocacy</t>
+        </is>
+      </c>
+      <c r="AM266" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN266" t="n">
+        <v>131</v>
+      </c>
+      <c r="AO266" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP266" t="n">
+        <v>334</v>
+      </c>
+      <c r="AQ266" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR266" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS266" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT266" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU266" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV266" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW266" t="inlineStr">
+        <is>
+          <t>3a232eaa-7cbc-4c27-aef7-25221f8a4bf1</t>
+        </is>
+      </c>
+      <c r="AX266" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>Scroll</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>Ordinary Papyrus</t>
+        </is>
+      </c>
+      <c r="C267" t="n">
+        <v>4</v>
+      </c>
+      <c r="D267" t="n">
+        <v>800</v>
+      </c>
+      <c r="E267" t="n">
+        <v>56</v>
+      </c>
+      <c r="F267" t="inlineStr">
+        <is>
+          <t>Elvish</t>
+        </is>
+      </c>
+      <c r="H267" t="inlineStr">
+        <is>
+          <t>Dungeon Bashing</t>
+        </is>
+      </c>
+      <c r="I267" t="inlineStr">
+        <is>
+          <t>Dungeon Bashing</t>
+        </is>
+      </c>
+      <c r="J267" t="n">
+        <v>4</v>
+      </c>
+      <c r="K267" t="n">
+        <v>0</v>
+      </c>
+      <c r="L267" t="n">
+        <v>5</v>
+      </c>
+      <c r="M267" t="n">
+        <v>0</v>
+      </c>
+      <c r="N267" t="n">
+        <v>1</v>
+      </c>
+      <c r="O267" t="n">
+        <v>3548</v>
+      </c>
+      <c r="P267" t="inlineStr">
+        <is>
+          <t>Communication as Regards Dungeon Bashing by Barbara Girardon</t>
+        </is>
+      </c>
+      <c r="Q267" t="inlineStr">
+        <is>
+          <t>Salim Salhi the Sour</t>
+        </is>
+      </c>
+      <c r="S267" s="11" t="inlineStr">
+        <is>
+          <t>Noe galad lagor eneth rhosc ist erib lhewig gaeruil aroed athrad meldir</t>
+        </is>
+      </c>
+      <c r="T267" t="n">
+        <v>5</v>
+      </c>
+      <c r="U267" t="n">
+        <v>5</v>
+      </c>
+      <c r="V267" t="n">
+        <v>562</v>
+      </c>
+      <c r="W267" t="n">
+        <v>25</v>
+      </c>
+      <c r="X267" t="n">
+        <v>24</v>
+      </c>
+      <c r="Y267" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AA267" t="inlineStr">
+        <is>
+          <t>the Sour</t>
+        </is>
+      </c>
+      <c r="AB267" t="inlineStr">
+        <is>
+          <t>Salim Salhi</t>
+        </is>
+      </c>
+      <c r="AC267" t="inlineStr">
+        <is>
+          <t>_names_arabic_surnames</t>
+        </is>
+      </c>
+      <c r="AE267" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ267" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK267" t="inlineStr">
+        <is>
+          <t>{communication} {conjunction_about} {topic} {conjunction_by} {person_1}</t>
+        </is>
+      </c>
+      <c r="AL267" t="inlineStr">
+        <is>
+          <t>Dungeon Bashing</t>
+        </is>
+      </c>
+      <c r="AM267" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AN267" t="n">
+        <v>248</v>
+      </c>
+      <c r="AO267" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="AP267" t="n">
+        <v>3300</v>
+      </c>
+      <c r="AQ267" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR267" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS267" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT267" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU267" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV267" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW267" t="inlineStr">
+        <is>
+          <t>840d616e-8c04-4d08-905f-917acedbb847</t>
+        </is>
+      </c>
+      <c r="AX267" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C268" t="n">
+        <v>4</v>
+      </c>
+      <c r="D268" t="n">
+        <v>2667</v>
+      </c>
+      <c r="E268" t="n">
+        <v>167</v>
+      </c>
+      <c r="F268" t="inlineStr">
+        <is>
+          <t>Regional</t>
+        </is>
+      </c>
+      <c r="H268" t="inlineStr">
+        <is>
+          <t>Dungeon Bashing</t>
+        </is>
+      </c>
+      <c r="I268" t="inlineStr">
+        <is>
+          <t>Dungeon Bashing</t>
+        </is>
+      </c>
+      <c r="J268" t="n">
+        <v>2</v>
+      </c>
+      <c r="K268" t="n">
+        <v>0</v>
+      </c>
+      <c r="L268" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="M268" t="n">
+        <v>0</v>
+      </c>
+      <c r="N268" t="n">
+        <v>1</v>
+      </c>
+      <c r="O268" t="n">
+        <v>1148</v>
+      </c>
+      <c r="P268" t="inlineStr">
+        <is>
+          <t>The Damnable Gluttony of The Dark Lord and Dungeon Bashing</t>
+        </is>
+      </c>
+      <c r="Q268" t="inlineStr">
+        <is>
+          <t>Eadwine Frink</t>
+        </is>
+      </c>
+      <c r="S268" s="10" t="inlineStr">
+        <is>
+          <t>Ἐστίν] ὀξείας τετραπλεύρων λζ΄ ιη΄ εὐθύγραμμον περιεχόμενον προσεκβληθεισῶν πέρατα ἴσαις σημεῖα λοιπὰς γωνία</t>
+        </is>
+      </c>
+      <c r="T268" t="n">
+        <v>15</v>
+      </c>
+      <c r="U268" t="n">
+        <v>15</v>
+      </c>
+      <c r="V268" t="n">
+        <v>35</v>
+      </c>
+      <c r="W268" t="n">
+        <v>296</v>
+      </c>
+      <c r="X268" t="n">
+        <v>295</v>
+      </c>
+      <c r="Y268" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="AB268" t="inlineStr">
+        <is>
+          <t>Eadwine Frink</t>
+        </is>
+      </c>
+      <c r="AC268" t="inlineStr">
+        <is>
+          <t>_names_anglo_saxon_surnames</t>
+        </is>
+      </c>
+      <c r="AE268" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ268" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK268" t="inlineStr">
+        <is>
+          <t>{the_1} {negative_1} of {person_evil} and {topic}</t>
+        </is>
+      </c>
+      <c r="AL268" t="inlineStr">
+        <is>
+          <t>Dungeon Bashing</t>
+        </is>
+      </c>
+      <c r="AM268" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN268" t="n">
+        <v>1041</v>
+      </c>
+      <c r="AO268" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP268" t="n">
+        <v>107</v>
+      </c>
+      <c r="AQ268" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR268" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS268" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT268" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU268" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV268" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW268" t="inlineStr">
+        <is>
+          <t>0f91395a-1bef-44ad-820a-038075ab5aa7</t>
+        </is>
+      </c>
+      <c r="AX268" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>Scroll</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C269" t="n">
+        <v>6</v>
+      </c>
+      <c r="D269" t="n">
+        <v>1334</v>
+      </c>
+      <c r="E269" t="n">
+        <v>93</v>
+      </c>
+      <c r="F269" t="inlineStr">
+        <is>
+          <t>Classical</t>
+        </is>
+      </c>
+      <c r="H269" t="inlineStr">
+        <is>
+          <t>Fighting Style</t>
+        </is>
+      </c>
+      <c r="I269" t="inlineStr">
+        <is>
+          <t>Fighting Style</t>
+        </is>
+      </c>
+      <c r="J269" t="n">
+        <v>4</v>
+      </c>
+      <c r="K269" t="n">
+        <v>0</v>
+      </c>
+      <c r="L269" t="n">
+        <v>3</v>
+      </c>
+      <c r="M269" t="n">
+        <v>0</v>
+      </c>
+      <c r="N269" t="n">
+        <v>1</v>
+      </c>
+      <c r="O269" t="n">
+        <v>3842</v>
+      </c>
+      <c r="P269" t="inlineStr">
+        <is>
+          <t>Victor Christensen and Peccancy: Aspects of Fighting Style</t>
+        </is>
+      </c>
+      <c r="Q269" t="inlineStr">
+        <is>
+          <t>Abel Charton</t>
+        </is>
+      </c>
+      <c r="S269" s="10" t="inlineStr">
+        <is>
+          <t>Pararentur copiam finem imperium gratulatione domi crudeliter</t>
+        </is>
+      </c>
+      <c r="T269" t="n">
+        <v>8</v>
+      </c>
+      <c r="U269" t="n">
+        <v>8</v>
+      </c>
+      <c r="V269" t="n">
+        <v>155</v>
+      </c>
+      <c r="W269" t="n">
+        <v>39</v>
+      </c>
+      <c r="X269" t="n">
+        <v>38</v>
+      </c>
+      <c r="Y269" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="AB269" t="inlineStr">
+        <is>
+          <t>Abel Charton</t>
+        </is>
+      </c>
+      <c r="AC269" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AE269" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ269" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK269" t="inlineStr">
+        <is>
+          <t>{person_1} and {negative_1}: Aspects of {topic}</t>
+        </is>
+      </c>
+      <c r="AL269" t="inlineStr">
+        <is>
+          <t>Fighting Style</t>
+        </is>
+      </c>
+      <c r="AM269" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="AN269" t="n">
+        <v>507</v>
+      </c>
+      <c r="AO269" t="n">
+        <v>10</v>
+      </c>
+      <c r="AP269" t="n">
+        <v>3335</v>
+      </c>
+      <c r="AQ269" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR269" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS269" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT269" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU269" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV269" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW269" t="inlineStr">
+        <is>
+          <t>76c4664c-9216-49c2-aed5-87a7907b1b30</t>
+        </is>
+      </c>
+      <c r="AX269" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C270" t="n">
+        <v>1</v>
+      </c>
+      <c r="D270" t="n">
+        <v>334</v>
+      </c>
+      <c r="E270" t="n">
+        <v>23</v>
+      </c>
+      <c r="F270" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H270" t="inlineStr">
+        <is>
+          <t>Knowledge (political economy)</t>
+        </is>
+      </c>
+      <c r="I270" t="inlineStr">
+        <is>
+          <t>Knowledge (political economy)</t>
+        </is>
+      </c>
+      <c r="J270" t="n">
+        <v>1</v>
+      </c>
+      <c r="K270" t="n">
+        <v>0</v>
+      </c>
+      <c r="L270" t="n">
+        <v>3</v>
+      </c>
+      <c r="M270" t="n">
+        <v>0</v>
+      </c>
+      <c r="N270" t="n">
+        <v>1</v>
+      </c>
+      <c r="O270" t="n">
+        <v>198</v>
+      </c>
+      <c r="P270" t="inlineStr">
+        <is>
+          <t>Adélard Gardet and Ungodliness: Aspects of Political Economy</t>
+        </is>
+      </c>
+      <c r="Q270" t="inlineStr">
+        <is>
+          <t>Father Romanus Gellia</t>
+        </is>
+      </c>
+      <c r="S270" s="10" t="inlineStr">
+        <is>
+          <t>Adélard Gardet and Ungodliness: Aspects of Political Economy</t>
+        </is>
+      </c>
+      <c r="T270" t="n">
+        <v>2</v>
+      </c>
+      <c r="U270" t="n">
+        <v>2</v>
+      </c>
+      <c r="V270" t="n">
+        <v>78</v>
+      </c>
+      <c r="W270" t="n">
+        <v>93</v>
+      </c>
+      <c r="X270" t="n">
+        <v>92</v>
+      </c>
+      <c r="Y270" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AB270" t="inlineStr">
+        <is>
+          <t>Romanus Gellia</t>
+        </is>
+      </c>
+      <c r="AC270" t="inlineStr">
+        <is>
+          <t>_names_roman_surnames</t>
+        </is>
+      </c>
+      <c r="AD270" t="inlineStr">
+        <is>
+          <t>Father</t>
+        </is>
+      </c>
+      <c r="AE270" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ270" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK270" t="inlineStr">
+        <is>
+          <t>{person_1} and {negative_1}: Aspects of {topic}</t>
+        </is>
+      </c>
+      <c r="AL270" t="inlineStr">
+        <is>
+          <t>Political Economy</t>
+        </is>
+      </c>
+      <c r="AM270" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN270" t="n">
+        <v>131</v>
+      </c>
+      <c r="AO270" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP270" t="n">
+        <v>67</v>
+      </c>
+      <c r="AQ270" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR270" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS270" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT270" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU270" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV270" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW270" t="inlineStr">
+        <is>
+          <t>c732a760-2b6f-46fc-a59b-02c253e880cb</t>
+        </is>
+      </c>
+      <c r="AX270" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C271" t="n">
+        <v>2</v>
+      </c>
+      <c r="D271" t="n">
+        <v>800</v>
+      </c>
+      <c r="E271" t="n">
+        <v>51</v>
+      </c>
+      <c r="F271" t="inlineStr">
+        <is>
+          <t>Classical</t>
+        </is>
+      </c>
+      <c r="H271" t="inlineStr">
+        <is>
+          <t>Martial Training</t>
+        </is>
+      </c>
+      <c r="I271" t="inlineStr">
+        <is>
+          <t>Martial Training</t>
+        </is>
+      </c>
+      <c r="J271" t="n">
+        <v>4</v>
+      </c>
+      <c r="K271" t="n">
+        <v>0</v>
+      </c>
+      <c r="L271" t="n">
+        <v>5</v>
+      </c>
+      <c r="M271" t="n">
+        <v>0</v>
+      </c>
+      <c r="N271" t="n">
+        <v>1</v>
+      </c>
+      <c r="O271" t="n">
+        <v>5296</v>
+      </c>
+      <c r="P271" t="inlineStr">
+        <is>
+          <t>Martial Training, a Telestic Circling</t>
+        </is>
+      </c>
+      <c r="Q271" t="inlineStr">
+        <is>
+          <t>Torhtsige Jansson the Scholar</t>
+        </is>
+      </c>
+      <c r="S271" s="10" t="inlineStr">
+        <is>
+          <t>Designari reliquisque contenderent quidam capitum nostrum rebus allobrogas liceri rapinis aperiam</t>
+        </is>
+      </c>
+      <c r="T271" t="n">
+        <v>5</v>
+      </c>
+      <c r="U271" t="n">
+        <v>5</v>
+      </c>
+      <c r="V271" t="n">
+        <v>12</v>
+      </c>
+      <c r="W271" t="n">
+        <v>4</v>
+      </c>
+      <c r="X271" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y271" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AA271" t="inlineStr">
+        <is>
+          <t>the Scholar</t>
+        </is>
+      </c>
+      <c r="AB271" t="inlineStr">
+        <is>
+          <t>Torhtsige Jansson</t>
+        </is>
+      </c>
+      <c r="AC271" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_male</t>
+        </is>
+      </c>
+      <c r="AE271" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ271" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK271" t="inlineStr">
+        <is>
+          <t>{topic}, a {adjective_1} {noun_1}</t>
+        </is>
+      </c>
+      <c r="AL271" t="inlineStr">
+        <is>
+          <t>Martial Training</t>
+        </is>
+      </c>
+      <c r="AM271" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN271" t="n">
+        <v>296</v>
+      </c>
+      <c r="AO271" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="AP271" t="n">
+        <v>5000</v>
+      </c>
+      <c r="AQ271" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR271" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS271" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT271" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU271" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV271" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW271" t="inlineStr">
+        <is>
+          <t>ac11a347-1f64-49db-b9bd-09d225262e81</t>
+        </is>
+      </c>
+      <c r="AX271" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C272" t="n">
+        <v>1</v>
+      </c>
+      <c r="D272" t="n">
+        <v>334</v>
+      </c>
+      <c r="E272" t="n">
+        <v>23</v>
+      </c>
+      <c r="F272" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H272" t="inlineStr">
+        <is>
+          <t>Esoteric: Soothsaying</t>
+        </is>
+      </c>
+      <c r="I272" t="inlineStr">
+        <is>
+          <t>Profession (chamberlain)</t>
+        </is>
+      </c>
+      <c r="J272" t="n">
+        <v>1</v>
+      </c>
+      <c r="K272" t="n">
+        <v>1</v>
+      </c>
+      <c r="L272" t="n">
+        <v>3</v>
+      </c>
+      <c r="M272" t="n">
+        <v>3</v>
+      </c>
+      <c r="N272" t="n">
+        <v>1</v>
+      </c>
+      <c r="O272" t="n">
+        <v>2015</v>
+      </c>
+      <c r="P272" t="inlineStr">
+        <is>
+          <t>The Arcane Sojourn of the Generation: Chamberlains of Note</t>
+        </is>
+      </c>
+      <c r="Q272" t="inlineStr">
+        <is>
+          <t>Brother Bartholomew Weatherby</t>
+        </is>
+      </c>
+      <c r="S272" s="10" t="inlineStr">
+        <is>
+          <t>The Arcane Sojourn of the Generation: Chamberlains of Note</t>
+        </is>
+      </c>
+      <c r="T272" t="n">
+        <v>2</v>
+      </c>
+      <c r="U272" t="n">
+        <v>2</v>
+      </c>
+      <c r="V272" t="n">
+        <v>40</v>
+      </c>
+      <c r="W272" t="n">
+        <v>19</v>
+      </c>
+      <c r="X272" t="n">
+        <v>18</v>
+      </c>
+      <c r="Y272" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AB272" t="inlineStr">
+        <is>
+          <t>Bartholomew Weatherby</t>
+        </is>
+      </c>
+      <c r="AC272" t="inlineStr">
+        <is>
+          <t>_names_english_surnames</t>
+        </is>
+      </c>
+      <c r="AD272" t="inlineStr">
+        <is>
+          <t>Brother</t>
+        </is>
+      </c>
+      <c r="AE272" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ272" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK272" t="inlineStr">
+        <is>
+          <t>The {adjective_1} {noun_1} of {noun_2}: {topic}</t>
+        </is>
+      </c>
+      <c r="AL272" t="inlineStr">
+        <is>
+          <t>Chamberlains of Note</t>
+        </is>
+      </c>
+      <c r="AM272" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN272" t="n">
+        <v>124</v>
+      </c>
+      <c r="AO272" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP272" t="n">
+        <v>221</v>
+      </c>
+      <c r="AQ272" t="n">
+        <v>2</v>
+      </c>
+      <c r="AR272" t="n">
+        <v>1670</v>
+      </c>
+      <c r="AS272" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT272" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU272" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV272" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW272" t="inlineStr">
+        <is>
+          <t>1dee4df5-a808-45a7-8a3c-b37bfd18cd10</t>
+        </is>
+      </c>
+      <c r="AX272" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>Tablet</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>Clay</t>
+        </is>
+      </c>
+      <c r="C273" t="n">
+        <v>1</v>
+      </c>
+      <c r="D273" t="n">
+        <v>1500</v>
+      </c>
+      <c r="E273" t="n">
+        <v>1125</v>
+      </c>
+      <c r="F273" t="inlineStr">
+        <is>
+          <t>Dwarven</t>
+        </is>
+      </c>
+      <c r="H273" t="inlineStr">
+        <is>
+          <t>Mountaineering</t>
+        </is>
+      </c>
+      <c r="I273" t="inlineStr">
+        <is>
+          <t>Mountaineering</t>
+        </is>
+      </c>
+      <c r="J273" t="n">
+        <v>3</v>
+      </c>
+      <c r="K273" t="n">
+        <v>0</v>
+      </c>
+      <c r="L273" t="n">
+        <v>2</v>
+      </c>
+      <c r="M273" t="n">
+        <v>0</v>
+      </c>
+      <c r="N273" t="n">
+        <v>1</v>
+      </c>
+      <c r="O273" t="n">
+        <v>3180</v>
+      </c>
+      <c r="P273" t="inlineStr">
+        <is>
+          <t>The Misdeeds of Ase Madsdotter, Considering Mountaineering</t>
+        </is>
+      </c>
+      <c r="Q273" t="inlineStr">
+        <is>
+          <t>Azeena Tariq</t>
+        </is>
+      </c>
+      <c r="S273" s="12" t="inlineStr">
+        <is>
+          <t>ᚾᛖᚲᚢᛖ ᛊᚢᛊᛈᛖᚾᛞᛁᛊᛊᛖ ᛊᚲᛖᛚᛖᚱᛁᛊᚲᚢᛖ ᛈᛖᛚᛚᛖᚾᛏᛖᛊᚲᚢᛖ ᚢᛁᚢᛖᚱᚱᚨ ᚲᚱᚨᛊ ᚢᛖᚾᛖᚾᚨᛏᛁᛊ ᚲᛟᚾᛞᛁᛗᛖᚾᛏᚢᛗ ᚨᚢᚲᛏᛟᚱ ᛏᛁᚾᚲᛁᛞᚢᚾᛏ</t>
+        </is>
+      </c>
+      <c r="T273" t="n">
+        <v>9</v>
+      </c>
+      <c r="U273" t="n">
+        <v>9</v>
+      </c>
+      <c r="V273" t="n">
+        <v>505</v>
+      </c>
+      <c r="W273" t="n">
+        <v>23</v>
+      </c>
+      <c r="X273" t="n">
+        <v>22</v>
+      </c>
+      <c r="Y273" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AB273" t="inlineStr">
+        <is>
+          <t>Azeena Tariq</t>
+        </is>
+      </c>
+      <c r="AC273" t="inlineStr">
+        <is>
+          <t>_names_arabic_surnames</t>
+        </is>
+      </c>
+      <c r="AE273" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ273" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="AK273" t="inlineStr">
+        <is>
+          <t>{the_1} {negative_1} of {person_1}, Considering {topic}</t>
+        </is>
+      </c>
+      <c r="AL273" t="inlineStr">
+        <is>
+          <t>Mountaineering</t>
+        </is>
+      </c>
+      <c r="AM273" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="AN273" t="n">
+        <v>1200</v>
+      </c>
+      <c r="AO273" t="n">
+        <v>4</v>
+      </c>
+      <c r="AP273" t="n">
+        <v>1980</v>
+      </c>
+      <c r="AQ273" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR273" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS273" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT273" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU273" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV273" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW273" t="inlineStr">
+        <is>
+          <t>8e389734-419c-48db-8475-3eb97bcd8235</t>
+        </is>
+      </c>
+      <c r="AX273" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C274" t="n">
+        <v>1</v>
+      </c>
+      <c r="D274" t="n">
+        <v>500</v>
+      </c>
+      <c r="E274" t="n">
+        <v>32</v>
+      </c>
+      <c r="F274" t="inlineStr">
+        <is>
+          <t>Classical</t>
+        </is>
+      </c>
+      <c r="H274" t="inlineStr">
+        <is>
+          <t>Siege Engineering</t>
+        </is>
+      </c>
+      <c r="I274" t="inlineStr">
+        <is>
+          <t>Siege Engineering</t>
+        </is>
+      </c>
+      <c r="J274" t="n">
+        <v>1</v>
+      </c>
+      <c r="K274" t="n">
+        <v>0</v>
+      </c>
+      <c r="L274" t="n">
+        <v>2</v>
+      </c>
+      <c r="M274" t="n">
+        <v>0</v>
+      </c>
+      <c r="N274" t="n">
+        <v>1</v>
+      </c>
+      <c r="O274" t="n">
+        <v>810</v>
+      </c>
+      <c r="P274" t="inlineStr">
+        <is>
+          <t>Trial of The Temptress with emphasis upon Siege Engineering</t>
+        </is>
+      </c>
+      <c r="Q274" t="inlineStr">
+        <is>
+          <t>Olanda Pettersson</t>
+        </is>
+      </c>
+      <c r="S274" s="10" t="inlineStr">
+        <is>
+          <t>Loquatur sem constituit murum recusare retineri rauracis proelium iterum pacem</t>
+        </is>
+      </c>
+      <c r="T274" t="n">
+        <v>3</v>
+      </c>
+      <c r="U274" t="n">
+        <v>3</v>
+      </c>
+      <c r="V274" t="n">
+        <v>385</v>
+      </c>
+      <c r="W274" t="n">
+        <v>1</v>
+      </c>
+      <c r="X274" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y274" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB274" t="inlineStr">
+        <is>
+          <t>Olanda Pettersson</t>
+        </is>
+      </c>
+      <c r="AC274" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_male</t>
+        </is>
+      </c>
+      <c r="AE274" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ274" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK274" t="inlineStr">
+        <is>
+          <t>{biography_starter} of {person_evil} with emphasis upon {topic}</t>
+        </is>
+      </c>
+      <c r="AL274" t="inlineStr">
+        <is>
+          <t>Siege Engineering</t>
+        </is>
+      </c>
+      <c r="AM274" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN274" t="n">
+        <v>185</v>
+      </c>
+      <c r="AO274" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AP274" t="n">
+        <v>625</v>
+      </c>
+      <c r="AQ274" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR274" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS274" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT274" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU274" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV274" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW274" t="inlineStr">
+        <is>
+          <t>7986e258-9115-4d01-9fbd-4e496eabac26</t>
+        </is>
+      </c>
+      <c r="AX274" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C275" t="n">
+        <v>2</v>
+      </c>
+      <c r="D275" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E275" t="n">
+        <v>63</v>
+      </c>
+      <c r="F275" t="inlineStr">
+        <is>
+          <t>Classical</t>
+        </is>
+      </c>
+      <c r="H275" t="inlineStr">
+        <is>
+          <t>Performance (epic poetry)</t>
+        </is>
+      </c>
+      <c r="I275" t="inlineStr">
+        <is>
+          <t>Performance (epic poetry)</t>
+        </is>
+      </c>
+      <c r="J275" t="n">
+        <v>3</v>
+      </c>
+      <c r="K275" t="n">
+        <v>0</v>
+      </c>
+      <c r="L275" t="n">
+        <v>3</v>
+      </c>
+      <c r="M275" t="n">
+        <v>0</v>
+      </c>
+      <c r="N275" t="n">
+        <v>1</v>
+      </c>
+      <c r="O275" t="n">
+        <v>1690</v>
+      </c>
+      <c r="P275" t="inlineStr">
+        <is>
+          <t>Treatise on Epic Poetry</t>
+        </is>
+      </c>
+      <c r="Q275" t="inlineStr">
+        <is>
+          <t>Mister Jude Docker</t>
+        </is>
+      </c>
+      <c r="S275" s="10" t="inlineStr">
+        <is>
+          <t>Praecipue ea fugit conloquendi dextro consecuti nobilissimi singulos orandi</t>
+        </is>
+      </c>
+      <c r="T275" t="n">
+        <v>6</v>
+      </c>
+      <c r="U275" t="n">
+        <v>6</v>
+      </c>
+      <c r="V275" t="n">
+        <v>39</v>
+      </c>
+      <c r="W275" t="n">
+        <v>16</v>
+      </c>
+      <c r="X275" t="n">
+        <v>15</v>
+      </c>
+      <c r="Y275" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AB275" t="inlineStr">
+        <is>
+          <t>Jude Docker</t>
+        </is>
+      </c>
+      <c r="AC275" t="inlineStr">
+        <is>
+          <t>_names_english_surnames</t>
+        </is>
+      </c>
+      <c r="AD275" t="inlineStr">
+        <is>
+          <t>Mister</t>
+        </is>
+      </c>
+      <c r="AE275" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ275" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK275" t="inlineStr">
+        <is>
+          <t>{study_on} on {topic}</t>
+        </is>
+      </c>
+      <c r="AL275" t="inlineStr">
+        <is>
+          <t>Epic Poetry</t>
+        </is>
+      </c>
+      <c r="AM275" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN275" t="n">
+        <v>370</v>
+      </c>
+      <c r="AO275" t="n">
+        <v>4</v>
+      </c>
+      <c r="AP275" t="n">
+        <v>1320</v>
+      </c>
+      <c r="AQ275" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR275" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS275" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT275" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU275" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV275" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW275" t="inlineStr">
+        <is>
+          <t>bb33dd5f-9e12-43fc-a796-34a02c8bc07a</t>
+        </is>
+      </c>
+      <c r="AX275" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C276" t="n">
+        <v>2</v>
+      </c>
+      <c r="D276" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E276" t="n">
+        <v>63</v>
+      </c>
+      <c r="F276" t="inlineStr">
+        <is>
+          <t>Classical</t>
+        </is>
+      </c>
+      <c r="G276" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H276" t="inlineStr">
+        <is>
+          <t>Labor (domestic)</t>
+        </is>
+      </c>
+      <c r="I276" t="inlineStr">
+        <is>
+          <t>Labor (domestic)</t>
+        </is>
+      </c>
+      <c r="J276" t="n">
+        <v>1</v>
+      </c>
+      <c r="K276" t="n">
+        <v>0</v>
+      </c>
+      <c r="L276" t="n">
+        <v>1</v>
+      </c>
+      <c r="M276" t="n">
+        <v>0</v>
+      </c>
+      <c r="N276" t="n">
+        <v>1</v>
+      </c>
+      <c r="O276" t="n">
+        <v>1370</v>
+      </c>
+      <c r="P276" t="inlineStr">
+        <is>
+          <t>The Imperfection of Raed Abd Manaf, on the Subject of Laboring as a Domestic</t>
+        </is>
+      </c>
+      <c r="Q276" t="inlineStr">
+        <is>
+          <t>Wilheard Read</t>
+        </is>
+      </c>
+      <c r="R276" t="inlineStr">
+        <is>
+          <t>Her Grace Anundr Olsdotter</t>
+        </is>
+      </c>
+      <c r="S276" s="10" t="inlineStr">
+        <is>
+          <t>Transfixis loquatur faciant fatum consilia quosque conscribit parvo intercludi oppugnaret castella quae fugae haberet ducimus vim terrenus</t>
+        </is>
+      </c>
+      <c r="T276" t="n">
+        <v>6</v>
+      </c>
+      <c r="U276" t="n">
+        <v>6</v>
+      </c>
+      <c r="V276" t="n">
+        <v>37</v>
+      </c>
+      <c r="W276" t="n">
+        <v>1</v>
+      </c>
+      <c r="X276" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y276" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB276" t="inlineStr">
+        <is>
+          <t>Wilheard Read</t>
+        </is>
+      </c>
+      <c r="AC276" t="inlineStr">
+        <is>
+          <t>_names_anglo_saxon_surnames</t>
+        </is>
+      </c>
+      <c r="AE276" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AF276" t="inlineStr">
+        <is>
+          <t>Anundr Olsdotter</t>
+        </is>
+      </c>
+      <c r="AG276" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_female</t>
+        </is>
+      </c>
+      <c r="AH276" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AI276" t="inlineStr">
+        <is>
+          <t>Her Grace</t>
+        </is>
+      </c>
+      <c r="AJ276" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK276" t="inlineStr">
+        <is>
+          <t>{the_1} {negative_1} of {person_1}, on the Subject of {topic}</t>
+        </is>
+      </c>
+      <c r="AL276" t="inlineStr">
+        <is>
+          <t>Laboring as a Domestic</t>
+        </is>
+      </c>
+      <c r="AM276" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN276" t="n">
+        <v>370</v>
+      </c>
+      <c r="AO276" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP276" t="n">
+        <v>1000</v>
+      </c>
+      <c r="AQ276" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR276" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS276" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT276" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU276" t="b">
+        <v>1</v>
+      </c>
+      <c r="AV276" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW276" t="inlineStr">
+        <is>
+          <t>d7ae7dbd-952b-48df-83a4-2ed33d1da1d1</t>
+        </is>
+      </c>
+      <c r="AX276" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C277" t="n">
+        <v>1</v>
+      </c>
+      <c r="D277" t="n">
+        <v>667</v>
+      </c>
+      <c r="E277" t="n">
+        <v>43</v>
+      </c>
+      <c r="F277" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H277" t="inlineStr">
+        <is>
+          <t>Swashbuckling</t>
+        </is>
+      </c>
+      <c r="I277" t="inlineStr">
+        <is>
+          <t>Swashbuckling</t>
+        </is>
+      </c>
+      <c r="J277" t="n">
+        <v>2</v>
+      </c>
+      <c r="K277" t="n">
+        <v>0</v>
+      </c>
+      <c r="L277" t="n">
+        <v>3</v>
+      </c>
+      <c r="M277" t="n">
+        <v>0</v>
+      </c>
+      <c r="N277" t="n">
+        <v>1</v>
+      </c>
+      <c r="O277" t="n">
+        <v>1095</v>
+      </c>
+      <c r="P277" t="inlineStr">
+        <is>
+          <t>Adventures in Swashbuckling</t>
+        </is>
+      </c>
+      <c r="Q277" t="inlineStr">
+        <is>
+          <t>Louis Hesketh the Crippled</t>
+        </is>
+      </c>
+      <c r="S277" s="10" t="inlineStr">
+        <is>
+          <t>Adventures in Swashbuckling</t>
+        </is>
+      </c>
+      <c r="T277" t="n">
+        <v>4</v>
+      </c>
+      <c r="U277" t="n">
+        <v>4</v>
+      </c>
+      <c r="V277" t="n">
+        <v>70</v>
+      </c>
+      <c r="W277" t="n">
+        <v>5</v>
+      </c>
+      <c r="X277" t="n">
+        <v>4</v>
+      </c>
+      <c r="Y277" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AA277" t="inlineStr">
+        <is>
+          <t>the Crippled</t>
+        </is>
+      </c>
+      <c r="AB277" t="inlineStr">
+        <is>
+          <t>Louis Hesketh</t>
+        </is>
+      </c>
+      <c r="AC277" t="inlineStr">
+        <is>
+          <t>_names_english_surnames</t>
+        </is>
+      </c>
+      <c r="AE277" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ277" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK277" t="inlineStr">
+        <is>
+          <t>{study_in} in {topic}</t>
+        </is>
+      </c>
+      <c r="AL277" t="inlineStr">
+        <is>
+          <t>Swashbuckling</t>
+        </is>
+      </c>
+      <c r="AM277" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN277" t="n">
+        <v>261</v>
+      </c>
+      <c r="AO277" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="AP277" t="n">
+        <v>834</v>
+      </c>
+      <c r="AQ277" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR277" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS277" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT277" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU277" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV277" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW277" t="inlineStr">
+        <is>
+          <t>133f23c8-95ea-4ecc-a918-8d1ec5612fc4</t>
+        </is>
+      </c>
+      <c r="AX277" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C278" t="n">
+        <v>2</v>
+      </c>
+      <c r="D278" t="n">
+        <v>1334</v>
+      </c>
+      <c r="E278" t="n">
+        <v>84</v>
+      </c>
+      <c r="F278" t="inlineStr">
+        <is>
+          <t>Elvish</t>
+        </is>
+      </c>
+      <c r="H278" t="inlineStr">
+        <is>
+          <t>Art (sculpture)</t>
+        </is>
+      </c>
+      <c r="I278" t="inlineStr">
+        <is>
+          <t>Art (sculpture)</t>
+        </is>
+      </c>
+      <c r="J278" t="n">
+        <v>1</v>
+      </c>
+      <c r="K278" t="n">
+        <v>0</v>
+      </c>
+      <c r="L278" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="M278" t="n">
+        <v>0</v>
+      </c>
+      <c r="N278" t="n">
+        <v>1</v>
+      </c>
+      <c r="O278" t="n">
+        <v>1161</v>
+      </c>
+      <c r="P278" t="inlineStr">
+        <is>
+          <t>The Rapturous Way: Creating Sculpture</t>
+        </is>
+      </c>
+      <c r="Q278" t="inlineStr">
+        <is>
+          <t>Hulda Pettersdotter</t>
+        </is>
+      </c>
+      <c r="S278" s="11" t="inlineStr">
+        <is>
+          <t>Amath ogol evyrn rui</t>
+        </is>
+      </c>
+      <c r="T278" t="n">
+        <v>8</v>
+      </c>
+      <c r="U278" t="n">
+        <v>8</v>
+      </c>
+      <c r="V278" t="n">
+        <v>90</v>
+      </c>
+      <c r="W278" t="n">
+        <v>3</v>
+      </c>
+      <c r="X278" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y278" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AB278" t="inlineStr">
+        <is>
+          <t>Hulda Pettersdotter</t>
+        </is>
+      </c>
+      <c r="AC278" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_female</t>
+        </is>
+      </c>
+      <c r="AE278" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ278" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK278" t="inlineStr">
+        <is>
+          <t>The {adjective_1} {noun_1}: {topic}</t>
+        </is>
+      </c>
+      <c r="AL278" t="inlineStr">
+        <is>
+          <t>Creating Sculpture</t>
+        </is>
+      </c>
+      <c r="AM278" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN278" t="n">
+        <v>494</v>
+      </c>
+      <c r="AO278" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP278" t="n">
+        <v>667</v>
+      </c>
+      <c r="AQ278" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR278" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS278" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT278" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU278" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV278" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW278" t="inlineStr">
+        <is>
+          <t>bbd12ad8-8757-4625-a4cd-361aa7d2b461</t>
+        </is>
+      </c>
+      <c r="AX278" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C279" t="n">
+        <v>1</v>
+      </c>
+      <c r="D279" t="n">
+        <v>500</v>
+      </c>
+      <c r="E279" t="n">
+        <v>32</v>
+      </c>
+      <c r="F279" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H279" t="inlineStr">
+        <is>
+          <t>Esoteric: Alchemy</t>
+        </is>
+      </c>
+      <c r="I279" t="inlineStr">
+        <is>
+          <t>Pass Without Trace</t>
+        </is>
+      </c>
+      <c r="J279" t="n">
+        <v>1</v>
+      </c>
+      <c r="K279" t="n">
+        <v>1</v>
+      </c>
+      <c r="L279" t="n">
+        <v>2</v>
+      </c>
+      <c r="M279" t="n">
+        <v>2</v>
+      </c>
+      <c r="N279" t="n">
+        <v>1</v>
+      </c>
+      <c r="O279" t="n">
+        <v>5810</v>
+      </c>
+      <c r="P279" t="inlineStr">
+        <is>
+          <t>Transactions as Regards Passing Unseen in ye Wildernesse from Ari Kristensen</t>
+        </is>
+      </c>
+      <c r="Q279" t="inlineStr">
+        <is>
+          <t>Benjamin Thomson the Lazy</t>
+        </is>
+      </c>
+      <c r="S279" s="10" t="inlineStr">
+        <is>
+          <t>Transactions as Regards Passing Unseen in ye Wildernesse from Ari Kristensen</t>
+        </is>
+      </c>
+      <c r="T279" t="n">
+        <v>3</v>
+      </c>
+      <c r="U279" t="n">
+        <v>3</v>
+      </c>
+      <c r="V279" t="n">
+        <v>20</v>
+      </c>
+      <c r="W279" t="n">
+        <v>1</v>
+      </c>
+      <c r="X279" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y279" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA279" t="inlineStr">
+        <is>
+          <t>the Lazy</t>
+        </is>
+      </c>
+      <c r="AB279" t="inlineStr">
+        <is>
+          <t>Benjamin Thomson</t>
+        </is>
+      </c>
+      <c r="AC279" t="inlineStr">
+        <is>
+          <t>_names_english_surnames</t>
+        </is>
+      </c>
+      <c r="AE279" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ279" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK279" t="inlineStr">
+        <is>
+          <t>{communication} {conjunction_about} {topic} {conjunction_by} {person_1}</t>
+        </is>
+      </c>
+      <c r="AL279" t="inlineStr">
+        <is>
+          <t>Passing Unseen in ye Wildernesse</t>
+        </is>
+      </c>
+      <c r="AM279" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN279" t="n">
+        <v>185</v>
+      </c>
+      <c r="AO279" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AP279" t="n">
+        <v>625</v>
+      </c>
+      <c r="AQ279" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AR279" t="n">
+        <v>5000</v>
+      </c>
+      <c r="AS279" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT279" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU279" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV279" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW279" t="inlineStr">
+        <is>
+          <t>acd69d07-c486-481b-9e54-af7da620d3a9</t>
+        </is>
+      </c>
+      <c r="AX279" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C280" t="n">
+        <v>1</v>
+      </c>
+      <c r="D280" t="n">
+        <v>500</v>
+      </c>
+      <c r="E280" t="n">
+        <v>32</v>
+      </c>
+      <c r="F280" t="inlineStr">
+        <is>
+          <t>Regional</t>
+        </is>
+      </c>
+      <c r="H280" t="inlineStr">
+        <is>
+          <t>Magical Engineering</t>
+        </is>
+      </c>
+      <c r="I280" t="inlineStr">
+        <is>
+          <t>Magical Engineering</t>
+        </is>
+      </c>
+      <c r="J280" t="n">
+        <v>2</v>
+      </c>
+      <c r="K280" t="n">
+        <v>0</v>
+      </c>
+      <c r="L280" t="n">
+        <v>4</v>
+      </c>
+      <c r="M280" t="n">
+        <v>0</v>
+      </c>
+      <c r="N280" t="n">
+        <v>1</v>
+      </c>
+      <c r="O280" t="n">
+        <v>1185</v>
+      </c>
+      <c r="P280" t="inlineStr">
+        <is>
+          <t>Correspondence of Lucia Cottia in Regard to Magical Engineering</t>
+        </is>
+      </c>
+      <c r="Q280" t="inlineStr">
+        <is>
+          <t>Duke Darius Mettia</t>
+        </is>
+      </c>
+      <c r="S280" s="10" t="inlineStr">
+        <is>
+          <t>Ἡμικυκλίου η΄ λγ΄ ἐλάσσονι τριῶν συστήσασθαι ἰσόπλευρον διαμέτρου λη΄ κα΄ τέμνωσιν ἐλάσσων</t>
+        </is>
+      </c>
+      <c r="T280" t="n">
+        <v>3</v>
+      </c>
+      <c r="U280" t="n">
+        <v>3</v>
+      </c>
+      <c r="V280" t="n">
+        <v>46</v>
+      </c>
+      <c r="W280" t="n">
+        <v>2</v>
+      </c>
+      <c r="X280" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y280" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AB280" t="inlineStr">
+        <is>
+          <t>Darius Mettia</t>
+        </is>
+      </c>
+      <c r="AC280" t="inlineStr">
+        <is>
+          <t>_names_roman_surnames</t>
+        </is>
+      </c>
+      <c r="AD280" t="inlineStr">
+        <is>
+          <t>Duke</t>
+        </is>
+      </c>
+      <c r="AE280" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ280" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK280" t="inlineStr">
+        <is>
+          <t>{communication} of {person_1} {conjunction_about} {topic}</t>
+        </is>
+      </c>
+      <c r="AL280" t="inlineStr">
+        <is>
+          <t>Magical Engineering</t>
+        </is>
+      </c>
+      <c r="AM280" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN280" t="n">
+        <v>185</v>
+      </c>
+      <c r="AO280" t="n">
+        <v>4</v>
+      </c>
+      <c r="AP280" t="n">
+        <v>1000</v>
+      </c>
+      <c r="AQ280" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR280" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS280" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT280" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU280" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV280" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW280" t="inlineStr">
+        <is>
+          <t>6d0eb4ed-ad72-4370-9609-ba58bbdf9df6</t>
+        </is>
+      </c>
+      <c r="AX280" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>Scroll</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>Ordinary Papyrus</t>
+        </is>
+      </c>
+      <c r="C281" t="n">
+        <v>4</v>
+      </c>
+      <c r="D281" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E281" t="n">
+        <v>68</v>
+      </c>
+      <c r="F281" t="inlineStr">
+        <is>
+          <t>Classical</t>
+        </is>
+      </c>
+      <c r="H281" t="inlineStr">
+        <is>
+          <t>Performance (epic poetry)</t>
+        </is>
+      </c>
+      <c r="I281" t="inlineStr">
+        <is>
+          <t>Performance (epic poetry)</t>
+        </is>
+      </c>
+      <c r="J281" t="n">
+        <v>1</v>
+      </c>
+      <c r="K281" t="n">
+        <v>0</v>
+      </c>
+      <c r="L281" t="n">
+        <v>1</v>
+      </c>
+      <c r="M281" t="n">
+        <v>0</v>
+      </c>
+      <c r="N281" t="n">
+        <v>1</v>
+      </c>
+      <c r="O281" t="n">
+        <v>560</v>
+      </c>
+      <c r="P281" t="inlineStr">
+        <is>
+          <t>Iyad Shams and Peccancy: Aspects of Epic Poetry</t>
+        </is>
+      </c>
+      <c r="Q281" t="inlineStr">
+        <is>
+          <t>Baug Jansson</t>
+        </is>
+      </c>
+      <c r="S281" s="10" t="inlineStr">
+        <is>
+          <t>Vitae queritur odisse exercitumque legionum commonefacit orgetorix commeatu adpetierit elementum pellentesque sementes</t>
+        </is>
+      </c>
+      <c r="T281" t="n">
+        <v>6</v>
+      </c>
+      <c r="U281" t="n">
+        <v>6</v>
+      </c>
+      <c r="V281" t="n">
+        <v>866</v>
+      </c>
+      <c r="W281" t="n">
+        <v>50</v>
+      </c>
+      <c r="X281" t="n">
+        <v>49</v>
+      </c>
+      <c r="Y281" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="AB281" t="inlineStr">
+        <is>
+          <t>Baug Jansson</t>
+        </is>
+      </c>
+      <c r="AC281" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_male</t>
+        </is>
+      </c>
+      <c r="AE281" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ281" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK281" t="inlineStr">
+        <is>
+          <t>{person_1} and {negative_1}: Aspects of {topic}</t>
+        </is>
+      </c>
+      <c r="AL281" t="inlineStr">
+        <is>
+          <t>Epic Poetry</t>
+        </is>
+      </c>
+      <c r="AM281" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AN281" t="n">
+        <v>310</v>
+      </c>
+      <c r="AO281" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP281" t="n">
+        <v>250</v>
+      </c>
+      <c r="AQ281" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR281" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS281" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT281" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU281" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV281" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW281" t="inlineStr">
+        <is>
+          <t>448ee59c-35c6-49c4-abf6-278195800663</t>
+        </is>
+      </c>
+      <c r="AX281" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C282" t="n">
+        <v>2</v>
+      </c>
+      <c r="D282" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E282" t="n">
+        <v>63</v>
+      </c>
+      <c r="F282" t="inlineStr">
+        <is>
+          <t>Classical</t>
+        </is>
+      </c>
+      <c r="H282" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
+      <c r="I282" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
+      <c r="J282" t="n">
+        <v>3</v>
+      </c>
+      <c r="K282" t="n">
+        <v>0</v>
+      </c>
+      <c r="L282" t="n">
+        <v>3</v>
+      </c>
+      <c r="M282" t="n">
+        <v>0</v>
+      </c>
+      <c r="N282" t="n">
+        <v>1</v>
+      </c>
+      <c r="O282" t="n">
+        <v>2390</v>
+      </c>
+      <c r="P282" t="inlineStr">
+        <is>
+          <t>The Telestic Winding: Engineering</t>
+        </is>
+      </c>
+      <c r="Q282" t="inlineStr">
+        <is>
+          <t>Eyfrod Jakobsson the Grotesque</t>
+        </is>
+      </c>
+      <c r="S282" s="10" t="inlineStr">
+        <is>
+          <t>Ei tigurini mandata facilem equitatus</t>
+        </is>
+      </c>
+      <c r="T282" t="n">
+        <v>6</v>
+      </c>
+      <c r="U282" t="n">
+        <v>6</v>
+      </c>
+      <c r="V282" t="n">
+        <v>42</v>
+      </c>
+      <c r="W282" t="n">
+        <v>4</v>
+      </c>
+      <c r="X282" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y282" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AA282" t="inlineStr">
+        <is>
+          <t>the Grotesque</t>
+        </is>
+      </c>
+      <c r="AB282" t="inlineStr">
+        <is>
+          <t>Eyfrod Jakobsson</t>
+        </is>
+      </c>
+      <c r="AC282" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_male</t>
+        </is>
+      </c>
+      <c r="AE282" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ282" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK282" t="inlineStr">
+        <is>
+          <t>The {adjective_1} {noun_1}: {topic}</t>
+        </is>
+      </c>
+      <c r="AL282" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
+      <c r="AM282" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN282" t="n">
+        <v>390</v>
+      </c>
+      <c r="AO282" t="n">
+        <v>4</v>
+      </c>
+      <c r="AP282" t="n">
+        <v>2000</v>
+      </c>
+      <c r="AQ282" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR282" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS282" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT282" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU282" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV282" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW282" t="inlineStr">
+        <is>
+          <t>6030b68e-4e7d-499f-8f1f-756bdfdf3604</t>
+        </is>
+      </c>
+      <c r="AX282" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
3rd rewrite of get_proper_random_book, using weighted random function
</commit_message>
<xml_diff>
--- a/books_spreadsheet_out.xlsx
+++ b/books_spreadsheet_out.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2160" yWindow="2160" windowWidth="21600" windowHeight="11295" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4560" yWindow="1665" windowWidth="21600" windowHeight="11295" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Book Hoard" sheetId="1" state="visible" r:id="rId1"/>
@@ -456,7 +456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AX21"/>
+  <dimension ref="A1:AX16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -498,8 +498,8 @@
     <col width="9.140625" customWidth="1" style="1" min="41" max="48"/>
     <col width="37.140625" customWidth="1" style="1" min="49" max="49"/>
     <col width="18.140625" customWidth="1" style="1" min="50" max="50"/>
-    <col width="9.140625" customWidth="1" style="1" min="51" max="60"/>
-    <col width="9.140625" customWidth="1" style="1" min="61" max="16384"/>
+    <col width="9.140625" customWidth="1" style="1" min="51" max="63"/>
+    <col width="9.140625" customWidth="1" style="1" min="64" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -762,31 +762,31 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Vellum</t>
+          <t>Parchment</t>
         </is>
       </c>
       <c r="C2" t="n">
         <v>2</v>
       </c>
       <c r="D2" t="n">
-        <v>1500</v>
+        <v>1334</v>
       </c>
       <c r="E2" t="n">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>Regional</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Sniping</t>
+          <t>Knowledge (occult)</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Sniping</t>
+          <t>Knowledge (occult)</t>
         </is>
       </c>
       <c r="J2" t="n">
@@ -796,7 +796,7 @@
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="M2" t="n">
         <v>0</v>
@@ -805,54 +805,49 @@
         <v>1</v>
       </c>
       <c r="O2" t="n">
-        <v>660</v>
+        <v>561</v>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>Epistles of Gamila Khouri and Déborah Houard Discoursing on Sniping</t>
+          <t>The Underground Extremity: Hidden Knowledge</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Fabricius Egnatia</t>
+          <t>Duilius Anneia</t>
         </is>
       </c>
       <c r="S2" s="10" t="inlineStr">
         <is>
-          <t>Epistles of Gamila Khouri and Déborah Houard Discoursing on Sniping</t>
+          <t>Σημεῖα τρίγωνον τεμεῖν κλίσις εὐθύγραμμος ὅρος δυσὶν ἄλλαι τῇ ὑπό κε΄</t>
         </is>
       </c>
       <c r="T2" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="U2" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="V2" t="n">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="W2" t="n">
-        <v>29</v>
+        <v>224</v>
       </c>
       <c r="X2" t="n">
-        <v>11</v>
+        <v>223</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="AA2" t="inlineStr">
-        <is>
-          <t>the Miniscule</t>
-        </is>
+        <v>0.05</v>
       </c>
       <c r="AB2" t="inlineStr">
         <is>
-          <t>Fabricius Egnatia</t>
-        </is>
-      </c>
-      <c r="AD2" t="inlineStr">
-        <is>
-          <t>Lord</t>
+          <t>Duilius Anneia</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>_names_roman_surnames</t>
         </is>
       </c>
       <c r="AE2" t="inlineStr">
@@ -865,25 +860,25 @@
       </c>
       <c r="AK2" t="inlineStr">
         <is>
-          <t>Final title passed in as: Epistles of Gamila Khouri and Déborah Houard Discoursing on Sniping</t>
+          <t>The {adjective_1} {noun_1}: {topic}</t>
         </is>
       </c>
       <c r="AL2" t="inlineStr">
         <is>
-          <t>Sniping</t>
+          <t>Hidden Knowledge</t>
         </is>
       </c>
       <c r="AM2" t="n">
-        <v>0.39</v>
+        <v>0.37</v>
       </c>
       <c r="AN2" t="n">
-        <v>585</v>
+        <v>494</v>
       </c>
       <c r="AO2" t="n">
         <v>1</v>
       </c>
       <c r="AP2" t="n">
-        <v>270</v>
+        <v>67</v>
       </c>
       <c r="AQ2" t="n">
         <v>0</v>
@@ -907,7 +902,7 @@
       </c>
       <c r="AW2" t="inlineStr">
         <is>
-          <t>1c8200ab-6aaf-47b0-8043-ce230b9ebf5b</t>
+          <t>8cabe910-b342-4c1b-a39f-cf9ebe255b8e</t>
         </is>
       </c>
       <c r="AX2" t="inlineStr">
@@ -924,42 +919,42 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Vellum</t>
+          <t>Copper Foil</t>
         </is>
       </c>
       <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>500</v>
+      </c>
+      <c r="E3" t="n">
+        <v>62</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Craft (book-binding)</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Craft (book-binding)</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
         <v>2</v>
       </c>
-      <c r="D3" t="n">
-        <v>1500</v>
-      </c>
-      <c r="E3" t="n">
-        <v>93</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Classical</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Land Surveying</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Land Surveying</t>
-        </is>
-      </c>
-      <c r="J3" t="n">
-        <v>1</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" t="n">
-        <v>1</v>
-      </c>
       <c r="M3" t="n">
         <v>0</v>
       </c>
@@ -967,44 +962,49 @@
         <v>1</v>
       </c>
       <c r="O3" t="n">
-        <v>997</v>
+        <v>247</v>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Land Surveying, a Heartening Cycle</t>
+          <t>The Regrettable Imperfection of The Dark Lord and Binding of Books</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Publius Salvidia</t>
+          <t>Cornelius Vorenia</t>
         </is>
       </c>
       <c r="S3" s="10" t="inlineStr">
         <is>
-          <t>Repertae accipere expeditior cursus enuntiatum fratres matrem legationi contendit a</t>
+          <t>The Regrettable Imperfection of The Dark Lord and Binding of Books</t>
         </is>
       </c>
       <c r="T3" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="U3" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="V3" t="n">
-        <v>286</v>
+        <v>48</v>
       </c>
       <c r="W3" t="n">
-        <v>18</v>
+        <v>216</v>
       </c>
       <c r="X3" t="n">
-        <v>14</v>
+        <v>215</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.33</v>
+        <v>0.05</v>
       </c>
       <c r="AB3" t="inlineStr">
         <is>
-          <t>Publius Salvidia</t>
+          <t>Cornelius Vorenia</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>_names_roman_surnames</t>
         </is>
       </c>
       <c r="AE3" t="inlineStr">
@@ -1013,29 +1013,29 @@
         </is>
       </c>
       <c r="AJ3" t="n">
-        <v>0.06</v>
+        <v>0.12</v>
       </c>
       <c r="AK3" t="inlineStr">
         <is>
-          <t>Final title passed in as: Land Surveying, a Heartening Cycle</t>
+          <t>{the_1} {negative_1} of {person_evil} and {topic}</t>
         </is>
       </c>
       <c r="AL3" t="inlineStr">
         <is>
-          <t>Land Surveying</t>
+          <t>Binding of Books</t>
         </is>
       </c>
       <c r="AM3" t="n">
-        <v>0.39</v>
+        <v>0.43</v>
       </c>
       <c r="AN3" t="n">
-        <v>585</v>
+        <v>215</v>
       </c>
       <c r="AO3" t="n">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="AP3" t="n">
-        <v>476</v>
+        <v>32</v>
       </c>
       <c r="AQ3" t="n">
         <v>0</v>
@@ -1059,7 +1059,7 @@
       </c>
       <c r="AW3" t="inlineStr">
         <is>
-          <t>942462a2-eba6-4c27-af3d-bf334a3699b9</t>
+          <t>f2ba2e2a-46c1-42e0-9760-263bb2674cc3</t>
         </is>
       </c>
       <c r="AX3" t="inlineStr">
@@ -1076,102 +1076,127 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Vellum</t>
+          <t>Parchment</t>
         </is>
       </c>
       <c r="C4" t="n">
         <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>750</v>
+        <v>500</v>
       </c>
       <c r="E4" t="n">
+        <v>32</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Regional</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Signaling</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Signaling</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>2</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>1</v>
+      </c>
+      <c r="O4" t="n">
+        <v>342</v>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>Experiences of Marcus Killingbeck and Signaling</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>Nihal Karib</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>The Venerable Thyra Karlsdotter</t>
+        </is>
+      </c>
+      <c r="S4" s="10" t="inlineStr">
+        <is>
+          <t>Λς΄ ἑκατέρα ὦσιν ἐφεστηκυῖα τριγώνῳ ὀρθῆς ἀρχῆς εὐθεῖά ἀμβλυγώνιον προσεκβληθείσης α΄ μς΄</t>
+        </is>
+      </c>
+      <c r="T4" t="n">
+        <v>3</v>
+      </c>
+      <c r="U4" t="n">
+        <v>3</v>
+      </c>
+      <c r="V4" t="n">
+        <v>78</v>
+      </c>
+      <c r="W4" t="n">
         <v>47</v>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Common</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Transmogrification</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Transmogrification</t>
-        </is>
-      </c>
-      <c r="J4" t="n">
-        <v>2</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" t="n">
-        <v>3</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" t="n">
-        <v>1</v>
-      </c>
-      <c r="O4" t="n">
-        <v>297</v>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>Mysteries of Transmogrifying</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>Brother Jacques Asselin the Black</t>
-        </is>
-      </c>
-      <c r="S4" s="10" t="inlineStr">
-        <is>
-          <t>Mysteries of Transmogrifying</t>
-        </is>
-      </c>
-      <c r="T4" t="n">
-        <v>5</v>
-      </c>
-      <c r="U4" t="n">
-        <v>5</v>
-      </c>
-      <c r="V4" t="n">
-        <v>23</v>
-      </c>
-      <c r="W4" t="n">
-        <v>358</v>
-      </c>
       <c r="X4" t="n">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="AA4" t="inlineStr">
-        <is>
-          <t>the Black</t>
-        </is>
+        <v>0.25</v>
       </c>
       <c r="AB4" t="inlineStr">
         <is>
-          <t>Jacques Asselin</t>
-        </is>
-      </c>
-      <c r="AD4" t="inlineStr">
-        <is>
-          <t>Brother</t>
+          <t>Nihal Karib</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>_names_arabic_surnames</t>
         </is>
       </c>
       <c r="AE4" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t>Thyra Karlsdotter</t>
+        </is>
+      </c>
+      <c r="AG4" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_female</t>
+        </is>
+      </c>
+      <c r="AH4" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AI4" t="inlineStr">
+        <is>
+          <t>The Venerable</t>
         </is>
       </c>
       <c r="AJ4" t="n">
@@ -1179,25 +1204,25 @@
       </c>
       <c r="AK4" t="inlineStr">
         <is>
-          <t>Final title passed in as: Mysteries of Transmogrifying</t>
+          <t>{biography_starter} of {person_1} and {topic}</t>
         </is>
       </c>
       <c r="AL4" t="inlineStr">
         <is>
-          <t>Transmogrifying</t>
+          <t>Signaling</t>
         </is>
       </c>
       <c r="AM4" t="n">
-        <v>0.39</v>
+        <v>0.37</v>
       </c>
       <c r="AN4" t="n">
-        <v>293</v>
+        <v>185</v>
       </c>
       <c r="AO4" t="n">
-        <v>2.5</v>
+        <v>1.25</v>
       </c>
       <c r="AP4" t="n">
-        <v>36</v>
+        <v>157</v>
       </c>
       <c r="AQ4" t="n">
         <v>0</v>
@@ -1212,7 +1237,7 @@
         <v>0</v>
       </c>
       <c r="AU4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV4" t="inlineStr">
         <is>
@@ -1221,7 +1246,7 @@
       </c>
       <c r="AW4" t="inlineStr">
         <is>
-          <t>888ab678-509e-4f06-ac1e-7eb53ae42dc8</t>
+          <t>90a46772-239c-4aef-94c0-b81262a6a92f</t>
         </is>
       </c>
       <c r="AX4" t="inlineStr">
@@ -1238,31 +1263,31 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Vellum</t>
+          <t>Parchment</t>
         </is>
       </c>
       <c r="C5" t="n">
         <v>2</v>
       </c>
       <c r="D5" t="n">
-        <v>1500</v>
+        <v>1334</v>
       </c>
       <c r="E5" t="n">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>Classical</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Sniping</t>
+          <t>Craft (tanning)</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Sniping</t>
+          <t>Craft (tanning)</t>
         </is>
       </c>
       <c r="J5" t="n">
@@ -1272,7 +1297,7 @@
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="M5" t="n">
         <v>0</v>
@@ -1281,54 +1306,49 @@
         <v>1</v>
       </c>
       <c r="O5" t="n">
-        <v>660</v>
+        <v>935</v>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Epistles of Gamila Khouri and Déborah Houard Discoursing on Sniping</t>
+          <t>The Damnable Evil of Hrothgar Holderman, in which case Touching Tanning is Given Particular Attention by Way of Instruction and Warning</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Fabricius Egnatia</t>
+          <t>Fróði Larsson</t>
         </is>
       </c>
       <c r="S5" s="10" t="inlineStr">
         <is>
-          <t>Epistles of Gamila Khouri and Déborah Houard Discoursing on Sniping</t>
+          <t>Ne oppida alpes placuit coniurationem liceret occaecati interpretibus omnino maximas muniebatur pugnare servitutem hostem a optimum potentatu respondit necessarii agendos</t>
         </is>
       </c>
       <c r="T5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="U5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="V5" t="n">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="W5" t="n">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="X5" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="AA5" t="inlineStr">
-        <is>
-          <t>the Sloppy</t>
-        </is>
+        <v>0.33</v>
       </c>
       <c r="AB5" t="inlineStr">
         <is>
-          <t>Fabricius Egnatia</t>
-        </is>
-      </c>
-      <c r="AD5" t="inlineStr">
-        <is>
-          <t>Magus</t>
+          <t>Fróði Larsson</t>
+        </is>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_male</t>
         </is>
       </c>
       <c r="AE5" t="inlineStr">
@@ -1341,25 +1361,25 @@
       </c>
       <c r="AK5" t="inlineStr">
         <is>
-          <t>Final title passed in as: Epistles of Gamila Khouri and Déborah Houard Discoursing on Sniping</t>
+          <t>{the_1} {negative_1} of {person_1}, in which case {conjunction_about} {topic} is Given Particular Attention by Way of Instruction and Warning</t>
         </is>
       </c>
       <c r="AL5" t="inlineStr">
         <is>
-          <t>Sniping</t>
+          <t>Tanning</t>
         </is>
       </c>
       <c r="AM5" t="n">
-        <v>0.39</v>
+        <v>0.37</v>
       </c>
       <c r="AN5" t="n">
-        <v>585</v>
+        <v>494</v>
       </c>
       <c r="AO5" t="n">
         <v>1</v>
       </c>
       <c r="AP5" t="n">
-        <v>270</v>
+        <v>441</v>
       </c>
       <c r="AQ5" t="n">
         <v>0</v>
@@ -1383,7 +1403,7 @@
       </c>
       <c r="AW5" t="inlineStr">
         <is>
-          <t>f712600a-228f-4c8a-8117-b8e85aea2687</t>
+          <t>679c09c9-bb9f-46f7-b346-32bcb84dbe28</t>
         </is>
       </c>
       <c r="AX5" t="inlineStr">
@@ -1400,7 +1420,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Gold Foil</t>
+          <t>Parchment</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -1410,7 +1430,7 @@
         <v>750</v>
       </c>
       <c r="E6" t="n">
-        <v>227</v>
+        <v>47</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -1419,45 +1439,45 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Esoteric: Judge’s Choice</t>
+          <t>Knowledge (astrology)</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Art (drawing)</t>
+          <t>Knowledge (astrology)</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M6" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="N6" t="n">
         <v>1</v>
       </c>
       <c r="O6" t="n">
-        <v>26663</v>
+        <v>466</v>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>Contemplation of Candle-Making</t>
+          <t>Transactions Respecting Astrology of Ecgberht Blakemore</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>His Holiness Hakim Ashour</t>
+          <t>The Honorable Hilda Drake the White</t>
         </is>
       </c>
       <c r="S6" s="10" t="inlineStr">
         <is>
-          <t>Contemplation of Candle-Making</t>
+          <t>Transactions Respecting Astrology of Ecgberht Blakemore</t>
         </is>
       </c>
       <c r="T6" t="n">
@@ -1467,62 +1487,72 @@
         <v>5</v>
       </c>
       <c r="V6" t="n">
-        <v>81</v>
+        <v>35</v>
       </c>
       <c r="W6" t="n">
-        <v>81</v>
+        <v>238</v>
       </c>
       <c r="X6" t="n">
-        <v>19</v>
+        <v>237</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>the White</t>
+        </is>
       </c>
       <c r="AB6" t="inlineStr">
         <is>
-          <t>Hakim Ashour</t>
+          <t>Hilda Drake</t>
+        </is>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>_names_anglo_saxon_surnames</t>
         </is>
       </c>
       <c r="AD6" t="inlineStr">
         <is>
-          <t>His Holiness</t>
+          <t>The Honorable</t>
         </is>
       </c>
       <c r="AE6" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="AJ6" t="n">
-        <v>0.3</v>
+        <v>0.06</v>
       </c>
       <c r="AK6" t="inlineStr">
         <is>
-          <t>Final title passed in as: Contemplation of Candle-Making</t>
+          <t>{communication} {conjunction_about} {topic} {conjunction_by} {person_1}</t>
         </is>
       </c>
       <c r="AL6" t="inlineStr">
         <is>
-          <t>Candle-Making</t>
+          <t>Astrology</t>
         </is>
       </c>
       <c r="AM6" t="n">
-        <v>30.31</v>
+        <v>0.37</v>
       </c>
       <c r="AN6" t="n">
-        <v>22733</v>
+        <v>278</v>
       </c>
       <c r="AO6" t="n">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="AP6" t="n">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="AQ6" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AR6" t="n">
-        <v>3750</v>
+        <v>0</v>
       </c>
       <c r="AS6" t="n">
         <v>0</v>
@@ -1540,7 +1570,7 @@
       </c>
       <c r="AW6" t="inlineStr">
         <is>
-          <t>aca69917-66b3-421d-988f-bb93508f0173</t>
+          <t>b1add46f-e75a-4139-9d35-49de7abdcdaa</t>
         </is>
       </c>
       <c r="AX6" t="inlineStr">
@@ -1557,41 +1587,41 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Vellum</t>
+          <t>Parchment</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" t="n">
-        <v>750</v>
+        <v>1500</v>
       </c>
       <c r="E7" t="n">
-        <v>47</v>
+        <v>93</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>Regional</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Transmogrification</t>
+          <t>Knowledge (occult)</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Transmogrification</t>
+          <t>Knowledge (occult)</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K7" t="n">
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M7" t="n">
         <v>0</v>
@@ -1600,54 +1630,49 @@
         <v>1</v>
       </c>
       <c r="O7" t="n">
-        <v>297</v>
+        <v>566</v>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Mysteries of Transmogrifying</t>
+          <t>The Underground Extremity: Hidden Knowledge</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Brother Jacques Asselin the Black</t>
+          <t>Duilius Anneia</t>
         </is>
       </c>
       <c r="S7" s="10" t="inlineStr">
         <is>
-          <t>Mysteries of Transmogrifying</t>
+          <t>Σημεῖα τρίγωνον τεμεῖν κλίσις εὐθύγραμμος ὅρος δυσὶν ἄλλαι τῇ ὑπό κε΄</t>
         </is>
       </c>
       <c r="T7" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="U7" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="V7" t="n">
-        <v>23</v>
+        <v>90</v>
       </c>
       <c r="W7" t="n">
-        <v>358</v>
+        <v>224</v>
       </c>
       <c r="X7" t="n">
-        <v>28</v>
+        <v>222</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="AA7" t="inlineStr">
-        <is>
-          <t>the Black</t>
-        </is>
+        <v>0.05</v>
       </c>
       <c r="AB7" t="inlineStr">
         <is>
-          <t>Jacques Asselin</t>
+          <t>Duilius Anneia</t>
         </is>
       </c>
       <c r="AD7" t="inlineStr">
         <is>
-          <t>Brother</t>
+          <t>Magus</t>
         </is>
       </c>
       <c r="AE7" t="inlineStr">
@@ -1660,25 +1685,25 @@
       </c>
       <c r="AK7" t="inlineStr">
         <is>
-          <t>Final title passed in as: Mysteries of Transmogrifying</t>
+          <t>Final title passed in as: The Underground Extremity: Hidden Knowledge</t>
         </is>
       </c>
       <c r="AL7" t="inlineStr">
         <is>
-          <t>Transmogrifying</t>
+          <t>Hidden Knowledge</t>
         </is>
       </c>
       <c r="AM7" t="n">
-        <v>0.39</v>
+        <v>0.37</v>
       </c>
       <c r="AN7" t="n">
-        <v>293</v>
+        <v>555</v>
       </c>
       <c r="AO7" t="n">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="AP7" t="n">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="AQ7" t="n">
         <v>0</v>
@@ -1702,7 +1727,7 @@
       </c>
       <c r="AW7" t="inlineStr">
         <is>
-          <t>297f406a-fa91-4374-85f6-9604740685a3</t>
+          <t>00874ee2-34ec-4fbe-bd2a-41d31b481f29</t>
         </is>
       </c>
       <c r="AX7" t="inlineStr">
@@ -1719,7 +1744,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Vellum</t>
+          <t>Parchment</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -1733,28 +1758,33 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
+          <t>Regional</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
           <t>Common</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Transmogrification</t>
+          <t>Signaling</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Transmogrification</t>
+          <t>Signaling</t>
         </is>
       </c>
       <c r="J8" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
         <v>2</v>
       </c>
-      <c r="K8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L8" t="n">
-        <v>3</v>
-      </c>
       <c r="M8" t="n">
         <v>0</v>
       </c>
@@ -1762,21 +1792,26 @@
         <v>1</v>
       </c>
       <c r="O8" t="n">
-        <v>297</v>
+        <v>354</v>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>Mysteries of Transmogrifying</t>
+          <t>Experiences of Marcus Killingbeck and Signaling</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Brother Jacques Asselin the Black</t>
+          <t>Nihal Karib</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>The Venerable Thyra Karlsdotter</t>
         </is>
       </c>
       <c r="S8" s="10" t="inlineStr">
         <is>
-          <t>Mysteries of Transmogrifying</t>
+          <t>Λς΄ ἑκατέρα ὦσιν ἐφεστηκυῖα τριγώνῳ ὀρθῆς ἀρχῆς εὐθεῖά ἀμβλυγώνιον προσεκβληθείσης α΄ μς΄</t>
         </is>
       </c>
       <c r="T8" t="n">
@@ -1786,35 +1821,50 @@
         <v>5</v>
       </c>
       <c r="V8" t="n">
-        <v>23</v>
+        <v>78</v>
       </c>
       <c r="W8" t="n">
-        <v>358</v>
+        <v>47</v>
       </c>
       <c r="X8" t="n">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="AA8" t="inlineStr">
-        <is>
-          <t>the Black</t>
-        </is>
+        <v>0.25</v>
       </c>
       <c r="AB8" t="inlineStr">
         <is>
-          <t>Jacques Asselin</t>
+          <t>Nihal Karib</t>
         </is>
       </c>
       <c r="AD8" t="inlineStr">
         <is>
-          <t>Brother</t>
+          <t>The Gracious</t>
         </is>
       </c>
       <c r="AE8" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AF8" t="inlineStr">
+        <is>
+          <t>Thyra Karlsdotter</t>
+        </is>
+      </c>
+      <c r="AG8" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_female</t>
+        </is>
+      </c>
+      <c r="AH8" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AI8" t="inlineStr">
+        <is>
+          <t>The Venerable</t>
         </is>
       </c>
       <c r="AJ8" t="n">
@@ -1822,25 +1872,25 @@
       </c>
       <c r="AK8" t="inlineStr">
         <is>
-          <t>Final title passed in as: Mysteries of Transmogrifying</t>
+          <t>Final title passed in as: Experiences of Marcus Killingbeck and Signaling</t>
         </is>
       </c>
       <c r="AL8" t="inlineStr">
         <is>
-          <t>Transmogrifying</t>
+          <t>Signaling</t>
         </is>
       </c>
       <c r="AM8" t="n">
-        <v>0.39</v>
+        <v>0.37</v>
       </c>
       <c r="AN8" t="n">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="AO8" t="n">
-        <v>2.5</v>
+        <v>1.25</v>
       </c>
       <c r="AP8" t="n">
-        <v>36</v>
+        <v>169</v>
       </c>
       <c r="AQ8" t="n">
         <v>0</v>
@@ -1855,7 +1905,7 @@
         <v>0</v>
       </c>
       <c r="AU8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV8" t="inlineStr">
         <is>
@@ -1864,7 +1914,7 @@
       </c>
       <c r="AW8" t="inlineStr">
         <is>
-          <t>940e0e7e-5912-467c-b3de-62414f31f453</t>
+          <t>37cea019-9d5b-465d-9df7-9ca59685f4a9</t>
         </is>
       </c>
       <c r="AX8" t="inlineStr">
@@ -1881,7 +1931,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Vellum</t>
+          <t>Parchment</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -1900,22 +1950,22 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Transmogrification</t>
+          <t>Knowledge (astrology)</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Transmogrification</t>
+          <t>Knowledge (astrology)</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K9" t="n">
         <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M9" t="n">
         <v>0</v>
@@ -1924,21 +1974,21 @@
         <v>1</v>
       </c>
       <c r="O9" t="n">
-        <v>297</v>
+        <v>503</v>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Mysteries of Transmogrifying</t>
+          <t>Transactions Respecting Astrology of Ecgberht Blakemore</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Brother Jacques Asselin the Black</t>
+          <t>The Honorable Hilda Drake the White</t>
         </is>
       </c>
       <c r="S9" s="10" t="inlineStr">
         <is>
-          <t>Mysteries of Transmogrifying</t>
+          <t>Transactions Respecting Astrology of Ecgberht Blakemore</t>
         </is>
       </c>
       <c r="T9" t="n">
@@ -1948,35 +1998,35 @@
         <v>5</v>
       </c>
       <c r="V9" t="n">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="W9" t="n">
-        <v>358</v>
+        <v>238</v>
       </c>
       <c r="X9" t="n">
-        <v>26</v>
+        <v>236</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="AA9" t="inlineStr">
         <is>
-          <t>the Black</t>
+          <t>the White</t>
         </is>
       </c>
       <c r="AB9" t="inlineStr">
         <is>
-          <t>Jacques Asselin</t>
+          <t>Hilda Drake</t>
         </is>
       </c>
       <c r="AD9" t="inlineStr">
         <is>
-          <t>Brother</t>
+          <t>The Honorable</t>
         </is>
       </c>
       <c r="AE9" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="AJ9" t="n">
@@ -1984,25 +2034,25 @@
       </c>
       <c r="AK9" t="inlineStr">
         <is>
-          <t>Final title passed in as: Mysteries of Transmogrifying</t>
+          <t>Final title passed in as: Transactions Respecting Astrology of Ecgberht Blakemore</t>
         </is>
       </c>
       <c r="AL9" t="inlineStr">
         <is>
-          <t>Transmogrifying</t>
+          <t>Astrology</t>
         </is>
       </c>
       <c r="AM9" t="n">
-        <v>0.39</v>
+        <v>0.37</v>
       </c>
       <c r="AN9" t="n">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="AO9" t="n">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="AP9" t="n">
-        <v>36</v>
+        <v>225</v>
       </c>
       <c r="AQ9" t="n">
         <v>0</v>
@@ -2026,7 +2076,7 @@
       </c>
       <c r="AW9" t="inlineStr">
         <is>
-          <t>13d9b0eb-a5e7-4792-b40a-e65e76a1ffba</t>
+          <t>3dbc18da-f360-49c0-92ab-35a699cee3ac</t>
         </is>
       </c>
       <c r="AX9" t="inlineStr">
@@ -2043,7 +2093,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Vellum</t>
+          <t>Copper Foil</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -2053,32 +2103,32 @@
         <v>750</v>
       </c>
       <c r="E10" t="n">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Classical</t>
+          <t>Common</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Dungeon Bashing</t>
+          <t>Craft (book-binding)</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Dungeon Bashing</t>
+          <t>Craft (book-binding)</t>
         </is>
       </c>
       <c r="J10" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
         <v>2</v>
       </c>
-      <c r="K10" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" t="n">
-        <v>3</v>
-      </c>
       <c r="M10" t="n">
         <v>0</v>
       </c>
@@ -2086,21 +2136,21 @@
         <v>1</v>
       </c>
       <c r="O10" t="n">
-        <v>351</v>
+        <v>249</v>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Embarking Dungeon Bashing</t>
+          <t>The Regrettable Imperfection of The Dark Lord and Binding of Books</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>His Lordship Hildigunnr Madsen</t>
+          <t>Cornelius Vorenia</t>
         </is>
       </c>
       <c r="S10" s="10" t="inlineStr">
         <is>
-          <t>Uxorem observari paratos famem</t>
+          <t>The Regrettable Imperfection of The Dark Lord and Binding of Books</t>
         </is>
       </c>
       <c r="T10" t="n">
@@ -2110,25 +2160,20 @@
         <v>5</v>
       </c>
       <c r="V10" t="n">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="W10" t="n">
-        <v>141</v>
+        <v>216</v>
       </c>
       <c r="X10" t="n">
-        <v>5</v>
+        <v>214</v>
       </c>
       <c r="Y10" t="n">
         <v>0.05</v>
       </c>
       <c r="AB10" t="inlineStr">
         <is>
-          <t>Hildigunnr Madsen</t>
-        </is>
-      </c>
-      <c r="AD10" t="inlineStr">
-        <is>
-          <t>His Lordship</t>
+          <t>Cornelius Vorenia</t>
         </is>
       </c>
       <c r="AE10" t="inlineStr">
@@ -2137,29 +2182,29 @@
         </is>
       </c>
       <c r="AJ10" t="n">
-        <v>0.06</v>
+        <v>0.12</v>
       </c>
       <c r="AK10" t="inlineStr">
         <is>
-          <t>Final title passed in as: Embarking Dungeon Bashing</t>
+          <t>Final title passed in as: The Regrettable Imperfection of The Dark Lord and Binding of Books</t>
         </is>
       </c>
       <c r="AL10" t="inlineStr">
         <is>
-          <t>Dungeon Bashing</t>
+          <t>Binding of Books</t>
         </is>
       </c>
       <c r="AM10" t="n">
-        <v>0.39</v>
+        <v>0.43</v>
       </c>
       <c r="AN10" t="n">
-        <v>293</v>
+        <v>323</v>
       </c>
       <c r="AO10" t="n">
-        <v>2.5</v>
+        <v>1.25</v>
       </c>
       <c r="AP10" t="n">
-        <v>90</v>
+        <v>34</v>
       </c>
       <c r="AQ10" t="n">
         <v>0</v>
@@ -2183,7 +2228,7 @@
       </c>
       <c r="AW10" t="inlineStr">
         <is>
-          <t>c6a2e7d3-a4e2-441d-b53f-998059484886</t>
+          <t>419e4f90-d967-4d0a-89ed-d3bc1826a52b</t>
         </is>
       </c>
       <c r="AX10" t="inlineStr">
@@ -2200,97 +2245,87 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Gold Foil</t>
+          <t>Parchment</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" t="n">
-        <v>750</v>
+        <v>1500</v>
       </c>
       <c r="E11" t="n">
-        <v>227</v>
+        <v>93</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>Regional</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Esoteric: Judge’s Choice</t>
+          <t>Knowledge (occult)</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Craft (baking)</t>
+          <t>Knowledge (occult)</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M11" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N11" t="n">
         <v>1</v>
       </c>
       <c r="O11" t="n">
-        <v>26663</v>
+        <v>566</v>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Contemplation of Candle-Making</t>
+          <t>The Underground Extremity: Hidden Knowledge</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>His Holiness Hakim Ashour</t>
+          <t>Duilius Anneia</t>
         </is>
       </c>
       <c r="S11" s="10" t="inlineStr">
         <is>
-          <t>Contemplation of Candle-Making</t>
+          <t>Σημεῖα τρίγωνον τεμεῖν κλίσις εὐθύγραμμος ὅρος δυσὶν ἄλλαι τῇ ὑπό κε΄</t>
         </is>
       </c>
       <c r="T11" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="U11" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="V11" t="n">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="W11" t="n">
-        <v>81</v>
+        <v>224</v>
       </c>
       <c r="X11" t="n">
-        <v>18</v>
+        <v>221</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="AA11" t="inlineStr">
-        <is>
-          <t>the Hooded</t>
-        </is>
+        <v>0.05</v>
       </c>
       <c r="AB11" t="inlineStr">
         <is>
-          <t>Hakim Ashour</t>
-        </is>
-      </c>
-      <c r="AD11" t="inlineStr">
-        <is>
-          <t>His Holiness</t>
+          <t>Duilius Anneia</t>
         </is>
       </c>
       <c r="AE11" t="inlineStr">
@@ -2299,35 +2334,35 @@
         </is>
       </c>
       <c r="AJ11" t="n">
-        <v>0.3</v>
+        <v>0.06</v>
       </c>
       <c r="AK11" t="inlineStr">
         <is>
-          <t>Final title passed in as: Contemplation of Candle-Making</t>
+          <t>Final title passed in as: The Underground Extremity: Hidden Knowledge</t>
         </is>
       </c>
       <c r="AL11" t="inlineStr">
         <is>
-          <t>Candle-Making</t>
+          <t>Hidden Knowledge</t>
         </is>
       </c>
       <c r="AM11" t="n">
-        <v>30.31</v>
+        <v>0.37</v>
       </c>
       <c r="AN11" t="n">
-        <v>22733</v>
+        <v>555</v>
       </c>
       <c r="AO11" t="n">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="AP11" t="n">
-        <v>180</v>
+        <v>72</v>
       </c>
       <c r="AQ11" t="n">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="AR11" t="n">
-        <v>3750</v>
+        <v>0</v>
       </c>
       <c r="AS11" t="n">
         <v>0</v>
@@ -2345,7 +2380,7 @@
       </c>
       <c r="AW11" t="inlineStr">
         <is>
-          <t>87bcd06a-b242-47fa-85a9-5622965ab916</t>
+          <t>cb6303c7-14ec-46f0-ac06-b749164204a2</t>
         </is>
       </c>
       <c r="AX11" t="inlineStr">
@@ -2366,13 +2401,13 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" t="n">
-        <v>1500</v>
+        <v>750</v>
       </c>
       <c r="E12" t="n">
-        <v>93</v>
+        <v>47</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -2381,23 +2416,23 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Knowledge (geography)</t>
+          <t>Knowledge (astrology)</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Knowledge (geography)</t>
+          <t>Knowledge (astrology)</t>
         </is>
       </c>
       <c r="J12" t="n">
+        <v>3</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
         <v>4</v>
       </c>
-      <c r="K12" t="n">
-        <v>0</v>
-      </c>
-      <c r="L12" t="n">
-        <v>3</v>
-      </c>
       <c r="M12" t="n">
         <v>0</v>
       </c>
@@ -2405,54 +2440,59 @@
         <v>1</v>
       </c>
       <c r="O12" t="n">
-        <v>3070</v>
+        <v>503</v>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Experiences of Hildebeorht Johnsen and Geography</t>
+          <t>Transactions Respecting Astrology of Ecgberht Blakemore</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>Baron Jamal Gharsallah</t>
+          <t>The Honorable Hilda Drake the White</t>
         </is>
       </c>
       <c r="S12" s="10" t="inlineStr">
         <is>
-          <t>Experiences of Hildebeorht Johnsen and Geography</t>
+          <t>Transactions Respecting Astrology of Ecgberht Blakemore</t>
         </is>
       </c>
       <c r="T12" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="U12" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="V12" t="n">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="W12" t="n">
-        <v>45</v>
+        <v>238</v>
       </c>
       <c r="X12" t="n">
-        <v>16</v>
+        <v>235</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.25</v>
+        <v>0.05</v>
+      </c>
+      <c r="AA12" t="inlineStr">
+        <is>
+          <t>the White</t>
+        </is>
       </c>
       <c r="AB12" t="inlineStr">
         <is>
-          <t>Jamal Gharsallah</t>
+          <t>Hilda Drake</t>
         </is>
       </c>
       <c r="AD12" t="inlineStr">
         <is>
-          <t>Baron</t>
+          <t>The Honorable</t>
         </is>
       </c>
       <c r="AE12" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="AJ12" t="n">
@@ -2460,25 +2500,25 @@
       </c>
       <c r="AK12" t="inlineStr">
         <is>
-          <t>Final title passed in as: Experiences of Hildebeorht Johnsen and Geography</t>
+          <t>Final title passed in as: Transactions Respecting Astrology of Ecgberht Blakemore</t>
         </is>
       </c>
       <c r="AL12" t="inlineStr">
         <is>
-          <t>Geography</t>
+          <t>Astrology</t>
         </is>
       </c>
       <c r="AM12" t="n">
         <v>0.37</v>
       </c>
       <c r="AN12" t="n">
-        <v>555</v>
+        <v>278</v>
       </c>
       <c r="AO12" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AP12" t="n">
-        <v>2700</v>
+        <v>225</v>
       </c>
       <c r="AQ12" t="n">
         <v>0</v>
@@ -2502,7 +2542,7 @@
       </c>
       <c r="AW12" t="inlineStr">
         <is>
-          <t>6882d4ff-76b8-47e0-8371-a703c08ba130</t>
+          <t>56889dd0-fd47-46f6-a898-7e00d4024e5f</t>
         </is>
       </c>
       <c r="AX12" t="inlineStr">
@@ -2523,13 +2563,13 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13" t="n">
-        <v>1500</v>
+        <v>750</v>
       </c>
       <c r="E13" t="n">
-        <v>93</v>
+        <v>47</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -2538,23 +2578,23 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Knowledge (geography)</t>
+          <t>Knowledge (astrology)</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Knowledge (geography)</t>
+          <t>Knowledge (astrology)</t>
         </is>
       </c>
       <c r="J13" t="n">
+        <v>3</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
         <v>4</v>
       </c>
-      <c r="K13" t="n">
-        <v>0</v>
-      </c>
-      <c r="L13" t="n">
-        <v>3</v>
-      </c>
       <c r="M13" t="n">
         <v>0</v>
       </c>
@@ -2562,59 +2602,59 @@
         <v>1</v>
       </c>
       <c r="O13" t="n">
-        <v>3070</v>
+        <v>503</v>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Experiences of Hildebeorht Johnsen and Geography</t>
+          <t>Transactions Respecting Astrology of Ecgberht Blakemore</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Baron Jamal Gharsallah</t>
+          <t>The Honorable Hilda Drake the White</t>
         </is>
       </c>
       <c r="S13" s="10" t="inlineStr">
         <is>
-          <t>Experiences of Hildebeorht Johnsen and Geography</t>
+          <t>Transactions Respecting Astrology of Ecgberht Blakemore</t>
         </is>
       </c>
       <c r="T13" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="U13" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="V13" t="n">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="W13" t="n">
-        <v>45</v>
+        <v>238</v>
       </c>
       <c r="X13" t="n">
-        <v>15</v>
+        <v>234</v>
       </c>
       <c r="Y13" t="n">
-        <v>0.25</v>
+        <v>0.05</v>
       </c>
       <c r="AA13" t="inlineStr">
         <is>
-          <t>the Lucky</t>
+          <t>the White</t>
         </is>
       </c>
       <c r="AB13" t="inlineStr">
         <is>
-          <t>Jamal Gharsallah</t>
+          <t>Hilda Drake</t>
         </is>
       </c>
       <c r="AD13" t="inlineStr">
         <is>
-          <t>Baron</t>
+          <t>The Honorable</t>
         </is>
       </c>
       <c r="AE13" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="AJ13" t="n">
@@ -2622,25 +2662,25 @@
       </c>
       <c r="AK13" t="inlineStr">
         <is>
-          <t>Final title passed in as: Experiences of Hildebeorht Johnsen and Geography</t>
+          <t>Final title passed in as: Transactions Respecting Astrology of Ecgberht Blakemore</t>
         </is>
       </c>
       <c r="AL13" t="inlineStr">
         <is>
-          <t>Geography</t>
+          <t>Astrology</t>
         </is>
       </c>
       <c r="AM13" t="n">
         <v>0.37</v>
       </c>
       <c r="AN13" t="n">
-        <v>555</v>
+        <v>278</v>
       </c>
       <c r="AO13" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AP13" t="n">
-        <v>2700</v>
+        <v>225</v>
       </c>
       <c r="AQ13" t="n">
         <v>0</v>
@@ -2664,7 +2704,7 @@
       </c>
       <c r="AW13" t="inlineStr">
         <is>
-          <t>790bceb0-d16f-491c-a33e-ddb9816f5753</t>
+          <t>e5ce532f-3c15-4eab-a714-7a4eaeb66b44</t>
         </is>
       </c>
       <c r="AX13" t="inlineStr">
@@ -2685,13 +2725,13 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>1500</v>
+        <v>750</v>
       </c>
       <c r="E14" t="n">
-        <v>93</v>
+        <v>47</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -2700,23 +2740,23 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Knowledge (geography)</t>
+          <t>Knowledge (astrology)</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Knowledge (geography)</t>
+          <t>Knowledge (astrology)</t>
         </is>
       </c>
       <c r="J14" t="n">
+        <v>3</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
         <v>4</v>
       </c>
-      <c r="K14" t="n">
-        <v>0</v>
-      </c>
-      <c r="L14" t="n">
-        <v>3</v>
-      </c>
       <c r="M14" t="n">
         <v>0</v>
       </c>
@@ -2724,54 +2764,59 @@
         <v>1</v>
       </c>
       <c r="O14" t="n">
-        <v>3070</v>
+        <v>503</v>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Experiences of Hildebeorht Johnsen and Geography</t>
+          <t>Transactions Respecting Astrology of Ecgberht Blakemore</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>Baron Jamal Gharsallah</t>
+          <t>The Honorable Hilda Drake the White</t>
         </is>
       </c>
       <c r="S14" s="10" t="inlineStr">
         <is>
-          <t>Experiences of Hildebeorht Johnsen and Geography</t>
+          <t>Transactions Respecting Astrology of Ecgberht Blakemore</t>
         </is>
       </c>
       <c r="T14" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="U14" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="V14" t="n">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="W14" t="n">
-        <v>45</v>
+        <v>238</v>
       </c>
       <c r="X14" t="n">
-        <v>14</v>
+        <v>233</v>
       </c>
       <c r="Y14" t="n">
-        <v>0.25</v>
+        <v>0.05</v>
+      </c>
+      <c r="AA14" t="inlineStr">
+        <is>
+          <t>the White</t>
+        </is>
       </c>
       <c r="AB14" t="inlineStr">
         <is>
-          <t>Jamal Gharsallah</t>
+          <t>Hilda Drake</t>
         </is>
       </c>
       <c r="AD14" t="inlineStr">
         <is>
-          <t>Baron</t>
+          <t>The Honorable</t>
         </is>
       </c>
       <c r="AE14" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="AJ14" t="n">
@@ -2779,25 +2824,25 @@
       </c>
       <c r="AK14" t="inlineStr">
         <is>
-          <t>Final title passed in as: Experiences of Hildebeorht Johnsen and Geography</t>
+          <t>Final title passed in as: Transactions Respecting Astrology of Ecgberht Blakemore</t>
         </is>
       </c>
       <c r="AL14" t="inlineStr">
         <is>
-          <t>Geography</t>
+          <t>Astrology</t>
         </is>
       </c>
       <c r="AM14" t="n">
         <v>0.37</v>
       </c>
       <c r="AN14" t="n">
-        <v>555</v>
+        <v>278</v>
       </c>
       <c r="AO14" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AP14" t="n">
-        <v>2700</v>
+        <v>225</v>
       </c>
       <c r="AQ14" t="n">
         <v>0</v>
@@ -2821,7 +2866,7 @@
       </c>
       <c r="AW14" t="inlineStr">
         <is>
-          <t>733adb2d-1261-481f-87d9-15ffb6b73293</t>
+          <t>e1b22fbf-6a91-424c-b5b9-c1a36dd9db13</t>
         </is>
       </c>
       <c r="AX14" t="inlineStr">
@@ -2838,7 +2883,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Vellum</t>
+          <t>Parchment</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -2852,17 +2897,17 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Ancient</t>
+          <t>Regional</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Craft (bow-making)</t>
+          <t>Knowledge (occult)</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Craft (bow-making)</t>
+          <t>Knowledge (occult)</t>
         </is>
       </c>
       <c r="J15" t="n">
@@ -2881,21 +2926,21 @@
         <v>1</v>
       </c>
       <c r="O15" t="n">
-        <v>536</v>
+        <v>566</v>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>The Eclipsed Gyre: Bowers Crafte</t>
+          <t>The Underground Extremity: Hidden Knowledge</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>Édith Gobet</t>
+          <t>Duilius Anneia</t>
         </is>
       </c>
       <c r="S15" s="10" t="inlineStr">
         <is>
-          <t>𐎧𐎨𐎬𐎤𐎭𐎠𐎤𐎮𐎽 𐎯𐎱𐎤𐏂𐎨𐎸𐎬 𐎭𐎤𐎢 𐎥𐎸𐎽𐎢𐎤</t>
+          <t>Σημεῖα τρίγωνον τεμεῖν κλίσις εὐθύγραμμος ὅρος δυσὶν ἄλλαι τῇ ὑπό κε΄</t>
         </is>
       </c>
       <c r="T15" t="n">
@@ -2905,25 +2950,25 @@
         <v>9</v>
       </c>
       <c r="V15" t="n">
-        <v>870</v>
+        <v>90</v>
       </c>
       <c r="W15" t="n">
-        <v>565</v>
+        <v>224</v>
       </c>
       <c r="X15" t="n">
-        <v>6</v>
+        <v>220</v>
       </c>
       <c r="Y15" t="n">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="AB15" t="inlineStr">
         <is>
-          <t>Édith Gobet</t>
+          <t>Duilius Anneia</t>
         </is>
       </c>
       <c r="AE15" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="AJ15" t="n">
@@ -2931,25 +2976,25 @@
       </c>
       <c r="AK15" t="inlineStr">
         <is>
-          <t>Final title passed in as: The Eclipsed Gyre: Bowers Crafte</t>
+          <t>Final title passed in as: The Underground Extremity: Hidden Knowledge</t>
         </is>
       </c>
       <c r="AL15" t="inlineStr">
         <is>
-          <t>Bowers Crafte</t>
+          <t>Hidden Knowledge</t>
         </is>
       </c>
       <c r="AM15" t="n">
-        <v>0.39</v>
+        <v>0.37</v>
       </c>
       <c r="AN15" t="n">
-        <v>585</v>
+        <v>555</v>
       </c>
       <c r="AO15" t="n">
         <v>1</v>
       </c>
       <c r="AP15" t="n">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="AQ15" t="n">
         <v>0</v>
@@ -2973,7 +3018,7 @@
       </c>
       <c r="AW15" t="inlineStr">
         <is>
-          <t>e3afbfca-f5f2-47b9-9091-a9a95ba01942</t>
+          <t>2143dd8f-7fc0-40e0-b0a3-3126adf08c3b</t>
         </is>
       </c>
       <c r="AX15" t="inlineStr">
@@ -2990,42 +3035,42 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Vellum</t>
+          <t>Copper Foil</t>
         </is>
       </c>
       <c r="C16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" t="n">
+        <v>750</v>
+      </c>
+      <c r="E16" t="n">
+        <v>92</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Craft (book-binding)</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Craft (book-binding)</t>
+        </is>
+      </c>
+      <c r="J16" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
         <v>2</v>
       </c>
-      <c r="D16" t="n">
-        <v>1500</v>
-      </c>
-      <c r="E16" t="n">
-        <v>93</v>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>Ancient</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>Craft (bow-making)</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>Craft (bow-making)</t>
-        </is>
-      </c>
-      <c r="J16" t="n">
-        <v>1</v>
-      </c>
-      <c r="K16" t="n">
-        <v>0</v>
-      </c>
-      <c r="L16" t="n">
-        <v>1</v>
-      </c>
       <c r="M16" t="n">
         <v>0</v>
       </c>
@@ -3033,75 +3078,80 @@
         <v>1</v>
       </c>
       <c r="O16" t="n">
-        <v>536</v>
+        <v>249</v>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>The Eclipsed Gyre: Bowers Crafte</t>
+          <t>The Regrettable Imperfection of The Dark Lord and Binding of Books</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>Édith Gobet</t>
+          <t>Cornelius Vorenia</t>
         </is>
       </c>
       <c r="S16" s="10" t="inlineStr">
         <is>
-          <t>𐎧𐎨𐎬𐎤𐎭𐎠𐎤𐎮𐎽 𐎯𐎱𐎤𐏂𐎨𐎸𐎬 𐎭𐎤𐎢 𐎥𐎸𐎽𐎢𐎤</t>
+          <t>The Regrettable Imperfection of The Dark Lord and Binding of Books</t>
         </is>
       </c>
       <c r="T16" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="U16" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="V16" t="n">
-        <v>870</v>
+        <v>48</v>
       </c>
       <c r="W16" t="n">
-        <v>565</v>
+        <v>216</v>
       </c>
       <c r="X16" t="n">
-        <v>5</v>
+        <v>213</v>
       </c>
       <c r="Y16" t="n">
-        <v>0.01</v>
+        <v>0.05</v>
+      </c>
+      <c r="AA16" t="inlineStr">
+        <is>
+          <t>the Merciful</t>
+        </is>
       </c>
       <c r="AB16" t="inlineStr">
         <is>
-          <t>Édith Gobet</t>
+          <t>Cornelius Vorenia</t>
         </is>
       </c>
       <c r="AE16" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="AJ16" t="n">
-        <v>0.06</v>
+        <v>0.12</v>
       </c>
       <c r="AK16" t="inlineStr">
         <is>
-          <t>Final title passed in as: The Eclipsed Gyre: Bowers Crafte</t>
+          <t>Final title passed in as: The Regrettable Imperfection of The Dark Lord and Binding of Books</t>
         </is>
       </c>
       <c r="AL16" t="inlineStr">
         <is>
-          <t>Bowers Crafte</t>
+          <t>Binding of Books</t>
         </is>
       </c>
       <c r="AM16" t="n">
-        <v>0.39</v>
+        <v>0.43</v>
       </c>
       <c r="AN16" t="n">
-        <v>585</v>
+        <v>323</v>
       </c>
       <c r="AO16" t="n">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="AP16" t="n">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="AQ16" t="n">
         <v>0</v>
@@ -3125,805 +3175,10 @@
       </c>
       <c r="AW16" t="inlineStr">
         <is>
-          <t>f43fd3bc-6572-4af6-91d9-32e348eabbe1</t>
+          <t>bd8b95a6-265f-47b1-962c-ba8829ee2bf5</t>
         </is>
       </c>
       <c r="AX16" t="inlineStr">
-        <is>
-          <t>has_been_archived</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Codex</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Parchment</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>2</v>
-      </c>
-      <c r="D17" t="n">
-        <v>1500</v>
-      </c>
-      <c r="E17" t="n">
-        <v>93</v>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Common</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>Knowledge (geography)</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>Knowledge (geography)</t>
-        </is>
-      </c>
-      <c r="J17" t="n">
-        <v>4</v>
-      </c>
-      <c r="K17" t="n">
-        <v>0</v>
-      </c>
-      <c r="L17" t="n">
-        <v>3</v>
-      </c>
-      <c r="M17" t="n">
-        <v>0</v>
-      </c>
-      <c r="N17" t="n">
-        <v>1</v>
-      </c>
-      <c r="O17" t="n">
-        <v>3070</v>
-      </c>
-      <c r="P17" t="inlineStr">
-        <is>
-          <t>Experiences of Hildebeorht Johnsen and Geography</t>
-        </is>
-      </c>
-      <c r="Q17" t="inlineStr">
-        <is>
-          <t>Baron Jamal Gharsallah</t>
-        </is>
-      </c>
-      <c r="S17" s="10" t="inlineStr">
-        <is>
-          <t>Experiences of Hildebeorht Johnsen and Geography</t>
-        </is>
-      </c>
-      <c r="T17" t="n">
-        <v>9</v>
-      </c>
-      <c r="U17" t="n">
-        <v>9</v>
-      </c>
-      <c r="V17" t="n">
-        <v>58</v>
-      </c>
-      <c r="W17" t="n">
-        <v>45</v>
-      </c>
-      <c r="X17" t="n">
-        <v>13</v>
-      </c>
-      <c r="Y17" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="AA17" t="inlineStr">
-        <is>
-          <t>the Ornate</t>
-        </is>
-      </c>
-      <c r="AB17" t="inlineStr">
-        <is>
-          <t>Jamal Gharsallah</t>
-        </is>
-      </c>
-      <c r="AD17" t="inlineStr">
-        <is>
-          <t>Baron</t>
-        </is>
-      </c>
-      <c r="AE17" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="AJ17" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="AK17" t="inlineStr">
-        <is>
-          <t>Final title passed in as: Experiences of Hildebeorht Johnsen and Geography</t>
-        </is>
-      </c>
-      <c r="AL17" t="inlineStr">
-        <is>
-          <t>Geography</t>
-        </is>
-      </c>
-      <c r="AM17" t="n">
-        <v>0.37</v>
-      </c>
-      <c r="AN17" t="n">
-        <v>555</v>
-      </c>
-      <c r="AO17" t="n">
-        <v>10</v>
-      </c>
-      <c r="AP17" t="n">
-        <v>2700</v>
-      </c>
-      <c r="AQ17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU17" t="b">
-        <v>0</v>
-      </c>
-      <c r="AV17" t="inlineStr">
-        <is>
-          <t>Standard</t>
-        </is>
-      </c>
-      <c r="AW17" t="inlineStr">
-        <is>
-          <t>c3c2098d-730f-40d8-93b6-253b49f24fe5</t>
-        </is>
-      </c>
-      <c r="AX17" t="inlineStr">
-        <is>
-          <t>has_been_archived</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Codex</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Vellum</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
-        <v>2</v>
-      </c>
-      <c r="D18" t="n">
-        <v>1500</v>
-      </c>
-      <c r="E18" t="n">
-        <v>93</v>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>Common</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>Sniping</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>Sniping</t>
-        </is>
-      </c>
-      <c r="J18" t="n">
-        <v>1</v>
-      </c>
-      <c r="K18" t="n">
-        <v>0</v>
-      </c>
-      <c r="L18" t="n">
-        <v>1</v>
-      </c>
-      <c r="M18" t="n">
-        <v>0</v>
-      </c>
-      <c r="N18" t="n">
-        <v>1</v>
-      </c>
-      <c r="O18" t="n">
-        <v>660</v>
-      </c>
-      <c r="P18" t="inlineStr">
-        <is>
-          <t>Epistles of Gamila Khouri and Déborah Houard Discoursing on Sniping</t>
-        </is>
-      </c>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>Fabricius Egnatia</t>
-        </is>
-      </c>
-      <c r="S18" s="10" t="inlineStr">
-        <is>
-          <t>Epistles of Gamila Khouri and Déborah Houard Discoursing on Sniping</t>
-        </is>
-      </c>
-      <c r="T18" t="n">
-        <v>9</v>
-      </c>
-      <c r="U18" t="n">
-        <v>9</v>
-      </c>
-      <c r="V18" t="n">
-        <v>32</v>
-      </c>
-      <c r="W18" t="n">
-        <v>29</v>
-      </c>
-      <c r="X18" t="n">
-        <v>8</v>
-      </c>
-      <c r="Y18" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="AB18" t="inlineStr">
-        <is>
-          <t>Fabricius Egnatia</t>
-        </is>
-      </c>
-      <c r="AD18" t="inlineStr">
-        <is>
-          <t>His Lordship</t>
-        </is>
-      </c>
-      <c r="AE18" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="AJ18" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="AK18" t="inlineStr">
-        <is>
-          <t>Final title passed in as: Epistles of Gamila Khouri and Déborah Houard Discoursing on Sniping</t>
-        </is>
-      </c>
-      <c r="AL18" t="inlineStr">
-        <is>
-          <t>Sniping</t>
-        </is>
-      </c>
-      <c r="AM18" t="n">
-        <v>0.39</v>
-      </c>
-      <c r="AN18" t="n">
-        <v>585</v>
-      </c>
-      <c r="AO18" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP18" t="n">
-        <v>270</v>
-      </c>
-      <c r="AQ18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU18" t="b">
-        <v>0</v>
-      </c>
-      <c r="AV18" t="inlineStr">
-        <is>
-          <t>Standard</t>
-        </is>
-      </c>
-      <c r="AW18" t="inlineStr">
-        <is>
-          <t>4ba1dea9-7196-42a1-935c-b8b915992f24</t>
-        </is>
-      </c>
-      <c r="AX18" t="inlineStr">
-        <is>
-          <t>has_been_archived</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Codex</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Gold Foil</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
-        <v>1</v>
-      </c>
-      <c r="D19" t="n">
-        <v>750</v>
-      </c>
-      <c r="E19" t="n">
-        <v>227</v>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>Common</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>Esoteric: Judge’s Choice</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>Performance (epic poetry)</t>
-        </is>
-      </c>
-      <c r="J19" t="n">
-        <v>2</v>
-      </c>
-      <c r="K19" t="n">
-        <v>1</v>
-      </c>
-      <c r="L19" t="n">
-        <v>3</v>
-      </c>
-      <c r="M19" t="n">
-        <v>2</v>
-      </c>
-      <c r="N19" t="n">
-        <v>1</v>
-      </c>
-      <c r="O19" t="n">
-        <v>26663</v>
-      </c>
-      <c r="P19" t="inlineStr">
-        <is>
-          <t>Contemplation of Candle-Making</t>
-        </is>
-      </c>
-      <c r="Q19" t="inlineStr">
-        <is>
-          <t>His Holiness Hakim Ashour</t>
-        </is>
-      </c>
-      <c r="S19" s="10" t="inlineStr">
-        <is>
-          <t>Contemplation of Candle-Making</t>
-        </is>
-      </c>
-      <c r="T19" t="n">
-        <v>5</v>
-      </c>
-      <c r="U19" t="n">
-        <v>5</v>
-      </c>
-      <c r="V19" t="n">
-        <v>81</v>
-      </c>
-      <c r="W19" t="n">
-        <v>81</v>
-      </c>
-      <c r="X19" t="n">
-        <v>12</v>
-      </c>
-      <c r="Y19" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="AB19" t="inlineStr">
-        <is>
-          <t>Hakim Ashour</t>
-        </is>
-      </c>
-      <c r="AD19" t="inlineStr">
-        <is>
-          <t>His Holiness</t>
-        </is>
-      </c>
-      <c r="AE19" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="AJ19" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="AK19" t="inlineStr">
-        <is>
-          <t>Final title passed in as: Contemplation of Candle-Making</t>
-        </is>
-      </c>
-      <c r="AL19" t="inlineStr">
-        <is>
-          <t>Candle-Making</t>
-        </is>
-      </c>
-      <c r="AM19" t="n">
-        <v>30.31</v>
-      </c>
-      <c r="AN19" t="n">
-        <v>22733</v>
-      </c>
-      <c r="AO19" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="AP19" t="n">
-        <v>180</v>
-      </c>
-      <c r="AQ19" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="AR19" t="n">
-        <v>3750</v>
-      </c>
-      <c r="AS19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU19" t="b">
-        <v>0</v>
-      </c>
-      <c r="AV19" t="inlineStr">
-        <is>
-          <t>Standard</t>
-        </is>
-      </c>
-      <c r="AW19" t="inlineStr">
-        <is>
-          <t>1e162bdb-11a1-45d4-a8d4-9d5e49fd6aa6</t>
-        </is>
-      </c>
-      <c r="AX19" t="inlineStr">
-        <is>
-          <t>has_been_archived</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Codex</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Gold Foil</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>1</v>
-      </c>
-      <c r="D20" t="n">
-        <v>750</v>
-      </c>
-      <c r="E20" t="n">
-        <v>227</v>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>Common</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>Esoteric: Judge’s Choice</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>Art (calligraphy)</t>
-        </is>
-      </c>
-      <c r="J20" t="n">
-        <v>2</v>
-      </c>
-      <c r="K20" t="n">
-        <v>1</v>
-      </c>
-      <c r="L20" t="n">
-        <v>3</v>
-      </c>
-      <c r="M20" t="n">
-        <v>4</v>
-      </c>
-      <c r="N20" t="n">
-        <v>1</v>
-      </c>
-      <c r="O20" t="n">
-        <v>26663</v>
-      </c>
-      <c r="P20" t="inlineStr">
-        <is>
-          <t>Contemplation of Candle-Making</t>
-        </is>
-      </c>
-      <c r="Q20" t="inlineStr">
-        <is>
-          <t>His Holiness Hakim Ashour</t>
-        </is>
-      </c>
-      <c r="S20" s="10" t="inlineStr">
-        <is>
-          <t>Contemplation of Candle-Making</t>
-        </is>
-      </c>
-      <c r="T20" t="n">
-        <v>5</v>
-      </c>
-      <c r="U20" t="n">
-        <v>5</v>
-      </c>
-      <c r="V20" t="n">
-        <v>81</v>
-      </c>
-      <c r="W20" t="n">
-        <v>81</v>
-      </c>
-      <c r="X20" t="n">
-        <v>11</v>
-      </c>
-      <c r="Y20" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="AB20" t="inlineStr">
-        <is>
-          <t>Hakim Ashour</t>
-        </is>
-      </c>
-      <c r="AD20" t="inlineStr">
-        <is>
-          <t>His Holiness</t>
-        </is>
-      </c>
-      <c r="AE20" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="AJ20" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="AK20" t="inlineStr">
-        <is>
-          <t>Final title passed in as: Contemplation of Candle-Making</t>
-        </is>
-      </c>
-      <c r="AL20" t="inlineStr">
-        <is>
-          <t>Candle-Making</t>
-        </is>
-      </c>
-      <c r="AM20" t="n">
-        <v>30.31</v>
-      </c>
-      <c r="AN20" t="n">
-        <v>22733</v>
-      </c>
-      <c r="AO20" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="AP20" t="n">
-        <v>180</v>
-      </c>
-      <c r="AQ20" t="n">
-        <v>5</v>
-      </c>
-      <c r="AR20" t="n">
-        <v>3750</v>
-      </c>
-      <c r="AS20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU20" t="b">
-        <v>0</v>
-      </c>
-      <c r="AV20" t="inlineStr">
-        <is>
-          <t>Standard</t>
-        </is>
-      </c>
-      <c r="AW20" t="inlineStr">
-        <is>
-          <t>1a96b0e7-fc17-49fd-a514-ed9537d7ca8a</t>
-        </is>
-      </c>
-      <c r="AX20" t="inlineStr">
-        <is>
-          <t>has_been_archived</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Codex</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Parchment</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>2</v>
-      </c>
-      <c r="D21" t="n">
-        <v>1500</v>
-      </c>
-      <c r="E21" t="n">
-        <v>93</v>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Common</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>Knowledge (geography)</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>Knowledge (geography)</t>
-        </is>
-      </c>
-      <c r="J21" t="n">
-        <v>4</v>
-      </c>
-      <c r="K21" t="n">
-        <v>0</v>
-      </c>
-      <c r="L21" t="n">
-        <v>3</v>
-      </c>
-      <c r="M21" t="n">
-        <v>0</v>
-      </c>
-      <c r="N21" t="n">
-        <v>1</v>
-      </c>
-      <c r="O21" t="n">
-        <v>3070</v>
-      </c>
-      <c r="P21" t="inlineStr">
-        <is>
-          <t>Experiences of Hildebeorht Johnsen and Geography</t>
-        </is>
-      </c>
-      <c r="Q21" t="inlineStr">
-        <is>
-          <t>Baron Jamal Gharsallah</t>
-        </is>
-      </c>
-      <c r="S21" s="10" t="inlineStr">
-        <is>
-          <t>Experiences of Hildebeorht Johnsen and Geography</t>
-        </is>
-      </c>
-      <c r="T21" t="n">
-        <v>9</v>
-      </c>
-      <c r="U21" t="n">
-        <v>9</v>
-      </c>
-      <c r="V21" t="n">
-        <v>58</v>
-      </c>
-      <c r="W21" t="n">
-        <v>45</v>
-      </c>
-      <c r="X21" t="n">
-        <v>12</v>
-      </c>
-      <c r="Y21" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="AA21" t="inlineStr">
-        <is>
-          <t>the Crippled</t>
-        </is>
-      </c>
-      <c r="AB21" t="inlineStr">
-        <is>
-          <t>Jamal Gharsallah</t>
-        </is>
-      </c>
-      <c r="AD21" t="inlineStr">
-        <is>
-          <t>Baron</t>
-        </is>
-      </c>
-      <c r="AE21" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="AJ21" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="AK21" t="inlineStr">
-        <is>
-          <t>Final title passed in as: Experiences of Hildebeorht Johnsen and Geography</t>
-        </is>
-      </c>
-      <c r="AL21" t="inlineStr">
-        <is>
-          <t>Geography</t>
-        </is>
-      </c>
-      <c r="AM21" t="n">
-        <v>0.37</v>
-      </c>
-      <c r="AN21" t="n">
-        <v>555</v>
-      </c>
-      <c r="AO21" t="n">
-        <v>10</v>
-      </c>
-      <c r="AP21" t="n">
-        <v>2700</v>
-      </c>
-      <c r="AQ21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU21" t="b">
-        <v>0</v>
-      </c>
-      <c r="AV21" t="inlineStr">
-        <is>
-          <t>Standard</t>
-        </is>
-      </c>
-      <c r="AW21" t="inlineStr">
-        <is>
-          <t>b056be1d-96bc-4a9b-8f1c-86f5a76ab0f6</t>
-        </is>
-      </c>
-      <c r="AX21" t="inlineStr">
         <is>
           <t>has_been_archived</t>
         </is>

</xml_diff>

<commit_message>
Still crushing bugs - needs save pandas table contents before archive to master
</commit_message>
<xml_diff>
--- a/books_spreadsheet_out.xlsx
+++ b/books_spreadsheet_out.xlsx
@@ -11,14 +11,14 @@
   <definedNames>
     <definedName name="GLS" localSheetId="0">'Book Hoard'!$A$1:$AV$1</definedName>
   </definedNames>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -40,6 +40,10 @@
     </font>
     <font>
       <b val="1"/>
+      <sz val="9"/>
+    </font>
+    <font>
+      <name val="Noto Sans Runic"/>
       <sz val="9"/>
     </font>
     <font>
@@ -67,7 +71,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -91,6 +95,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,10 +461,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AX11"/>
+  <dimension ref="A1:AX21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15.75"/>
@@ -498,8 +503,8 @@
     <col width="9.140625" customWidth="1" style="1" min="41" max="48"/>
     <col width="37.140625" customWidth="1" style="1" min="49" max="49"/>
     <col width="18.140625" customWidth="1" style="1" min="50" max="50"/>
-    <col width="9.140625" customWidth="1" style="1" min="51" max="68"/>
-    <col width="9.140625" customWidth="1" style="1" min="69" max="16384"/>
+    <col width="9.140625" customWidth="1" style="1" min="51" max="72"/>
+    <col width="9.140625" customWidth="1" style="1" min="73" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -757,97 +762,102 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Codex</t>
+          <t>Scroll</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Vellum</t>
+          <t>Parchment</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D2" t="n">
-        <v>1000</v>
+        <v>1334</v>
       </c>
       <c r="E2" t="n">
-        <v>63</v>
+        <v>93</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Regional</t>
+          <t>Dwarven</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Esoteric: Soothsaying</t>
+          <t>Profession (chamberlain)</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Performance (singing)</t>
+          <t>Profession (chamberlain)</t>
         </is>
       </c>
       <c r="J2" t="n">
         <v>1</v>
       </c>
       <c r="K2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="M2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N2" t="n">
         <v>1</v>
       </c>
       <c r="O2" t="n">
-        <v>5890</v>
+        <v>495</v>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>The Wickedness of Hróðulfr Johnsdotter, Considering Singing</t>
+          <t>Transactions Discoursing on Chamberlain's Craft from Æðelwulf Notleigh</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Lina Baghdadi</t>
+          <t>Viviane Fonder the Harried</t>
         </is>
       </c>
       <c r="S2" s="10" t="inlineStr">
         <is>
-          <t>Γραμμὴ πλειόνων εἰσὶν ἀμβλεῖα παρὰ λοιπαῖς εὐθύγραμμά ἐλάττονες</t>
+          <t>ᛞᛁᚲᛏᚢᛗ ᛞᛟᚾᛖᚲ ᚲᚢᚱᚨᛒᛁᛏᚢᚱ ᛞᛟᚨᛗ ᛚᛖᚲᛏᚢᛊ ᛞᚨᛈᛁᛒᚢᛊ ᛊᛟᛚᛚᛁᚲᛁᛏᚢᛞᛁᚾ ᛖᚢ ᚱᛁᛊᚢᛊ ᛈᚱᛁᛗᛁᛊ ᛈᛟᚱᛏᚨ ᛖᚱᚨᛏ</t>
         </is>
       </c>
       <c r="T2" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="U2" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="V2" t="n">
-        <v>45</v>
+        <v>905</v>
       </c>
       <c r="W2" t="n">
-        <v>2</v>
+        <v>755</v>
       </c>
       <c r="X2" t="n">
-        <v>1</v>
+        <v>754</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.5</v>
+        <v>0.01</v>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>the Harried</t>
+        </is>
       </c>
       <c r="AB2" t="inlineStr">
         <is>
-          <t>Lina Baghdadi</t>
+          <t>Viviane Fonder</t>
         </is>
       </c>
       <c r="AC2" t="inlineStr">
         <is>
-          <t>_names_arabic_surnames</t>
+          <t>_names_french_surnames</t>
         </is>
       </c>
       <c r="AE2" t="inlineStr">
@@ -860,31 +870,31 @@
       </c>
       <c r="AK2" t="inlineStr">
         <is>
-          <t>{the_1} {negative_1} of {person_1}, Considering {topic}</t>
+          <t>{communication} {conjunction_about} {topic} {conjunction_by} {person_1}</t>
         </is>
       </c>
       <c r="AL2" t="inlineStr">
         <is>
-          <t>Singing</t>
+          <t>Chamberlain's Craft</t>
         </is>
       </c>
       <c r="AM2" t="n">
-        <v>0.39</v>
+        <v>0.36</v>
       </c>
       <c r="AN2" t="n">
-        <v>390</v>
+        <v>481</v>
       </c>
       <c r="AO2" t="n">
         <v>1</v>
       </c>
       <c r="AP2" t="n">
-        <v>500</v>
+        <v>14</v>
       </c>
       <c r="AQ2" t="n">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="AR2" t="n">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="AS2" t="n">
         <v>0</v>
@@ -902,7 +912,7 @@
       </c>
       <c r="AW2" t="inlineStr">
         <is>
-          <t>efacfe2c-40cb-466d-a411-c46438869134</t>
+          <t>124ee267-b893-4e9e-b77b-ddce832eae1a</t>
         </is>
       </c>
       <c r="AX2" t="inlineStr">
@@ -919,31 +929,31 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Silver Foil</t>
+          <t>Parchment</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>195</v>
+        <v>1334</v>
       </c>
       <c r="E3" t="n">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>Classical</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Knowledge (architecture)</t>
+          <t>Caving</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Knowledge (architecture)</t>
+          <t>Caving</t>
         </is>
       </c>
       <c r="J3" t="n">
@@ -953,89 +963,89 @@
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>2</v>
+        <v>0.75</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>0.39</v>
+        <v>1</v>
       </c>
       <c r="O3" t="n">
-        <v>366</v>
+        <v>1828</v>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>The Peccability of Félicité Legot, Considering Architecture</t>
+          <t>The History of Mozar the Conqueror and Caving</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Ealhstan Miller</t>
-        </is>
-      </c>
-      <c r="S3" s="10" t="inlineStr">
-        <is>
-          <t>The Peccability of Félicité Legot, Considering Architecture</t>
+          <t>Leila Chausson</t>
+        </is>
+      </c>
+      <c r="S3" s="11" t="inlineStr">
+        <is>
+          <t>Fusce pabulationibus liceri munera existimabat reprehenderit spectat inter propterea</t>
         </is>
       </c>
       <c r="T3" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="U3" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="V3" t="n">
-        <v>43</v>
+        <v>386</v>
       </c>
       <c r="W3" t="n">
-        <v>152</v>
+        <v>1</v>
       </c>
       <c r="X3" t="n">
-        <v>151</v>
+        <v>0</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="AB3" t="inlineStr">
         <is>
-          <t>Ealhstan Miller</t>
+          <t>Leila Chausson</t>
         </is>
       </c>
       <c r="AC3" t="inlineStr">
         <is>
-          <t>_names_anglo_saxon_surnames</t>
+          <t>_names_french_surnames</t>
         </is>
       </c>
       <c r="AE3" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="AJ3" t="n">
-        <v>0.15</v>
+        <v>0.06</v>
       </c>
       <c r="AK3" t="inlineStr">
         <is>
-          <t>{the_1} {negative_1} of {person_1}, Considering {topic}</t>
+          <t>{biography_starter} of {person_famous} and {topic}</t>
         </is>
       </c>
       <c r="AL3" t="inlineStr">
         <is>
-          <t>Architecture</t>
+          <t>Caving</t>
         </is>
       </c>
       <c r="AM3" t="n">
-        <v>1.81</v>
+        <v>0.37</v>
       </c>
       <c r="AN3" t="n">
-        <v>905</v>
+        <v>494</v>
       </c>
       <c r="AO3" t="n">
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="AP3" t="n">
-        <v>32</v>
+        <v>1334</v>
       </c>
       <c r="AQ3" t="n">
         <v>0</v>
@@ -1059,7 +1069,7 @@
       </c>
       <c r="AW3" t="inlineStr">
         <is>
-          <t>aad276f6-22db-4551-b4e2-fa3498833bd6</t>
+          <t>64e05c50-e2bf-4bf8-9684-c0af68d68567</t>
         </is>
       </c>
       <c r="AX3" t="inlineStr">
@@ -1076,41 +1086,41 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Parchment</t>
+          <t>Gold Foil</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>1000</v>
+        <v>750</v>
       </c>
       <c r="E4" t="n">
-        <v>63</v>
+        <v>227</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Classical</t>
+          <t>Common</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Animal Training (dogs)</t>
+          <t>Knowledge (astrology)</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Animal Training (dogs)</t>
+          <t>Knowledge (astrology)</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M4" t="n">
         <v>0</v>
@@ -1119,80 +1129,80 @@
         <v>1</v>
       </c>
       <c r="O4" t="n">
-        <v>1370</v>
+        <v>23971</v>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Letters of Dagfinnr Jørgensen Concerning Canine Reproof</t>
+          <t>Epistles With Reference to Astrology of Prune Loyer</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Victoria Skeat</t>
-        </is>
-      </c>
-      <c r="S4" s="10" t="inlineStr">
-        <is>
-          <t>Renuntiatur labienus confirmare cognitis persuadent ut apr optimus</t>
+          <t>Frea Eriksdotter</t>
+        </is>
+      </c>
+      <c r="S4" s="11" t="inlineStr">
+        <is>
+          <t>Epistles With Reference to Astrology of Prune Loyer</t>
         </is>
       </c>
       <c r="T4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V4" t="n">
-        <v>494</v>
+        <v>38</v>
       </c>
       <c r="W4" t="n">
+        <v>8</v>
+      </c>
+      <c r="X4" t="n">
+        <v>7</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>Frea Eriksdotter</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_female</t>
+        </is>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ4" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AK4" t="inlineStr">
+        <is>
+          <t>{communication} {conjunction_about} {topic} {conjunction_by} {person_1}</t>
+        </is>
+      </c>
+      <c r="AL4" t="inlineStr">
+        <is>
+          <t>Astrology</t>
+        </is>
+      </c>
+      <c r="AM4" t="n">
+        <v>30.31</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>22733</v>
+      </c>
+      <c r="AO4" t="n">
         <v>5</v>
       </c>
-      <c r="X4" t="n">
-        <v>4</v>
-      </c>
-      <c r="Y4" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="AB4" t="inlineStr">
-        <is>
-          <t>Victoria Skeat</t>
-        </is>
-      </c>
-      <c r="AC4" t="inlineStr">
-        <is>
-          <t>_names_english_surnames</t>
-        </is>
-      </c>
-      <c r="AE4" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="AJ4" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="AK4" t="inlineStr">
-        <is>
-          <t>{communication} of {person_1} {conjunction_about} {topic}</t>
-        </is>
-      </c>
-      <c r="AL4" t="inlineStr">
-        <is>
-          <t>Canine Reproof</t>
-        </is>
-      </c>
-      <c r="AM4" t="n">
-        <v>0.37</v>
-      </c>
-      <c r="AN4" t="n">
-        <v>370</v>
-      </c>
-      <c r="AO4" t="n">
-        <v>2</v>
-      </c>
       <c r="AP4" t="n">
-        <v>1000</v>
+        <v>1238</v>
       </c>
       <c r="AQ4" t="n">
         <v>0</v>
@@ -1216,7 +1226,7 @@
       </c>
       <c r="AW4" t="inlineStr">
         <is>
-          <t>2c5d8ff8-9c61-4ed8-b52f-5cb0acf86286</t>
+          <t>97409c73-9b39-45c9-bb5a-dce853df5acd</t>
         </is>
       </c>
       <c r="AX4" t="inlineStr">
@@ -1233,41 +1243,41 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Parchment</t>
+          <t>Vellum</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" t="n">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="E5" t="n">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>Classical</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Fighting Style</t>
+          <t>Arcane Dabbling</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Fighting Style</t>
+          <t>Arcane Dabbling</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K5" t="n">
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M5" t="n">
         <v>0</v>
@@ -1276,49 +1286,54 @@
         <v>1</v>
       </c>
       <c r="O5" t="n">
-        <v>498</v>
+        <v>2890</v>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Transactions of Galla Betitia Respecting Fighting Style</t>
+          <t>Correspondence in Regard to Arcane Dabbling by Faustine Baffier</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Michèle Bourbeau</t>
-        </is>
-      </c>
-      <c r="S5" s="10" t="inlineStr">
-        <is>
-          <t>Transactions of Galla Betitia Respecting Fighting Style</t>
+          <t>Her Holiness Gunna Thomsdotter</t>
+        </is>
+      </c>
+      <c r="S5" s="11" t="inlineStr">
+        <is>
+          <t>Brevi volebant deorum testem tempore necessitatibus sociosqu altitudinem paulatim galliae muniendi</t>
         </is>
       </c>
       <c r="T5" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="U5" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="V5" t="n">
+        <v>496</v>
+      </c>
+      <c r="W5" t="n">
+        <v>45</v>
+      </c>
+      <c r="X5" t="n">
         <v>44</v>
       </c>
-      <c r="W5" t="n">
-        <v>4</v>
-      </c>
-      <c r="X5" t="n">
-        <v>3</v>
-      </c>
       <c r="Y5" t="n">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AB5" t="inlineStr">
         <is>
-          <t>Michèle Bourbeau</t>
+          <t>Gunna Thomsdotter</t>
         </is>
       </c>
       <c r="AC5" t="inlineStr">
         <is>
-          <t>_names_french_surnames</t>
+          <t>_names_norse_surnames_female</t>
+        </is>
+      </c>
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t>Her Holiness</t>
         </is>
       </c>
       <c r="AE5" t="inlineStr">
@@ -1331,25 +1346,25 @@
       </c>
       <c r="AK5" t="inlineStr">
         <is>
-          <t>{communication} of {person_1} {conjunction_about} {topic}</t>
+          <t>{communication} {conjunction_about} {topic} {conjunction_by} {person_1}</t>
         </is>
       </c>
       <c r="AL5" t="inlineStr">
         <is>
-          <t>Fighting Style</t>
+          <t>Arcane Dabbling</t>
         </is>
       </c>
       <c r="AM5" t="n">
-        <v>0.37</v>
+        <v>0.39</v>
       </c>
       <c r="AN5" t="n">
-        <v>185</v>
+        <v>390</v>
       </c>
       <c r="AO5" t="n">
-        <v>1.25</v>
+        <v>10</v>
       </c>
       <c r="AP5" t="n">
-        <v>313</v>
+        <v>2500</v>
       </c>
       <c r="AQ5" t="n">
         <v>0</v>
@@ -1373,7 +1388,7 @@
       </c>
       <c r="AW5" t="inlineStr">
         <is>
-          <t>a6cfd56d-91e9-439b-9142-87082a3cad57</t>
+          <t>12a2fca1-6877-478b-a6b1-102179ea1484</t>
         </is>
       </c>
       <c r="AX5" t="inlineStr">
@@ -1385,36 +1400,36 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Codex</t>
+          <t>Scroll</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Parchment</t>
+          <t>Fine Papyrus</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D6" t="n">
-        <v>500</v>
+        <v>1334</v>
       </c>
       <c r="E6" t="n">
-        <v>32</v>
+        <v>93</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>Dwarven</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Craft (basket-making)</t>
+          <t>Knowledge (political economy)</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Craft (basket-making)</t>
+          <t>Knowledge (political economy)</t>
         </is>
       </c>
       <c r="J6" t="n">
@@ -1424,7 +1439,7 @@
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>2</v>
+        <v>0.75</v>
       </c>
       <c r="M6" t="n">
         <v>0</v>
@@ -1433,54 +1448,54 @@
         <v>1</v>
       </c>
       <c r="O6" t="n">
-        <v>342</v>
+        <v>508</v>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>Critiquing The Crafte of Making Baskets: a Jolly Determination</t>
+          <t>A Treatise on Political Economy</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Antoinette Chaumette</t>
+          <t>Cynemær Currington</t>
         </is>
       </c>
       <c r="S6" s="10" t="inlineStr">
         <is>
-          <t>Critiquing The Crafte of Making Baskets: a Jolly Determination</t>
+          <t>ᛚᛁᚷᚢᛚᚨ ᛈᛟᚱᛏᚨ ᛁᚾᛏᛖᚱᛞᚢᛗ ᚲᛟᛗᛗᛟᛞᛟ ᛈᚱᛁᛗᛁᛊ ᚢᛖᛚ ᛗᚨᚲᛊᛁᛗᚢᛊ ᛖᚢᛁᛊᛗᛟᛞ ᚠᚢᛊᚲᛖ</t>
         </is>
       </c>
       <c r="T6" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="U6" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="V6" t="n">
-        <v>172</v>
+        <v>657</v>
       </c>
       <c r="W6" t="n">
-        <v>49</v>
+        <v>234</v>
       </c>
       <c r="X6" t="n">
-        <v>48</v>
+        <v>233</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.25</v>
+        <v>0.05</v>
       </c>
       <c r="AB6" t="inlineStr">
         <is>
-          <t>Antoinette Chaumette</t>
+          <t>Cynemær Currington</t>
         </is>
       </c>
       <c r="AC6" t="inlineStr">
         <is>
-          <t>_names_french_surnames</t>
+          <t>_names_anglo_saxon_surnames</t>
         </is>
       </c>
       <c r="AE6" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="AJ6" t="n">
@@ -1488,25 +1503,25 @@
       </c>
       <c r="AK6" t="inlineStr">
         <is>
-          <t>{verbing} {topic}: a {adjective_1} {noun_1}</t>
+          <t>{study_on} on {topic}</t>
         </is>
       </c>
       <c r="AL6" t="inlineStr">
         <is>
-          <t>The Crafte of Making Baskets</t>
+          <t>Political Economy</t>
         </is>
       </c>
       <c r="AM6" t="n">
-        <v>0.37</v>
+        <v>0.33</v>
       </c>
       <c r="AN6" t="n">
-        <v>185</v>
+        <v>441</v>
       </c>
       <c r="AO6" t="n">
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="AP6" t="n">
-        <v>157</v>
+        <v>67</v>
       </c>
       <c r="AQ6" t="n">
         <v>0</v>
@@ -1530,7 +1545,7 @@
       </c>
       <c r="AW6" t="inlineStr">
         <is>
-          <t>5ffae90a-f6d1-4689-ae4d-0c000fbb5ff6</t>
+          <t>78205b9a-86f5-4446-bd0d-d96c6e5f404f</t>
         </is>
       </c>
       <c r="AX6" t="inlineStr">
@@ -1542,36 +1557,36 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Codex</t>
+          <t>Scroll</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Vellum</t>
+          <t>Parchment</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D7" t="n">
-        <v>1334</v>
+        <v>1500</v>
       </c>
       <c r="E7" t="n">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Regional</t>
+          <t>Dwarven</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Knowledge (history)</t>
+          <t>Profession (chamberlain)</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Knowledge (history)</t>
+          <t>Profession (chamberlain)</t>
         </is>
       </c>
       <c r="J7" t="n">
@@ -1581,7 +1596,7 @@
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="M7" t="n">
         <v>0</v>
@@ -1590,54 +1605,49 @@
         <v>1</v>
       </c>
       <c r="O7" t="n">
-        <v>855</v>
+        <v>496</v>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Concert of Constantinople</t>
+          <t>Transactions Discoursing on Chamberlain's Craft from Æðelwulf Notleigh</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Madam Lise Hérault</t>
+          <t>Viviane Fonder the Harried</t>
         </is>
       </c>
       <c r="S7" s="10" t="inlineStr">
         <is>
-          <t>Πέρατα βάσεως κάθετον παραπληρώματα σχημάτων</t>
+          <t>ᛞᛁᚲᛏᚢᛗ ᛞᛟᚾᛖᚲ ᚲᚢᚱᚨᛒᛁᛏᚢᚱ ᛞᛟᚨᛗ ᛚᛖᚲᛏᚢᛊ ᛞᚨᛈᛁᛒᚢᛊ ᛊᛟᛚᛚᛁᚲᛁᛏᚢᛞᛁᚾ ᛖᚢ ᚱᛁᛊᚢᛊ ᛈᚱᛁᛗᛁᛊ ᛈᛟᚱᛏᚨ ᛖᚱᚨᛏ</t>
         </is>
       </c>
       <c r="T7" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="U7" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="V7" t="n">
-        <v>31</v>
+        <v>905</v>
       </c>
       <c r="W7" t="n">
-        <v>45</v>
+        <v>755</v>
       </c>
       <c r="X7" t="n">
-        <v>44</v>
+        <v>753</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.25</v>
+        <v>0.01</v>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>the Harried</t>
+        </is>
       </c>
       <c r="AB7" t="inlineStr">
         <is>
-          <t>Lise Hérault</t>
-        </is>
-      </c>
-      <c r="AC7" t="inlineStr">
-        <is>
-          <t>_names_french_surnames</t>
-        </is>
-      </c>
-      <c r="AD7" t="inlineStr">
-        <is>
-          <t>Madam</t>
+          <t>Viviane Fonder</t>
         </is>
       </c>
       <c r="AE7" t="inlineStr">
@@ -1650,25 +1660,25 @@
       </c>
       <c r="AK7" t="inlineStr">
         <is>
-          <t>{history_of} {place_city}</t>
+          <t>Final title passed in as: Transactions Discoursing on Chamberlain's Craft from Æðelwulf Notleigh</t>
         </is>
       </c>
       <c r="AL7" t="inlineStr">
         <is>
-          <t>History</t>
+          <t>Chamberlain's Craft</t>
         </is>
       </c>
       <c r="AM7" t="n">
-        <v>0.39</v>
+        <v>0.36</v>
       </c>
       <c r="AN7" t="n">
-        <v>521</v>
+        <v>540</v>
       </c>
       <c r="AO7" t="n">
         <v>1</v>
       </c>
       <c r="AP7" t="n">
-        <v>334</v>
+        <v>15</v>
       </c>
       <c r="AQ7" t="n">
         <v>0</v>
@@ -1692,7 +1702,7 @@
       </c>
       <c r="AW7" t="inlineStr">
         <is>
-          <t>65ae5975-44b9-486a-87bf-e50f3055c3a1</t>
+          <t>1efbea20-a31c-4c08-a32e-a76d89b9a4c8</t>
         </is>
       </c>
       <c r="AX7" t="inlineStr">
@@ -1709,41 +1719,41 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Fine Papyrus</t>
+          <t>Parchment</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D8" t="n">
-        <v>750</v>
+        <v>1500</v>
       </c>
       <c r="E8" t="n">
-        <v>51</v>
+        <v>102</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>Dwarven</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Mountaineering</t>
+          <t>Profession (chamberlain)</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Mountaineering</t>
+          <t>Profession (chamberlain)</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K8" t="n">
         <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M8" t="n">
         <v>0</v>
@@ -1752,49 +1762,49 @@
         <v>1</v>
       </c>
       <c r="O8" t="n">
-        <v>623</v>
+        <v>496</v>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>Exchanges With Regard to Mountaineering of Corneille Duvivier</t>
+          <t>Transactions Discoursing on Chamberlain's Craft from Æðelwulf Notleigh</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Svanhild Olofsdotter</t>
+          <t>Viviane Fonder the Harried</t>
         </is>
       </c>
       <c r="S8" s="10" t="inlineStr">
         <is>
-          <t>Exchanges With Regard to Mountaineering of Corneille Duvivier</t>
+          <t>ᛞᛁᚲᛏᚢᛗ ᛞᛟᚾᛖᚲ ᚲᚢᚱᚨᛒᛁᛏᚢᚱ ᛞᛟᚨᛗ ᛚᛖᚲᛏᚢᛊ ᛞᚨᛈᛁᛒᚢᛊ ᛊᛟᛚᛚᛁᚲᛁᛏᚢᛞᛁᚾ ᛖᚢ ᚱᛁᛊᚢᛊ ᛈᚱᛁᛗᛁᛊ ᛈᛟᚱᛏᚨ ᛖᚱᚨᛏ</t>
         </is>
       </c>
       <c r="T8" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="U8" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="V8" t="n">
-        <v>71</v>
+        <v>905</v>
       </c>
       <c r="W8" t="n">
-        <v>55</v>
+        <v>755</v>
       </c>
       <c r="X8" t="n">
-        <v>54</v>
+        <v>752</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.1</v>
+        <v>0.01</v>
+      </c>
+      <c r="AA8" t="inlineStr">
+        <is>
+          <t>the Harried</t>
+        </is>
       </c>
       <c r="AB8" t="inlineStr">
         <is>
-          <t>Svanhild Olofsdotter</t>
-        </is>
-      </c>
-      <c r="AC8" t="inlineStr">
-        <is>
-          <t>_names_norse_surnames_female</t>
+          <t>Viviane Fonder</t>
         </is>
       </c>
       <c r="AE8" t="inlineStr">
@@ -1807,25 +1817,25 @@
       </c>
       <c r="AK8" t="inlineStr">
         <is>
-          <t>{communication} {conjunction_about} {topic} {conjunction_by} {person_1}</t>
+          <t>Final title passed in as: Transactions Discoursing on Chamberlain's Craft from Æðelwulf Notleigh</t>
         </is>
       </c>
       <c r="AL8" t="inlineStr">
         <is>
-          <t>Mountaineering</t>
+          <t>Chamberlain's Craft</t>
         </is>
       </c>
       <c r="AM8" t="n">
-        <v>0.33</v>
+        <v>0.36</v>
       </c>
       <c r="AN8" t="n">
-        <v>248</v>
+        <v>540</v>
       </c>
       <c r="AO8" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AP8" t="n">
-        <v>375</v>
+        <v>15</v>
       </c>
       <c r="AQ8" t="n">
         <v>0</v>
@@ -1849,7 +1859,7 @@
       </c>
       <c r="AW8" t="inlineStr">
         <is>
-          <t>1b6692eb-3367-42b5-8b5d-bbca3dcb43b5</t>
+          <t>01b07f48-433d-4c9b-a961-c64d0f755552</t>
         </is>
       </c>
       <c r="AX8" t="inlineStr">
@@ -1866,31 +1876,31 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Parchment</t>
+          <t>Gold Foil</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>1000</v>
+        <v>750</v>
       </c>
       <c r="E9" t="n">
-        <v>63</v>
+        <v>227</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Classical</t>
+          <t>Common</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Healing</t>
+          <t>Knowledge (astrology)</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Healing</t>
+          <t>Knowledge (astrology)</t>
         </is>
       </c>
       <c r="J9" t="n">
@@ -1900,7 +1910,7 @@
         <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M9" t="n">
         <v>0</v>
@@ -1909,80 +1919,75 @@
         <v>1</v>
       </c>
       <c r="O9" t="n">
-        <v>570</v>
+        <v>24219</v>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>A Multitude of Iniquity of Fenris Olsson, on the Subject of Healing</t>
+          <t>Epistles With Reference to Astrology of Prune Loyer</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Njáll Andersson</t>
-        </is>
-      </c>
-      <c r="S9" s="10" t="inlineStr">
-        <is>
-          <t>Ipsam superatos alariis imperium acies interesset metiri conlaturus incolumem aliquo finem alieno morati missurum egestas</t>
+          <t>Frea Eriksdotter</t>
+        </is>
+      </c>
+      <c r="S9" s="11" t="inlineStr">
+        <is>
+          <t>Epistles With Reference to Astrology of Prune Loyer</t>
         </is>
       </c>
       <c r="T9" t="n">
+        <v>5</v>
+      </c>
+      <c r="U9" t="n">
+        <v>5</v>
+      </c>
+      <c r="V9" t="n">
+        <v>38</v>
+      </c>
+      <c r="W9" t="n">
+        <v>8</v>
+      </c>
+      <c r="X9" t="n">
         <v>6</v>
       </c>
-      <c r="U9" t="n">
-        <v>6</v>
-      </c>
-      <c r="V9" t="n">
-        <v>44</v>
-      </c>
-      <c r="W9" t="n">
-        <v>111</v>
-      </c>
-      <c r="X9" t="n">
-        <v>110</v>
-      </c>
       <c r="Y9" t="n">
-        <v>0.05</v>
+        <v>0.33</v>
       </c>
       <c r="AB9" t="inlineStr">
         <is>
-          <t>Njáll Andersson</t>
-        </is>
-      </c>
-      <c r="AC9" t="inlineStr">
-        <is>
-          <t>_names_norse_surnames_male</t>
+          <t>Frea Eriksdotter</t>
         </is>
       </c>
       <c r="AE9" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="AJ9" t="n">
-        <v>0.06</v>
+        <v>0.3</v>
       </c>
       <c r="AK9" t="inlineStr">
         <is>
-          <t>{the_1} {negative_1} of {person_1}, on the Subject of {topic}</t>
+          <t>Final title passed in as: Epistles With Reference to Astrology of Prune Loyer</t>
         </is>
       </c>
       <c r="AL9" t="inlineStr">
         <is>
-          <t>Healing</t>
+          <t>Astrology</t>
         </is>
       </c>
       <c r="AM9" t="n">
-        <v>0.37</v>
+        <v>30.31</v>
       </c>
       <c r="AN9" t="n">
-        <v>370</v>
+        <v>22733</v>
       </c>
       <c r="AO9" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AP9" t="n">
-        <v>200</v>
+        <v>1486</v>
       </c>
       <c r="AQ9" t="n">
         <v>0</v>
@@ -2006,7 +2011,7 @@
       </c>
       <c r="AW9" t="inlineStr">
         <is>
-          <t>1063b58d-b025-406f-b562-9d8d7bcbe8b1</t>
+          <t>4cff1e5c-a153-44f6-9ac4-f1b089b150bb</t>
         </is>
       </c>
       <c r="AX9" t="inlineStr">
@@ -2023,41 +2028,41 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Parchment</t>
+          <t>Gold Foil</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>1000</v>
+        <v>750</v>
       </c>
       <c r="E10" t="n">
-        <v>63</v>
+        <v>227</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Regional</t>
+          <t>Common</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Righteous Turning</t>
+          <t>Knowledge (astrology)</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Righteous Turning</t>
+          <t>Knowledge (astrology)</t>
         </is>
       </c>
       <c r="J10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K10" t="n">
         <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M10" t="n">
         <v>0</v>
@@ -2066,80 +2071,75 @@
         <v>1</v>
       </c>
       <c r="O10" t="n">
-        <v>2370</v>
+        <v>24219</v>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>The Disguised Quest of Want: Righteous Turning</t>
+          <t>Epistles With Reference to Astrology of Prune Loyer</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Sergius Campatia</t>
-        </is>
-      </c>
-      <c r="S10" s="10" t="inlineStr">
-        <is>
-          <t>Γραμμαὶ περιέχουσαι ἀπεναντίον ἐντὸς κάθετος</t>
+          <t>Frea Eriksdotter</t>
+        </is>
+      </c>
+      <c r="S10" s="11" t="inlineStr">
+        <is>
+          <t>Epistles With Reference to Astrology of Prune Loyer</t>
         </is>
       </c>
       <c r="T10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V10" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="W10" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="X10" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Y10" t="n">
-        <v>1</v>
+        <v>0.33</v>
       </c>
       <c r="AB10" t="inlineStr">
         <is>
-          <t>Sergius Campatia</t>
-        </is>
-      </c>
-      <c r="AC10" t="inlineStr">
-        <is>
-          <t>_names_roman_surnames</t>
+          <t>Frea Eriksdotter</t>
         </is>
       </c>
       <c r="AE10" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="AJ10" t="n">
-        <v>0.06</v>
+        <v>0.3</v>
       </c>
       <c r="AK10" t="inlineStr">
         <is>
-          <t>The {adjective_1} {noun_1} of {noun_2}: {topic}</t>
+          <t>Final title passed in as: Epistles With Reference to Astrology of Prune Loyer</t>
         </is>
       </c>
       <c r="AL10" t="inlineStr">
         <is>
-          <t>Righteous Turning</t>
+          <t>Astrology</t>
         </is>
       </c>
       <c r="AM10" t="n">
-        <v>0.37</v>
+        <v>30.31</v>
       </c>
       <c r="AN10" t="n">
-        <v>370</v>
+        <v>22733</v>
       </c>
       <c r="AO10" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AP10" t="n">
-        <v>2000</v>
+        <v>1486</v>
       </c>
       <c r="AQ10" t="n">
         <v>0</v>
@@ -2163,7 +2163,7 @@
       </c>
       <c r="AW10" t="inlineStr">
         <is>
-          <t>76fc3ae8-9e4d-441c-938c-e93578e9c972</t>
+          <t>49108554-3651-4eae-a016-20d2e588d7ad</t>
         </is>
       </c>
       <c r="AX10" t="inlineStr">
@@ -2180,41 +2180,41 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Parchment</t>
+          <t>Gold Foil</t>
         </is>
       </c>
       <c r="C11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" t="n">
+        <v>750</v>
+      </c>
+      <c r="E11" t="n">
+        <v>227</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Knowledge (astrology)</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Knowledge (astrology)</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
         <v>3</v>
       </c>
-      <c r="D11" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E11" t="n">
-        <v>125</v>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Common</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>Caving</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>Caving</t>
-        </is>
-      </c>
-      <c r="J11" t="n">
-        <v>2</v>
-      </c>
       <c r="K11" t="n">
         <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M11" t="n">
         <v>0</v>
@@ -2223,49 +2223,54 @@
         <v>1</v>
       </c>
       <c r="O11" t="n">
-        <v>2060</v>
+        <v>24219</v>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>The Festive Sensing of Unease: Caving</t>
+          <t>Epistles With Reference to Astrology of Prune Loyer</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>Priscilla Atinia</t>
-        </is>
-      </c>
-      <c r="S11" s="10" t="inlineStr">
-        <is>
-          <t>The Festive Sensing of Unease: Caving</t>
+          <t>Frea Eriksdotter</t>
+        </is>
+      </c>
+      <c r="S11" s="11" t="inlineStr">
+        <is>
+          <t>Epistles With Reference to Astrology of Prune Loyer</t>
         </is>
       </c>
       <c r="T11" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="U11" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="V11" t="n">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="W11" t="n">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="X11" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="Y11" t="n">
         <v>0.33</v>
       </c>
+      <c r="AA11" t="inlineStr">
+        <is>
+          <t>the Worthy</t>
+        </is>
+      </c>
       <c r="AB11" t="inlineStr">
         <is>
-          <t>Priscilla Atinia</t>
-        </is>
-      </c>
-      <c r="AC11" t="inlineStr">
-        <is>
-          <t>_names_roman_surnames</t>
+          <t>Frea Eriksdotter</t>
+        </is>
+      </c>
+      <c r="AD11" t="inlineStr">
+        <is>
+          <t>Her Grace</t>
         </is>
       </c>
       <c r="AE11" t="inlineStr">
@@ -2274,56 +2279,1631 @@
         </is>
       </c>
       <c r="AJ11" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AK11" t="inlineStr">
+        <is>
+          <t>Final title passed in as: Epistles With Reference to Astrology of Prune Loyer</t>
+        </is>
+      </c>
+      <c r="AL11" t="inlineStr">
+        <is>
+          <t>Astrology</t>
+        </is>
+      </c>
+      <c r="AM11" t="n">
+        <v>30.31</v>
+      </c>
+      <c r="AN11" t="n">
+        <v>22733</v>
+      </c>
+      <c r="AO11" t="n">
+        <v>5</v>
+      </c>
+      <c r="AP11" t="n">
+        <v>1486</v>
+      </c>
+      <c r="AQ11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU11" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV11" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW11" t="inlineStr">
+        <is>
+          <t>ffca2522-1caf-46ea-a566-c041452148bd</t>
+        </is>
+      </c>
+      <c r="AX11" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Scroll</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>6</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1500</v>
+      </c>
+      <c r="E12" t="n">
+        <v>102</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Dwarven</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Profession (chamberlain)</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Profession (chamberlain)</t>
+        </is>
+      </c>
+      <c r="J12" t="n">
+        <v>1</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>1</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>1</v>
+      </c>
+      <c r="O12" t="n">
+        <v>496</v>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>Transactions Discoursing on Chamberlain's Craft from Æðelwulf Notleigh</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>Viviane Fonder the Harried</t>
+        </is>
+      </c>
+      <c r="S12" s="10" t="inlineStr">
+        <is>
+          <t>ᛞᛁᚲᛏᚢᛗ ᛞᛟᚾᛖᚲ ᚲᚢᚱᚨᛒᛁᛏᚢᚱ ᛞᛟᚨᛗ ᛚᛖᚲᛏᚢᛊ ᛞᚨᛈᛁᛒᚢᛊ ᛊᛟᛚᛚᛁᚲᛁᛏᚢᛞᛁᚾ ᛖᚢ ᚱᛁᛊᚢᛊ ᛈᚱᛁᛗᛁᛊ ᛈᛟᚱᛏᚨ ᛖᚱᚨᛏ</t>
+        </is>
+      </c>
+      <c r="T12" t="n">
+        <v>9</v>
+      </c>
+      <c r="U12" t="n">
+        <v>9</v>
+      </c>
+      <c r="V12" t="n">
+        <v>905</v>
+      </c>
+      <c r="W12" t="n">
+        <v>755</v>
+      </c>
+      <c r="X12" t="n">
+        <v>753</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AA12" t="inlineStr">
+        <is>
+          <t>the Harried</t>
+        </is>
+      </c>
+      <c r="AB12" t="inlineStr">
+        <is>
+          <t>Viviane Fonder</t>
+        </is>
+      </c>
+      <c r="AE12" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ12" t="n">
         <v>0.06</v>
       </c>
-      <c r="AK11" t="inlineStr">
-        <is>
-          <t>The {adjective_1} {noun_1} of {noun_2}: {topic}</t>
-        </is>
-      </c>
-      <c r="AL11" t="inlineStr">
-        <is>
-          <t>Caving</t>
-        </is>
-      </c>
-      <c r="AM11" t="n">
-        <v>0.37</v>
-      </c>
-      <c r="AN11" t="n">
-        <v>740</v>
-      </c>
-      <c r="AO11" t="n">
-        <v>2</v>
-      </c>
-      <c r="AP11" t="n">
-        <v>1320</v>
-      </c>
-      <c r="AQ11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU11" t="b">
-        <v>0</v>
-      </c>
-      <c r="AV11" t="inlineStr">
+      <c r="AK12" t="inlineStr">
+        <is>
+          <t>Final title passed in as: Transactions Discoursing on Chamberlain's Craft from Æðelwulf Notleigh</t>
+        </is>
+      </c>
+      <c r="AL12" t="inlineStr">
+        <is>
+          <t>Chamberlain's Craft</t>
+        </is>
+      </c>
+      <c r="AM12" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="AN12" t="n">
+        <v>540</v>
+      </c>
+      <c r="AO12" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP12" t="n">
+        <v>15</v>
+      </c>
+      <c r="AQ12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU12" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV12" t="inlineStr">
         <is>
           <t>Standard</t>
         </is>
       </c>
-      <c r="AW11" t="inlineStr">
-        <is>
-          <t>6ceeec79-a31f-4daf-b22c-e1e91fbe0797</t>
-        </is>
-      </c>
-      <c r="AX11" t="inlineStr">
+      <c r="AW12" t="inlineStr">
+        <is>
+          <t>2dad2f32-d1b5-47fc-b5d4-a2754788058c</t>
+        </is>
+      </c>
+      <c r="AX12" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Gold Foil</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" t="n">
+        <v>750</v>
+      </c>
+      <c r="E13" t="n">
+        <v>227</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Knowledge (astrology)</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Knowledge (astrology)</t>
+        </is>
+      </c>
+      <c r="J13" t="n">
+        <v>3</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>4</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>1</v>
+      </c>
+      <c r="O13" t="n">
+        <v>24219</v>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>Epistles With Reference to Astrology of Prune Loyer</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>Frea Eriksdotter</t>
+        </is>
+      </c>
+      <c r="S13" s="11" t="inlineStr">
+        <is>
+          <t>Epistles With Reference to Astrology of Prune Loyer</t>
+        </is>
+      </c>
+      <c r="T13" t="n">
+        <v>5</v>
+      </c>
+      <c r="U13" t="n">
+        <v>5</v>
+      </c>
+      <c r="V13" t="n">
+        <v>38</v>
+      </c>
+      <c r="W13" t="n">
+        <v>8</v>
+      </c>
+      <c r="X13" t="n">
+        <v>6</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AB13" t="inlineStr">
+        <is>
+          <t>Frea Eriksdotter</t>
+        </is>
+      </c>
+      <c r="AE13" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ13" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AK13" t="inlineStr">
+        <is>
+          <t>Final title passed in as: Epistles With Reference to Astrology of Prune Loyer</t>
+        </is>
+      </c>
+      <c r="AL13" t="inlineStr">
+        <is>
+          <t>Astrology</t>
+        </is>
+      </c>
+      <c r="AM13" t="n">
+        <v>30.31</v>
+      </c>
+      <c r="AN13" t="n">
+        <v>22733</v>
+      </c>
+      <c r="AO13" t="n">
+        <v>5</v>
+      </c>
+      <c r="AP13" t="n">
+        <v>1486</v>
+      </c>
+      <c r="AQ13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU13" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV13" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW13" t="inlineStr">
+        <is>
+          <t>a9cc58e4-653c-4bc9-aef0-3d3b4dad14bf</t>
+        </is>
+      </c>
+      <c r="AX13" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Gold Foil</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" t="n">
+        <v>750</v>
+      </c>
+      <c r="E14" t="n">
+        <v>227</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Knowledge (astrology)</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Knowledge (astrology)</t>
+        </is>
+      </c>
+      <c r="J14" t="n">
+        <v>3</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>4</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>1</v>
+      </c>
+      <c r="O14" t="n">
+        <v>24219</v>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>Epistles With Reference to Astrology of Prune Loyer</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>Frea Eriksdotter</t>
+        </is>
+      </c>
+      <c r="S14" s="11" t="inlineStr">
+        <is>
+          <t>Epistles With Reference to Astrology of Prune Loyer</t>
+        </is>
+      </c>
+      <c r="T14" t="n">
+        <v>5</v>
+      </c>
+      <c r="U14" t="n">
+        <v>5</v>
+      </c>
+      <c r="V14" t="n">
+        <v>38</v>
+      </c>
+      <c r="W14" t="n">
+        <v>8</v>
+      </c>
+      <c r="X14" t="n">
+        <v>5</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AB14" t="inlineStr">
+        <is>
+          <t>Frea Eriksdotter</t>
+        </is>
+      </c>
+      <c r="AD14" t="inlineStr">
+        <is>
+          <t>Saint</t>
+        </is>
+      </c>
+      <c r="AE14" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ14" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AK14" t="inlineStr">
+        <is>
+          <t>Final title passed in as: Epistles With Reference to Astrology of Prune Loyer</t>
+        </is>
+      </c>
+      <c r="AL14" t="inlineStr">
+        <is>
+          <t>Astrology</t>
+        </is>
+      </c>
+      <c r="AM14" t="n">
+        <v>30.31</v>
+      </c>
+      <c r="AN14" t="n">
+        <v>22733</v>
+      </c>
+      <c r="AO14" t="n">
+        <v>5</v>
+      </c>
+      <c r="AP14" t="n">
+        <v>1486</v>
+      </c>
+      <c r="AQ14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU14" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV14" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW14" t="inlineStr">
+        <is>
+          <t>a2d6e388-a219-4f25-9f84-44895e3b0a8c</t>
+        </is>
+      </c>
+      <c r="AX14" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Scroll</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>6</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1500</v>
+      </c>
+      <c r="E15" t="n">
+        <v>102</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Dwarven</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Profession (chamberlain)</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Profession (chamberlain)</t>
+        </is>
+      </c>
+      <c r="J15" t="n">
+        <v>1</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>1</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
+        <v>1</v>
+      </c>
+      <c r="O15" t="n">
+        <v>496</v>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>Transactions Discoursing on Chamberlain's Craft from Æðelwulf Notleigh</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>Viviane Fonder the Harried</t>
+        </is>
+      </c>
+      <c r="S15" s="10" t="inlineStr">
+        <is>
+          <t>ᛞᛁᚲᛏᚢᛗ ᛞᛟᚾᛖᚲ ᚲᚢᚱᚨᛒᛁᛏᚢᚱ ᛞᛟᚨᛗ ᛚᛖᚲᛏᚢᛊ ᛞᚨᛈᛁᛒᚢᛊ ᛊᛟᛚᛚᛁᚲᛁᛏᚢᛞᛁᚾ ᛖᚢ ᚱᛁᛊᚢᛊ ᛈᚱᛁᛗᛁᛊ ᛈᛟᚱᛏᚨ ᛖᚱᚨᛏ</t>
+        </is>
+      </c>
+      <c r="T15" t="n">
+        <v>9</v>
+      </c>
+      <c r="U15" t="n">
+        <v>9</v>
+      </c>
+      <c r="V15" t="n">
+        <v>905</v>
+      </c>
+      <c r="W15" t="n">
+        <v>755</v>
+      </c>
+      <c r="X15" t="n">
+        <v>752</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AA15" t="inlineStr">
+        <is>
+          <t>the Harried</t>
+        </is>
+      </c>
+      <c r="AB15" t="inlineStr">
+        <is>
+          <t>Viviane Fonder</t>
+        </is>
+      </c>
+      <c r="AD15" t="inlineStr">
+        <is>
+          <t>The Divine</t>
+        </is>
+      </c>
+      <c r="AE15" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ15" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK15" t="inlineStr">
+        <is>
+          <t>Final title passed in as: Transactions Discoursing on Chamberlain's Craft from Æðelwulf Notleigh</t>
+        </is>
+      </c>
+      <c r="AL15" t="inlineStr">
+        <is>
+          <t>Chamberlain's Craft</t>
+        </is>
+      </c>
+      <c r="AM15" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="AN15" t="n">
+        <v>540</v>
+      </c>
+      <c r="AO15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP15" t="n">
+        <v>15</v>
+      </c>
+      <c r="AQ15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU15" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV15" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW15" t="inlineStr">
+        <is>
+          <t>bed79272-808e-481e-9198-dccbc1fe1cc4</t>
+        </is>
+      </c>
+      <c r="AX15" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Scroll</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>6</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1500</v>
+      </c>
+      <c r="E16" t="n">
+        <v>102</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Dwarven</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Profession (chamberlain)</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Profession (chamberlain)</t>
+        </is>
+      </c>
+      <c r="J16" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>1</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>1</v>
+      </c>
+      <c r="O16" t="n">
+        <v>496</v>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>Transactions Discoursing on Chamberlain's Craft from Æðelwulf Notleigh</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>Viviane Fonder the Harried</t>
+        </is>
+      </c>
+      <c r="S16" s="10" t="inlineStr">
+        <is>
+          <t>ᛞᛁᚲᛏᚢᛗ ᛞᛟᚾᛖᚲ ᚲᚢᚱᚨᛒᛁᛏᚢᚱ ᛞᛟᚨᛗ ᛚᛖᚲᛏᚢᛊ ᛞᚨᛈᛁᛒᚢᛊ ᛊᛟᛚᛚᛁᚲᛁᛏᚢᛞᛁᚾ ᛖᚢ ᚱᛁᛊᚢᛊ ᛈᚱᛁᛗᛁᛊ ᛈᛟᚱᛏᚨ ᛖᚱᚨᛏ</t>
+        </is>
+      </c>
+      <c r="T16" t="n">
+        <v>9</v>
+      </c>
+      <c r="U16" t="n">
+        <v>9</v>
+      </c>
+      <c r="V16" t="n">
+        <v>905</v>
+      </c>
+      <c r="W16" t="n">
+        <v>755</v>
+      </c>
+      <c r="X16" t="n">
+        <v>751</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AA16" t="inlineStr">
+        <is>
+          <t>the Harried</t>
+        </is>
+      </c>
+      <c r="AB16" t="inlineStr">
+        <is>
+          <t>Viviane Fonder</t>
+        </is>
+      </c>
+      <c r="AE16" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ16" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK16" t="inlineStr">
+        <is>
+          <t>Final title passed in as: Transactions Discoursing on Chamberlain's Craft from Æðelwulf Notleigh</t>
+        </is>
+      </c>
+      <c r="AL16" t="inlineStr">
+        <is>
+          <t>Chamberlain's Craft</t>
+        </is>
+      </c>
+      <c r="AM16" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="AN16" t="n">
+        <v>540</v>
+      </c>
+      <c r="AO16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP16" t="n">
+        <v>15</v>
+      </c>
+      <c r="AQ16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV16" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW16" t="inlineStr">
+        <is>
+          <t>5af6d365-a31c-4000-ba7d-4e1547ccf505</t>
+        </is>
+      </c>
+      <c r="AX16" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Scroll</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Fine Papyrus</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>6</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1500</v>
+      </c>
+      <c r="E17" t="n">
+        <v>102</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Dwarven</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Knowledge (political economy)</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Knowledge (political economy)</t>
+        </is>
+      </c>
+      <c r="J17" t="n">
+        <v>1</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" t="n">
+        <v>1</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O17" t="n">
+        <v>513</v>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>A Treatise on Political Economy</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>Cynemær Currington</t>
+        </is>
+      </c>
+      <c r="S17" s="10" t="inlineStr">
+        <is>
+          <t>ᛚᛁᚷᚢᛚᚨ ᛈᛟᚱᛏᚨ ᛁᚾᛏᛖᚱᛞᚢᛗ ᚲᛟᛗᛗᛟᛞᛟ ᛈᚱᛁᛗᛁᛊ ᚢᛖᛚ ᛗᚨᚲᛊᛁᛗᚢᛊ ᛖᚢᛁᛊᛗᛟᛞ ᚠᚢᛊᚲᛖ</t>
+        </is>
+      </c>
+      <c r="T17" t="n">
+        <v>9</v>
+      </c>
+      <c r="U17" t="n">
+        <v>9</v>
+      </c>
+      <c r="V17" t="n">
+        <v>657</v>
+      </c>
+      <c r="W17" t="n">
+        <v>234</v>
+      </c>
+      <c r="X17" t="n">
+        <v>232</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="AA17" t="inlineStr">
+        <is>
+          <t>the Wide-eyed</t>
+        </is>
+      </c>
+      <c r="AB17" t="inlineStr">
+        <is>
+          <t>Cynemær Currington</t>
+        </is>
+      </c>
+      <c r="AD17" t="inlineStr">
+        <is>
+          <t>The Gracious</t>
+        </is>
+      </c>
+      <c r="AE17" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ17" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK17" t="inlineStr">
+        <is>
+          <t>Final title passed in as: A Treatise on Political Economy</t>
+        </is>
+      </c>
+      <c r="AL17" t="inlineStr">
+        <is>
+          <t>Political Economy</t>
+        </is>
+      </c>
+      <c r="AM17" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AN17" t="n">
+        <v>495</v>
+      </c>
+      <c r="AO17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP17" t="n">
+        <v>72</v>
+      </c>
+      <c r="AQ17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU17" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV17" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW17" t="inlineStr">
+        <is>
+          <t>6145b0f7-eb48-4719-aeff-c18c77feb705</t>
+        </is>
+      </c>
+      <c r="AX17" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Scroll</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Fine Papyrus</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>6</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1500</v>
+      </c>
+      <c r="E18" t="n">
+        <v>102</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Dwarven</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Knowledge (political economy)</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Knowledge (political economy)</t>
+        </is>
+      </c>
+      <c r="J18" t="n">
+        <v>1</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" t="n">
+        <v>1</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" t="n">
+        <v>1</v>
+      </c>
+      <c r="O18" t="n">
+        <v>513</v>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>A Treatise on Political Economy</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>Cynemær Currington</t>
+        </is>
+      </c>
+      <c r="S18" s="10" t="inlineStr">
+        <is>
+          <t>ᛚᛁᚷᚢᛚᚨ ᛈᛟᚱᛏᚨ ᛁᚾᛏᛖᚱᛞᚢᛗ ᚲᛟᛗᛗᛟᛞᛟ ᛈᚱᛁᛗᛁᛊ ᚢᛖᛚ ᛗᚨᚲᛊᛁᛗᚢᛊ ᛖᚢᛁᛊᛗᛟᛞ ᚠᚢᛊᚲᛖ</t>
+        </is>
+      </c>
+      <c r="T18" t="n">
+        <v>9</v>
+      </c>
+      <c r="U18" t="n">
+        <v>9</v>
+      </c>
+      <c r="V18" t="n">
+        <v>657</v>
+      </c>
+      <c r="W18" t="n">
+        <v>234</v>
+      </c>
+      <c r="X18" t="n">
+        <v>231</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="AB18" t="inlineStr">
+        <is>
+          <t>Cynemær Currington</t>
+        </is>
+      </c>
+      <c r="AE18" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ18" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK18" t="inlineStr">
+        <is>
+          <t>Final title passed in as: A Treatise on Political Economy</t>
+        </is>
+      </c>
+      <c r="AL18" t="inlineStr">
+        <is>
+          <t>Political Economy</t>
+        </is>
+      </c>
+      <c r="AM18" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AN18" t="n">
+        <v>495</v>
+      </c>
+      <c r="AO18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP18" t="n">
+        <v>72</v>
+      </c>
+      <c r="AQ18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV18" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW18" t="inlineStr">
+        <is>
+          <t>5bc05a32-b71a-4e28-91fc-d78d43a5d7bc</t>
+        </is>
+      </c>
+      <c r="AX18" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Scroll</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Fine Papyrus</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>6</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1500</v>
+      </c>
+      <c r="E19" t="n">
+        <v>102</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Dwarven</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Knowledge (political economy)</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Knowledge (political economy)</t>
+        </is>
+      </c>
+      <c r="J19" t="n">
+        <v>1</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" t="n">
+        <v>1</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0</v>
+      </c>
+      <c r="N19" t="n">
+        <v>1</v>
+      </c>
+      <c r="O19" t="n">
+        <v>513</v>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>A Treatise on Political Economy</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>Cynemær Currington</t>
+        </is>
+      </c>
+      <c r="S19" s="10" t="inlineStr">
+        <is>
+          <t>ᛚᛁᚷᚢᛚᚨ ᛈᛟᚱᛏᚨ ᛁᚾᛏᛖᚱᛞᚢᛗ ᚲᛟᛗᛗᛟᛞᛟ ᛈᚱᛁᛗᛁᛊ ᚢᛖᛚ ᛗᚨᚲᛊᛁᛗᚢᛊ ᛖᚢᛁᛊᛗᛟᛞ ᚠᚢᛊᚲᛖ</t>
+        </is>
+      </c>
+      <c r="T19" t="n">
+        <v>9</v>
+      </c>
+      <c r="U19" t="n">
+        <v>9</v>
+      </c>
+      <c r="V19" t="n">
+        <v>657</v>
+      </c>
+      <c r="W19" t="n">
+        <v>234</v>
+      </c>
+      <c r="X19" t="n">
+        <v>230</v>
+      </c>
+      <c r="Y19" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="AB19" t="inlineStr">
+        <is>
+          <t>Cynemær Currington</t>
+        </is>
+      </c>
+      <c r="AD19" t="inlineStr">
+        <is>
+          <t>His Honor</t>
+        </is>
+      </c>
+      <c r="AE19" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ19" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK19" t="inlineStr">
+        <is>
+          <t>Final title passed in as: A Treatise on Political Economy</t>
+        </is>
+      </c>
+      <c r="AL19" t="inlineStr">
+        <is>
+          <t>Political Economy</t>
+        </is>
+      </c>
+      <c r="AM19" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AN19" t="n">
+        <v>495</v>
+      </c>
+      <c r="AO19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP19" t="n">
+        <v>72</v>
+      </c>
+      <c r="AQ19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV19" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW19" t="inlineStr">
+        <is>
+          <t>d095144c-1d8d-48c8-8315-3d11898b73bd</t>
+        </is>
+      </c>
+      <c r="AX19" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Scroll</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>6</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1500</v>
+      </c>
+      <c r="E20" t="n">
+        <v>102</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Dwarven</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Profession (chamberlain)</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Profession (chamberlain)</t>
+        </is>
+      </c>
+      <c r="J20" t="n">
+        <v>1</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" t="n">
+        <v>1</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" t="n">
+        <v>1</v>
+      </c>
+      <c r="O20" t="n">
+        <v>496</v>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>Transactions Discoursing on Chamberlain's Craft from Æðelwulf Notleigh</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>Viviane Fonder the Harried</t>
+        </is>
+      </c>
+      <c r="S20" s="10" t="inlineStr">
+        <is>
+          <t>ᛞᛁᚲᛏᚢᛗ ᛞᛟᚾᛖᚲ ᚲᚢᚱᚨᛒᛁᛏᚢᚱ ᛞᛟᚨᛗ ᛚᛖᚲᛏᚢᛊ ᛞᚨᛈᛁᛒᚢᛊ ᛊᛟᛚᛚᛁᚲᛁᛏᚢᛞᛁᚾ ᛖᚢ ᚱᛁᛊᚢᛊ ᛈᚱᛁᛗᛁᛊ ᛈᛟᚱᛏᚨ ᛖᚱᚨᛏ</t>
+        </is>
+      </c>
+      <c r="T20" t="n">
+        <v>9</v>
+      </c>
+      <c r="U20" t="n">
+        <v>9</v>
+      </c>
+      <c r="V20" t="n">
+        <v>905</v>
+      </c>
+      <c r="W20" t="n">
+        <v>755</v>
+      </c>
+      <c r="X20" t="n">
+        <v>753</v>
+      </c>
+      <c r="Y20" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AA20" t="inlineStr">
+        <is>
+          <t>the Harried</t>
+        </is>
+      </c>
+      <c r="AB20" t="inlineStr">
+        <is>
+          <t>Viviane Fonder</t>
+        </is>
+      </c>
+      <c r="AD20" t="inlineStr">
+        <is>
+          <t>Lady</t>
+        </is>
+      </c>
+      <c r="AE20" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ20" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK20" t="inlineStr">
+        <is>
+          <t>Final title passed in as: Transactions Discoursing on Chamberlain's Craft from Æðelwulf Notleigh</t>
+        </is>
+      </c>
+      <c r="AL20" t="inlineStr">
+        <is>
+          <t>Chamberlain's Craft</t>
+        </is>
+      </c>
+      <c r="AM20" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="AN20" t="n">
+        <v>540</v>
+      </c>
+      <c r="AO20" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP20" t="n">
+        <v>15</v>
+      </c>
+      <c r="AQ20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU20" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV20" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW20" t="inlineStr">
+        <is>
+          <t>c0bfd151-b893-4834-b09c-7c74b4402796</t>
+        </is>
+      </c>
+      <c r="AX20" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Scroll</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>6</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1500</v>
+      </c>
+      <c r="E21" t="n">
+        <v>102</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Dwarven</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Profession (chamberlain)</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Profession (chamberlain)</t>
+        </is>
+      </c>
+      <c r="J21" t="n">
+        <v>1</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" t="n">
+        <v>1</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" t="n">
+        <v>1</v>
+      </c>
+      <c r="O21" t="n">
+        <v>496</v>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>Transactions Discoursing on Chamberlain's Craft from Æðelwulf Notleigh</t>
+        </is>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>Viviane Fonder the Harried</t>
+        </is>
+      </c>
+      <c r="S21" s="10" t="inlineStr">
+        <is>
+          <t>ᛞᛁᚲᛏᚢᛗ ᛞᛟᚾᛖᚲ ᚲᚢᚱᚨᛒᛁᛏᚢᚱ ᛞᛟᚨᛗ ᛚᛖᚲᛏᚢᛊ ᛞᚨᛈᛁᛒᚢᛊ ᛊᛟᛚᛚᛁᚲᛁᛏᚢᛞᛁᚾ ᛖᚢ ᚱᛁᛊᚢᛊ ᛈᚱᛁᛗᛁᛊ ᛈᛟᚱᛏᚨ ᛖᚱᚨᛏ</t>
+        </is>
+      </c>
+      <c r="T21" t="n">
+        <v>9</v>
+      </c>
+      <c r="U21" t="n">
+        <v>9</v>
+      </c>
+      <c r="V21" t="n">
+        <v>905</v>
+      </c>
+      <c r="W21" t="n">
+        <v>755</v>
+      </c>
+      <c r="X21" t="n">
+        <v>752</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AA21" t="inlineStr">
+        <is>
+          <t>the Harried</t>
+        </is>
+      </c>
+      <c r="AB21" t="inlineStr">
+        <is>
+          <t>Viviane Fonder</t>
+        </is>
+      </c>
+      <c r="AE21" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ21" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK21" t="inlineStr">
+        <is>
+          <t>Final title passed in as: Transactions Discoursing on Chamberlain's Craft from Æðelwulf Notleigh</t>
+        </is>
+      </c>
+      <c r="AL21" t="inlineStr">
+        <is>
+          <t>Chamberlain's Craft</t>
+        </is>
+      </c>
+      <c r="AM21" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="AN21" t="n">
+        <v>540</v>
+      </c>
+      <c r="AO21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP21" t="n">
+        <v>15</v>
+      </c>
+      <c r="AQ21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV21" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW21" t="inlineStr">
+        <is>
+          <t>91aabc05-bb1a-4014-ab63-91391b6c26d0</t>
+        </is>
+      </c>
+      <c r="AX21" t="inlineStr">
         <is>
           <t>has_been_archived</t>
         </is>

</xml_diff>

<commit_message>
Error checking works. Testing works. Default Settings files in folder
</commit_message>
<xml_diff>
--- a/books_spreadsheet_out.xlsx
+++ b/books_spreadsheet_out.xlsx
@@ -466,7 +466,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AX101"/>
+  <dimension ref="A1:AX131"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
       <selection activeCell="S2" sqref="S2"/>
@@ -16724,6 +16724,4826 @@
         </is>
       </c>
     </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C102" t="n">
+        <v>1</v>
+      </c>
+      <c r="D102" t="n">
+        <v>500</v>
+      </c>
+      <c r="E102" t="n">
+        <v>32</v>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>Classical</t>
+        </is>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>Craft (brewing)</t>
+        </is>
+      </c>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>Craft (brewing)</t>
+        </is>
+      </c>
+      <c r="J102" t="n">
+        <v>1</v>
+      </c>
+      <c r="K102" t="n">
+        <v>0</v>
+      </c>
+      <c r="L102" t="n">
+        <v>2</v>
+      </c>
+      <c r="M102" t="n">
+        <v>0</v>
+      </c>
+      <c r="N102" t="n">
+        <v>1</v>
+      </c>
+      <c r="O102" t="n">
+        <v>342</v>
+      </c>
+      <c r="P102" t="inlineStr">
+        <is>
+          <t>Experiences of Léontine Gérard and Brewing</t>
+        </is>
+      </c>
+      <c r="Q102" t="inlineStr">
+        <is>
+          <t>Jordane Soyer</t>
+        </is>
+      </c>
+      <c r="S102" s="10" t="inlineStr">
+        <is>
+          <t>Sueborum pervenerunt reperiebat mercede visae nuptum deditione referrent consequatur?</t>
+        </is>
+      </c>
+      <c r="T102" t="n">
+        <v>3</v>
+      </c>
+      <c r="U102" t="n">
+        <v>3</v>
+      </c>
+      <c r="V102" t="n">
+        <v>141</v>
+      </c>
+      <c r="W102" t="n">
+        <v>33</v>
+      </c>
+      <c r="X102" t="n">
+        <v>32</v>
+      </c>
+      <c r="Y102" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="AB102" t="inlineStr">
+        <is>
+          <t>Jordane Soyer</t>
+        </is>
+      </c>
+      <c r="AC102" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AE102" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ102" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK102" t="inlineStr">
+        <is>
+          <t>{biography_starter} of {person_1} and {topic}</t>
+        </is>
+      </c>
+      <c r="AL102" t="inlineStr">
+        <is>
+          <t>Brewing</t>
+        </is>
+      </c>
+      <c r="AM102" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN102" t="n">
+        <v>185</v>
+      </c>
+      <c r="AO102" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AP102" t="n">
+        <v>157</v>
+      </c>
+      <c r="AQ102" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR102" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS102" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT102" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU102" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV102" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW102" t="inlineStr">
+        <is>
+          <t>bdaec664-d4ab-44f2-982b-9af09ae69718</t>
+        </is>
+      </c>
+      <c r="AX102" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C103" t="n">
+        <v>2</v>
+      </c>
+      <c r="D103" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E103" t="n">
+        <v>63</v>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>Esoteric: Theology</t>
+        </is>
+      </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>Trap Finding</t>
+        </is>
+      </c>
+      <c r="J103" t="n">
+        <v>2</v>
+      </c>
+      <c r="K103" t="n">
+        <v>1</v>
+      </c>
+      <c r="L103" t="n">
+        <v>2</v>
+      </c>
+      <c r="M103" t="n">
+        <v>2</v>
+      </c>
+      <c r="N103" t="n">
+        <v>1</v>
+      </c>
+      <c r="O103" t="n">
+        <v>5890</v>
+      </c>
+      <c r="P103" t="inlineStr">
+        <is>
+          <t>Experiences of The Temptress with emphasis upon Trap Finding</t>
+        </is>
+      </c>
+      <c r="Q103" t="inlineStr">
+        <is>
+          <t>Khawla Islambouli the Fearless</t>
+        </is>
+      </c>
+      <c r="S103" s="10" t="inlineStr">
+        <is>
+          <t>Experiences of The Temptress with emphasis upon Trap Finding</t>
+        </is>
+      </c>
+      <c r="T103" t="n">
+        <v>6</v>
+      </c>
+      <c r="U103" t="n">
+        <v>6</v>
+      </c>
+      <c r="V103" t="n">
+        <v>56</v>
+      </c>
+      <c r="W103" t="n">
+        <v>45</v>
+      </c>
+      <c r="X103" t="n">
+        <v>44</v>
+      </c>
+      <c r="Y103" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="AA103" t="inlineStr">
+        <is>
+          <t>the Fearless</t>
+        </is>
+      </c>
+      <c r="AB103" t="inlineStr">
+        <is>
+          <t>Khawla Islambouli</t>
+        </is>
+      </c>
+      <c r="AC103" t="inlineStr">
+        <is>
+          <t>_names_arabic_surnames</t>
+        </is>
+      </c>
+      <c r="AE103" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ103" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK103" t="inlineStr">
+        <is>
+          <t>{biography_starter} of {person_evil} with emphasis upon {topic}</t>
+        </is>
+      </c>
+      <c r="AL103" t="inlineStr">
+        <is>
+          <t>Trap Finding</t>
+        </is>
+      </c>
+      <c r="AM103" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN103" t="n">
+        <v>390</v>
+      </c>
+      <c r="AO103" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP103" t="n">
+        <v>500</v>
+      </c>
+      <c r="AQ103" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AR103" t="n">
+        <v>5000</v>
+      </c>
+      <c r="AS103" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT103" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU103" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV103" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW103" t="inlineStr">
+        <is>
+          <t>aae2b81b-d050-4d39-9fa6-8a7457486e56</t>
+        </is>
+      </c>
+      <c r="AX103" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C104" t="n">
+        <v>2</v>
+      </c>
+      <c r="D104" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E104" t="n">
+        <v>63</v>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>Classical</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>Labor (barber)</t>
+        </is>
+      </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>Labor (barber)</t>
+        </is>
+      </c>
+      <c r="J104" t="n">
+        <v>1</v>
+      </c>
+      <c r="K104" t="n">
+        <v>0</v>
+      </c>
+      <c r="L104" t="n">
+        <v>1</v>
+      </c>
+      <c r="M104" t="n">
+        <v>0</v>
+      </c>
+      <c r="N104" t="n">
+        <v>1</v>
+      </c>
+      <c r="O104" t="n">
+        <v>720</v>
+      </c>
+      <c r="P104" t="inlineStr">
+        <is>
+          <t>Communication Concerning Barbering from Noëlle Sharpe</t>
+        </is>
+      </c>
+      <c r="Q104" t="inlineStr">
+        <is>
+          <t>Saint Æthelweard Halderman</t>
+        </is>
+      </c>
+      <c r="S104" s="10" t="inlineStr">
+        <is>
+          <t>Prima optime insilirent concedi eas sumi equitatu oceano occasum pugna</t>
+        </is>
+      </c>
+      <c r="T104" t="n">
+        <v>6</v>
+      </c>
+      <c r="U104" t="n">
+        <v>6</v>
+      </c>
+      <c r="V104" t="n">
+        <v>90</v>
+      </c>
+      <c r="W104" t="n">
+        <v>19</v>
+      </c>
+      <c r="X104" t="n">
+        <v>18</v>
+      </c>
+      <c r="Y104" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AB104" t="inlineStr">
+        <is>
+          <t>Æthelweard Halderman</t>
+        </is>
+      </c>
+      <c r="AC104" t="inlineStr">
+        <is>
+          <t>_names_anglo_saxon_surnames</t>
+        </is>
+      </c>
+      <c r="AD104" t="inlineStr">
+        <is>
+          <t>Saint</t>
+        </is>
+      </c>
+      <c r="AE104" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ104" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK104" t="inlineStr">
+        <is>
+          <t>{communication} {conjunction_about} {topic} {conjunction_by} {person_1}</t>
+        </is>
+      </c>
+      <c r="AL104" t="inlineStr">
+        <is>
+          <t>Barbering</t>
+        </is>
+      </c>
+      <c r="AM104" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN104" t="n">
+        <v>390</v>
+      </c>
+      <c r="AO104" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP104" t="n">
+        <v>330</v>
+      </c>
+      <c r="AQ104" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR104" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS104" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT104" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU104" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV104" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW104" t="inlineStr">
+        <is>
+          <t>6c915ef8-c58b-4053-b3f2-a55b4f1ecb4b</t>
+        </is>
+      </c>
+      <c r="AX104" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C105" t="n">
+        <v>1</v>
+      </c>
+      <c r="D105" t="n">
+        <v>500</v>
+      </c>
+      <c r="E105" t="n">
+        <v>32</v>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>Classical</t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>Lockpicking</t>
+        </is>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>Lockpicking</t>
+        </is>
+      </c>
+      <c r="J105" t="n">
+        <v>1</v>
+      </c>
+      <c r="K105" t="n">
+        <v>0</v>
+      </c>
+      <c r="L105" t="n">
+        <v>2</v>
+      </c>
+      <c r="M105" t="n">
+        <v>0</v>
+      </c>
+      <c r="N105" t="n">
+        <v>1</v>
+      </c>
+      <c r="O105" t="n">
+        <v>392</v>
+      </c>
+      <c r="P105" t="inlineStr">
+        <is>
+          <t>Epistles Respecting Locks without Keys , a Commentary on That Which Came From the Pen of Alba Vinicia</t>
+        </is>
+      </c>
+      <c r="Q105" t="inlineStr">
+        <is>
+          <t>Antonia Faenia</t>
+        </is>
+      </c>
+      <c r="S105" s="10" t="inlineStr">
+        <is>
+          <t>Consule paucis milibus multo aspernatur praesentium bellum ob viso inscientibus dolorem occulto coepit malesuada perrumpere totis spiritus helvetios tristique cognoverant uterque</t>
+        </is>
+      </c>
+      <c r="T105" t="n">
+        <v>3</v>
+      </c>
+      <c r="U105" t="n">
+        <v>3</v>
+      </c>
+      <c r="V105" t="n">
+        <v>62</v>
+      </c>
+      <c r="W105" t="n">
+        <v>11</v>
+      </c>
+      <c r="X105" t="n">
+        <v>10</v>
+      </c>
+      <c r="Y105" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AB105" t="inlineStr">
+        <is>
+          <t>Antonia Faenia</t>
+        </is>
+      </c>
+      <c r="AC105" t="inlineStr">
+        <is>
+          <t>_names_roman_surnames</t>
+        </is>
+      </c>
+      <c r="AE105" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ105" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK105" t="inlineStr">
+        <is>
+          <t>{communication} {conjunction_about} {topic} {conjunction_by} {person_1}</t>
+        </is>
+      </c>
+      <c r="AL105" t="inlineStr">
+        <is>
+          <t>Locks without Keys</t>
+        </is>
+      </c>
+      <c r="AM105" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN105" t="n">
+        <v>185</v>
+      </c>
+      <c r="AO105" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AP105" t="n">
+        <v>207</v>
+      </c>
+      <c r="AQ105" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR105" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS105" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT105" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU105" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV105" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW105" t="inlineStr">
+        <is>
+          <t>e3f6fd50-a098-48bd-8e0d-33e44b6f4c4f</t>
+        </is>
+      </c>
+      <c r="AX105" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C106" t="n">
+        <v>2</v>
+      </c>
+      <c r="D106" t="n">
+        <v>1334</v>
+      </c>
+      <c r="E106" t="n">
+        <v>84</v>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>Eavesdropping</t>
+        </is>
+      </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>Eavesdropping</t>
+        </is>
+      </c>
+      <c r="J106" t="n">
+        <v>1</v>
+      </c>
+      <c r="K106" t="n">
+        <v>0</v>
+      </c>
+      <c r="L106" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="M106" t="n">
+        <v>0</v>
+      </c>
+      <c r="N106" t="n">
+        <v>1</v>
+      </c>
+      <c r="O106" t="n">
+        <v>1855</v>
+      </c>
+      <c r="P106" t="inlineStr">
+        <is>
+          <t>The Disguised Progress of This Period: On the Dropping of Eaves for Gardners and Gaffers</t>
+        </is>
+      </c>
+      <c r="Q106" t="inlineStr">
+        <is>
+          <t>Louka Mabille</t>
+        </is>
+      </c>
+      <c r="S106" s="10" t="inlineStr">
+        <is>
+          <t>The Disguised Progress of This Period: On the Dropping of Eaves for Gardners and Gaffers</t>
+        </is>
+      </c>
+      <c r="T106" t="n">
+        <v>8</v>
+      </c>
+      <c r="U106" t="n">
+        <v>8</v>
+      </c>
+      <c r="V106" t="n">
+        <v>41</v>
+      </c>
+      <c r="W106" t="n">
+        <v>1</v>
+      </c>
+      <c r="X106" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y106" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB106" t="inlineStr">
+        <is>
+          <t>Louka Mabille</t>
+        </is>
+      </c>
+      <c r="AC106" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AE106" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ106" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK106" t="inlineStr">
+        <is>
+          <t>The {adjective_1} {noun_1} of {noun_2}: {topic}</t>
+        </is>
+      </c>
+      <c r="AL106" t="inlineStr">
+        <is>
+          <t>On the Dropping of Eaves for Gardners and Gaffers</t>
+        </is>
+      </c>
+      <c r="AM106" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN106" t="n">
+        <v>521</v>
+      </c>
+      <c r="AO106" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP106" t="n">
+        <v>1334</v>
+      </c>
+      <c r="AQ106" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR106" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS106" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT106" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU106" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV106" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW106" t="inlineStr">
+        <is>
+          <t>2ac5324a-a507-4b79-8da0-1a51cccbee60</t>
+        </is>
+      </c>
+      <c r="AX106" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C107" t="n">
+        <v>4</v>
+      </c>
+      <c r="D107" t="n">
+        <v>3000</v>
+      </c>
+      <c r="E107" t="n">
+        <v>186</v>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>Esoteric: Theology</t>
+        </is>
+      </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>Animal Training (falcons)</t>
+        </is>
+      </c>
+      <c r="J107" t="n">
+        <v>3</v>
+      </c>
+      <c r="K107" t="n">
+        <v>1</v>
+      </c>
+      <c r="L107" t="n">
+        <v>1</v>
+      </c>
+      <c r="M107" t="n">
+        <v>3</v>
+      </c>
+      <c r="N107" t="n">
+        <v>1</v>
+      </c>
+      <c r="O107" t="n">
+        <v>22170</v>
+      </c>
+      <c r="P107" t="inlineStr">
+        <is>
+          <t>Martyrdom of The Dark Lord with emphasis upon Noble Art of Falconry</t>
+        </is>
+      </c>
+      <c r="Q107" t="inlineStr">
+        <is>
+          <t>His Honor Muhannad Farhat</t>
+        </is>
+      </c>
+      <c r="S107" s="10" t="inlineStr">
+        <is>
+          <t>Martyrdom of The Dark Lord with emphasis upon Noble Art of Falconry</t>
+        </is>
+      </c>
+      <c r="T107" t="n">
+        <v>17</v>
+      </c>
+      <c r="U107" t="n">
+        <v>17</v>
+      </c>
+      <c r="V107" t="n">
+        <v>36</v>
+      </c>
+      <c r="W107" t="n">
+        <v>2</v>
+      </c>
+      <c r="X107" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y107" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AB107" t="inlineStr">
+        <is>
+          <t>Muhannad Farhat</t>
+        </is>
+      </c>
+      <c r="AC107" t="inlineStr">
+        <is>
+          <t>_names_arabic_surnames</t>
+        </is>
+      </c>
+      <c r="AD107" t="inlineStr">
+        <is>
+          <t>His Honor</t>
+        </is>
+      </c>
+      <c r="AE107" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ107" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK107" t="inlineStr">
+        <is>
+          <t>{biography_starter} of {person_evil} with emphasis upon {topic}</t>
+        </is>
+      </c>
+      <c r="AL107" t="inlineStr">
+        <is>
+          <t>Noble Art of Falconry</t>
+        </is>
+      </c>
+      <c r="AM107" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN107" t="n">
+        <v>1170</v>
+      </c>
+      <c r="AO107" t="n">
+        <v>4</v>
+      </c>
+      <c r="AP107" t="n">
+        <v>6000</v>
+      </c>
+      <c r="AQ107" t="n">
+        <v>2</v>
+      </c>
+      <c r="AR107" t="n">
+        <v>15000</v>
+      </c>
+      <c r="AS107" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT107" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU107" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV107" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW107" t="inlineStr">
+        <is>
+          <t>9affcabd-d577-4783-b271-5af52e300d0c</t>
+        </is>
+      </c>
+      <c r="AX107" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C108" t="n">
+        <v>2</v>
+      </c>
+      <c r="D108" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E108" t="n">
+        <v>63</v>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>Classical</t>
+        </is>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>Land Surveying</t>
+        </is>
+      </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>Land Surveying</t>
+        </is>
+      </c>
+      <c r="J108" t="n">
+        <v>2</v>
+      </c>
+      <c r="K108" t="n">
+        <v>0</v>
+      </c>
+      <c r="L108" t="n">
+        <v>2</v>
+      </c>
+      <c r="M108" t="n">
+        <v>0</v>
+      </c>
+      <c r="N108" t="n">
+        <v>1</v>
+      </c>
+      <c r="O108" t="n">
+        <v>490</v>
+      </c>
+      <c r="P108" t="inlineStr">
+        <is>
+          <t>Condemnation of Queen Kalissa and Land Surveying</t>
+        </is>
+      </c>
+      <c r="Q108" t="inlineStr">
+        <is>
+          <t>Uhtric Fisc</t>
+        </is>
+      </c>
+      <c r="S108" s="10" t="inlineStr">
+        <is>
+          <t>Sequanos summam misit cruciatus legatis datis acies</t>
+        </is>
+      </c>
+      <c r="T108" t="n">
+        <v>6</v>
+      </c>
+      <c r="U108" t="n">
+        <v>6</v>
+      </c>
+      <c r="V108" t="n">
+        <v>91</v>
+      </c>
+      <c r="W108" t="n">
+        <v>185</v>
+      </c>
+      <c r="X108" t="n">
+        <v>184</v>
+      </c>
+      <c r="Y108" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="AB108" t="inlineStr">
+        <is>
+          <t>Uhtric Fisc</t>
+        </is>
+      </c>
+      <c r="AC108" t="inlineStr">
+        <is>
+          <t>_names_anglo_saxon_surnames</t>
+        </is>
+      </c>
+      <c r="AE108" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ108" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK108" t="inlineStr">
+        <is>
+          <t>{biography_starter} of {person_famous} and {topic}</t>
+        </is>
+      </c>
+      <c r="AL108" t="inlineStr">
+        <is>
+          <t>Land Surveying</t>
+        </is>
+      </c>
+      <c r="AM108" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN108" t="n">
+        <v>390</v>
+      </c>
+      <c r="AO108" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP108" t="n">
+        <v>100</v>
+      </c>
+      <c r="AQ108" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR108" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS108" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT108" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU108" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV108" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW108" t="inlineStr">
+        <is>
+          <t>4abefa9f-c74e-4424-b888-edfba838392a</t>
+        </is>
+      </c>
+      <c r="AX108" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C109" t="n">
+        <v>1</v>
+      </c>
+      <c r="D109" t="n">
+        <v>500</v>
+      </c>
+      <c r="E109" t="n">
+        <v>32</v>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>Regional</t>
+        </is>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>Craft (basket-making)</t>
+        </is>
+      </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>Craft (basket-making)</t>
+        </is>
+      </c>
+      <c r="J109" t="n">
+        <v>1</v>
+      </c>
+      <c r="K109" t="n">
+        <v>0</v>
+      </c>
+      <c r="L109" t="n">
+        <v>2</v>
+      </c>
+      <c r="M109" t="n">
+        <v>0</v>
+      </c>
+      <c r="N109" t="n">
+        <v>1</v>
+      </c>
+      <c r="O109" t="n">
+        <v>508</v>
+      </c>
+      <c r="P109" t="inlineStr">
+        <is>
+          <t>The Underground Passage of Foreboding: The Crafte of Making Baskets</t>
+        </is>
+      </c>
+      <c r="Q109" t="inlineStr">
+        <is>
+          <t>Her Ladyship Inga Johansdotter</t>
+        </is>
+      </c>
+      <c r="S109" s="10" t="inlineStr">
+        <is>
+          <t>Ε΄ λοιπαῖς ἀρχῆς ἀλλήλοις μέρη ἀφ' ἴση ἀφελεῖν τὰς γραμμή</t>
+        </is>
+      </c>
+      <c r="T109" t="n">
+        <v>3</v>
+      </c>
+      <c r="U109" t="n">
+        <v>3</v>
+      </c>
+      <c r="V109" t="n">
+        <v>48</v>
+      </c>
+      <c r="W109" t="n">
+        <v>4</v>
+      </c>
+      <c r="X109" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y109" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AB109" t="inlineStr">
+        <is>
+          <t>Inga Johansdotter</t>
+        </is>
+      </c>
+      <c r="AC109" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_female</t>
+        </is>
+      </c>
+      <c r="AD109" t="inlineStr">
+        <is>
+          <t>Her Ladyship</t>
+        </is>
+      </c>
+      <c r="AE109" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ109" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK109" t="inlineStr">
+        <is>
+          <t>The {adjective_1} {noun_1} of {noun_2}: {topic}</t>
+        </is>
+      </c>
+      <c r="AL109" t="inlineStr">
+        <is>
+          <t>The Crafte of Making Baskets</t>
+        </is>
+      </c>
+      <c r="AM109" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN109" t="n">
+        <v>195</v>
+      </c>
+      <c r="AO109" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AP109" t="n">
+        <v>313</v>
+      </c>
+      <c r="AQ109" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR109" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS109" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT109" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU109" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV109" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW109" t="inlineStr">
+        <is>
+          <t>a726cea9-2787-44e2-b083-1cae60493043</t>
+        </is>
+      </c>
+      <c r="AX109" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>Scroll</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C110" t="n">
+        <v>3</v>
+      </c>
+      <c r="D110" t="n">
+        <v>667</v>
+      </c>
+      <c r="E110" t="n">
+        <v>47</v>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>Dwarven</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>Classical</t>
+        </is>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>Knowledge (history)</t>
+        </is>
+      </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>Knowledge (history)</t>
+        </is>
+      </c>
+      <c r="J110" t="n">
+        <v>2</v>
+      </c>
+      <c r="K110" t="n">
+        <v>0</v>
+      </c>
+      <c r="L110" t="n">
+        <v>3</v>
+      </c>
+      <c r="M110" t="n">
+        <v>0</v>
+      </c>
+      <c r="N110" t="n">
+        <v>1</v>
+      </c>
+      <c r="O110" t="n">
+        <v>792</v>
+      </c>
+      <c r="P110" t="inlineStr">
+        <is>
+          <t>Synod of the Germanies</t>
+        </is>
+      </c>
+      <c r="Q110" t="inlineStr">
+        <is>
+          <t>Ophélie Boissonade</t>
+        </is>
+      </c>
+      <c r="R110" t="inlineStr">
+        <is>
+          <t>Mister Tiberius Numeria</t>
+        </is>
+      </c>
+      <c r="S110" s="11" t="inlineStr">
+        <is>
+          <t>ᛗᛁ ᚢᛚᛚᚨᛗᚲᛟᚱᛈᛖᚱ ᛏᛖᛗᛈᚢᛊ ᚲᛟᛜᚢᛖ</t>
+        </is>
+      </c>
+      <c r="T110" t="n">
+        <v>4</v>
+      </c>
+      <c r="U110" t="n">
+        <v>4</v>
+      </c>
+      <c r="V110" t="n">
+        <v>1942</v>
+      </c>
+      <c r="W110" t="n">
+        <v>19</v>
+      </c>
+      <c r="X110" t="n">
+        <v>18</v>
+      </c>
+      <c r="Y110" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AB110" t="inlineStr">
+        <is>
+          <t>Ophélie Boissonade</t>
+        </is>
+      </c>
+      <c r="AC110" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AE110" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AF110" t="inlineStr">
+        <is>
+          <t>Tiberius Numeria</t>
+        </is>
+      </c>
+      <c r="AG110" t="inlineStr">
+        <is>
+          <t>_names_roman_surnames</t>
+        </is>
+      </c>
+      <c r="AH110" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AI110" t="inlineStr">
+        <is>
+          <t>Mister</t>
+        </is>
+      </c>
+      <c r="AJ110" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK110" t="inlineStr">
+        <is>
+          <t>{history_of} {place_nation}</t>
+        </is>
+      </c>
+      <c r="AL110" t="inlineStr">
+        <is>
+          <t>History</t>
+        </is>
+      </c>
+      <c r="AM110" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="AN110" t="n">
+        <v>241</v>
+      </c>
+      <c r="AO110" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="AP110" t="n">
+        <v>551</v>
+      </c>
+      <c r="AQ110" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR110" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS110" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT110" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU110" t="b">
+        <v>1</v>
+      </c>
+      <c r="AV110" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW110" t="inlineStr">
+        <is>
+          <t>35000fc6-11aa-4807-a469-05c3c1611484</t>
+        </is>
+      </c>
+      <c r="AX110" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C111" t="n">
+        <v>2</v>
+      </c>
+      <c r="D111" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E111" t="n">
+        <v>63</v>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>Tracking</t>
+        </is>
+      </c>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>Tracking</t>
+        </is>
+      </c>
+      <c r="J111" t="n">
+        <v>2</v>
+      </c>
+      <c r="K111" t="n">
+        <v>0</v>
+      </c>
+      <c r="L111" t="n">
+        <v>2</v>
+      </c>
+      <c r="M111" t="n">
+        <v>0</v>
+      </c>
+      <c r="N111" t="n">
+        <v>1</v>
+      </c>
+      <c r="O111" t="n">
+        <v>1390</v>
+      </c>
+      <c r="P111" t="inlineStr">
+        <is>
+          <t>Tracking and the Age</t>
+        </is>
+      </c>
+      <c r="Q111" t="inlineStr">
+        <is>
+          <t>The Honorable Alcide Montel</t>
+        </is>
+      </c>
+      <c r="S111" s="10" t="inlineStr">
+        <is>
+          <t>Tracking and the Age</t>
+        </is>
+      </c>
+      <c r="T111" t="n">
+        <v>6</v>
+      </c>
+      <c r="U111" t="n">
+        <v>6</v>
+      </c>
+      <c r="V111" t="n">
+        <v>16</v>
+      </c>
+      <c r="W111" t="n">
+        <v>3</v>
+      </c>
+      <c r="X111" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y111" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AB111" t="inlineStr">
+        <is>
+          <t>Alcide Montel</t>
+        </is>
+      </c>
+      <c r="AC111" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AD111" t="inlineStr">
+        <is>
+          <t>The Honorable</t>
+        </is>
+      </c>
+      <c r="AE111" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ111" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK111" t="inlineStr">
+        <is>
+          <t>{topic} and {noun_2}</t>
+        </is>
+      </c>
+      <c r="AL111" t="inlineStr">
+        <is>
+          <t>Tracking</t>
+        </is>
+      </c>
+      <c r="AM111" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN111" t="n">
+        <v>390</v>
+      </c>
+      <c r="AO111" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP111" t="n">
+        <v>1000</v>
+      </c>
+      <c r="AQ111" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR111" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS111" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT111" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU111" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV111" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW111" t="inlineStr">
+        <is>
+          <t>06fd26ec-9e90-499a-99a3-3604662da428</t>
+        </is>
+      </c>
+      <c r="AX111" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C112" t="n">
+        <v>2</v>
+      </c>
+      <c r="D112" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E112" t="n">
+        <v>63</v>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>Regional</t>
+        </is>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>Performance (playing instruments)</t>
+        </is>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>Performance (playing instruments)</t>
+        </is>
+      </c>
+      <c r="J112" t="n">
+        <v>2</v>
+      </c>
+      <c r="K112" t="n">
+        <v>0</v>
+      </c>
+      <c r="L112" t="n">
+        <v>2</v>
+      </c>
+      <c r="M112" t="n">
+        <v>0</v>
+      </c>
+      <c r="N112" t="n">
+        <v>1</v>
+      </c>
+      <c r="O112" t="n">
+        <v>1390</v>
+      </c>
+      <c r="P112" t="inlineStr">
+        <is>
+          <t>Transactions of Maude Bonneton and Ely Lewis Relating to The Seductive Lute</t>
+        </is>
+      </c>
+      <c r="Q112" t="inlineStr">
+        <is>
+          <t>Jeannine Petit</t>
+        </is>
+      </c>
+      <c r="S112" s="10" t="inlineStr">
+        <is>
+          <t>Καλεῖται ὦσιν ἄνισα τετραγώνοις τοῖς μέρους ἐμπίπτουσα ἐκβαλεῖν μζ΄ τὴν πλευρῶν</t>
+        </is>
+      </c>
+      <c r="T112" t="n">
+        <v>6</v>
+      </c>
+      <c r="U112" t="n">
+        <v>6</v>
+      </c>
+      <c r="V112" t="n">
+        <v>39</v>
+      </c>
+      <c r="W112" t="n">
+        <v>2</v>
+      </c>
+      <c r="X112" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y112" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AB112" t="inlineStr">
+        <is>
+          <t>Jeannine Petit</t>
+        </is>
+      </c>
+      <c r="AC112" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AE112" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ112" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK112" t="inlineStr">
+        <is>
+          <t>{communication} of {person_1} and {person_2} {conjunction_about} {topic}</t>
+        </is>
+      </c>
+      <c r="AL112" t="inlineStr">
+        <is>
+          <t>The Seductive Lute</t>
+        </is>
+      </c>
+      <c r="AM112" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN112" t="n">
+        <v>390</v>
+      </c>
+      <c r="AO112" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP112" t="n">
+        <v>1000</v>
+      </c>
+      <c r="AQ112" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR112" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS112" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT112" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU112" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV112" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW112" t="inlineStr">
+        <is>
+          <t>303bbe27-3521-4ce8-a78e-2f6490911d04</t>
+        </is>
+      </c>
+      <c r="AX112" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C113" t="n">
+        <v>2</v>
+      </c>
+      <c r="D113" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E113" t="n">
+        <v>63</v>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>Regional</t>
+        </is>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>Collegiate Wizardry</t>
+        </is>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>Collegiate Wizardry</t>
+        </is>
+      </c>
+      <c r="J113" t="n">
+        <v>1</v>
+      </c>
+      <c r="K113" t="n">
+        <v>0</v>
+      </c>
+      <c r="L113" t="n">
+        <v>1</v>
+      </c>
+      <c r="M113" t="n">
+        <v>0</v>
+      </c>
+      <c r="N113" t="n">
+        <v>1</v>
+      </c>
+      <c r="O113" t="n">
+        <v>870</v>
+      </c>
+      <c r="P113" t="inlineStr">
+        <is>
+          <t>Searches in Collegiate Wizardry</t>
+        </is>
+      </c>
+      <c r="Q113" t="inlineStr">
+        <is>
+          <t>Ambroise Lavaud</t>
+        </is>
+      </c>
+      <c r="S113" s="10" t="inlineStr">
+        <is>
+          <t>Γωνίας ἐφέστηκεν ιθ΄ εἰσιν ἴσον ἑτερόμηκες ἐστίν συσταθῶσιν μεταλαμβανομένας]</t>
+        </is>
+      </c>
+      <c r="T113" t="n">
+        <v>6</v>
+      </c>
+      <c r="U113" t="n">
+        <v>6</v>
+      </c>
+      <c r="V113" t="n">
+        <v>33</v>
+      </c>
+      <c r="W113" t="n">
+        <v>3</v>
+      </c>
+      <c r="X113" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y113" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AB113" t="inlineStr">
+        <is>
+          <t>Ambroise Lavaud</t>
+        </is>
+      </c>
+      <c r="AC113" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AE113" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ113" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK113" t="inlineStr">
+        <is>
+          <t>{study_in} in {topic}</t>
+        </is>
+      </c>
+      <c r="AL113" t="inlineStr">
+        <is>
+          <t>Collegiate Wizardry</t>
+        </is>
+      </c>
+      <c r="AM113" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN113" t="n">
+        <v>370</v>
+      </c>
+      <c r="AO113" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP113" t="n">
+        <v>500</v>
+      </c>
+      <c r="AQ113" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR113" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS113" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT113" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU113" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV113" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW113" t="inlineStr">
+        <is>
+          <t>59331f52-fb76-4805-98dc-516f24814ea0</t>
+        </is>
+      </c>
+      <c r="AX113" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C114" t="n">
+        <v>2</v>
+      </c>
+      <c r="D114" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E114" t="n">
+        <v>63</v>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H114" t="inlineStr">
+        <is>
+          <t>Command</t>
+        </is>
+      </c>
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>Command</t>
+        </is>
+      </c>
+      <c r="J114" t="n">
+        <v>1</v>
+      </c>
+      <c r="K114" t="n">
+        <v>0</v>
+      </c>
+      <c r="L114" t="n">
+        <v>1</v>
+      </c>
+      <c r="M114" t="n">
+        <v>0</v>
+      </c>
+      <c r="N114" t="n">
+        <v>1</v>
+      </c>
+      <c r="O114" t="n">
+        <v>620</v>
+      </c>
+      <c r="P114" t="inlineStr">
+        <is>
+          <t>Apologia of The Dark Lord with emphasis upon Exercising Command</t>
+        </is>
+      </c>
+      <c r="Q114" t="inlineStr">
+        <is>
+          <t>Didier Lucroy</t>
+        </is>
+      </c>
+      <c r="S114" s="10" t="inlineStr">
+        <is>
+          <t>Apologia of The Dark Lord with emphasis upon Exercising Command</t>
+        </is>
+      </c>
+      <c r="T114" t="n">
+        <v>6</v>
+      </c>
+      <c r="U114" t="n">
+        <v>6</v>
+      </c>
+      <c r="V114" t="n">
+        <v>17</v>
+      </c>
+      <c r="W114" t="n">
+        <v>45</v>
+      </c>
+      <c r="X114" t="n">
+        <v>44</v>
+      </c>
+      <c r="Y114" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="AB114" t="inlineStr">
+        <is>
+          <t>Didier Lucroy</t>
+        </is>
+      </c>
+      <c r="AC114" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AE114" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ114" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK114" t="inlineStr">
+        <is>
+          <t>{biography_starter} of {person_evil} with emphasis upon {topic}</t>
+        </is>
+      </c>
+      <c r="AL114" t="inlineStr">
+        <is>
+          <t>Exercising Command</t>
+        </is>
+      </c>
+      <c r="AM114" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN114" t="n">
+        <v>370</v>
+      </c>
+      <c r="AO114" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP114" t="n">
+        <v>250</v>
+      </c>
+      <c r="AQ114" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR114" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS114" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT114" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU114" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV114" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW114" t="inlineStr">
+        <is>
+          <t>708a41e9-b405-42fd-add1-368bd5f4b9f6</t>
+        </is>
+      </c>
+      <c r="AX114" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C115" t="n">
+        <v>2</v>
+      </c>
+      <c r="D115" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E115" t="n">
+        <v>63</v>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>Regional</t>
+        </is>
+      </c>
+      <c r="H115" t="inlineStr">
+        <is>
+          <t>Land Surveying</t>
+        </is>
+      </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>Land Surveying</t>
+        </is>
+      </c>
+      <c r="J115" t="n">
+        <v>2</v>
+      </c>
+      <c r="K115" t="n">
+        <v>0</v>
+      </c>
+      <c r="L115" t="n">
+        <v>2</v>
+      </c>
+      <c r="M115" t="n">
+        <v>0</v>
+      </c>
+      <c r="N115" t="n">
+        <v>1</v>
+      </c>
+      <c r="O115" t="n">
+        <v>570</v>
+      </c>
+      <c r="P115" t="inlineStr">
+        <is>
+          <t>The Misdeeds of Patricia Tituria, in which case Concerning Land Surveying is Given Particular Attention by Way of Instruction and Warning</t>
+        </is>
+      </c>
+      <c r="Q115" t="inlineStr">
+        <is>
+          <t>Torny Jensdotter</t>
+        </is>
+      </c>
+      <c r="S115" s="10" t="inlineStr">
+        <is>
+          <t>Οὔτε ἴσας προσεκβληθεισῶν τοῖς ὅλον μείζονας σχημάτων τραπέζια μόνας κέντρῳ τετραγώνοις τῆς ὑποτεινούσης ἣν ἐκ μβ΄ ἐπιφάνεια ὀρθὴν παραλληλογράμμων περιέχουσιν ἐστίν] μέρος ἐστι σημεῖα</t>
+        </is>
+      </c>
+      <c r="T115" t="n">
+        <v>6</v>
+      </c>
+      <c r="U115" t="n">
+        <v>6</v>
+      </c>
+      <c r="V115" t="n">
+        <v>50</v>
+      </c>
+      <c r="W115" t="n">
+        <v>72</v>
+      </c>
+      <c r="X115" t="n">
+        <v>71</v>
+      </c>
+      <c r="Y115" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AB115" t="inlineStr">
+        <is>
+          <t>Torny Jensdotter</t>
+        </is>
+      </c>
+      <c r="AC115" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_female</t>
+        </is>
+      </c>
+      <c r="AE115" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ115" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK115" t="inlineStr">
+        <is>
+          <t>{the_1} {negative_1} of {person_1}, in which case {conjunction_about} {topic} is Given Particular Attention by Way of Instruction and Warning</t>
+        </is>
+      </c>
+      <c r="AL115" t="inlineStr">
+        <is>
+          <t>Land Surveying</t>
+        </is>
+      </c>
+      <c r="AM115" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN115" t="n">
+        <v>370</v>
+      </c>
+      <c r="AO115" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP115" t="n">
+        <v>200</v>
+      </c>
+      <c r="AQ115" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR115" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS115" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT115" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU115" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV115" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW115" t="inlineStr">
+        <is>
+          <t>d1f3e1b9-508a-41cf-a39c-e7b674b0e8dd</t>
+        </is>
+      </c>
+      <c r="AX115" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C116" t="n">
+        <v>1</v>
+      </c>
+      <c r="D116" t="n">
+        <v>500</v>
+      </c>
+      <c r="E116" t="n">
+        <v>32</v>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H116" t="inlineStr">
+        <is>
+          <t>Combat Trickery</t>
+        </is>
+      </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>Combat Trickery</t>
+        </is>
+      </c>
+      <c r="J116" t="n">
+        <v>2</v>
+      </c>
+      <c r="K116" t="n">
+        <v>0</v>
+      </c>
+      <c r="L116" t="n">
+        <v>4</v>
+      </c>
+      <c r="M116" t="n">
+        <v>0</v>
+      </c>
+      <c r="N116" t="n">
+        <v>1</v>
+      </c>
+      <c r="O116" t="n">
+        <v>845</v>
+      </c>
+      <c r="P116" t="inlineStr">
+        <is>
+          <t>Debates in Combat Trickery</t>
+        </is>
+      </c>
+      <c r="Q116" t="inlineStr">
+        <is>
+          <t>Brother Bartholomew Slaughter</t>
+        </is>
+      </c>
+      <c r="S116" s="10" t="inlineStr">
+        <is>
+          <t>Debates in Combat Trickery</t>
+        </is>
+      </c>
+      <c r="T116" t="n">
+        <v>3</v>
+      </c>
+      <c r="U116" t="n">
+        <v>3</v>
+      </c>
+      <c r="V116" t="n">
+        <v>49</v>
+      </c>
+      <c r="W116" t="n">
+        <v>20</v>
+      </c>
+      <c r="X116" t="n">
+        <v>19</v>
+      </c>
+      <c r="Y116" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AB116" t="inlineStr">
+        <is>
+          <t>Bartholomew Slaughter</t>
+        </is>
+      </c>
+      <c r="AC116" t="inlineStr">
+        <is>
+          <t>_names_anglo_saxon_surnames</t>
+        </is>
+      </c>
+      <c r="AD116" t="inlineStr">
+        <is>
+          <t>Brother</t>
+        </is>
+      </c>
+      <c r="AE116" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ116" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK116" t="inlineStr">
+        <is>
+          <t>{study_in} in {topic}</t>
+        </is>
+      </c>
+      <c r="AL116" t="inlineStr">
+        <is>
+          <t>Combat Trickery</t>
+        </is>
+      </c>
+      <c r="AM116" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN116" t="n">
+        <v>185</v>
+      </c>
+      <c r="AO116" t="n">
+        <v>4</v>
+      </c>
+      <c r="AP116" t="n">
+        <v>660</v>
+      </c>
+      <c r="AQ116" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR116" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS116" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT116" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU116" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV116" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW116" t="inlineStr">
+        <is>
+          <t>b32f146c-b3be-4d26-9c21-5c12a33005be</t>
+        </is>
+      </c>
+      <c r="AX116" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C117" t="n">
+        <v>2</v>
+      </c>
+      <c r="D117" t="n">
+        <v>1334</v>
+      </c>
+      <c r="E117" t="n">
+        <v>84</v>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>Regional</t>
+        </is>
+      </c>
+      <c r="H117" t="inlineStr">
+        <is>
+          <t>Labor (mining)</t>
+        </is>
+      </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>Labor (mining)</t>
+        </is>
+      </c>
+      <c r="J117" t="n">
+        <v>1</v>
+      </c>
+      <c r="K117" t="n">
+        <v>0</v>
+      </c>
+      <c r="L117" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="M117" t="n">
+        <v>0</v>
+      </c>
+      <c r="N117" t="n">
+        <v>1</v>
+      </c>
+      <c r="O117" t="n">
+        <v>1188</v>
+      </c>
+      <c r="P117" t="inlineStr">
+        <is>
+          <t>The Regrettable Misdeeds of Justus Appia, Considering Mining</t>
+        </is>
+      </c>
+      <c r="Q117" t="inlineStr">
+        <is>
+          <t>Her Honor Ennia Ofania Harefoot</t>
+        </is>
+      </c>
+      <c r="S117" s="10" t="inlineStr">
+        <is>
+          <t>Ἐφεξῆς συσταθήσονται συνεχὲς πλευρᾷ ἁπτομένων ἐστι πέρατα ἒνοιαι</t>
+        </is>
+      </c>
+      <c r="T117" t="n">
+        <v>8</v>
+      </c>
+      <c r="U117" t="n">
+        <v>8</v>
+      </c>
+      <c r="V117" t="n">
+        <v>37</v>
+      </c>
+      <c r="W117" t="n">
+        <v>3</v>
+      </c>
+      <c r="X117" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y117" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AA117" t="inlineStr">
+        <is>
+          <t>Harefoot</t>
+        </is>
+      </c>
+      <c r="AB117" t="inlineStr">
+        <is>
+          <t>Ennia Ofania</t>
+        </is>
+      </c>
+      <c r="AC117" t="inlineStr">
+        <is>
+          <t>_names_roman_surnames</t>
+        </is>
+      </c>
+      <c r="AD117" t="inlineStr">
+        <is>
+          <t>Her Honor</t>
+        </is>
+      </c>
+      <c r="AE117" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ117" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK117" t="inlineStr">
+        <is>
+          <t>{the_1} {negative_1} of {person_1}, Considering {topic}</t>
+        </is>
+      </c>
+      <c r="AL117" t="inlineStr">
+        <is>
+          <t>Mining</t>
+        </is>
+      </c>
+      <c r="AM117" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN117" t="n">
+        <v>521</v>
+      </c>
+      <c r="AO117" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP117" t="n">
+        <v>667</v>
+      </c>
+      <c r="AQ117" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR117" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS117" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT117" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU117" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV117" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW117" t="inlineStr">
+        <is>
+          <t>ba99603a-cc21-4f3e-a371-889e18037b97</t>
+        </is>
+      </c>
+      <c r="AX117" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C118" t="n">
+        <v>1</v>
+      </c>
+      <c r="D118" t="n">
+        <v>500</v>
+      </c>
+      <c r="E118" t="n">
+        <v>32</v>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>Classical</t>
+        </is>
+      </c>
+      <c r="H118" t="inlineStr">
+        <is>
+          <t>Knowledge (occult)</t>
+        </is>
+      </c>
+      <c r="I118" t="inlineStr">
+        <is>
+          <t>Knowledge (occult)</t>
+        </is>
+      </c>
+      <c r="J118" t="n">
+        <v>1</v>
+      </c>
+      <c r="K118" t="n">
+        <v>0</v>
+      </c>
+      <c r="L118" t="n">
+        <v>2</v>
+      </c>
+      <c r="M118" t="n">
+        <v>0</v>
+      </c>
+      <c r="N118" t="n">
+        <v>1</v>
+      </c>
+      <c r="O118" t="n">
+        <v>402</v>
+      </c>
+      <c r="P118" t="inlineStr">
+        <is>
+          <t>Life of The Temptress with emphasis upon Occult Knowledge</t>
+        </is>
+      </c>
+      <c r="Q118" t="inlineStr">
+        <is>
+          <t>The Venerable Freyja Andersdotter</t>
+        </is>
+      </c>
+      <c r="S118" s="10" t="inlineStr">
+        <is>
+          <t>Meritos immortalium edere potirentur progressus iura se imperare rem</t>
+        </is>
+      </c>
+      <c r="T118" t="n">
+        <v>3</v>
+      </c>
+      <c r="U118" t="n">
+        <v>3</v>
+      </c>
+      <c r="V118" t="n">
+        <v>120</v>
+      </c>
+      <c r="W118" t="n">
+        <v>12</v>
+      </c>
+      <c r="X118" t="n">
+        <v>11</v>
+      </c>
+      <c r="Y118" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AB118" t="inlineStr">
+        <is>
+          <t>Freyja Andersdotter</t>
+        </is>
+      </c>
+      <c r="AC118" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_female</t>
+        </is>
+      </c>
+      <c r="AD118" t="inlineStr">
+        <is>
+          <t>The Venerable</t>
+        </is>
+      </c>
+      <c r="AE118" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ118" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK118" t="inlineStr">
+        <is>
+          <t>{biography_starter} of {person_evil} with emphasis upon {topic}</t>
+        </is>
+      </c>
+      <c r="AL118" t="inlineStr">
+        <is>
+          <t>Occult Knowledge</t>
+        </is>
+      </c>
+      <c r="AM118" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN118" t="n">
+        <v>195</v>
+      </c>
+      <c r="AO118" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AP118" t="n">
+        <v>207</v>
+      </c>
+      <c r="AQ118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU118" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV118" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW118" t="inlineStr">
+        <is>
+          <t>53d581a1-6d42-49fa-b77e-7a88b6531fa6</t>
+        </is>
+      </c>
+      <c r="AX118" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C119" t="n">
+        <v>2</v>
+      </c>
+      <c r="D119" t="n">
+        <v>340</v>
+      </c>
+      <c r="E119" t="n">
+        <v>22</v>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H119" t="inlineStr">
+        <is>
+          <t>Intimidation</t>
+        </is>
+      </c>
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>Intimidation</t>
+        </is>
+      </c>
+      <c r="J119" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="K119" t="n">
+        <v>0</v>
+      </c>
+      <c r="L119" t="n">
+        <v>4</v>
+      </c>
+      <c r="M119" t="n">
+        <v>0</v>
+      </c>
+      <c r="N119" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="O119" t="n">
+        <v>296</v>
+      </c>
+      <c r="P119" t="inlineStr">
+        <is>
+          <t>Adventures of The Temptress with emphasis upon Intimidation</t>
+        </is>
+      </c>
+      <c r="Q119" t="inlineStr">
+        <is>
+          <t>Lady Fenal Pachachi</t>
+        </is>
+      </c>
+      <c r="S119" s="10" t="inlineStr">
+        <is>
+          <t>Adventures of The Temptress with emphasis upon Intimidation</t>
+        </is>
+      </c>
+      <c r="T119" t="n">
+        <v>2</v>
+      </c>
+      <c r="U119" t="n">
+        <v>2</v>
+      </c>
+      <c r="V119" t="n">
+        <v>93</v>
+      </c>
+      <c r="W119" t="n">
+        <v>107</v>
+      </c>
+      <c r="X119" t="n">
+        <v>106</v>
+      </c>
+      <c r="Y119" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="AB119" t="inlineStr">
+        <is>
+          <t>Fenal Pachachi</t>
+        </is>
+      </c>
+      <c r="AC119" t="inlineStr">
+        <is>
+          <t>_names_arabic_surnames</t>
+        </is>
+      </c>
+      <c r="AD119" t="inlineStr">
+        <is>
+          <t>Lady</t>
+        </is>
+      </c>
+      <c r="AE119" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ119" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK119" t="inlineStr">
+        <is>
+          <t>{biography_starter} of {person_evil} with emphasis upon {topic}</t>
+        </is>
+      </c>
+      <c r="AL119" t="inlineStr">
+        <is>
+          <t>Intimidation</t>
+        </is>
+      </c>
+      <c r="AM119" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN119" t="n">
+        <v>370</v>
+      </c>
+      <c r="AO119" t="n">
+        <v>10</v>
+      </c>
+      <c r="AP119" t="n">
+        <v>500</v>
+      </c>
+      <c r="AQ119" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR119" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS119" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT119" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU119" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV119" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW119" t="inlineStr">
+        <is>
+          <t>d8b0b28e-b6a3-4483-89d9-2bf70ca53cbe</t>
+        </is>
+      </c>
+      <c r="AX119" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C120" t="n">
+        <v>1</v>
+      </c>
+      <c r="D120" t="n">
+        <v>500</v>
+      </c>
+      <c r="E120" t="n">
+        <v>32</v>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>Classical</t>
+        </is>
+      </c>
+      <c r="H120" t="inlineStr">
+        <is>
+          <t>Dungeon Bashing</t>
+        </is>
+      </c>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>Dungeon Bashing</t>
+        </is>
+      </c>
+      <c r="J120" t="n">
+        <v>1</v>
+      </c>
+      <c r="K120" t="n">
+        <v>0</v>
+      </c>
+      <c r="L120" t="n">
+        <v>2</v>
+      </c>
+      <c r="M120" t="n">
+        <v>0</v>
+      </c>
+      <c r="N120" t="n">
+        <v>1</v>
+      </c>
+      <c r="O120" t="n">
+        <v>810</v>
+      </c>
+      <c r="P120" t="inlineStr">
+        <is>
+          <t>Dungeon Bashing and Aversion</t>
+        </is>
+      </c>
+      <c r="Q120" t="inlineStr">
+        <is>
+          <t>Her Holiness Marwa Al-Ashwal</t>
+        </is>
+      </c>
+      <c r="S120" s="10" t="inlineStr">
+        <is>
+          <t>Re maximis potenti obaeratosque damnatum class effeminandos matura</t>
+        </is>
+      </c>
+      <c r="T120" t="n">
+        <v>3</v>
+      </c>
+      <c r="U120" t="n">
+        <v>3</v>
+      </c>
+      <c r="V120" t="n">
+        <v>46</v>
+      </c>
+      <c r="W120" t="n">
+        <v>1</v>
+      </c>
+      <c r="X120" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y120" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB120" t="inlineStr">
+        <is>
+          <t>Marwa Al-Ashwal</t>
+        </is>
+      </c>
+      <c r="AC120" t="inlineStr">
+        <is>
+          <t>_names_arabic_surnames</t>
+        </is>
+      </c>
+      <c r="AD120" t="inlineStr">
+        <is>
+          <t>Her Holiness</t>
+        </is>
+      </c>
+      <c r="AE120" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ120" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK120" t="inlineStr">
+        <is>
+          <t>{topic} and {noun_2}</t>
+        </is>
+      </c>
+      <c r="AL120" t="inlineStr">
+        <is>
+          <t>Dungeon Bashing</t>
+        </is>
+      </c>
+      <c r="AM120" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN120" t="n">
+        <v>185</v>
+      </c>
+      <c r="AO120" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AP120" t="n">
+        <v>625</v>
+      </c>
+      <c r="AQ120" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR120" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS120" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT120" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU120" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV120" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW120" t="inlineStr">
+        <is>
+          <t>cd8c58ef-baf5-43d9-90fc-224679b7153a</t>
+        </is>
+      </c>
+      <c r="AX120" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C121" t="n">
+        <v>3</v>
+      </c>
+      <c r="D121" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E121" t="n">
+        <v>125</v>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H121" t="inlineStr">
+        <is>
+          <t>Performance (epic poetry)</t>
+        </is>
+      </c>
+      <c r="I121" t="inlineStr">
+        <is>
+          <t>Performance (epic poetry)</t>
+        </is>
+      </c>
+      <c r="J121" t="n">
+        <v>2</v>
+      </c>
+      <c r="K121" t="n">
+        <v>0</v>
+      </c>
+      <c r="L121" t="n">
+        <v>1</v>
+      </c>
+      <c r="M121" t="n">
+        <v>0</v>
+      </c>
+      <c r="N121" t="n">
+        <v>1</v>
+      </c>
+      <c r="O121" t="n">
+        <v>2060</v>
+      </c>
+      <c r="P121" t="inlineStr">
+        <is>
+          <t>The Lusts of Asgard Haugen, on the Subject of Epic Poetry</t>
+        </is>
+      </c>
+      <c r="Q121" t="inlineStr">
+        <is>
+          <t>Thorin Jørgensdotter</t>
+        </is>
+      </c>
+      <c r="S121" s="10" t="inlineStr">
+        <is>
+          <t>The Lusts of Asgard Haugen, on the Subject of Epic Poetry</t>
+        </is>
+      </c>
+      <c r="T121" t="n">
+        <v>12</v>
+      </c>
+      <c r="U121" t="n">
+        <v>12</v>
+      </c>
+      <c r="V121" t="n">
+        <v>25</v>
+      </c>
+      <c r="W121" t="n">
+        <v>6</v>
+      </c>
+      <c r="X121" t="n">
+        <v>5</v>
+      </c>
+      <c r="Y121" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AB121" t="inlineStr">
+        <is>
+          <t>Thorin Jørgensdotter</t>
+        </is>
+      </c>
+      <c r="AC121" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_female</t>
+        </is>
+      </c>
+      <c r="AE121" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ121" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK121" t="inlineStr">
+        <is>
+          <t>{the_1} {negative_1} of {person_1}, on the Subject of {topic}</t>
+        </is>
+      </c>
+      <c r="AL121" t="inlineStr">
+        <is>
+          <t>Epic Poetry</t>
+        </is>
+      </c>
+      <c r="AM121" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN121" t="n">
+        <v>740</v>
+      </c>
+      <c r="AO121" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP121" t="n">
+        <v>1320</v>
+      </c>
+      <c r="AQ121" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR121" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS121" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT121" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU121" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV121" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW121" t="inlineStr">
+        <is>
+          <t>001f75d3-c7f7-4bb7-9d8a-8863a5456f12</t>
+        </is>
+      </c>
+      <c r="AX121" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C122" t="n">
+        <v>1</v>
+      </c>
+      <c r="D122" t="n">
+        <v>334</v>
+      </c>
+      <c r="E122" t="n">
+        <v>23</v>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H122" t="inlineStr">
+        <is>
+          <t>Art (mosaic)</t>
+        </is>
+      </c>
+      <c r="I122" t="inlineStr">
+        <is>
+          <t>Art (mosaic)</t>
+        </is>
+      </c>
+      <c r="J122" t="n">
+        <v>1</v>
+      </c>
+      <c r="K122" t="n">
+        <v>0</v>
+      </c>
+      <c r="L122" t="n">
+        <v>3</v>
+      </c>
+      <c r="M122" t="n">
+        <v>0</v>
+      </c>
+      <c r="N122" t="n">
+        <v>1</v>
+      </c>
+      <c r="O122" t="n">
+        <v>352</v>
+      </c>
+      <c r="P122" t="inlineStr">
+        <is>
+          <t>Musing on Designing Mosaics</t>
+        </is>
+      </c>
+      <c r="Q122" t="inlineStr">
+        <is>
+          <t>Hróarr Karlsson</t>
+        </is>
+      </c>
+      <c r="S122" s="10" t="inlineStr">
+        <is>
+          <t>Musing on Designing Mosaics</t>
+        </is>
+      </c>
+      <c r="T122" t="n">
+        <v>2</v>
+      </c>
+      <c r="U122" t="n">
+        <v>2</v>
+      </c>
+      <c r="V122" t="n">
+        <v>24</v>
+      </c>
+      <c r="W122" t="n">
+        <v>9</v>
+      </c>
+      <c r="X122" t="n">
+        <v>8</v>
+      </c>
+      <c r="Y122" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AB122" t="inlineStr">
+        <is>
+          <t>Hróarr Karlsson</t>
+        </is>
+      </c>
+      <c r="AC122" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_male</t>
+        </is>
+      </c>
+      <c r="AE122" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ122" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK122" t="inlineStr">
+        <is>
+          <t>{study_on} on {topic}</t>
+        </is>
+      </c>
+      <c r="AL122" t="inlineStr">
+        <is>
+          <t>Designing Mosaics</t>
+        </is>
+      </c>
+      <c r="AM122" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN122" t="n">
+        <v>131</v>
+      </c>
+      <c r="AO122" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP122" t="n">
+        <v>221</v>
+      </c>
+      <c r="AQ122" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR122" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS122" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT122" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU122" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV122" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW122" t="inlineStr">
+        <is>
+          <t>21c1c5f1-aee3-4001-b671-2552537fd913</t>
+        </is>
+      </c>
+      <c r="AX122" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C123" t="n">
+        <v>1</v>
+      </c>
+      <c r="D123" t="n">
+        <v>334</v>
+      </c>
+      <c r="E123" t="n">
+        <v>23</v>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>Classical</t>
+        </is>
+      </c>
+      <c r="H123" t="inlineStr">
+        <is>
+          <t>Military Strategy</t>
+        </is>
+      </c>
+      <c r="I123" t="inlineStr">
+        <is>
+          <t>Military Strategy</t>
+        </is>
+      </c>
+      <c r="J123" t="n">
+        <v>1</v>
+      </c>
+      <c r="K123" t="n">
+        <v>0</v>
+      </c>
+      <c r="L123" t="n">
+        <v>3</v>
+      </c>
+      <c r="M123" t="n">
+        <v>0</v>
+      </c>
+      <c r="N123" t="n">
+        <v>1</v>
+      </c>
+      <c r="O123" t="n">
+        <v>191</v>
+      </c>
+      <c r="P123" t="inlineStr">
+        <is>
+          <t>Apologia of The Temptress with emphasis upon Military Strategy</t>
+        </is>
+      </c>
+      <c r="Q123" t="inlineStr">
+        <is>
+          <t>Mister Fasolt Andersson</t>
+        </is>
+      </c>
+      <c r="S123" s="10" t="inlineStr">
+        <is>
+          <t>Vacare frumenta constiterunt propinquosque conterri gerunt posuere</t>
+        </is>
+      </c>
+      <c r="T123" t="n">
+        <v>2</v>
+      </c>
+      <c r="U123" t="n">
+        <v>2</v>
+      </c>
+      <c r="V123" t="n">
+        <v>50</v>
+      </c>
+      <c r="W123" t="n">
+        <v>90</v>
+      </c>
+      <c r="X123" t="n">
+        <v>89</v>
+      </c>
+      <c r="Y123" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AB123" t="inlineStr">
+        <is>
+          <t>Fasolt Andersson</t>
+        </is>
+      </c>
+      <c r="AC123" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_male</t>
+        </is>
+      </c>
+      <c r="AD123" t="inlineStr">
+        <is>
+          <t>Mister</t>
+        </is>
+      </c>
+      <c r="AE123" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ123" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK123" t="inlineStr">
+        <is>
+          <t>{biography_starter} of {person_evil} with emphasis upon {topic}</t>
+        </is>
+      </c>
+      <c r="AL123" t="inlineStr">
+        <is>
+          <t>Military Strategy</t>
+        </is>
+      </c>
+      <c r="AM123" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN123" t="n">
+        <v>124</v>
+      </c>
+      <c r="AO123" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP123" t="n">
+        <v>67</v>
+      </c>
+      <c r="AQ123" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR123" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS123" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT123" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU123" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV123" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW123" t="inlineStr">
+        <is>
+          <t>3e2f0970-b506-47f8-9b3b-218c4f152bf2</t>
+        </is>
+      </c>
+      <c r="AX123" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>Scroll</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C124" t="n">
+        <v>12</v>
+      </c>
+      <c r="D124" t="n">
+        <v>3000</v>
+      </c>
+      <c r="E124" t="n">
+        <v>204</v>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>Ancient</t>
+        </is>
+      </c>
+      <c r="H124" t="inlineStr">
+        <is>
+          <t>Knowledge (architecture)</t>
+        </is>
+      </c>
+      <c r="I124" t="inlineStr">
+        <is>
+          <t>Knowledge (architecture)</t>
+        </is>
+      </c>
+      <c r="J124" t="n">
+        <v>3</v>
+      </c>
+      <c r="K124" t="n">
+        <v>0</v>
+      </c>
+      <c r="L124" t="n">
+        <v>1</v>
+      </c>
+      <c r="M124" t="n">
+        <v>0</v>
+      </c>
+      <c r="N124" t="n">
+        <v>1</v>
+      </c>
+      <c r="O124" t="n">
+        <v>13080</v>
+      </c>
+      <c r="P124" t="inlineStr">
+        <is>
+          <t>The Sufferings of Rahal the Sunsoul and Architecture</t>
+        </is>
+      </c>
+      <c r="Q124" t="inlineStr">
+        <is>
+          <t>Magister Hamza Dziri</t>
+        </is>
+      </c>
+      <c r="S124" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">𐎸𐎱𐎭𐎠 𐎬𐎤𐏂𐎸𐎽 𐎠 𐎢𐎮𐎬𐎬𐎮𐎣𐎮 𐎵𐎤𐎧𐎨𐎢𐎸𐎫𐎠 𐏂𐎨𐎭𐎢𐎨𐎣𐎸𐎭𐏂 </t>
+        </is>
+      </c>
+      <c r="T124" t="n">
+        <v>17</v>
+      </c>
+      <c r="U124" t="n">
+        <v>17</v>
+      </c>
+      <c r="V124" t="n">
+        <v>1748</v>
+      </c>
+      <c r="W124" t="n">
+        <v>1</v>
+      </c>
+      <c r="X124" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y124" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB124" t="inlineStr">
+        <is>
+          <t>Hamza Dziri</t>
+        </is>
+      </c>
+      <c r="AC124" t="inlineStr">
+        <is>
+          <t>_names_arabic_surnames</t>
+        </is>
+      </c>
+      <c r="AD124" t="inlineStr">
+        <is>
+          <t>Magister</t>
+        </is>
+      </c>
+      <c r="AE124" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ124" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK124" t="inlineStr">
+        <is>
+          <t>{biography_starter} of {person_famous} and {topic}</t>
+        </is>
+      </c>
+      <c r="AL124" t="inlineStr">
+        <is>
+          <t>Architecture</t>
+        </is>
+      </c>
+      <c r="AM124" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="AN124" t="n">
+        <v>1080</v>
+      </c>
+      <c r="AO124" t="n">
+        <v>4</v>
+      </c>
+      <c r="AP124" t="n">
+        <v>12000</v>
+      </c>
+      <c r="AQ124" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR124" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS124" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT124" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU124" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV124" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW124" t="inlineStr">
+        <is>
+          <t>29d4fa75-53b3-4a94-babf-69d6bede6606</t>
+        </is>
+      </c>
+      <c r="AX124" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C125" t="n">
+        <v>3</v>
+      </c>
+      <c r="D125" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E125" t="n">
+        <v>125</v>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H125" t="inlineStr">
+        <is>
+          <t>Craft (leatherworking)</t>
+        </is>
+      </c>
+      <c r="I125" t="inlineStr">
+        <is>
+          <t>Craft (leatherworking)</t>
+        </is>
+      </c>
+      <c r="J125" t="n">
+        <v>2</v>
+      </c>
+      <c r="K125" t="n">
+        <v>0</v>
+      </c>
+      <c r="L125" t="n">
+        <v>1</v>
+      </c>
+      <c r="M125" t="n">
+        <v>0</v>
+      </c>
+      <c r="N125" t="n">
+        <v>1</v>
+      </c>
+      <c r="O125" t="n">
+        <v>2060</v>
+      </c>
+      <c r="P125" t="inlineStr">
+        <is>
+          <t>Journeying to Leatherworking: a Jovial Wish</t>
+        </is>
+      </c>
+      <c r="Q125" t="inlineStr">
+        <is>
+          <t>Pascale Illouz</t>
+        </is>
+      </c>
+      <c r="S125" s="10" t="inlineStr">
+        <is>
+          <t>Journeying to Leatherworking: a Jovial Wish</t>
+        </is>
+      </c>
+      <c r="T125" t="n">
+        <v>12</v>
+      </c>
+      <c r="U125" t="n">
+        <v>12</v>
+      </c>
+      <c r="V125" t="n">
+        <v>29</v>
+      </c>
+      <c r="W125" t="n">
+        <v>13</v>
+      </c>
+      <c r="X125" t="n">
+        <v>12</v>
+      </c>
+      <c r="Y125" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AB125" t="inlineStr">
+        <is>
+          <t>Pascale Illouz</t>
+        </is>
+      </c>
+      <c r="AC125" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AE125" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ125" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK125" t="inlineStr">
+        <is>
+          <t>{verbing} {topic}: a {adjective_1} {noun_1}</t>
+        </is>
+      </c>
+      <c r="AL125" t="inlineStr">
+        <is>
+          <t>Leatherworking</t>
+        </is>
+      </c>
+      <c r="AM125" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN125" t="n">
+        <v>740</v>
+      </c>
+      <c r="AO125" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP125" t="n">
+        <v>1320</v>
+      </c>
+      <c r="AQ125" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR125" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS125" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT125" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU125" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV125" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW125" t="inlineStr">
+        <is>
+          <t>3b12a247-b836-4229-8acc-55a0f82247e8</t>
+        </is>
+      </c>
+      <c r="AX125" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C126" t="n">
+        <v>2</v>
+      </c>
+      <c r="D126" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E126" t="n">
+        <v>63</v>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H126" t="inlineStr">
+        <is>
+          <t>Blind Fighting</t>
+        </is>
+      </c>
+      <c r="I126" t="inlineStr">
+        <is>
+          <t>Blind Fighting</t>
+        </is>
+      </c>
+      <c r="J126" t="n">
+        <v>2</v>
+      </c>
+      <c r="K126" t="n">
+        <v>0</v>
+      </c>
+      <c r="L126" t="n">
+        <v>2</v>
+      </c>
+      <c r="M126" t="n">
+        <v>0</v>
+      </c>
+      <c r="N126" t="n">
+        <v>1</v>
+      </c>
+      <c r="O126" t="n">
+        <v>490</v>
+      </c>
+      <c r="P126" t="inlineStr">
+        <is>
+          <t>Experiences of Rahal the Sunsoul and Blind Fighting</t>
+        </is>
+      </c>
+      <c r="Q126" t="inlineStr">
+        <is>
+          <t>Arwa Kaddouri</t>
+        </is>
+      </c>
+      <c r="S126" s="10" t="inlineStr">
+        <is>
+          <t>Experiences of Rahal the Sunsoul and Blind Fighting</t>
+        </is>
+      </c>
+      <c r="T126" t="n">
+        <v>6</v>
+      </c>
+      <c r="U126" t="n">
+        <v>6</v>
+      </c>
+      <c r="V126" t="n">
+        <v>82</v>
+      </c>
+      <c r="W126" t="n">
+        <v>138</v>
+      </c>
+      <c r="X126" t="n">
+        <v>137</v>
+      </c>
+      <c r="Y126" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="AB126" t="inlineStr">
+        <is>
+          <t>Arwa Kaddouri</t>
+        </is>
+      </c>
+      <c r="AC126" t="inlineStr">
+        <is>
+          <t>_names_arabic_surnames</t>
+        </is>
+      </c>
+      <c r="AE126" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ126" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK126" t="inlineStr">
+        <is>
+          <t>{biography_starter} of {person_famous} and {topic}</t>
+        </is>
+      </c>
+      <c r="AL126" t="inlineStr">
+        <is>
+          <t>Blind Fighting</t>
+        </is>
+      </c>
+      <c r="AM126" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN126" t="n">
+        <v>390</v>
+      </c>
+      <c r="AO126" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP126" t="n">
+        <v>100</v>
+      </c>
+      <c r="AQ126" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR126" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS126" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT126" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU126" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV126" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW126" t="inlineStr">
+        <is>
+          <t>cf894ce3-83dd-4851-870f-9d44a828e75a</t>
+        </is>
+      </c>
+      <c r="AX126" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C127" t="n">
+        <v>2</v>
+      </c>
+      <c r="D127" t="n">
+        <v>1334</v>
+      </c>
+      <c r="E127" t="n">
+        <v>84</v>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H127" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
+      <c r="I127" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
+      <c r="J127" t="n">
+        <v>1</v>
+      </c>
+      <c r="K127" t="n">
+        <v>0</v>
+      </c>
+      <c r="L127" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="M127" t="n">
+        <v>0</v>
+      </c>
+      <c r="N127" t="n">
+        <v>1</v>
+      </c>
+      <c r="O127" t="n">
+        <v>855</v>
+      </c>
+      <c r="P127" t="inlineStr">
+        <is>
+          <t>Engineering and Cowardice</t>
+        </is>
+      </c>
+      <c r="Q127" t="inlineStr">
+        <is>
+          <t>Aurélia Duret</t>
+        </is>
+      </c>
+      <c r="S127" s="10" t="inlineStr">
+        <is>
+          <t>Engineering and Cowardice</t>
+        </is>
+      </c>
+      <c r="T127" t="n">
+        <v>8</v>
+      </c>
+      <c r="U127" t="n">
+        <v>8</v>
+      </c>
+      <c r="V127" t="n">
+        <v>48</v>
+      </c>
+      <c r="W127" t="n">
+        <v>42</v>
+      </c>
+      <c r="X127" t="n">
+        <v>41</v>
+      </c>
+      <c r="Y127" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="AB127" t="inlineStr">
+        <is>
+          <t>Aurélia Duret</t>
+        </is>
+      </c>
+      <c r="AC127" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AE127" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ127" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK127" t="inlineStr">
+        <is>
+          <t>{topic} and {noun_2}</t>
+        </is>
+      </c>
+      <c r="AL127" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
+      <c r="AM127" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN127" t="n">
+        <v>521</v>
+      </c>
+      <c r="AO127" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP127" t="n">
+        <v>334</v>
+      </c>
+      <c r="AQ127" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR127" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS127" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT127" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU127" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV127" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW127" t="inlineStr">
+        <is>
+          <t>00fa4195-c42e-4719-981e-a363135ef1f8</t>
+        </is>
+      </c>
+      <c r="AX127" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C128" t="n">
+        <v>3</v>
+      </c>
+      <c r="D128" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E128" t="n">
+        <v>125</v>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>Regional</t>
+        </is>
+      </c>
+      <c r="H128" t="inlineStr">
+        <is>
+          <t>Performance (dancing)</t>
+        </is>
+      </c>
+      <c r="I128" t="inlineStr">
+        <is>
+          <t>Performance (dancing)</t>
+        </is>
+      </c>
+      <c r="J128" t="n">
+        <v>2</v>
+      </c>
+      <c r="K128" t="n">
+        <v>0</v>
+      </c>
+      <c r="L128" t="n">
+        <v>1</v>
+      </c>
+      <c r="M128" t="n">
+        <v>0</v>
+      </c>
+      <c r="N128" t="n">
+        <v>1</v>
+      </c>
+      <c r="O128" t="n">
+        <v>780</v>
+      </c>
+      <c r="P128" t="inlineStr">
+        <is>
+          <t>So Thou Believest Thou Canst Dance?, a Delicate Pilgrimage</t>
+        </is>
+      </c>
+      <c r="Q128" t="inlineStr">
+        <is>
+          <t>Her Holiness Mardochée Bechard</t>
+        </is>
+      </c>
+      <c r="S128" s="10" t="inlineStr">
+        <is>
+          <t>Ὀρθή ζ΄ βάσει δοθέντι μὲν κη΄ δοθεῖσαν ἐπίπεδον γραμμαὶ τριγώνων δύο περιέχουσαι παράλληλοί ἐκτὸς</t>
+        </is>
+      </c>
+      <c r="T128" t="n">
+        <v>12</v>
+      </c>
+      <c r="U128" t="n">
+        <v>12</v>
+      </c>
+      <c r="V128" t="n">
+        <v>47</v>
+      </c>
+      <c r="W128" t="n">
+        <v>601</v>
+      </c>
+      <c r="X128" t="n">
+        <v>600</v>
+      </c>
+      <c r="Y128" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AB128" t="inlineStr">
+        <is>
+          <t>Mardochée Bechard</t>
+        </is>
+      </c>
+      <c r="AC128" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AD128" t="inlineStr">
+        <is>
+          <t>Her Holiness</t>
+        </is>
+      </c>
+      <c r="AE128" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ128" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK128" t="inlineStr">
+        <is>
+          <t>{topic}, a {adjective_1} {noun_1}</t>
+        </is>
+      </c>
+      <c r="AL128" t="inlineStr">
+        <is>
+          <t>So Thou Believest Thou Canst Dance?</t>
+        </is>
+      </c>
+      <c r="AM128" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN128" t="n">
+        <v>740</v>
+      </c>
+      <c r="AO128" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP128" t="n">
+        <v>40</v>
+      </c>
+      <c r="AQ128" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR128" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS128" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT128" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU128" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV128" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW128" t="inlineStr">
+        <is>
+          <t>bced3b13-f0ba-4100-8170-57dae9cc9cf1</t>
+        </is>
+      </c>
+      <c r="AX128" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C129" t="n">
+        <v>1</v>
+      </c>
+      <c r="D129" t="n">
+        <v>500</v>
+      </c>
+      <c r="E129" t="n">
+        <v>32</v>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>Classical</t>
+        </is>
+      </c>
+      <c r="H129" t="inlineStr">
+        <is>
+          <t>Eavesdropping</t>
+        </is>
+      </c>
+      <c r="I129" t="inlineStr">
+        <is>
+          <t>Eavesdropping</t>
+        </is>
+      </c>
+      <c r="J129" t="n">
+        <v>1</v>
+      </c>
+      <c r="K129" t="n">
+        <v>0</v>
+      </c>
+      <c r="L129" t="n">
+        <v>2</v>
+      </c>
+      <c r="M129" t="n">
+        <v>0</v>
+      </c>
+      <c r="N129" t="n">
+        <v>1</v>
+      </c>
+      <c r="O129" t="n">
+        <v>392</v>
+      </c>
+      <c r="P129" t="inlineStr">
+        <is>
+          <t>Antiquities of Lira the Flamekeeper and Eavesdropping</t>
+        </is>
+      </c>
+      <c r="Q129" t="inlineStr">
+        <is>
+          <t>Joffrey Fremont</t>
+        </is>
+      </c>
+      <c r="S129" s="10" t="inlineStr">
+        <is>
+          <t>Intervallo quosque utebatur cassium convenerant quidam concilium isdem minime solis vicissent didicisse</t>
+        </is>
+      </c>
+      <c r="T129" t="n">
+        <v>3</v>
+      </c>
+      <c r="U129" t="n">
+        <v>3</v>
+      </c>
+      <c r="V129" t="n">
+        <v>396</v>
+      </c>
+      <c r="W129" t="n">
+        <v>12</v>
+      </c>
+      <c r="X129" t="n">
+        <v>11</v>
+      </c>
+      <c r="Y129" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AB129" t="inlineStr">
+        <is>
+          <t>Joffrey Fremont</t>
+        </is>
+      </c>
+      <c r="AC129" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AE129" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ129" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK129" t="inlineStr">
+        <is>
+          <t>{biography_starter} of {person_famous} and {topic}</t>
+        </is>
+      </c>
+      <c r="AL129" t="inlineStr">
+        <is>
+          <t>Eavesdropping</t>
+        </is>
+      </c>
+      <c r="AM129" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN129" t="n">
+        <v>185</v>
+      </c>
+      <c r="AO129" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AP129" t="n">
+        <v>207</v>
+      </c>
+      <c r="AQ129" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR129" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS129" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT129" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU129" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV129" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW129" t="inlineStr">
+        <is>
+          <t>55b2f579-be8a-440e-bc1f-a3284be0357e</t>
+        </is>
+      </c>
+      <c r="AX129" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C130" t="n">
+        <v>1</v>
+      </c>
+      <c r="D130" t="n">
+        <v>500</v>
+      </c>
+      <c r="E130" t="n">
+        <v>32</v>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>Regional</t>
+        </is>
+      </c>
+      <c r="H130" t="inlineStr">
+        <is>
+          <t>Esoteric: Alchemy</t>
+        </is>
+      </c>
+      <c r="I130" t="inlineStr">
+        <is>
+          <t>Familiar</t>
+        </is>
+      </c>
+      <c r="J130" t="n">
+        <v>1</v>
+      </c>
+      <c r="K130" t="n">
+        <v>1</v>
+      </c>
+      <c r="L130" t="n">
+        <v>2</v>
+      </c>
+      <c r="M130" t="n">
+        <v>2</v>
+      </c>
+      <c r="N130" t="n">
+        <v>1</v>
+      </c>
+      <c r="O130" t="n">
+        <v>5820</v>
+      </c>
+      <c r="P130" t="inlineStr">
+        <is>
+          <t>The Damnable Gluttony of Priscilla Curtia, on the Subject of Familiar</t>
+        </is>
+      </c>
+      <c r="Q130" t="inlineStr">
+        <is>
+          <t>The Divine Halim Mahjoub</t>
+        </is>
+      </c>
+      <c r="S130" s="10" t="inlineStr">
+        <is>
+          <t>Ἀφαιρεθῇ περιεχομένην μείζων ἔσται πλευραί ἔχει καὶ αὐταῖς χωρίον ὀρθὴ μείζονές κείμεναι ἰσόπλευρον</t>
+        </is>
+      </c>
+      <c r="T130" t="n">
+        <v>3</v>
+      </c>
+      <c r="U130" t="n">
+        <v>3</v>
+      </c>
+      <c r="V130" t="n">
+        <v>14</v>
+      </c>
+      <c r="W130" t="n">
+        <v>1</v>
+      </c>
+      <c r="X130" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y130" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB130" t="inlineStr">
+        <is>
+          <t>Halim Mahjoub</t>
+        </is>
+      </c>
+      <c r="AC130" t="inlineStr">
+        <is>
+          <t>_names_arabic_surnames</t>
+        </is>
+      </c>
+      <c r="AD130" t="inlineStr">
+        <is>
+          <t>The Divine</t>
+        </is>
+      </c>
+      <c r="AE130" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ130" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK130" t="inlineStr">
+        <is>
+          <t>{the_1} {negative_1} of {person_1}, on the Subject of {topic}</t>
+        </is>
+      </c>
+      <c r="AL130" t="inlineStr">
+        <is>
+          <t>Familiar</t>
+        </is>
+      </c>
+      <c r="AM130" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN130" t="n">
+        <v>195</v>
+      </c>
+      <c r="AO130" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AP130" t="n">
+        <v>625</v>
+      </c>
+      <c r="AQ130" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AR130" t="n">
+        <v>5000</v>
+      </c>
+      <c r="AS130" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT130" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU130" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV130" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW130" t="inlineStr">
+        <is>
+          <t>13d749d1-a386-4afc-8b1f-2972d8f38ccc</t>
+        </is>
+      </c>
+      <c r="AX130" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C131" t="n">
+        <v>3</v>
+      </c>
+      <c r="D131" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E131" t="n">
+        <v>125</v>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>Classical</t>
+        </is>
+      </c>
+      <c r="H131" t="inlineStr">
+        <is>
+          <t>Battle Magic</t>
+        </is>
+      </c>
+      <c r="I131" t="inlineStr">
+        <is>
+          <t>Battle Magic</t>
+        </is>
+      </c>
+      <c r="J131" t="n">
+        <v>4</v>
+      </c>
+      <c r="K131" t="n">
+        <v>0</v>
+      </c>
+      <c r="L131" t="n">
+        <v>2</v>
+      </c>
+      <c r="M131" t="n">
+        <v>0</v>
+      </c>
+      <c r="N131" t="n">
+        <v>1</v>
+      </c>
+      <c r="O131" t="n">
+        <v>980</v>
+      </c>
+      <c r="P131" t="inlineStr">
+        <is>
+          <t>Condemnation of Bahruz the Prophet and Sorcerie and the Field of Battle</t>
+        </is>
+      </c>
+      <c r="Q131" t="inlineStr">
+        <is>
+          <t>Timothée Périer the Weak</t>
+        </is>
+      </c>
+      <c r="S131" s="10" t="inlineStr">
+        <is>
+          <t>Perfacile santonos ii catenis ultro praeerant uti deducat committeret duis oppidum dicunt</t>
+        </is>
+      </c>
+      <c r="T131" t="n">
+        <v>12</v>
+      </c>
+      <c r="U131" t="n">
+        <v>12</v>
+      </c>
+      <c r="V131" t="n">
+        <v>30</v>
+      </c>
+      <c r="W131" t="n">
+        <v>708</v>
+      </c>
+      <c r="X131" t="n">
+        <v>707</v>
+      </c>
+      <c r="Y131" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AA131" t="inlineStr">
+        <is>
+          <t>the Weak</t>
+        </is>
+      </c>
+      <c r="AB131" t="inlineStr">
+        <is>
+          <t>Timothée Périer</t>
+        </is>
+      </c>
+      <c r="AC131" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AE131" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ131" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK131" t="inlineStr">
+        <is>
+          <t>{biography_starter} of {person_famous} and {topic}</t>
+        </is>
+      </c>
+      <c r="AL131" t="inlineStr">
+        <is>
+          <t>Sorcerie and the Field of Battle</t>
+        </is>
+      </c>
+      <c r="AM131" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN131" t="n">
+        <v>780</v>
+      </c>
+      <c r="AO131" t="n">
+        <v>10</v>
+      </c>
+      <c r="AP131" t="n">
+        <v>200</v>
+      </c>
+      <c r="AQ131" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR131" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS131" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT131" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU131" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV131" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW131" t="inlineStr">
+        <is>
+          <t>1939e5e5-4f0f-4147-818f-166247fde7ab</t>
+        </is>
+      </c>
+      <c r="AX131" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
book batch and book horde both work; saving prefs or restoring or discarding all work in main fantasy_books.py code
</commit_message>
<xml_diff>
--- a/books_spreadsheet_out.xlsx
+++ b/books_spreadsheet_out.xlsx
@@ -466,7 +466,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AX231"/>
+  <dimension ref="A1:AX252"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
       <selection activeCell="S2" sqref="S2"/>
@@ -37279,6 +37279,3383 @@
         </is>
       </c>
     </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>Silver Foil</t>
+        </is>
+      </c>
+      <c r="C232" t="n">
+        <v>1</v>
+      </c>
+      <c r="D232" t="n">
+        <v>500</v>
+      </c>
+      <c r="E232" t="n">
+        <v>77</v>
+      </c>
+      <c r="F232" t="inlineStr">
+        <is>
+          <t>Regional</t>
+        </is>
+      </c>
+      <c r="H232" t="inlineStr">
+        <is>
+          <t>Profession (banker)</t>
+        </is>
+      </c>
+      <c r="I232" t="inlineStr">
+        <is>
+          <t>Profession (banker)</t>
+        </is>
+      </c>
+      <c r="J232" t="n">
+        <v>2</v>
+      </c>
+      <c r="K232" t="n">
+        <v>0</v>
+      </c>
+      <c r="L232" t="n">
+        <v>4</v>
+      </c>
+      <c r="M232" t="n">
+        <v>0</v>
+      </c>
+      <c r="N232" t="n">
+        <v>1</v>
+      </c>
+      <c r="O232" t="n">
+        <v>925</v>
+      </c>
+      <c r="P232" t="inlineStr">
+        <is>
+          <t>Embarking Banking: a Enraptured Committal</t>
+        </is>
+      </c>
+      <c r="Q232" t="inlineStr">
+        <is>
+          <t>Chester Becker</t>
+        </is>
+      </c>
+      <c r="S232" s="10" t="inlineStr">
+        <is>
+          <t>Ἐκβαλλομένας βάσιν ἔτι πλευρᾷ πεπερασμένης δυσὶ περὶ κέντρῳ τινι τοῦ</t>
+        </is>
+      </c>
+      <c r="T232" t="n">
+        <v>3</v>
+      </c>
+      <c r="U232" t="n">
+        <v>3</v>
+      </c>
+      <c r="V232" t="n">
+        <v>37</v>
+      </c>
+      <c r="W232" t="n">
+        <v>986</v>
+      </c>
+      <c r="X232" t="n">
+        <v>985</v>
+      </c>
+      <c r="Y232" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AB232" t="inlineStr">
+        <is>
+          <t>Chester Becker</t>
+        </is>
+      </c>
+      <c r="AC232" t="inlineStr">
+        <is>
+          <t>_names_english_surnames</t>
+        </is>
+      </c>
+      <c r="AE232" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ232" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="AK232" t="inlineStr">
+        <is>
+          <t>{verbing} {topic}: a {adjective_1} {noun_1}</t>
+        </is>
+      </c>
+      <c r="AL232" t="inlineStr">
+        <is>
+          <t>Banking</t>
+        </is>
+      </c>
+      <c r="AM232" t="n">
+        <v>1.81</v>
+      </c>
+      <c r="AN232" t="n">
+        <v>905</v>
+      </c>
+      <c r="AO232" t="n">
+        <v>4</v>
+      </c>
+      <c r="AP232" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ232" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR232" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS232" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT232" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU232" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV232" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW232" t="inlineStr">
+        <is>
+          <t>a7fb40bf-67ab-4b60-ab66-ffe05111e4d1</t>
+        </is>
+      </c>
+      <c r="AX232" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C233" t="n">
+        <v>2</v>
+      </c>
+      <c r="D233" t="n">
+        <v>1334</v>
+      </c>
+      <c r="E233" t="n">
+        <v>84</v>
+      </c>
+      <c r="F233" t="inlineStr">
+        <is>
+          <t>Elvish</t>
+        </is>
+      </c>
+      <c r="H233" t="inlineStr">
+        <is>
+          <t>Loremastery</t>
+        </is>
+      </c>
+      <c r="I233" t="inlineStr">
+        <is>
+          <t>Loremastery</t>
+        </is>
+      </c>
+      <c r="J233" t="n">
+        <v>1</v>
+      </c>
+      <c r="K233" t="n">
+        <v>0</v>
+      </c>
+      <c r="L233" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="M233" t="n">
+        <v>0</v>
+      </c>
+      <c r="N233" t="n">
+        <v>1</v>
+      </c>
+      <c r="O233" t="n">
+        <v>828</v>
+      </c>
+      <c r="P233" t="inlineStr">
+        <is>
+          <t>Loremastery and Despair</t>
+        </is>
+      </c>
+      <c r="Q233" t="inlineStr">
+        <is>
+          <t>Hallbjǫrn Johansen the Supine</t>
+        </is>
+      </c>
+      <c r="S233" s="12" t="inlineStr">
+        <is>
+          <t>Linnyd uidefnin raug</t>
+        </is>
+      </c>
+      <c r="T233" t="n">
+        <v>8</v>
+      </c>
+      <c r="U233" t="n">
+        <v>8</v>
+      </c>
+      <c r="V233" t="n">
+        <v>93</v>
+      </c>
+      <c r="W233" t="n">
+        <v>47</v>
+      </c>
+      <c r="X233" t="n">
+        <v>46</v>
+      </c>
+      <c r="Y233" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="AA233" t="inlineStr">
+        <is>
+          <t>the Supine</t>
+        </is>
+      </c>
+      <c r="AB233" t="inlineStr">
+        <is>
+          <t>Hallbjǫrn Johansen</t>
+        </is>
+      </c>
+      <c r="AC233" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_male</t>
+        </is>
+      </c>
+      <c r="AE233" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ233" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK233" t="inlineStr">
+        <is>
+          <t>{topic} and {noun_2}</t>
+        </is>
+      </c>
+      <c r="AL233" t="inlineStr">
+        <is>
+          <t>Loremastery</t>
+        </is>
+      </c>
+      <c r="AM233" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN233" t="n">
+        <v>494</v>
+      </c>
+      <c r="AO233" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP233" t="n">
+        <v>334</v>
+      </c>
+      <c r="AQ233" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR233" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS233" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT233" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU233" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV233" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW233" t="inlineStr">
+        <is>
+          <t>90e67af1-09fd-4adb-816c-3b92096b3b5a</t>
+        </is>
+      </c>
+      <c r="AX233" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C234" t="n">
+        <v>1</v>
+      </c>
+      <c r="D234" t="n">
+        <v>500</v>
+      </c>
+      <c r="E234" t="n">
+        <v>32</v>
+      </c>
+      <c r="F234" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H234" t="inlineStr">
+        <is>
+          <t>Profession (torturer)</t>
+        </is>
+      </c>
+      <c r="I234" t="inlineStr">
+        <is>
+          <t>Profession (torturer)</t>
+        </is>
+      </c>
+      <c r="J234" t="n">
+        <v>1</v>
+      </c>
+      <c r="K234" t="n">
+        <v>0</v>
+      </c>
+      <c r="L234" t="n">
+        <v>2</v>
+      </c>
+      <c r="M234" t="n">
+        <v>0</v>
+      </c>
+      <c r="N234" t="n">
+        <v>1</v>
+      </c>
+      <c r="O234" t="n">
+        <v>392</v>
+      </c>
+      <c r="P234" t="inlineStr">
+        <is>
+          <t>The Regrettable Evildoing of The Temptress and Interogating</t>
+        </is>
+      </c>
+      <c r="Q234" t="inlineStr">
+        <is>
+          <t>Roger Sørensen the Thoughtful</t>
+        </is>
+      </c>
+      <c r="S234" s="10" t="inlineStr">
+        <is>
+          <t>The Regrettable Evildoing of The Temptress and Interogating</t>
+        </is>
+      </c>
+      <c r="T234" t="n">
+        <v>3</v>
+      </c>
+      <c r="U234" t="n">
+        <v>3</v>
+      </c>
+      <c r="V234" t="n">
+        <v>48</v>
+      </c>
+      <c r="W234" t="n">
+        <v>16</v>
+      </c>
+      <c r="X234" t="n">
+        <v>15</v>
+      </c>
+      <c r="Y234" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AA234" t="inlineStr">
+        <is>
+          <t>the Thoughtful</t>
+        </is>
+      </c>
+      <c r="AB234" t="inlineStr">
+        <is>
+          <t>Roger Sørensen</t>
+        </is>
+      </c>
+      <c r="AC234" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_male</t>
+        </is>
+      </c>
+      <c r="AE234" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ234" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK234" t="inlineStr">
+        <is>
+          <t>{the_1} {negative_1} of {person_evil} and {topic}</t>
+        </is>
+      </c>
+      <c r="AL234" t="inlineStr">
+        <is>
+          <t>Interogating</t>
+        </is>
+      </c>
+      <c r="AM234" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN234" t="n">
+        <v>185</v>
+      </c>
+      <c r="AO234" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AP234" t="n">
+        <v>207</v>
+      </c>
+      <c r="AQ234" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR234" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS234" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT234" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU234" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV234" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW234" t="inlineStr">
+        <is>
+          <t>0f37a3b0-32d7-4013-8eb7-f67309bdf967</t>
+        </is>
+      </c>
+      <c r="AX234" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C235" t="n">
+        <v>2</v>
+      </c>
+      <c r="D235" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E235" t="n">
+        <v>63</v>
+      </c>
+      <c r="F235" t="inlineStr">
+        <is>
+          <t>Ancient</t>
+        </is>
+      </c>
+      <c r="H235" t="inlineStr">
+        <is>
+          <t>Labor (domestic)</t>
+        </is>
+      </c>
+      <c r="I235" t="inlineStr">
+        <is>
+          <t>Labor (domestic)</t>
+        </is>
+      </c>
+      <c r="J235" t="n">
+        <v>3</v>
+      </c>
+      <c r="K235" t="n">
+        <v>0</v>
+      </c>
+      <c r="L235" t="n">
+        <v>3</v>
+      </c>
+      <c r="M235" t="n">
+        <v>0</v>
+      </c>
+      <c r="N235" t="n">
+        <v>1</v>
+      </c>
+      <c r="O235" t="n">
+        <v>1370</v>
+      </c>
+      <c r="P235" t="inlineStr">
+        <is>
+          <t>Condemnation of The Dark Lord with emphasis upon Serving the Great and Good</t>
+        </is>
+      </c>
+      <c r="Q235" t="inlineStr">
+        <is>
+          <t>Loulia Murad</t>
+        </is>
+      </c>
+      <c r="S235" s="10" t="inlineStr">
+        <is>
+          <t>𐎽𐎮𐎫𐎫𐎨𐎢𐎨𐏂𐎸𐎣𐎨𐎭 𐎱𐎧𐎮𐎭𐎢𐎸𐎽 𐎢𐎮𐎭𐎽𐎤𐎢𐏂𐎤𐏂𐎸𐎱 𐎫𐎤𐎮 𐎠𐎭𐏂</t>
+        </is>
+      </c>
+      <c r="T235" t="n">
+        <v>6</v>
+      </c>
+      <c r="U235" t="n">
+        <v>6</v>
+      </c>
+      <c r="V235" t="n">
+        <v>11</v>
+      </c>
+      <c r="W235" t="n">
+        <v>39</v>
+      </c>
+      <c r="X235" t="n">
+        <v>38</v>
+      </c>
+      <c r="Y235" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="AB235" t="inlineStr">
+        <is>
+          <t>Loulia Murad</t>
+        </is>
+      </c>
+      <c r="AC235" t="inlineStr">
+        <is>
+          <t>_names_arabic_surnames</t>
+        </is>
+      </c>
+      <c r="AE235" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ235" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK235" t="inlineStr">
+        <is>
+          <t>{biography_starter} of {person_evil} with emphasis upon {topic}</t>
+        </is>
+      </c>
+      <c r="AL235" t="inlineStr">
+        <is>
+          <t>Serving the Great and Good</t>
+        </is>
+      </c>
+      <c r="AM235" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN235" t="n">
+        <v>370</v>
+      </c>
+      <c r="AO235" t="n">
+        <v>4</v>
+      </c>
+      <c r="AP235" t="n">
+        <v>1000</v>
+      </c>
+      <c r="AQ235" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR235" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS235" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT235" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU235" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV235" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW235" t="inlineStr">
+        <is>
+          <t>554c562a-1676-4e78-89aa-a96feff4f0e0</t>
+        </is>
+      </c>
+      <c r="AX235" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>Scroll</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C236" t="n">
+        <v>4</v>
+      </c>
+      <c r="D236" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E236" t="n">
+        <v>68</v>
+      </c>
+      <c r="F236" t="inlineStr">
+        <is>
+          <t>Elvish</t>
+        </is>
+      </c>
+      <c r="H236" t="inlineStr">
+        <is>
+          <t>Caving</t>
+        </is>
+      </c>
+      <c r="I236" t="inlineStr">
+        <is>
+          <t>Caving</t>
+        </is>
+      </c>
+      <c r="J236" t="n">
+        <v>1</v>
+      </c>
+      <c r="K236" t="n">
+        <v>0</v>
+      </c>
+      <c r="L236" t="n">
+        <v>1</v>
+      </c>
+      <c r="M236" t="n">
+        <v>0</v>
+      </c>
+      <c r="N236" t="n">
+        <v>1</v>
+      </c>
+      <c r="O236" t="n">
+        <v>610</v>
+      </c>
+      <c r="P236" t="inlineStr">
+        <is>
+          <t>Reasonings in Caving</t>
+        </is>
+      </c>
+      <c r="Q236" t="inlineStr">
+        <is>
+          <t>Juliette Leclère</t>
+        </is>
+      </c>
+      <c r="S236" s="12" t="inlineStr">
+        <is>
+          <t>Rhysc mîr thŷr arwen gwest bedhryn flaid galadhremmin</t>
+        </is>
+      </c>
+      <c r="T236" t="n">
+        <v>6</v>
+      </c>
+      <c r="U236" t="n">
+        <v>6</v>
+      </c>
+      <c r="V236" t="n">
+        <v>336</v>
+      </c>
+      <c r="W236" t="n">
+        <v>31</v>
+      </c>
+      <c r="X236" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y236" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="AB236" t="inlineStr">
+        <is>
+          <t>Juliette Leclère</t>
+        </is>
+      </c>
+      <c r="AC236" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AE236" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ236" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK236" t="inlineStr">
+        <is>
+          <t>{study_in} in {topic}</t>
+        </is>
+      </c>
+      <c r="AL236" t="inlineStr">
+        <is>
+          <t>Caving</t>
+        </is>
+      </c>
+      <c r="AM236" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="AN236" t="n">
+        <v>360</v>
+      </c>
+      <c r="AO236" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP236" t="n">
+        <v>250</v>
+      </c>
+      <c r="AQ236" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR236" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS236" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT236" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU236" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV236" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW236" t="inlineStr">
+        <is>
+          <t>d225c47c-f372-42ef-a267-ed6d1f679224</t>
+        </is>
+      </c>
+      <c r="AX236" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C237" t="n">
+        <v>1</v>
+      </c>
+      <c r="D237" t="n">
+        <v>750</v>
+      </c>
+      <c r="E237" t="n">
+        <v>47</v>
+      </c>
+      <c r="F237" t="inlineStr">
+        <is>
+          <t>Ancient</t>
+        </is>
+      </c>
+      <c r="H237" t="inlineStr">
+        <is>
+          <t>Blind Fighting</t>
+        </is>
+      </c>
+      <c r="I237" t="inlineStr">
+        <is>
+          <t>Blind Fighting</t>
+        </is>
+      </c>
+      <c r="J237" t="n">
+        <v>3</v>
+      </c>
+      <c r="K237" t="n">
+        <v>0</v>
+      </c>
+      <c r="L237" t="n">
+        <v>4</v>
+      </c>
+      <c r="M237" t="n">
+        <v>0</v>
+      </c>
+      <c r="N237" t="n">
+        <v>1</v>
+      </c>
+      <c r="O237" t="n">
+        <v>1231</v>
+      </c>
+      <c r="P237" t="inlineStr">
+        <is>
+          <t>The Insecure Bounds of Vacancy: Blind Fighting</t>
+        </is>
+      </c>
+      <c r="Q237" t="inlineStr">
+        <is>
+          <t>Duchess Víðarr Jansdotter the Victorious</t>
+        </is>
+      </c>
+      <c r="S237" s="10" t="inlineStr">
+        <is>
+          <t>𐎸𐏂 𐎽𐎸𐎽𐎢𐎨𐎯𐎨𐏂 𐎭𐎨𐎽𐎨 𐎣𐎨𐎢𐏂𐎸𐎬 𐎥𐎠𐎬𐎤𐎽 𐎬𐎮𐎫𐎫𐎨𐎽 𐎢𐎮𐎭</t>
+        </is>
+      </c>
+      <c r="T237" t="n">
+        <v>5</v>
+      </c>
+      <c r="U237" t="n">
+        <v>5</v>
+      </c>
+      <c r="V237" t="n">
+        <v>30</v>
+      </c>
+      <c r="W237" t="n">
+        <v>43</v>
+      </c>
+      <c r="X237" t="n">
+        <v>42</v>
+      </c>
+      <c r="Y237" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="AA237" t="inlineStr">
+        <is>
+          <t>the Victorious</t>
+        </is>
+      </c>
+      <c r="AB237" t="inlineStr">
+        <is>
+          <t>Víðarr Jansdotter</t>
+        </is>
+      </c>
+      <c r="AC237" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_female</t>
+        </is>
+      </c>
+      <c r="AD237" t="inlineStr">
+        <is>
+          <t>Duchess</t>
+        </is>
+      </c>
+      <c r="AE237" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ237" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK237" t="inlineStr">
+        <is>
+          <t>The {adjective_1} {noun_1} of {noun_2}: {topic}</t>
+        </is>
+      </c>
+      <c r="AL237" t="inlineStr">
+        <is>
+          <t>Blind Fighting</t>
+        </is>
+      </c>
+      <c r="AM237" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN237" t="n">
+        <v>293</v>
+      </c>
+      <c r="AO237" t="n">
+        <v>5</v>
+      </c>
+      <c r="AP237" t="n">
+        <v>938</v>
+      </c>
+      <c r="AQ237" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR237" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS237" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT237" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU237" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV237" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW237" t="inlineStr">
+        <is>
+          <t>63d868a4-7088-4579-ba1c-96d5cbac1d54</t>
+        </is>
+      </c>
+      <c r="AX237" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C238" t="n">
+        <v>2</v>
+      </c>
+      <c r="D238" t="n">
+        <v>790</v>
+      </c>
+      <c r="E238" t="n">
+        <v>50</v>
+      </c>
+      <c r="F238" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H238" t="inlineStr">
+        <is>
+          <t>Loremastery</t>
+        </is>
+      </c>
+      <c r="I238" t="inlineStr">
+        <is>
+          <t>Loremastery</t>
+        </is>
+      </c>
+      <c r="J238" t="n">
+        <v>1</v>
+      </c>
+      <c r="K238" t="n">
+        <v>0</v>
+      </c>
+      <c r="L238" t="n">
+        <v>1</v>
+      </c>
+      <c r="M238" t="n">
+        <v>0</v>
+      </c>
+      <c r="N238" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="O238" t="n">
+        <v>348</v>
+      </c>
+      <c r="P238" t="inlineStr">
+        <is>
+          <t>The Ulterior Duty: Loremastery</t>
+        </is>
+      </c>
+      <c r="Q238" t="inlineStr">
+        <is>
+          <t>Baron Magnar Jensen</t>
+        </is>
+      </c>
+      <c r="S238" s="10" t="inlineStr">
+        <is>
+          <t>The Ulterior Duty: Loremastery</t>
+        </is>
+      </c>
+      <c r="T238" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="U238" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="V238" t="n">
+        <v>52</v>
+      </c>
+      <c r="W238" t="n">
+        <v>161</v>
+      </c>
+      <c r="X238" t="n">
+        <v>160</v>
+      </c>
+      <c r="Y238" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="AB238" t="inlineStr">
+        <is>
+          <t>Magnar Jensen</t>
+        </is>
+      </c>
+      <c r="AC238" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_male</t>
+        </is>
+      </c>
+      <c r="AD238" t="inlineStr">
+        <is>
+          <t>Baron</t>
+        </is>
+      </c>
+      <c r="AE238" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ238" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK238" t="inlineStr">
+        <is>
+          <t>The {adjective_1} {noun_1}: {topic}</t>
+        </is>
+      </c>
+      <c r="AL238" t="inlineStr">
+        <is>
+          <t>Loremastery</t>
+        </is>
+      </c>
+      <c r="AM238" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN238" t="n">
+        <v>390</v>
+      </c>
+      <c r="AO238" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP238" t="n">
+        <v>50</v>
+      </c>
+      <c r="AQ238" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR238" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS238" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT238" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU238" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV238" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW238" t="inlineStr">
+        <is>
+          <t>b7656904-1a76-4b4d-bab9-8323eb1d2bdc</t>
+        </is>
+      </c>
+      <c r="AX238" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C239" t="n">
+        <v>3</v>
+      </c>
+      <c r="D239" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E239" t="n">
+        <v>125</v>
+      </c>
+      <c r="F239" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H239" t="inlineStr">
+        <is>
+          <t>Battle Magic</t>
+        </is>
+      </c>
+      <c r="I239" t="inlineStr">
+        <is>
+          <t>Battle Magic</t>
+        </is>
+      </c>
+      <c r="J239" t="n">
+        <v>2</v>
+      </c>
+      <c r="K239" t="n">
+        <v>0</v>
+      </c>
+      <c r="L239" t="n">
+        <v>1</v>
+      </c>
+      <c r="M239" t="n">
+        <v>0</v>
+      </c>
+      <c r="N239" t="n">
+        <v>1</v>
+      </c>
+      <c r="O239" t="n">
+        <v>1780</v>
+      </c>
+      <c r="P239" t="inlineStr">
+        <is>
+          <t>The Wickedness of The Temptress and Sorcerie and the Field of Battle</t>
+        </is>
+      </c>
+      <c r="Q239" t="inlineStr">
+        <is>
+          <t>Arnviðr Pettersen the Misty</t>
+        </is>
+      </c>
+      <c r="S239" s="10" t="inlineStr">
+        <is>
+          <t>The Wickedness of The Temptress and Sorcerie and the Field of Battle</t>
+        </is>
+      </c>
+      <c r="T239" t="n">
+        <v>12</v>
+      </c>
+      <c r="U239" t="n">
+        <v>12</v>
+      </c>
+      <c r="V239" t="n">
+        <v>48</v>
+      </c>
+      <c r="W239" t="n">
+        <v>28</v>
+      </c>
+      <c r="X239" t="n">
+        <v>27</v>
+      </c>
+      <c r="Y239" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="AA239" t="inlineStr">
+        <is>
+          <t>the Misty</t>
+        </is>
+      </c>
+      <c r="AB239" t="inlineStr">
+        <is>
+          <t>Arnviðr Pettersen</t>
+        </is>
+      </c>
+      <c r="AC239" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_male</t>
+        </is>
+      </c>
+      <c r="AE239" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ239" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK239" t="inlineStr">
+        <is>
+          <t>{the_1} {negative_1} of {person_evil} and {topic}</t>
+        </is>
+      </c>
+      <c r="AL239" t="inlineStr">
+        <is>
+          <t>Sorcerie and the Field of Battle</t>
+        </is>
+      </c>
+      <c r="AM239" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN239" t="n">
+        <v>780</v>
+      </c>
+      <c r="AO239" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP239" t="n">
+        <v>1000</v>
+      </c>
+      <c r="AQ239" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR239" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS239" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT239" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU239" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV239" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW239" t="inlineStr">
+        <is>
+          <t>b76a092d-4c93-426d-96fd-020f43e75e67</t>
+        </is>
+      </c>
+      <c r="AX239" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C240" t="n">
+        <v>1</v>
+      </c>
+      <c r="D240" t="n">
+        <v>500</v>
+      </c>
+      <c r="E240" t="n">
+        <v>32</v>
+      </c>
+      <c r="F240" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H240" t="inlineStr">
+        <is>
+          <t>Craft (wheelwright)</t>
+        </is>
+      </c>
+      <c r="I240" t="inlineStr">
+        <is>
+          <t>Craft (wheelwright)</t>
+        </is>
+      </c>
+      <c r="J240" t="n">
+        <v>1</v>
+      </c>
+      <c r="K240" t="n">
+        <v>0</v>
+      </c>
+      <c r="L240" t="n">
+        <v>2</v>
+      </c>
+      <c r="M240" t="n">
+        <v>0</v>
+      </c>
+      <c r="N240" t="n">
+        <v>1</v>
+      </c>
+      <c r="O240" t="n">
+        <v>227</v>
+      </c>
+      <c r="P240" t="inlineStr">
+        <is>
+          <t>A Treatise on Wheelwrighting</t>
+        </is>
+      </c>
+      <c r="Q240" t="inlineStr">
+        <is>
+          <t>Gontran Baffier</t>
+        </is>
+      </c>
+      <c r="S240" s="10" t="inlineStr">
+        <is>
+          <t>A Treatise on Wheelwrighting</t>
+        </is>
+      </c>
+      <c r="T240" t="n">
+        <v>3</v>
+      </c>
+      <c r="U240" t="n">
+        <v>3</v>
+      </c>
+      <c r="V240" t="n">
+        <v>13</v>
+      </c>
+      <c r="W240" t="n">
+        <v>173</v>
+      </c>
+      <c r="X240" t="n">
+        <v>172</v>
+      </c>
+      <c r="Y240" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="AB240" t="inlineStr">
+        <is>
+          <t>Gontran Baffier</t>
+        </is>
+      </c>
+      <c r="AC240" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AE240" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ240" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK240" t="inlineStr">
+        <is>
+          <t>{study_on} on {topic}</t>
+        </is>
+      </c>
+      <c r="AL240" t="inlineStr">
+        <is>
+          <t>Wheelwrighting</t>
+        </is>
+      </c>
+      <c r="AM240" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN240" t="n">
+        <v>195</v>
+      </c>
+      <c r="AO240" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AP240" t="n">
+        <v>32</v>
+      </c>
+      <c r="AQ240" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR240" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS240" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT240" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU240" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV240" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW240" t="inlineStr">
+        <is>
+          <t>3871a760-7cda-4c13-85d1-6d770cbcbd3e</t>
+        </is>
+      </c>
+      <c r="AX240" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C241" t="n">
+        <v>1</v>
+      </c>
+      <c r="D241" t="n">
+        <v>500</v>
+      </c>
+      <c r="E241" t="n">
+        <v>32</v>
+      </c>
+      <c r="F241" t="inlineStr">
+        <is>
+          <t>Classical</t>
+        </is>
+      </c>
+      <c r="H241" t="inlineStr">
+        <is>
+          <t>Profession (judge)</t>
+        </is>
+      </c>
+      <c r="I241" t="inlineStr">
+        <is>
+          <t>Profession (judge)</t>
+        </is>
+      </c>
+      <c r="J241" t="n">
+        <v>1</v>
+      </c>
+      <c r="K241" t="n">
+        <v>0</v>
+      </c>
+      <c r="L241" t="n">
+        <v>2</v>
+      </c>
+      <c r="M241" t="n">
+        <v>0</v>
+      </c>
+      <c r="N241" t="n">
+        <v>1</v>
+      </c>
+      <c r="O241" t="n">
+        <v>202</v>
+      </c>
+      <c r="P241" t="inlineStr">
+        <is>
+          <t>The Transgressions of Agrippa Titucia, on the Subject of Judging</t>
+        </is>
+      </c>
+      <c r="Q241" t="inlineStr">
+        <is>
+          <t>The Venerable Manlius Condetia</t>
+        </is>
+      </c>
+      <c r="S241" s="10" t="inlineStr">
+        <is>
+          <t>Animosque animum iurando frumenta disponit celerrime sociorum eripi milites avaritiam</t>
+        </is>
+      </c>
+      <c r="T241" t="n">
+        <v>3</v>
+      </c>
+      <c r="U241" t="n">
+        <v>3</v>
+      </c>
+      <c r="V241" t="n">
+        <v>81</v>
+      </c>
+      <c r="W241" t="n">
+        <v>769</v>
+      </c>
+      <c r="X241" t="n">
+        <v>768</v>
+      </c>
+      <c r="Y241" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AB241" t="inlineStr">
+        <is>
+          <t>Manlius Condetia</t>
+        </is>
+      </c>
+      <c r="AC241" t="inlineStr">
+        <is>
+          <t>_names_roman_surnames</t>
+        </is>
+      </c>
+      <c r="AD241" t="inlineStr">
+        <is>
+          <t>The Venerable</t>
+        </is>
+      </c>
+      <c r="AE241" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ241" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK241" t="inlineStr">
+        <is>
+          <t>{the_1} {negative_1} of {person_1}, on the Subject of {topic}</t>
+        </is>
+      </c>
+      <c r="AL241" t="inlineStr">
+        <is>
+          <t>Judging</t>
+        </is>
+      </c>
+      <c r="AM241" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN241" t="n">
+        <v>195</v>
+      </c>
+      <c r="AO241" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AP241" t="n">
+        <v>7</v>
+      </c>
+      <c r="AQ241" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR241" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS241" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT241" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU241" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV241" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW241" t="inlineStr">
+        <is>
+          <t>4e0d3928-6a26-4a6e-a77e-1af606e3c582</t>
+        </is>
+      </c>
+      <c r="AX241" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C242" t="n">
+        <v>1</v>
+      </c>
+      <c r="D242" t="n">
+        <v>500</v>
+      </c>
+      <c r="E242" t="n">
+        <v>32</v>
+      </c>
+      <c r="F242" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H242" t="inlineStr">
+        <is>
+          <t>Seafaring</t>
+        </is>
+      </c>
+      <c r="I242" t="inlineStr">
+        <is>
+          <t>Seafaring</t>
+        </is>
+      </c>
+      <c r="J242" t="n">
+        <v>1</v>
+      </c>
+      <c r="K242" t="n">
+        <v>0</v>
+      </c>
+      <c r="L242" t="n">
+        <v>2</v>
+      </c>
+      <c r="M242" t="n">
+        <v>0</v>
+      </c>
+      <c r="N242" t="n">
+        <v>1</v>
+      </c>
+      <c r="O242" t="n">
+        <v>352</v>
+      </c>
+      <c r="P242" t="inlineStr">
+        <is>
+          <t>The Undercover Gyre of Phobias: Seafaring</t>
+        </is>
+      </c>
+      <c r="Q242" t="inlineStr">
+        <is>
+          <t>Magus Manu Bruguès</t>
+        </is>
+      </c>
+      <c r="S242" s="10" t="inlineStr">
+        <is>
+          <t>The Undercover Gyre of Phobias: Seafaring</t>
+        </is>
+      </c>
+      <c r="T242" t="n">
+        <v>3</v>
+      </c>
+      <c r="U242" t="n">
+        <v>3</v>
+      </c>
+      <c r="V242" t="n">
+        <v>50</v>
+      </c>
+      <c r="W242" t="n">
+        <v>46</v>
+      </c>
+      <c r="X242" t="n">
+        <v>45</v>
+      </c>
+      <c r="Y242" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="AB242" t="inlineStr">
+        <is>
+          <t>Manu Bruguès</t>
+        </is>
+      </c>
+      <c r="AC242" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AD242" t="inlineStr">
+        <is>
+          <t>Magus</t>
+        </is>
+      </c>
+      <c r="AE242" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ242" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK242" t="inlineStr">
+        <is>
+          <t>The {adjective_1} {noun_1} of {noun_2}: {topic}</t>
+        </is>
+      </c>
+      <c r="AL242" t="inlineStr">
+        <is>
+          <t>Seafaring</t>
+        </is>
+      </c>
+      <c r="AM242" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN242" t="n">
+        <v>195</v>
+      </c>
+      <c r="AO242" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AP242" t="n">
+        <v>157</v>
+      </c>
+      <c r="AQ242" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR242" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS242" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT242" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU242" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV242" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW242" t="inlineStr">
+        <is>
+          <t>35df4b32-9a7d-4dd4-99a8-3cea005d29ba</t>
+        </is>
+      </c>
+      <c r="AX242" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C243" t="n">
+        <v>1</v>
+      </c>
+      <c r="D243" t="n">
+        <v>667</v>
+      </c>
+      <c r="E243" t="n">
+        <v>43</v>
+      </c>
+      <c r="F243" t="inlineStr">
+        <is>
+          <t>Regional</t>
+        </is>
+      </c>
+      <c r="H243" t="inlineStr">
+        <is>
+          <t>Trapping</t>
+        </is>
+      </c>
+      <c r="I243" t="inlineStr">
+        <is>
+          <t>Trapping</t>
+        </is>
+      </c>
+      <c r="J243" t="n">
+        <v>2</v>
+      </c>
+      <c r="K243" t="n">
+        <v>0</v>
+      </c>
+      <c r="L243" t="n">
+        <v>3</v>
+      </c>
+      <c r="M243" t="n">
+        <v>0</v>
+      </c>
+      <c r="N243" t="n">
+        <v>1</v>
+      </c>
+      <c r="O243" t="n">
+        <v>798</v>
+      </c>
+      <c r="P243" t="inlineStr">
+        <is>
+          <t>Trapping and This Period</t>
+        </is>
+      </c>
+      <c r="Q243" t="inlineStr">
+        <is>
+          <t>The Gracious Leofstan Smythe</t>
+        </is>
+      </c>
+      <c r="S243" s="10" t="inlineStr">
+        <is>
+          <t>Ἀφελεῖν εἰσιν αὐτό δὲ περιφέρεια] περιέχουσιν προσπίπτουσαι εὐθειῶν</t>
+        </is>
+      </c>
+      <c r="T243" t="n">
+        <v>4</v>
+      </c>
+      <c r="U243" t="n">
+        <v>4</v>
+      </c>
+      <c r="V243" t="n">
+        <v>57</v>
+      </c>
+      <c r="W243" t="n">
+        <v>9</v>
+      </c>
+      <c r="X243" t="n">
+        <v>8</v>
+      </c>
+      <c r="Y243" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AB243" t="inlineStr">
+        <is>
+          <t>Leofstan Smythe</t>
+        </is>
+      </c>
+      <c r="AC243" t="inlineStr">
+        <is>
+          <t>_names_anglo_saxon_surnames</t>
+        </is>
+      </c>
+      <c r="AD243" t="inlineStr">
+        <is>
+          <t>The Gracious</t>
+        </is>
+      </c>
+      <c r="AE243" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ243" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK243" t="inlineStr">
+        <is>
+          <t>{topic} and {noun_2}</t>
+        </is>
+      </c>
+      <c r="AL243" t="inlineStr">
+        <is>
+          <t>Trapping</t>
+        </is>
+      </c>
+      <c r="AM243" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN243" t="n">
+        <v>247</v>
+      </c>
+      <c r="AO243" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="AP243" t="n">
+        <v>551</v>
+      </c>
+      <c r="AQ243" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR243" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS243" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT243" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU243" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV243" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW243" t="inlineStr">
+        <is>
+          <t>a6047632-ca85-4699-903d-ccf94fcfd3bc</t>
+        </is>
+      </c>
+      <c r="AX243" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>Tablet</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>Clay</t>
+        </is>
+      </c>
+      <c r="C244" t="n">
+        <v>1</v>
+      </c>
+      <c r="D244" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E244" t="n">
+        <v>750</v>
+      </c>
+      <c r="F244" t="inlineStr">
+        <is>
+          <t>Ancient</t>
+        </is>
+      </c>
+      <c r="H244" t="inlineStr">
+        <is>
+          <t>Military Strategy</t>
+        </is>
+      </c>
+      <c r="I244" t="inlineStr">
+        <is>
+          <t>Military Strategy</t>
+        </is>
+      </c>
+      <c r="J244" t="n">
+        <v>1</v>
+      </c>
+      <c r="K244" t="n">
+        <v>0</v>
+      </c>
+      <c r="L244" t="n">
+        <v>1</v>
+      </c>
+      <c r="M244" t="n">
+        <v>0</v>
+      </c>
+      <c r="N244" t="n">
+        <v>1</v>
+      </c>
+      <c r="O244" t="n">
+        <v>900</v>
+      </c>
+      <c r="P244" t="inlineStr">
+        <is>
+          <t>The Undercover Expedition of Agitation: Military Strategy</t>
+        </is>
+      </c>
+      <c r="Q244" t="inlineStr">
+        <is>
+          <t>Þone Thomsen the Mysterious</t>
+        </is>
+      </c>
+      <c r="S244" s="10" t="inlineStr">
+        <is>
+          <t>𐎽𐎸𐎽𐎯𐎤𐎭𐎣𐎨𐎽𐎽𐎤 𐎢𐎮𐎭𐎦𐎸𐎤 𐏂𐎠𐎢𐎨𐏂𐎨 𐎡𐎫𐎠𐎭𐎣𐎨𐏂 𐎤𐏍 𐎣𐎨𐎠</t>
+        </is>
+      </c>
+      <c r="T244" t="n">
+        <v>6</v>
+      </c>
+      <c r="U244" t="n">
+        <v>6</v>
+      </c>
+      <c r="V244" t="n">
+        <v>2585</v>
+      </c>
+      <c r="W244" t="n">
+        <v>64</v>
+      </c>
+      <c r="X244" t="n">
+        <v>63</v>
+      </c>
+      <c r="Y244" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AA244" t="inlineStr">
+        <is>
+          <t>the Mysterious</t>
+        </is>
+      </c>
+      <c r="AB244" t="inlineStr">
+        <is>
+          <t>Þone Thomsen</t>
+        </is>
+      </c>
+      <c r="AC244" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_male</t>
+        </is>
+      </c>
+      <c r="AE244" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ244" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="AK244" t="inlineStr">
+        <is>
+          <t>The {adjective_1} {noun_1} of {noun_2}: {topic}</t>
+        </is>
+      </c>
+      <c r="AL244" t="inlineStr">
+        <is>
+          <t>Military Strategy</t>
+        </is>
+      </c>
+      <c r="AM244" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="AN244" t="n">
+        <v>800</v>
+      </c>
+      <c r="AO244" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP244" t="n">
+        <v>100</v>
+      </c>
+      <c r="AQ244" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR244" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS244" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT244" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU244" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV244" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW244" t="inlineStr">
+        <is>
+          <t>a8b8bb21-323f-4e29-9ce0-d9f9f40b7cf7</t>
+        </is>
+      </c>
+      <c r="AX244" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C245" t="n">
+        <v>1</v>
+      </c>
+      <c r="D245" t="n">
+        <v>500</v>
+      </c>
+      <c r="E245" t="n">
+        <v>32</v>
+      </c>
+      <c r="F245" t="inlineStr">
+        <is>
+          <t>Classical</t>
+        </is>
+      </c>
+      <c r="H245" t="inlineStr">
+        <is>
+          <t>Craft (saddlery)</t>
+        </is>
+      </c>
+      <c r="I245" t="inlineStr">
+        <is>
+          <t>Craft (saddlery)</t>
+        </is>
+      </c>
+      <c r="J245" t="n">
+        <v>1</v>
+      </c>
+      <c r="K245" t="n">
+        <v>0</v>
+      </c>
+      <c r="L245" t="n">
+        <v>2</v>
+      </c>
+      <c r="M245" t="n">
+        <v>0</v>
+      </c>
+      <c r="N245" t="n">
+        <v>1</v>
+      </c>
+      <c r="O245" t="n">
+        <v>258</v>
+      </c>
+      <c r="P245" t="inlineStr">
+        <is>
+          <t>Thoughts on Saddlery</t>
+        </is>
+      </c>
+      <c r="Q245" t="inlineStr">
+        <is>
+          <t>The Venerable Raymonde Biémouret the Loud</t>
+        </is>
+      </c>
+      <c r="S245" s="10" t="inlineStr">
+        <is>
+          <t>Adesse alariis facilisi allobrogibus conventu</t>
+        </is>
+      </c>
+      <c r="T245" t="n">
+        <v>3</v>
+      </c>
+      <c r="U245" t="n">
+        <v>3</v>
+      </c>
+      <c r="V245" t="n">
+        <v>45</v>
+      </c>
+      <c r="W245" t="n">
+        <v>54</v>
+      </c>
+      <c r="X245" t="n">
+        <v>53</v>
+      </c>
+      <c r="Y245" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AA245" t="inlineStr">
+        <is>
+          <t>the Loud</t>
+        </is>
+      </c>
+      <c r="AB245" t="inlineStr">
+        <is>
+          <t>Raymonde Biémouret</t>
+        </is>
+      </c>
+      <c r="AC245" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AD245" t="inlineStr">
+        <is>
+          <t>The Venerable</t>
+        </is>
+      </c>
+      <c r="AE245" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ245" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK245" t="inlineStr">
+        <is>
+          <t>{study_on} on {topic}</t>
+        </is>
+      </c>
+      <c r="AL245" t="inlineStr">
+        <is>
+          <t>Saddlery</t>
+        </is>
+      </c>
+      <c r="AM245" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN245" t="n">
+        <v>195</v>
+      </c>
+      <c r="AO245" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AP245" t="n">
+        <v>63</v>
+      </c>
+      <c r="AQ245" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR245" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS245" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT245" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU245" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV245" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW245" t="inlineStr">
+        <is>
+          <t>28236bd7-a85b-4b86-9cd1-8c45ed403ef8</t>
+        </is>
+      </c>
+      <c r="AX245" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C246" t="n">
+        <v>1</v>
+      </c>
+      <c r="D246" t="n">
+        <v>667</v>
+      </c>
+      <c r="E246" t="n">
+        <v>43</v>
+      </c>
+      <c r="F246" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H246" t="inlineStr">
+        <is>
+          <t>Esoteric: Judge’s Choice</t>
+        </is>
+      </c>
+      <c r="I246" t="inlineStr">
+        <is>
+          <t>Performance (dancing)</t>
+        </is>
+      </c>
+      <c r="J246" t="n">
+        <v>2</v>
+      </c>
+      <c r="K246" t="n">
+        <v>1</v>
+      </c>
+      <c r="L246" t="n">
+        <v>3</v>
+      </c>
+      <c r="M246" t="n">
+        <v>2</v>
+      </c>
+      <c r="N246" t="n">
+        <v>1</v>
+      </c>
+      <c r="O246" t="n">
+        <v>8599</v>
+      </c>
+      <c r="P246" t="inlineStr">
+        <is>
+          <t>The Imperfection of Revna Thomsdotter, in which case Apropos of Dancing is Given Particular Attention by Way of Instruction and Warning</t>
+        </is>
+      </c>
+      <c r="Q246" t="inlineStr">
+        <is>
+          <t>Rosette Proux</t>
+        </is>
+      </c>
+      <c r="S246" s="10" t="inlineStr">
+        <is>
+          <t>The Imperfection of Revna Thomsdotter, in which case Apropos of Dancing is Given Particular Attention by Way of Instruction and Warning</t>
+        </is>
+      </c>
+      <c r="T246" t="n">
+        <v>4</v>
+      </c>
+      <c r="U246" t="n">
+        <v>4</v>
+      </c>
+      <c r="V246" t="n">
+        <v>35</v>
+      </c>
+      <c r="W246" t="n">
+        <v>1</v>
+      </c>
+      <c r="X246" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y246" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB246" t="inlineStr">
+        <is>
+          <t>Rosette Proux</t>
+        </is>
+      </c>
+      <c r="AC246" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AE246" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ246" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK246" t="inlineStr">
+        <is>
+          <t>{the_1} {negative_1} of {person_1}, in which case {conjunction_about} {topic} is Given Particular Attention by Way of Instruction and Warning</t>
+        </is>
+      </c>
+      <c r="AL246" t="inlineStr">
+        <is>
+          <t>Dancing</t>
+        </is>
+      </c>
+      <c r="AM246" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN246" t="n">
+        <v>261</v>
+      </c>
+      <c r="AO246" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="AP246" t="n">
+        <v>1668</v>
+      </c>
+      <c r="AQ246" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AR246" t="n">
+        <v>6670</v>
+      </c>
+      <c r="AS246" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT246" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU246" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV246" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW246" t="inlineStr">
+        <is>
+          <t>2c2a19b5-eb49-4c49-8b88-42bc6149c09b</t>
+        </is>
+      </c>
+      <c r="AX246" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>Silver Foil</t>
+        </is>
+      </c>
+      <c r="C247" t="n">
+        <v>1</v>
+      </c>
+      <c r="D247" t="n">
+        <v>500</v>
+      </c>
+      <c r="E247" t="n">
+        <v>77</v>
+      </c>
+      <c r="F247" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H247" t="inlineStr">
+        <is>
+          <t>Gambling</t>
+        </is>
+      </c>
+      <c r="I247" t="inlineStr">
+        <is>
+          <t>Gambling</t>
+        </is>
+      </c>
+      <c r="J247" t="n">
+        <v>1</v>
+      </c>
+      <c r="K247" t="n">
+        <v>0</v>
+      </c>
+      <c r="L247" t="n">
+        <v>2</v>
+      </c>
+      <c r="M247" t="n">
+        <v>0</v>
+      </c>
+      <c r="N247" t="n">
+        <v>1</v>
+      </c>
+      <c r="O247" t="n">
+        <v>968</v>
+      </c>
+      <c r="P247" t="inlineStr">
+        <is>
+          <t>The Wickedness of Aelfled Kristensen, in which case Discoursing on Gambling is Given Particular Attention by Way of Instruction and Warning</t>
+        </is>
+      </c>
+      <c r="Q247" t="inlineStr">
+        <is>
+          <t>Maecia Longinia</t>
+        </is>
+      </c>
+      <c r="S247" s="10" t="inlineStr">
+        <is>
+          <t>The Wickedness of Aelfled Kristensen, in which case Discoursing on Gambling is Given Particular Attention by Way of Instruction and Warning</t>
+        </is>
+      </c>
+      <c r="T247" t="n">
+        <v>3</v>
+      </c>
+      <c r="U247" t="n">
+        <v>3</v>
+      </c>
+      <c r="V247" t="n">
+        <v>15</v>
+      </c>
+      <c r="W247" t="n">
+        <v>69</v>
+      </c>
+      <c r="X247" t="n">
+        <v>68</v>
+      </c>
+      <c r="Y247" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AB247" t="inlineStr">
+        <is>
+          <t>Maecia Longinia</t>
+        </is>
+      </c>
+      <c r="AC247" t="inlineStr">
+        <is>
+          <t>_names_roman_surnames</t>
+        </is>
+      </c>
+      <c r="AE247" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ247" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="AK247" t="inlineStr">
+        <is>
+          <t>{the_1} {negative_1} of {person_1}, in which case {conjunction_about} {topic} is Given Particular Attention by Way of Instruction and Warning</t>
+        </is>
+      </c>
+      <c r="AL247" t="inlineStr">
+        <is>
+          <t>Gambling</t>
+        </is>
+      </c>
+      <c r="AM247" t="n">
+        <v>1.81</v>
+      </c>
+      <c r="AN247" t="n">
+        <v>905</v>
+      </c>
+      <c r="AO247" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AP247" t="n">
+        <v>63</v>
+      </c>
+      <c r="AQ247" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR247" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS247" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT247" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU247" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV247" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW247" t="inlineStr">
+        <is>
+          <t>1de2cafa-0492-465d-add2-d45b2ef52e56</t>
+        </is>
+      </c>
+      <c r="AX247" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C248" t="n">
+        <v>2</v>
+      </c>
+      <c r="D248" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E248" t="n">
+        <v>63</v>
+      </c>
+      <c r="F248" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H248" t="inlineStr">
+        <is>
+          <t>Animal Training (dogs)</t>
+        </is>
+      </c>
+      <c r="I248" t="inlineStr">
+        <is>
+          <t>Animal Training (dogs)</t>
+        </is>
+      </c>
+      <c r="J248" t="n">
+        <v>1</v>
+      </c>
+      <c r="K248" t="n">
+        <v>0</v>
+      </c>
+      <c r="L248" t="n">
+        <v>1</v>
+      </c>
+      <c r="M248" t="n">
+        <v>0</v>
+      </c>
+      <c r="N248" t="n">
+        <v>1</v>
+      </c>
+      <c r="O248" t="n">
+        <v>490</v>
+      </c>
+      <c r="P248" t="inlineStr">
+        <is>
+          <t>Training of Dogs, a Abstruse Revelation</t>
+        </is>
+      </c>
+      <c r="Q248" t="inlineStr">
+        <is>
+          <t>Sybille Mazet</t>
+        </is>
+      </c>
+      <c r="S248" s="10" t="inlineStr">
+        <is>
+          <t>Training of Dogs, a Abstruse Revelation</t>
+        </is>
+      </c>
+      <c r="T248" t="n">
+        <v>6</v>
+      </c>
+      <c r="U248" t="n">
+        <v>6</v>
+      </c>
+      <c r="V248" t="n">
+        <v>20</v>
+      </c>
+      <c r="W248" t="n">
+        <v>87</v>
+      </c>
+      <c r="X248" t="n">
+        <v>86</v>
+      </c>
+      <c r="Y248" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AB248" t="inlineStr">
+        <is>
+          <t>Sybille Mazet</t>
+        </is>
+      </c>
+      <c r="AC248" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AE248" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ248" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK248" t="inlineStr">
+        <is>
+          <t>{topic}, a {adjective_1} {noun_1}</t>
+        </is>
+      </c>
+      <c r="AL248" t="inlineStr">
+        <is>
+          <t>Training of Dogs</t>
+        </is>
+      </c>
+      <c r="AM248" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN248" t="n">
+        <v>390</v>
+      </c>
+      <c r="AO248" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP248" t="n">
+        <v>100</v>
+      </c>
+      <c r="AQ248" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR248" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS248" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT248" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU248" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV248" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW248" t="inlineStr">
+        <is>
+          <t>0564fada-c0b1-49eb-9af7-f9c1fa5ee285</t>
+        </is>
+      </c>
+      <c r="AX248" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C249" t="n">
+        <v>1</v>
+      </c>
+      <c r="D249" t="n">
+        <v>334</v>
+      </c>
+      <c r="E249" t="n">
+        <v>23</v>
+      </c>
+      <c r="F249" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H249" t="inlineStr">
+        <is>
+          <t>Labor (construction)</t>
+        </is>
+      </c>
+      <c r="I249" t="inlineStr">
+        <is>
+          <t>Labor (construction)</t>
+        </is>
+      </c>
+      <c r="J249" t="n">
+        <v>1</v>
+      </c>
+      <c r="K249" t="n">
+        <v>0</v>
+      </c>
+      <c r="L249" t="n">
+        <v>3</v>
+      </c>
+      <c r="M249" t="n">
+        <v>0</v>
+      </c>
+      <c r="N249" t="n">
+        <v>1</v>
+      </c>
+      <c r="O249" t="n">
+        <v>458</v>
+      </c>
+      <c r="P249" t="inlineStr">
+        <is>
+          <t>Condemnation of Queen Kalissa and Construction</t>
+        </is>
+      </c>
+      <c r="Q249" t="inlineStr">
+        <is>
+          <t>Isolf Pedersen One-eye</t>
+        </is>
+      </c>
+      <c r="S249" s="10" t="inlineStr">
+        <is>
+          <t>Condemnation of Queen Kalissa and Construction</t>
+        </is>
+      </c>
+      <c r="T249" t="n">
+        <v>2</v>
+      </c>
+      <c r="U249" t="n">
+        <v>2</v>
+      </c>
+      <c r="V249" t="n">
+        <v>30</v>
+      </c>
+      <c r="W249" t="n">
+        <v>5</v>
+      </c>
+      <c r="X249" t="n">
+        <v>4</v>
+      </c>
+      <c r="Y249" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AA249" t="inlineStr">
+        <is>
+          <t>One-eye</t>
+        </is>
+      </c>
+      <c r="AB249" t="inlineStr">
+        <is>
+          <t>Isolf Pedersen</t>
+        </is>
+      </c>
+      <c r="AC249" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_male</t>
+        </is>
+      </c>
+      <c r="AE249" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ249" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK249" t="inlineStr">
+        <is>
+          <t>{biography_starter} of {person_famous} and {topic}</t>
+        </is>
+      </c>
+      <c r="AL249" t="inlineStr">
+        <is>
+          <t>Construction</t>
+        </is>
+      </c>
+      <c r="AM249" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN249" t="n">
+        <v>124</v>
+      </c>
+      <c r="AO249" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP249" t="n">
+        <v>334</v>
+      </c>
+      <c r="AQ249" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR249" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS249" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT249" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU249" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV249" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW249" t="inlineStr">
+        <is>
+          <t>99c35f31-f673-4f9b-b853-6038258218af</t>
+        </is>
+      </c>
+      <c r="AX249" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C250" t="n">
+        <v>1</v>
+      </c>
+      <c r="D250" t="n">
+        <v>500</v>
+      </c>
+      <c r="E250" t="n">
+        <v>32</v>
+      </c>
+      <c r="F250" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H250" t="inlineStr">
+        <is>
+          <t>Military Strategy</t>
+        </is>
+      </c>
+      <c r="I250" t="inlineStr">
+        <is>
+          <t>Military Strategy</t>
+        </is>
+      </c>
+      <c r="J250" t="n">
+        <v>1</v>
+      </c>
+      <c r="K250" t="n">
+        <v>0</v>
+      </c>
+      <c r="L250" t="n">
+        <v>2</v>
+      </c>
+      <c r="M250" t="n">
+        <v>0</v>
+      </c>
+      <c r="N250" t="n">
+        <v>1</v>
+      </c>
+      <c r="O250" t="n">
+        <v>248</v>
+      </c>
+      <c r="P250" t="inlineStr">
+        <is>
+          <t>The Damnable Immorality of Sabine Baugé, on the Subject of Military Strategy</t>
+        </is>
+      </c>
+      <c r="Q250" t="inlineStr">
+        <is>
+          <t>The Gracious Arvakl Thomsen</t>
+        </is>
+      </c>
+      <c r="S250" s="10" t="inlineStr">
+        <is>
+          <t>The Damnable Immorality of Sabine Baugé, on the Subject of Military Strategy</t>
+        </is>
+      </c>
+      <c r="T250" t="n">
+        <v>3</v>
+      </c>
+      <c r="U250" t="n">
+        <v>3</v>
+      </c>
+      <c r="V250" t="n">
+        <v>94</v>
+      </c>
+      <c r="W250" t="n">
+        <v>62</v>
+      </c>
+      <c r="X250" t="n">
+        <v>61</v>
+      </c>
+      <c r="Y250" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AB250" t="inlineStr">
+        <is>
+          <t>Arvakl Thomsen</t>
+        </is>
+      </c>
+      <c r="AC250" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_male</t>
+        </is>
+      </c>
+      <c r="AD250" t="inlineStr">
+        <is>
+          <t>The Gracious</t>
+        </is>
+      </c>
+      <c r="AE250" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ250" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK250" t="inlineStr">
+        <is>
+          <t>{the_1} {negative_1} of {person_1}, on the Subject of {topic}</t>
+        </is>
+      </c>
+      <c r="AL250" t="inlineStr">
+        <is>
+          <t>Military Strategy</t>
+        </is>
+      </c>
+      <c r="AM250" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN250" t="n">
+        <v>185</v>
+      </c>
+      <c r="AO250" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AP250" t="n">
+        <v>63</v>
+      </c>
+      <c r="AQ250" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR250" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS250" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT250" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU250" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV250" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW250" t="inlineStr">
+        <is>
+          <t>adf5fe48-6a6b-4310-922b-d8a9a7c86571</t>
+        </is>
+      </c>
+      <c r="AX250" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>Scroll</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>Ordinary Papyrus</t>
+        </is>
+      </c>
+      <c r="C251" t="n">
+        <v>4</v>
+      </c>
+      <c r="D251" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E251" t="n">
+        <v>68</v>
+      </c>
+      <c r="F251" t="inlineStr">
+        <is>
+          <t>Ancient</t>
+        </is>
+      </c>
+      <c r="H251" t="inlineStr">
+        <is>
+          <t>Craft (cobbling)</t>
+        </is>
+      </c>
+      <c r="I251" t="inlineStr">
+        <is>
+          <t>Craft (cobbling)</t>
+        </is>
+      </c>
+      <c r="J251" t="n">
+        <v>3</v>
+      </c>
+      <c r="K251" t="n">
+        <v>0</v>
+      </c>
+      <c r="L251" t="n">
+        <v>3</v>
+      </c>
+      <c r="M251" t="n">
+        <v>0</v>
+      </c>
+      <c r="N251" t="n">
+        <v>1</v>
+      </c>
+      <c r="O251" t="n">
+        <v>1630</v>
+      </c>
+      <c r="P251" t="inlineStr">
+        <is>
+          <t>Investigations in Why Doth the Children of the Cobbler Never Have Shoes?</t>
+        </is>
+      </c>
+      <c r="Q251" t="inlineStr">
+        <is>
+          <t>Julius Equitia</t>
+        </is>
+      </c>
+      <c r="S251" s="10" t="inlineStr">
+        <is>
+          <t>𐎯𐎱𐎮𐎨𐎭 𐎣𐎨𐎦𐎭𐎨𐎽𐎽𐎨𐎬 𐎣𐎨𐎠𐎬 𐎨𐎭𐏂𐎤𐎱𐎣𐎸𐎬 𐎯𐎮𐎽𐎸𐎤𐎱𐎤 𐎠𐎢</t>
+        </is>
+      </c>
+      <c r="T251" t="n">
+        <v>6</v>
+      </c>
+      <c r="U251" t="n">
+        <v>6</v>
+      </c>
+      <c r="V251" t="n">
+        <v>867</v>
+      </c>
+      <c r="W251" t="n">
+        <v>16</v>
+      </c>
+      <c r="X251" t="n">
+        <v>15</v>
+      </c>
+      <c r="Y251" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AB251" t="inlineStr">
+        <is>
+          <t>Julius Equitia</t>
+        </is>
+      </c>
+      <c r="AC251" t="inlineStr">
+        <is>
+          <t>_names_roman_surnames</t>
+        </is>
+      </c>
+      <c r="AE251" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ251" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK251" t="inlineStr">
+        <is>
+          <t>{study_in} in {topic}</t>
+        </is>
+      </c>
+      <c r="AL251" t="inlineStr">
+        <is>
+          <t>Why Doth the Children of the Cobbler Never Have Shoes?</t>
+        </is>
+      </c>
+      <c r="AM251" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AN251" t="n">
+        <v>310</v>
+      </c>
+      <c r="AO251" t="n">
+        <v>4</v>
+      </c>
+      <c r="AP251" t="n">
+        <v>1320</v>
+      </c>
+      <c r="AQ251" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR251" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS251" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT251" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU251" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV251" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW251" t="inlineStr">
+        <is>
+          <t>eba3025b-3caa-40ce-8df1-781b5a14f6ae</t>
+        </is>
+      </c>
+      <c r="AX251" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C252" t="n">
+        <v>1</v>
+      </c>
+      <c r="D252" t="n">
+        <v>667</v>
+      </c>
+      <c r="E252" t="n">
+        <v>43</v>
+      </c>
+      <c r="F252" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H252" t="inlineStr">
+        <is>
+          <t>Esoteric: Loremastery</t>
+        </is>
+      </c>
+      <c r="I252" t="inlineStr">
+        <is>
+          <t>Profession (chamberlain)</t>
+        </is>
+      </c>
+      <c r="J252" t="n">
+        <v>2</v>
+      </c>
+      <c r="K252" t="n">
+        <v>1</v>
+      </c>
+      <c r="L252" t="n">
+        <v>3</v>
+      </c>
+      <c r="M252" t="n">
+        <v>2</v>
+      </c>
+      <c r="N252" t="n">
+        <v>1</v>
+      </c>
+      <c r="O252" t="n">
+        <v>8585</v>
+      </c>
+      <c r="P252" t="inlineStr">
+        <is>
+          <t>The Crimes of The Temptress and Chamberlain's Craft</t>
+        </is>
+      </c>
+      <c r="Q252" t="inlineStr">
+        <is>
+          <t>Her Grace Aurora Turpilia XI</t>
+        </is>
+      </c>
+      <c r="S252" s="10" t="inlineStr">
+        <is>
+          <t>The Crimes of The Temptress and Chamberlain's Craft</t>
+        </is>
+      </c>
+      <c r="T252" t="n">
+        <v>4</v>
+      </c>
+      <c r="U252" t="n">
+        <v>4</v>
+      </c>
+      <c r="V252" t="n">
+        <v>14</v>
+      </c>
+      <c r="W252" t="n">
+        <v>1</v>
+      </c>
+      <c r="X252" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y252" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA252" t="inlineStr">
+        <is>
+          <t>XI</t>
+        </is>
+      </c>
+      <c r="AB252" t="inlineStr">
+        <is>
+          <t>Aurora Turpilia</t>
+        </is>
+      </c>
+      <c r="AC252" t="inlineStr">
+        <is>
+          <t>_names_roman_surnames</t>
+        </is>
+      </c>
+      <c r="AD252" t="inlineStr">
+        <is>
+          <t>Her Grace</t>
+        </is>
+      </c>
+      <c r="AE252" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ252" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK252" t="inlineStr">
+        <is>
+          <t>{the_1} {negative_1} of {person_evil} and {topic}</t>
+        </is>
+      </c>
+      <c r="AL252" t="inlineStr">
+        <is>
+          <t>Chamberlain's Craft</t>
+        </is>
+      </c>
+      <c r="AM252" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN252" t="n">
+        <v>247</v>
+      </c>
+      <c r="AO252" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="AP252" t="n">
+        <v>1668</v>
+      </c>
+      <c r="AQ252" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AR252" t="n">
+        <v>6670</v>
+      </c>
+      <c r="AS252" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT252" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU252" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV252" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW252" t="inlineStr">
+        <is>
+          <t>c3aca3c7-ce06-44a9-ad74-3ee9bd5aa1d2</t>
+        </is>
+      </c>
+      <c r="AX252" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Create new master file if not existing
</commit_message>
<xml_diff>
--- a/books_spreadsheet_out.xlsx
+++ b/books_spreadsheet_out.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\My Documents\Greg Documents\Programming\Python 3\fantasy_books_workspace\fantasy_books\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC0D6060-1F21-495B-8A44-4C6540F7B67C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD02EAA-994C-44FA-81A0-BE1BBC692ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Book Hoard" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Book Hoard" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -176,7 +177,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,6 +189,14 @@
       <b/>
       <sz val="9"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Segoe UI Historic"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Tengwar Annatar"/>
     </font>
   </fonts>
   <fills count="2">
@@ -210,9 +219,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,7 +526,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AX1"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AX20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -675,6 +698,63 @@
         <v>49</v>
       </c>
     </row>
+    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="S2" s="2"/>
+    </row>
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="S3" s="2"/>
+    </row>
+    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="S4" s="2"/>
+    </row>
+    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="S5" s="2"/>
+    </row>
+    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="S6" s="2"/>
+    </row>
+    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="S7" s="2"/>
+    </row>
+    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="S8" s="2"/>
+    </row>
+    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="S9" s="2"/>
+    </row>
+    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="S10" s="2"/>
+    </row>
+    <row r="11" spans="1:50" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="S11" s="3"/>
+    </row>
+    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="S12" s="2"/>
+    </row>
+    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="S13" s="2"/>
+    </row>
+    <row r="14" spans="1:50" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="S14" s="3"/>
+    </row>
+    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="S15" s="2"/>
+    </row>
+    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="S16" s="2"/>
+    </row>
+    <row r="17" spans="19:19" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="S17" s="3"/>
+    </row>
+    <row r="18" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S18" s="2"/>
+    </row>
+    <row r="19" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S19" s="2"/>
+    </row>
+    <row r="20" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S20" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Zero all out; replace deprecated delete sheet call with correct one from openpyxl
</commit_message>
<xml_diff>
--- a/books_spreadsheet_out.xlsx
+++ b/books_spreadsheet_out.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\My Documents\Greg Documents\Programming\Python 3\fantasy_books_workspace\fantasy_books\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3333EF38-6D6B-4D59-B894-5F697ED87C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99438C2E-33D3-49C2-97A2-416E9075E47A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -580,8 +580,8 @@
     <col min="41" max="48" width="9.140625" style="1" customWidth="1"/>
     <col min="49" max="49" width="37.140625" style="1" customWidth="1"/>
     <col min="50" max="50" width="18.140625" style="1" customWidth="1"/>
-    <col min="51" max="59" width="9.140625" style="1" customWidth="1"/>
-    <col min="60" max="16384" width="9.140625" style="1"/>
+    <col min="51" max="60" width="9.140625" style="1" customWidth="1"/>
+    <col min="61" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.25">

</xml_diff>